<commit_message>
Finished reworking all classes with their level 2 Talents, based on the new Exhaust-based systems. Started work on Level 4 talents. Got a lot of ideas done in Ideas.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="307">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -134,7 +134,13 @@
     <t>Heal</t>
   </si>
   <si>
-    <t>Save or half (50% chance)</t>
+    <t>Save or half (50% chance) (+35%)</t>
+  </si>
+  <si>
+    <t>Pet Attack</t>
+  </si>
+  <si>
+    <t>Pet Attack (Unique)</t>
   </si>
   <si>
     <t>Crowd Control</t>
@@ -206,6 +212,15 @@
     <t>Silence + 1</t>
   </si>
   <si>
+    <t>Talent</t>
+  </si>
+  <si>
+    <t>Snare + 0.75 Damage</t>
+  </si>
+  <si>
+    <t>Stun + 0.3 Damage</t>
+  </si>
+  <si>
     <t>Monster Stats By Rating</t>
   </si>
   <si>
@@ -299,16 +314,7 @@
     <t>1d12 + 2</t>
   </si>
   <si>
-    <t xml:space="preserve">1d8 + </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3d8 + </t>
-  </si>
-  <si>
-    <t>2d8 + 3</t>
-  </si>
-  <si>
-    <t>2d6 + 7</t>
+    <t>1d6 + 3</t>
   </si>
   <si>
     <t>XP Rules</t>
@@ -320,6 +326,9 @@
 equivalent.</t>
   </si>
   <si>
+    <t>1d6 + 2</t>
+  </si>
+  <si>
     <t>Level</t>
   </si>
   <si>
@@ -329,13 +338,45 @@
     <t>Bonuses</t>
   </si>
   <si>
-    <t>+1 Damage</t>
-  </si>
-  <si>
-    <t>+1 Stat</t>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>Talent (1)</t>
+  </si>
+  <si>
+    <t>4.5 + 3 = 7</t>
+  </si>
+  <si>
+    <t>+1 Stat
++1 Feat
++1 Training Point</t>
+  </si>
+  <si>
+    <t>10 + 3 = 13</t>
+  </si>
+  <si>
+    <t>Talent (2)</t>
+  </si>
+  <si>
+    <t>10 = 10</t>
   </si>
   <si>
     <t>Action Surge</t>
+  </si>
+  <si>
+    <t>Talent (3)</t>
+  </si>
+  <si>
+    <t>4.5 + 3 = 7 + 7 = 14</t>
+  </si>
+  <si>
+    <t>Talent (4)</t>
+  </si>
+  <si>
+    <t>Talent (1, 2 or 3)</t>
+  </si>
+  <si>
+    <t>Talent (5)</t>
   </si>
   <si>
     <t>XP Reward per Difficulty</t>
@@ -907,10 +948,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1092,11 +1133,95 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1108,8 +1233,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1123,29 +1263,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1154,83 +1271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1251,7 +1292,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,55 +1454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,115 +1466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1625,6 +1666,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1634,11 +1714,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1658,56 +1744,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1716,7 +1757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1734,134 +1775,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="20" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2078,12 +2119,42 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2120,15 +2191,30 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2147,40 +2233,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2195,9 +2251,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2248,6 +2301,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2576,20 +2632,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:N107"/>
+  <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7333333333333" customWidth="1"/>
-    <col min="2" max="2" width="17.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="19.752380952381" customWidth="1"/>
     <col min="3" max="3" width="24.4666666666667" customWidth="1"/>
     <col min="4" max="4" width="25.9619047619048" customWidth="1"/>
     <col min="5" max="5" width="30.8" customWidth="1"/>
-    <col min="6" max="6" width="26.0857142857143" customWidth="1"/>
+    <col min="6" max="6" width="33.5428571428571" customWidth="1"/>
     <col min="7" max="7" width="27.952380952381" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="10" width="17.4285714285714" customWidth="1"/>
@@ -2611,13 +2667,13 @@
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
-      <c r="L3" s="73" t="s">
+      <c r="L3" s="77" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="73"/>
+      <c r="N3" s="77"/>
     </row>
     <row r="4" ht="15.75" spans="2:14">
       <c r="B4" s="29" t="s">
@@ -2632,13 +2688,13 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="L4" s="73" t="s">
+      <c r="L4" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="73"/>
+      <c r="N4" s="77"/>
     </row>
     <row r="5" ht="15.75" spans="2:14">
       <c r="B5" s="32" t="s">
@@ -2653,7 +2709,7 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="33"/>
-      <c r="L5" s="73" t="s">
+      <c r="L5" s="77" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="68" t="s">
@@ -2672,7 +2728,7 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="L6" s="73" t="s">
+      <c r="L6" s="77" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="68" t="s">
@@ -2684,7 +2740,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="113" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="68" t="s">
@@ -2700,11 +2756,11 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="108" t="s">
+      <c r="L8" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="108"/>
-      <c r="N8" s="73"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="41" t="s">
@@ -2736,13 +2792,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="123" t="s">
+      <c r="A10" s="127" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="124" t="s">
+      <c r="C10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -2754,24 +2810,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="124" t="s">
+      <c r="G10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="109">
+      <c r="I10" s="114">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="127" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -2783,24 +2839,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="124" t="s">
+      <c r="G11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="109">
+      <c r="I11" s="114">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="125" t="s">
+      <c r="A12" s="129" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="126" t="s">
+      <c r="C12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -2812,13 +2868,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="126" t="s">
+      <c r="G12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="110">
+      <c r="I12" s="115">
         <v>11.5</v>
       </c>
     </row>
@@ -2898,7 +2954,7 @@
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="66"/>
-      <c r="K18" s="73"/>
+      <c r="K18" s="77"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">
       <c r="A19" s="61">
@@ -2921,7 +2977,7 @@
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="68"/>
-      <c r="K19" s="73"/>
+      <c r="K19" s="77"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
       <c r="A20" s="61">
@@ -2944,7 +3000,7 @@
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="66"/>
-      <c r="K20" s="73"/>
+      <c r="K20" s="77"/>
     </row>
     <row r="21" ht="15.75" spans="1:11">
       <c r="A21" s="61">
@@ -2967,7 +3023,7 @@
       </c>
       <c r="G21" s="47"/>
       <c r="H21" s="68"/>
-      <c r="K21" s="73"/>
+      <c r="K21" s="77"/>
     </row>
     <row r="22" ht="16.5" spans="1:11">
       <c r="A22" s="69">
@@ -2990,561 +3046,535 @@
       </c>
       <c r="G22" s="47"/>
       <c r="H22" s="68"/>
-      <c r="K22" s="73"/>
-    </row>
-    <row r="23" ht="16.5" spans="1:11">
-      <c r="A23" s="72"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-    </row>
-    <row r="24" ht="15.75" spans="1:12">
-      <c r="A24" s="74"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="75" t="s">
+      <c r="K22" s="77"/>
+    </row>
+    <row r="23" ht="15.75" spans="1:11">
+      <c r="A23" s="72">
+        <v>1</v>
+      </c>
+      <c r="B23" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="112"/>
-    </row>
-    <row r="25" ht="16.5" spans="1:12">
-      <c r="A25" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="78" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="79" t="s">
+      <c r="C23" s="74">
+        <v>6</v>
+      </c>
+      <c r="D23" s="73">
+        <v>2</v>
+      </c>
+      <c r="E23" s="75"/>
+      <c r="F23" s="76">
+        <v>3</v>
+      </c>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+    </row>
+    <row r="24" ht="16.5" spans="1:11">
+      <c r="A24" s="78">
+        <v>1</v>
+      </c>
+      <c r="B24" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="114"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="46">
-        <v>0</v>
-      </c>
-      <c r="B26" s="47">
-        <v>0</v>
-      </c>
-      <c r="C26" s="81" t="s">
+      <c r="C24" s="80">
+        <v>8</v>
+      </c>
+      <c r="D24" s="79">
+        <v>4</v>
+      </c>
+      <c r="E24" s="81"/>
+      <c r="F24" s="82">
+        <v>5.5</v>
+      </c>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+    </row>
+    <row r="25" ht="16.5" spans="1:11">
+      <c r="A25" s="83"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+    </row>
+    <row r="26" ht="15.75" spans="1:12">
+      <c r="A26" s="84"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="82"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="111"/>
+      <c r="J26" s="110"/>
       <c r="K26" s="64"/>
-      <c r="L26" s="112"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="B27" s="47">
-        <v>0</v>
-      </c>
-      <c r="C27" s="83" t="s">
+      <c r="L26" s="116"/>
+    </row>
+    <row r="27" ht="16.5" spans="1:12">
+      <c r="A27" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="112"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="47">
         <v>0</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="84" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="84"/>
-      <c r="J28" s="115"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="110"/>
       <c r="K28" s="64"/>
-      <c r="L28" s="112"/>
+      <c r="L28" s="116"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="B29" s="47">
         <v>0</v>
       </c>
-      <c r="B29" s="47">
-        <v>1</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="47" t="s">
-        <v>51</v>
-      </c>
+      <c r="C29" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
       <c r="J29" s="48"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="112"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="116"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
+        <v>1</v>
+      </c>
+      <c r="B30" s="47">
+        <v>0</v>
+      </c>
+      <c r="C30" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="95" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="94"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="116"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="46">
+        <v>0</v>
+      </c>
+      <c r="B31" s="47">
+        <v>1</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="47"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="116"/>
+      <c r="L31" s="116"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="46">
         <v>0.5</v>
       </c>
-      <c r="B30" s="47">
+      <c r="B32" s="47">
         <v>1</v>
       </c>
-      <c r="C30" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="47" t="s">
+      <c r="C32" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="120"/>
+      <c r="K32" s="116"/>
+      <c r="L32" s="116"/>
+    </row>
+    <row r="33" ht="15.75" spans="1:12">
+      <c r="A33" s="51">
+        <v>1</v>
+      </c>
+      <c r="B33" s="52">
+        <v>1</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="116"/>
+      <c r="L33" s="116"/>
+    </row>
+    <row r="34" ht="15.75" spans="1:14">
+      <c r="A34" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="97">
+        <v>1</v>
+      </c>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+    </row>
+    <row r="35" ht="15.75" spans="1:11">
+      <c r="A35" s="99">
+        <v>1</v>
+      </c>
+      <c r="B35" s="100" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="116"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="112"/>
-    </row>
-    <row r="31" ht="15.75" spans="1:12">
-      <c r="A31" s="51">
+      <c r="D35" s="101"/>
+      <c r="E35" s="101"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="68"/>
+    </row>
+    <row r="36" ht="16.5" spans="1:11">
+      <c r="A36" s="69">
         <v>1</v>
       </c>
-      <c r="B31" s="52">
-        <v>1</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="H31" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="K31" s="112"/>
-      <c r="L31" s="112"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="47"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-    </row>
-    <row r="33" ht="16.5" spans="1:11">
-      <c r="A33" s="68"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="68"/>
-    </row>
-    <row r="34" ht="16.5" spans="1:11">
-      <c r="A34" s="68"/>
-      <c r="C34" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="88"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="68"/>
-    </row>
-    <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="72"/>
-      <c r="B35" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="58" t="s">
+      <c r="B36" s="102" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D36" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="88" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="H35" s="90">
-        <v>20</v>
-      </c>
-      <c r="I35" s="127" t="s">
-        <v>71</v>
-      </c>
-      <c r="J35" s="117"/>
-      <c r="K35" s="117"/>
-    </row>
-    <row r="36" ht="15.75" spans="1:11">
-      <c r="A36" s="72"/>
-      <c r="B36" s="46">
-        <v>25</v>
-      </c>
-      <c r="C36" s="64">
-        <v>6</v>
-      </c>
-      <c r="D36" s="64">
-        <v>4</v>
-      </c>
-      <c r="E36" s="64">
-        <v>1.5</v>
-      </c>
-      <c r="F36" s="91">
-        <v>12</v>
-      </c>
-      <c r="G36" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="H36" s="68">
-        <v>4</v>
-      </c>
-      <c r="I36" s="128" t="s">
-        <v>73</v>
-      </c>
-      <c r="J36" s="47"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="53"/>
       <c r="K36" s="68"/>
     </row>
     <row r="37" ht="15.75" spans="1:11">
-      <c r="A37" s="72"/>
-      <c r="B37" s="46">
-        <v>50</v>
-      </c>
-      <c r="C37" s="64">
-        <v>12</v>
-      </c>
-      <c r="D37" s="64">
-        <v>4</v>
-      </c>
-      <c r="E37" s="64">
-        <v>2.5</v>
-      </c>
-      <c r="F37" s="91">
-        <v>12</v>
-      </c>
-      <c r="G37" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="H37" s="68">
-        <v>10</v>
-      </c>
-      <c r="I37" s="68"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="47"/>
       <c r="J37" s="47"/>
       <c r="K37" s="68"/>
     </row>
-    <row r="38" ht="15.75" spans="1:11">
-      <c r="A38" s="72"/>
-      <c r="B38" s="46">
-        <v>75</v>
-      </c>
-      <c r="C38" s="64">
-        <v>18</v>
-      </c>
-      <c r="D38" s="64">
-        <v>4</v>
-      </c>
-      <c r="E38" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="91">
-        <v>12</v>
-      </c>
-      <c r="G38" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="68">
-        <v>12</v>
-      </c>
-      <c r="I38" s="68"/>
+    <row r="38" ht="16.5" spans="1:11">
+      <c r="A38" s="68"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="47"/>
       <c r="J38" s="47"/>
       <c r="K38" s="68"/>
     </row>
-    <row r="39" ht="15.75" spans="1:11">
-      <c r="A39" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="92">
-        <v>100</v>
-      </c>
-      <c r="C39" s="64">
-        <v>24</v>
-      </c>
-      <c r="D39" s="64">
-        <v>4</v>
-      </c>
-      <c r="E39" s="86">
-        <v>4.5</v>
-      </c>
-      <c r="F39" s="91">
-        <v>12</v>
-      </c>
-      <c r="G39" s="68"/>
+    <row r="39" ht="16.5" spans="1:11">
+      <c r="A39" s="68"/>
+      <c r="C39" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="100"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68" t="s">
+        <v>69</v>
+      </c>
       <c r="H39" s="68"/>
-      <c r="I39" s="47"/>
+      <c r="I39" s="68"/>
       <c r="J39" s="47"/>
       <c r="K39" s="68"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
-      <c r="A40" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="93">
-        <v>125</v>
-      </c>
-      <c r="C40" s="64">
-        <v>28</v>
-      </c>
-      <c r="D40" s="64">
-        <v>4</v>
-      </c>
-      <c r="E40" s="86" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="91">
-        <v>12</v>
-      </c>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="68"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="84" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" s="105">
+        <v>20</v>
+      </c>
+      <c r="I40" s="131" t="s">
+        <v>76</v>
+      </c>
+      <c r="J40" s="121"/>
+      <c r="K40" s="121"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
-      <c r="A41" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="93">
-        <v>150</v>
+      <c r="A41" s="83"/>
+      <c r="B41" s="46">
+        <v>25</v>
       </c>
       <c r="C41" s="64">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D41" s="64">
         <v>4</v>
       </c>
-      <c r="E41" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="91">
+      <c r="E41" s="64">
+        <v>1.5</v>
+      </c>
+      <c r="F41" s="106">
         <v>12</v>
       </c>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="47"/>
+      <c r="G41" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="68">
+        <v>4</v>
+      </c>
+      <c r="I41" s="132" t="s">
+        <v>78</v>
+      </c>
       <c r="J41" s="47"/>
       <c r="K41" s="68"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
-      <c r="A42" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="93">
-        <v>175</v>
+      <c r="A42" s="83"/>
+      <c r="B42" s="46">
+        <v>50</v>
       </c>
       <c r="C42" s="64">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D42" s="64">
         <v>4</v>
       </c>
-      <c r="E42" s="86" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="91">
+      <c r="E42" s="64">
+        <v>2.5</v>
+      </c>
+      <c r="F42" s="106">
         <v>12</v>
       </c>
-      <c r="G42" s="68"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
+      <c r="G42" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" s="68">
+        <v>10</v>
+      </c>
+      <c r="I42" s="68"/>
       <c r="J42" s="47"/>
       <c r="K42" s="68"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="93">
-        <v>200</v>
+      <c r="A43" s="83"/>
+      <c r="B43" s="46">
+        <v>75</v>
       </c>
       <c r="C43" s="64">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D43" s="64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="91">
-        <v>13</v>
+        <v>80</v>
+      </c>
+      <c r="F43" s="106">
+        <v>12</v>
       </c>
       <c r="G43" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
+        <v>81</v>
+      </c>
+      <c r="H43" s="68">
+        <v>12</v>
+      </c>
+      <c r="I43" s="68"/>
       <c r="J43" s="47"/>
       <c r="K43" s="68"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
-      <c r="A44" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="92">
-        <v>225</v>
+      <c r="A44" s="83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="107">
+        <v>100</v>
       </c>
       <c r="C44" s="64">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D44" s="64">
-        <v>5</v>
-      </c>
-      <c r="E44" s="64">
-        <v>8.25</v>
-      </c>
-      <c r="F44" s="91">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="E44" s="103">
+        <v>4.5</v>
+      </c>
+      <c r="F44" s="106">
+        <v>12</v>
       </c>
       <c r="G44" s="68"/>
-      <c r="H44" s="47"/>
+      <c r="H44" s="68"/>
       <c r="I44" s="47"/>
       <c r="J44" s="47"/>
       <c r="K44" s="68"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
-      <c r="A45" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="46">
-        <v>250</v>
-      </c>
-      <c r="C45" s="47">
-        <v>58</v>
-      </c>
-      <c r="D45" s="47">
-        <v>5</v>
-      </c>
-      <c r="E45" s="47">
-        <v>9</v>
-      </c>
-      <c r="F45" s="48">
-        <v>13</v>
-      </c>
-      <c r="G45" s="86"/>
-      <c r="H45" s="47"/>
+      <c r="A45" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="108">
+        <v>125</v>
+      </c>
+      <c r="C45" s="64">
+        <v>28</v>
+      </c>
+      <c r="D45" s="64">
+        <v>4</v>
+      </c>
+      <c r="E45" s="103" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="106">
+        <v>12</v>
+      </c>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
       <c r="I45" s="47"/>
       <c r="J45" s="47"/>
       <c r="K45" s="68"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
-      <c r="A46" s="72" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="46">
-        <v>275</v>
-      </c>
-      <c r="C46" s="47">
-        <v>66</v>
-      </c>
-      <c r="D46" s="47">
-        <v>5</v>
-      </c>
-      <c r="E46" s="47">
-        <v>9.5</v>
-      </c>
-      <c r="F46" s="48">
-        <v>13</v>
+      <c r="A46" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="108">
+        <v>150</v>
+      </c>
+      <c r="C46" s="64">
+        <v>32</v>
+      </c>
+      <c r="D46" s="64">
+        <v>4</v>
+      </c>
+      <c r="E46" s="103" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="106">
+        <v>12</v>
       </c>
       <c r="G46" s="68"/>
       <c r="H46" s="68"/>
@@ -3552,261 +3582,334 @@
       <c r="J46" s="47"/>
       <c r="K46" s="68"/>
     </row>
-    <row r="47" ht="15.75" spans="1:13">
-      <c r="A47" s="72" t="s">
+    <row r="47" ht="15.75" spans="1:11">
+      <c r="A47" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="108">
+        <v>175</v>
+      </c>
+      <c r="C47" s="64">
+        <v>36</v>
+      </c>
+      <c r="D47" s="64">
+        <v>4</v>
+      </c>
+      <c r="E47" s="103" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="106">
+        <v>12</v>
+      </c>
+      <c r="G47" s="68"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="68"/>
+    </row>
+    <row r="48" ht="15.75" spans="1:11">
+      <c r="A48" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="108">
+        <v>200</v>
+      </c>
+      <c r="C48" s="64">
+        <v>42</v>
+      </c>
+      <c r="D48" s="64">
+        <v>5</v>
+      </c>
+      <c r="E48" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="46">
-        <v>300</v>
-      </c>
-      <c r="C47" s="47">
-        <v>73</v>
-      </c>
-      <c r="D47" s="47">
-        <v>5</v>
-      </c>
-      <c r="E47" s="47">
-        <v>10</v>
-      </c>
-      <c r="F47" s="48">
-        <v>14</v>
-      </c>
-      <c r="G47" s="47">
+      <c r="F48" s="106">
         <v>13</v>
       </c>
-      <c r="H47" s="68"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="73"/>
-      <c r="K47" s="73"/>
-      <c r="M47" s="68"/>
-    </row>
-    <row r="48" ht="16.5" spans="1:13">
-      <c r="A48" s="72" t="s">
+      <c r="G48" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="51">
-        <v>325</v>
-      </c>
-      <c r="C48" s="52">
-        <v>85</v>
-      </c>
-      <c r="D48" s="52">
-        <v>5</v>
-      </c>
-      <c r="E48" s="52">
-        <v>10.75</v>
-      </c>
-      <c r="F48" s="53">
-        <v>14</v>
-      </c>
-      <c r="G48" s="47"/>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
-      <c r="M48" s="68"/>
-    </row>
-    <row r="49" ht="15.75" spans="2:13">
-      <c r="B49" s="94">
-        <v>350</v>
-      </c>
-      <c r="C49" s="95">
-        <v>61</v>
-      </c>
-      <c r="D49" s="96">
+      <c r="J48" s="47"/>
+      <c r="K48" s="68"/>
+    </row>
+    <row r="49" ht="15.75" spans="1:11">
+      <c r="A49" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="107">
+        <v>225</v>
+      </c>
+      <c r="C49" s="64">
+        <v>50</v>
+      </c>
+      <c r="D49" s="64">
         <v>5</v>
       </c>
-      <c r="E49" s="96">
-        <v>11.5</v>
-      </c>
-      <c r="F49" s="97">
-        <v>14</v>
-      </c>
-      <c r="G49" s="47"/>
+      <c r="E49" s="64">
+        <v>8.25</v>
+      </c>
+      <c r="F49" s="106">
+        <v>13</v>
+      </c>
+      <c r="G49" s="68"/>
       <c r="H49" s="47"/>
       <c r="I49" s="47"/>
-      <c r="M49" s="68"/>
-    </row>
-    <row r="50" ht="15.75" spans="2:9">
-      <c r="B50" s="92">
-        <v>375</v>
-      </c>
-      <c r="C50" s="98">
-        <v>66</v>
-      </c>
-      <c r="D50" s="99">
+      <c r="J49" s="47"/>
+      <c r="K49" s="68"/>
+    </row>
+    <row r="50" ht="15.75" spans="1:11">
+      <c r="A50" s="83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="46">
+        <v>250</v>
+      </c>
+      <c r="C50" s="47">
+        <v>58</v>
+      </c>
+      <c r="D50" s="47">
         <v>5</v>
       </c>
       <c r="E50" s="47">
-        <v>12.25</v>
-      </c>
-      <c r="F50" s="100">
-        <v>14</v>
-      </c>
-      <c r="G50" s="47"/>
+        <v>9</v>
+      </c>
+      <c r="F50" s="48">
+        <v>13</v>
+      </c>
+      <c r="G50" s="103"/>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
-    </row>
-    <row r="51" spans="2:9">
+      <c r="J50" s="47"/>
+      <c r="K50" s="68"/>
+    </row>
+    <row r="51" ht="15.75" spans="1:11">
+      <c r="A51" s="83" t="s">
+        <v>94</v>
+      </c>
       <c r="B51" s="46">
-        <v>400</v>
-      </c>
-      <c r="C51" s="98">
-        <v>71</v>
-      </c>
-      <c r="D51" s="64">
+        <v>275</v>
+      </c>
+      <c r="C51" s="47">
+        <v>66</v>
+      </c>
+      <c r="D51" s="47">
         <v>5</v>
       </c>
       <c r="E51" s="47">
+        <v>9.5</v>
+      </c>
+      <c r="F51" s="48">
         <v>13</v>
       </c>
-      <c r="F51" s="100">
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="68"/>
+    </row>
+    <row r="52" ht="15.75" spans="1:13">
+      <c r="A52" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="46">
+        <v>300</v>
+      </c>
+      <c r="C52" s="47">
+        <v>73</v>
+      </c>
+      <c r="D52" s="47">
+        <v>5</v>
+      </c>
+      <c r="E52" s="47">
+        <v>10</v>
+      </c>
+      <c r="F52" s="48">
         <v>14</v>
       </c>
-      <c r="G51" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-    </row>
-    <row r="52" spans="2:9">
-      <c r="B52" s="46">
-        <v>425</v>
-      </c>
-      <c r="C52" s="98">
-        <v>78</v>
-      </c>
-      <c r="D52" s="101">
+      <c r="G52" s="47">
+        <v>13</v>
+      </c>
+      <c r="H52" s="68"/>
+      <c r="I52" s="68"/>
+      <c r="J52" s="77"/>
+      <c r="K52" s="77"/>
+      <c r="M52" s="68"/>
+    </row>
+    <row r="53" ht="16.5" spans="1:13">
+      <c r="A53" s="83" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="51">
+        <v>325</v>
+      </c>
+      <c r="C53" s="52">
+        <v>85</v>
+      </c>
+      <c r="D53" s="52">
         <v>5</v>
       </c>
-      <c r="E52" s="47">
-        <v>13.5</v>
-      </c>
-      <c r="F52" s="100">
-        <v>14</v>
-      </c>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-    </row>
-    <row r="53" spans="2:9">
-      <c r="B53" s="46">
-        <v>450</v>
-      </c>
-      <c r="C53" s="98">
-        <v>85</v>
-      </c>
-      <c r="D53" s="101">
-        <v>5</v>
-      </c>
-      <c r="E53" s="47">
-        <v>14</v>
-      </c>
-      <c r="F53" s="100">
+      <c r="E53" s="52">
+        <v>10.75</v>
+      </c>
+      <c r="F53" s="53">
         <v>14</v>
       </c>
       <c r="G53" s="47"/>
       <c r="H53" s="47"/>
       <c r="I53" s="47"/>
-    </row>
-    <row r="54" spans="2:9">
-      <c r="B54" s="93">
-        <v>475</v>
-      </c>
-      <c r="C54" s="98">
-        <v>92</v>
-      </c>
-      <c r="D54" s="64">
+      <c r="M53" s="68"/>
+    </row>
+    <row r="54" ht="15.75" spans="2:13">
+      <c r="B54" s="109">
+        <v>350</v>
+      </c>
+      <c r="C54" s="58">
+        <v>61</v>
+      </c>
+      <c r="D54" s="58">
         <v>5</v>
       </c>
-      <c r="E54" s="47">
-        <v>14.5</v>
-      </c>
-      <c r="F54" s="100">
+      <c r="E54" s="58">
+        <v>11.5</v>
+      </c>
+      <c r="F54" s="110">
         <v>14</v>
       </c>
-      <c r="G54" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="G54" s="47"/>
       <c r="H54" s="47"/>
       <c r="I54" s="47"/>
-    </row>
-    <row r="55" ht="16.5" spans="2:9">
-      <c r="B55" s="102">
-        <v>500</v>
-      </c>
-      <c r="C55" s="103">
-        <v>99</v>
-      </c>
-      <c r="D55" s="104">
+      <c r="M54" s="68"/>
+    </row>
+    <row r="55" ht="15.75" spans="2:9">
+      <c r="B55" s="107">
+        <v>375</v>
+      </c>
+      <c r="C55" s="47">
+        <v>66</v>
+      </c>
+      <c r="D55" s="64">
         <v>5</v>
       </c>
-      <c r="E55" s="105">
-        <v>15.25</v>
-      </c>
-      <c r="F55" s="106">
+      <c r="E55" s="47">
+        <v>12.25</v>
+      </c>
+      <c r="F55" s="48">
         <v>14</v>
       </c>
       <c r="G55" s="47"/>
       <c r="H55" s="47"/>
       <c r="I55" s="47"/>
     </row>
-    <row r="56" spans="5:9">
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
+    <row r="56" spans="2:9">
+      <c r="B56" s="46">
+        <v>400</v>
+      </c>
+      <c r="C56" s="47">
+        <v>71</v>
+      </c>
+      <c r="D56" s="64">
+        <v>5</v>
+      </c>
+      <c r="E56" s="47">
+        <v>13</v>
+      </c>
+      <c r="F56" s="48">
+        <v>14</v>
+      </c>
+      <c r="G56" s="47" t="s">
+        <v>97</v>
+      </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
     </row>
-    <row r="57" spans="5:9">
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
+    <row r="57" spans="2:9">
+      <c r="B57" s="46">
+        <v>425</v>
+      </c>
+      <c r="C57" s="47">
+        <v>78</v>
+      </c>
+      <c r="D57" s="64">
+        <v>5</v>
+      </c>
+      <c r="E57" s="47">
+        <v>13.5</v>
+      </c>
+      <c r="F57" s="48">
+        <v>14</v>
+      </c>
       <c r="G57" s="47"/>
       <c r="H57" s="47"/>
       <c r="I57" s="47"/>
     </row>
-    <row r="58" spans="5:9">
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47" t="s">
-        <v>94</v>
-      </c>
+    <row r="58" spans="2:9">
+      <c r="B58" s="46">
+        <v>450</v>
+      </c>
+      <c r="C58" s="47">
+        <v>85</v>
+      </c>
+      <c r="D58" s="64">
+        <v>5</v>
+      </c>
+      <c r="E58" s="47">
+        <v>14</v>
+      </c>
+      <c r="F58" s="48">
+        <v>14</v>
+      </c>
+      <c r="G58" s="47"/>
       <c r="H58" s="47"/>
       <c r="I58" s="47"/>
     </row>
-    <row r="59" spans="3:9">
-      <c r="C59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59">
-        <v>15.5</v>
+    <row r="59" spans="2:9">
+      <c r="B59" s="108">
+        <v>475</v>
+      </c>
+      <c r="C59" s="47">
+        <v>92</v>
+      </c>
+      <c r="D59" s="64">
+        <v>5</v>
       </c>
       <c r="E59" s="47">
-        <v>12.25</v>
-      </c>
-      <c r="F59" s="107"/>
-      <c r="G59" s="47"/>
+        <v>14.5</v>
+      </c>
+      <c r="F59" s="48">
+        <v>14</v>
+      </c>
+      <c r="G59" s="47" t="s">
+        <v>98</v>
+      </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
     </row>
-    <row r="60" spans="4:9">
-      <c r="D60">
+    <row r="60" ht="16.5" spans="2:9">
+      <c r="B60" s="111">
+        <v>500</v>
+      </c>
+      <c r="C60" s="52">
+        <v>99</v>
+      </c>
+      <c r="D60" s="52">
+        <v>5</v>
+      </c>
+      <c r="E60" s="52">
+        <v>15.25</v>
+      </c>
+      <c r="F60" s="53">
         <v>14</v>
       </c>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
       <c r="G60" s="47"/>
       <c r="H60" s="47"/>
       <c r="I60" s="47"/>
     </row>
     <row r="61" spans="5:9">
-      <c r="E61" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="G61" s="47">
-        <v>12.25</v>
-      </c>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
       <c r="H61" s="47"/>
       <c r="I61" s="47"/>
     </row>
@@ -3820,24 +3923,27 @@
     <row r="63" spans="5:9">
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
+      <c r="G63" s="47">
+        <v>13.5</v>
+      </c>
       <c r="H63" s="47"/>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="3:9">
-      <c r="C64" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
+    <row r="64" spans="4:9">
+      <c r="D64">
+        <v>13</v>
+      </c>
+      <c r="E64" s="47">
+        <v>10</v>
+      </c>
+      <c r="F64" s="112" t="s">
+        <v>99</v>
+      </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
       <c r="I64" s="47"/>
     </row>
-    <row r="65" ht="102" customHeight="1" spans="3:9">
-      <c r="C65" s="118" t="s">
-        <v>99</v>
-      </c>
+    <row r="65" spans="5:9">
       <c r="E65" s="47"/>
       <c r="F65" s="47"/>
       <c r="G65" s="47"/>
@@ -3851,149 +3957,90 @@
       <c r="H66" s="47"/>
       <c r="I66" s="47"/>
     </row>
-    <row r="67" ht="15.75" spans="1:14">
-      <c r="A67" s="119"/>
-      <c r="B67" s="89"/>
-      <c r="C67" s="120"/>
-      <c r="D67" s="120"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="68"/>
-      <c r="K67" s="68"/>
-      <c r="M67" s="47"/>
-      <c r="N67" s="47"/>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="A68" s="47"/>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
+    <row r="67" spans="5:9">
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+    </row>
+    <row r="68" spans="5:9">
       <c r="E68" s="47"/>
       <c r="F68" s="47"/>
       <c r="G68" s="47"/>
       <c r="H68" s="47"/>
       <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-      <c r="K68" s="47"/>
-      <c r="M68" s="47"/>
-      <c r="N68" s="47"/>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="A69" s="47"/>
-      <c r="B69" s="47" t="s">
+    </row>
+    <row r="69" spans="3:9">
+      <c r="C69" s="47" t="s">
         <v>100</v>
-      </c>
-      <c r="C69" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D69" s="47" t="s">
-        <v>102</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
       <c r="G69" s="47"/>
       <c r="H69" s="47"/>
       <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="47"/>
-      <c r="M69" s="47"/>
-      <c r="N69" s="47"/>
-    </row>
-    <row r="70" spans="1:14">
-      <c r="A70" s="47"/>
-      <c r="B70" s="47">
-        <v>1</v>
-      </c>
-      <c r="C70" s="47">
-        <v>20</v>
-      </c>
-      <c r="D70" s="47"/>
+    </row>
+    <row r="70" ht="102" customHeight="1" spans="3:9">
+      <c r="C70" s="122" t="s">
+        <v>101</v>
+      </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
       <c r="G70" s="47"/>
       <c r="H70" s="47"/>
       <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="47"/>
-      <c r="L70" s="47"/>
-      <c r="M70" s="47"/>
-      <c r="N70" s="47"/>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="A71" s="47"/>
-      <c r="B71" s="47">
-        <v>2</v>
-      </c>
-      <c r="C71" s="47">
-        <v>25</v>
-      </c>
-      <c r="D71" s="47"/>
+    </row>
+    <row r="71" spans="5:9">
       <c r="E71" s="47"/>
       <c r="F71" s="47"/>
       <c r="G71" s="47"/>
       <c r="H71" s="47"/>
       <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="47"/>
-      <c r="L71" s="47"/>
-      <c r="M71" s="47"/>
-      <c r="N71" s="47"/>
-    </row>
-    <row r="72" spans="1:14">
-      <c r="A72" s="47"/>
-      <c r="B72" s="47">
-        <v>3</v>
-      </c>
-      <c r="C72" s="47">
-        <v>30</v>
-      </c>
-      <c r="D72" s="124" t="s">
-        <v>103</v>
-      </c>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="47"/>
-      <c r="J72" s="47"/>
-      <c r="K72" s="47"/>
+    </row>
+    <row r="72" ht="15.75" spans="1:14">
+      <c r="A72" s="123"/>
+      <c r="B72" s="104"/>
+      <c r="C72" s="124"/>
+      <c r="D72" s="124"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="68"/>
+      <c r="K72" s="68"/>
       <c r="M72" s="47"/>
       <c r="N72" s="47"/>
     </row>
-    <row r="73" ht="15.75" spans="1:14">
-      <c r="A73" s="119"/>
-      <c r="B73" s="47">
-        <v>4</v>
-      </c>
-      <c r="C73" s="47">
-        <v>35</v>
-      </c>
-      <c r="D73" s="124" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="121"/>
-      <c r="F73" s="121"/>
-      <c r="G73" s="121"/>
-      <c r="H73" s="121"/>
-      <c r="I73" s="121"/>
-      <c r="J73" s="121"/>
-      <c r="K73" s="121"/>
-      <c r="L73" s="121"/>
+    <row r="73" spans="1:14">
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
+      <c r="K73" s="47"/>
       <c r="M73" s="47"/>
       <c r="N73" s="47"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
-      <c r="B74" s="47">
-        <v>5</v>
-      </c>
-      <c r="C74" s="47">
-        <v>40</v>
-      </c>
-      <c r="D74" s="47"/>
+      <c r="B74" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D74" s="47" t="s">
+        <v>105</v>
+      </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
       <c r="G74" s="47"/>
@@ -4007,13 +4054,13 @@
     <row r="75" spans="1:14">
       <c r="A75" s="47"/>
       <c r="B75" s="47">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C75" s="47">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4029,15 +4076,21 @@
     <row r="76" spans="1:14">
       <c r="A76" s="47"/>
       <c r="B76" s="47">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C76" s="47">
-        <v>50</v>
-      </c>
-      <c r="D76" s="47"/>
+        <v>25</v>
+      </c>
+      <c r="D76" s="47" t="s">
+        <v>107</v>
+      </c>
       <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
+      <c r="F76" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="G76" s="47">
+        <v>3.5</v>
+      </c>
       <c r="H76" s="47"/>
       <c r="I76" s="47"/>
       <c r="J76" s="47"/>
@@ -4046,51 +4099,66 @@
       <c r="M76" s="47"/>
       <c r="N76" s="47"/>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" ht="45" spans="1:14">
       <c r="A77" s="47"/>
       <c r="B77" s="47">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C77" s="47">
-        <v>55</v>
-      </c>
-      <c r="D77" s="124" t="s">
-        <v>104</v>
+        <v>30</v>
+      </c>
+      <c r="D77" s="133" t="s">
+        <v>109</v>
       </c>
       <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
+      <c r="F77" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G77" s="47">
+        <v>9</v>
+      </c>
       <c r="H77" s="47"/>
       <c r="I77" s="47"/>
       <c r="J77" s="47"/>
       <c r="K77" s="47"/>
-    </row>
-    <row r="78" spans="1:11">
-      <c r="A78" s="47"/>
+      <c r="M77" s="47"/>
+      <c r="N77" s="47"/>
+    </row>
+    <row r="78" ht="15.75" spans="1:14">
+      <c r="A78" s="123"/>
       <c r="B78" s="47">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C78" s="47">
-        <v>60</v>
-      </c>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="47"/>
-      <c r="H78" s="47"/>
-      <c r="I78" s="47"/>
-      <c r="J78" s="47"/>
-      <c r="K78" s="47"/>
-    </row>
-    <row r="79" spans="1:11">
+        <v>35</v>
+      </c>
+      <c r="D78" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" s="125"/>
+      <c r="F78" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G78" s="125"/>
+      <c r="H78" s="125"/>
+      <c r="I78" s="125"/>
+      <c r="J78" s="125"/>
+      <c r="K78" s="125"/>
+      <c r="L78" s="125"/>
+      <c r="M78" s="47"/>
+      <c r="N78" s="47"/>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="47"/>
       <c r="B79" s="47">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" s="47">
-        <v>65</v>
-      </c>
-      <c r="D79" s="47"/>
+        <v>40</v>
+      </c>
+      <c r="D79" s="47" t="s">
+        <v>113</v>
+      </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
       <c r="G79" s="47"/>
@@ -4098,26 +4166,44 @@
       <c r="I79" s="47"/>
       <c r="J79" s="47"/>
       <c r="K79" s="47"/>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="47"/>
-      <c r="B80" s="47"/>
-      <c r="C80" s="47"/>
+      <c r="B80" s="47">
+        <v>6</v>
+      </c>
+      <c r="C80" s="47">
+        <v>45</v>
+      </c>
       <c r="D80" s="47" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
+      <c r="F80" s="47" t="s">
+        <v>115</v>
+      </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
       <c r="I80" s="47"/>
       <c r="J80" s="47"/>
       <c r="K80" s="47"/>
-    </row>
-    <row r="81" spans="2:11">
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="47"/>
+    </row>
+    <row r="81" ht="45" spans="1:14">
+      <c r="A81" s="47"/>
+      <c r="B81" s="47">
+        <v>7</v>
+      </c>
+      <c r="C81" s="47">
+        <v>50</v>
+      </c>
+      <c r="D81" s="133" t="s">
+        <v>109</v>
+      </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
       <c r="G81" s="47"/>
@@ -4125,11 +4211,21 @@
       <c r="I81" s="47"/>
       <c r="J81" s="47"/>
       <c r="K81" s="47"/>
-    </row>
-    <row r="82" spans="2:11">
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
+      <c r="L81" s="47"/>
+      <c r="M81" s="47"/>
+      <c r="N81" s="47"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="47"/>
+      <c r="B82" s="47">
+        <v>8</v>
+      </c>
+      <c r="C82" s="47">
+        <v>55</v>
+      </c>
+      <c r="D82" s="47" t="s">
+        <v>116</v>
+      </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
       <c r="G82" s="47"/>
@@ -4138,10 +4234,17 @@
       <c r="J82" s="47"/>
       <c r="K82" s="47"/>
     </row>
-    <row r="83" spans="2:11">
-      <c r="B83" s="47"/>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
+    <row r="83" spans="1:11">
+      <c r="A83" s="47"/>
+      <c r="B83" s="47">
+        <v>9</v>
+      </c>
+      <c r="C83" s="47">
+        <v>60</v>
+      </c>
+      <c r="D83" s="47" t="s">
+        <v>117</v>
+      </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
       <c r="G83" s="47"/>
@@ -4150,10 +4253,17 @@
       <c r="J83" s="47"/>
       <c r="K83" s="47"/>
     </row>
-    <row r="84" spans="2:11">
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
+    <row r="84" spans="1:11">
+      <c r="A84" s="47"/>
+      <c r="B84" s="47">
+        <v>10</v>
+      </c>
+      <c r="C84" s="47">
+        <v>65</v>
+      </c>
+      <c r="D84" s="47" t="s">
+        <v>118</v>
+      </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
       <c r="G84" s="47"/>
@@ -4162,10 +4272,13 @@
       <c r="J84" s="47"/>
       <c r="K84" s="47"/>
     </row>
-    <row r="85" spans="2:11">
+    <row r="85" spans="1:11">
+      <c r="A85" s="47"/>
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="47" t="s">
+        <v>119</v>
+      </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
       <c r="G85" s="47"/>
@@ -4246,13 +4359,19 @@
       <c r="J91" s="47"/>
       <c r="K91" s="47"/>
     </row>
-    <row r="92" spans="9:11">
+    <row r="92" spans="2:11">
+      <c r="B92" s="47"/>
+      <c r="C92" s="47"/>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="47"/>
+      <c r="G92" s="47"/>
+      <c r="H92" s="47"/>
       <c r="I92" s="47"/>
       <c r="J92" s="47"/>
       <c r="K92" s="47"/>
     </row>
-    <row r="93" spans="1:11">
-      <c r="A93" s="47"/>
+    <row r="93" spans="2:11">
       <c r="B93" s="47"/>
       <c r="C93" s="47"/>
       <c r="D93" s="47"/>
@@ -4264,8 +4383,7 @@
       <c r="J93" s="47"/>
       <c r="K93" s="47"/>
     </row>
-    <row r="94" spans="1:11">
-      <c r="A94" s="47"/>
+    <row r="94" spans="2:11">
       <c r="B94" s="47"/>
       <c r="C94" s="47"/>
       <c r="D94" s="47"/>
@@ -4277,46 +4395,71 @@
       <c r="J94" s="47"/>
       <c r="K94" s="47"/>
     </row>
-    <row r="95" spans="2:6">
+    <row r="95" spans="2:11">
       <c r="B95" s="47"/>
       <c r="C95" s="47"/>
       <c r="D95" s="47"/>
       <c r="E95" s="47"/>
       <c r="F95" s="47"/>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="47"/>
+      <c r="G95" s="47"/>
+      <c r="H95" s="47"/>
+      <c r="I95" s="47"/>
+      <c r="J95" s="47"/>
+      <c r="K95" s="47"/>
+    </row>
+    <row r="96" spans="2:11">
       <c r="B96" s="47"/>
       <c r="C96" s="47"/>
       <c r="D96" s="47"/>
       <c r="E96" s="47"/>
       <c r="F96" s="47"/>
-    </row>
-    <row r="97" spans="3:6">
-      <c r="C97" s="47"/>
-      <c r="D97" s="47"/>
-      <c r="E97" s="47"/>
-      <c r="F97" s="47"/>
-    </row>
-    <row r="98" spans="3:6">
+      <c r="G96" s="47"/>
+      <c r="H96" s="47"/>
+      <c r="I96" s="47"/>
+      <c r="J96" s="47"/>
+      <c r="K96" s="47"/>
+    </row>
+    <row r="97" spans="9:11">
+      <c r="I97" s="47"/>
+      <c r="J97" s="47"/>
+      <c r="K97" s="47"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="47"/>
+      <c r="B98" s="47"/>
       <c r="C98" s="47"/>
       <c r="D98" s="47"/>
-      <c r="E98" s="122"/>
-      <c r="F98" s="122"/>
-    </row>
-    <row r="99" spans="3:6">
+      <c r="E98" s="47"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="47"/>
+      <c r="H98" s="47"/>
+      <c r="I98" s="47"/>
+      <c r="J98" s="47"/>
+      <c r="K98" s="47"/>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="47"/>
+      <c r="B99" s="47"/>
       <c r="C99" s="47"/>
       <c r="D99" s="47"/>
       <c r="E99" s="47"/>
       <c r="F99" s="47"/>
-    </row>
-    <row r="100" spans="3:6">
+      <c r="G99" s="47"/>
+      <c r="H99" s="47"/>
+      <c r="I99" s="47"/>
+      <c r="J99" s="47"/>
+      <c r="K99" s="47"/>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="47"/>
       <c r="C100" s="47"/>
       <c r="D100" s="47"/>
       <c r="E100" s="47"/>
       <c r="F100" s="47"/>
     </row>
-    <row r="101" spans="3:6">
+    <row r="101" spans="1:6">
+      <c r="A101" s="47"/>
+      <c r="B101" s="47"/>
       <c r="C101" s="47"/>
       <c r="D101" s="47"/>
       <c r="E101" s="47"/>
@@ -4331,8 +4474,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="47"/>
-      <c r="F103" s="47"/>
+      <c r="E103" s="126"/>
+      <c r="F103" s="126"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4357,6 +4500,36 @@
       <c r="D107" s="47"/>
       <c r="E107" s="47"/>
       <c r="F107" s="47"/>
+    </row>
+    <row r="108" spans="3:6">
+      <c r="C108" s="47"/>
+      <c r="D108" s="47"/>
+      <c r="E108" s="47"/>
+      <c r="F108" s="47"/>
+    </row>
+    <row r="109" spans="3:6">
+      <c r="C109" s="47"/>
+      <c r="D109" s="47"/>
+      <c r="E109" s="47"/>
+      <c r="F109" s="47"/>
+    </row>
+    <row r="110" spans="3:6">
+      <c r="C110" s="47"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="47"/>
+    </row>
+    <row r="111" spans="3:6">
+      <c r="C111" s="47"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="47"/>
+      <c r="F111" s="47"/>
+    </row>
+    <row r="112" spans="3:6">
+      <c r="C112" s="47"/>
+      <c r="D112" s="47"/>
+      <c r="E112" s="47"/>
+      <c r="F112" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -4368,13 +4541,13 @@
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="D80:G80"/>
-    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="B86:C86"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -4387,7 +4560,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4406,31 +4579,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4438,28 +4611,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4467,28 +4640,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4496,28 +4669,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4525,28 +4698,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4554,28 +4727,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4583,28 +4756,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4612,28 +4785,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4641,28 +4814,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4670,28 +4843,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4699,28 +4872,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4728,28 +4901,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4757,28 +4930,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -4786,33 +4959,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -4844,34 +5017,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -4879,31 +5052,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -4911,31 +5084,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -4943,31 +5116,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -4975,31 +5148,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5007,31 +5180,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5039,31 +5212,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5071,31 +5244,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5103,31 +5276,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5135,31 +5308,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5167,31 +5340,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5199,31 +5372,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5231,31 +5404,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5263,63 +5436,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the react website.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="308">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Save or half (50% chance) (+35%)</t>
+  </si>
+  <si>
+    <t>4d4 + Main Stat</t>
   </si>
   <si>
     <t>Pet Attack</t>
@@ -948,10 +951,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1140,8 +1143,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1155,16 +1174,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1173,22 +1184,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1209,6 +1204,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1222,29 +1225,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1264,7 +1244,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1298,13 +1301,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1316,19 +1313,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1340,19 +1325,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,7 +1361,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1388,61 +1433,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,25 +1475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1657,26 +1660,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1705,11 +1700,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1746,9 +1747,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1757,152 +1760,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2128,29 +2131,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2200,13 +2182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2634,8 +2610,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2667,13 +2643,13 @@
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
-      <c r="L3" s="77" t="s">
+      <c r="L3" s="75" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="77"/>
+      <c r="N3" s="75"/>
     </row>
     <row r="4" ht="15.75" spans="2:14">
       <c r="B4" s="29" t="s">
@@ -2688,13 +2664,13 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="75" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="77"/>
+      <c r="N4" s="75"/>
     </row>
     <row r="5" ht="15.75" spans="2:14">
       <c r="B5" s="32" t="s">
@@ -2709,7 +2685,7 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="33"/>
-      <c r="L5" s="77" t="s">
+      <c r="L5" s="75" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="68" t="s">
@@ -2728,7 +2704,7 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="L6" s="77" t="s">
+      <c r="L6" s="75" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="68" t="s">
@@ -2740,7 +2716,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="113" t="s">
+      <c r="L7" s="104" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="68" t="s">
@@ -2756,11 +2732,11 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="113" t="s">
+      <c r="L8" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="113"/>
-      <c r="N8" s="77"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="75"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="41" t="s">
@@ -2792,13 +2768,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="118" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="119" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -2810,24 +2786,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="128" t="s">
+      <c r="G10" s="119" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="114">
+      <c r="I10" s="105">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="118" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="119" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -2839,24 +2815,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="128" t="s">
+      <c r="G11" s="119" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="114">
+      <c r="I11" s="105">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="120" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="121" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -2868,13 +2844,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="130" t="s">
+      <c r="G12" s="121" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="115">
+      <c r="I12" s="106">
         <v>11.5</v>
       </c>
     </row>
@@ -2954,7 +2930,7 @@
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="66"/>
-      <c r="K18" s="77"/>
+      <c r="K18" s="75"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">
       <c r="A19" s="61">
@@ -2975,9 +2951,11 @@
       <c r="F19" s="65">
         <v>11</v>
       </c>
-      <c r="G19" s="47"/>
+      <c r="G19" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="H19" s="68"/>
-      <c r="K19" s="77"/>
+      <c r="K19" s="75"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
       <c r="A20" s="61">
@@ -3000,7 +2978,7 @@
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="66"/>
-      <c r="K20" s="77"/>
+      <c r="K20" s="75"/>
     </row>
     <row r="21" ht="15.75" spans="1:11">
       <c r="A21" s="61">
@@ -3023,7 +3001,7 @@
       </c>
       <c r="G21" s="47"/>
       <c r="H21" s="68"/>
-      <c r="K21" s="77"/>
+      <c r="K21" s="75"/>
     </row>
     <row r="22" ht="16.5" spans="1:11">
       <c r="A22" s="69">
@@ -3046,14 +3024,14 @@
       </c>
       <c r="G22" s="47"/>
       <c r="H22" s="68"/>
-      <c r="K22" s="77"/>
+      <c r="K22" s="75"/>
     </row>
     <row r="23" ht="15.75" spans="1:11">
       <c r="A23" s="72">
         <v>1</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="74">
         <v>6</v>
@@ -3061,84 +3039,86 @@
       <c r="D23" s="73">
         <v>2</v>
       </c>
-      <c r="E23" s="75"/>
-      <c r="F23" s="76">
+      <c r="E23" s="58"/>
+      <c r="F23" s="59">
         <v>3</v>
       </c>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
     </row>
     <row r="24" ht="16.5" spans="1:11">
-      <c r="A24" s="78">
+      <c r="A24" s="69">
         <v>1</v>
       </c>
-      <c r="B24" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="80">
+      <c r="B24" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="71">
         <v>8</v>
       </c>
-      <c r="D24" s="79">
+      <c r="D24" s="70">
         <v>4</v>
       </c>
-      <c r="E24" s="81"/>
-      <c r="F24" s="82">
+      <c r="E24" s="52"/>
+      <c r="F24" s="50">
         <v>5.5</v>
       </c>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
     </row>
     <row r="25" ht="16.5" spans="1:11">
-      <c r="A25" s="83"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="68"/>
       <c r="C25" s="68"/>
       <c r="D25" s="68"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
     </row>
     <row r="26" ht="15.75" spans="1:12">
-      <c r="A26" s="84"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="58"/>
-      <c r="C26" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="86"/>
+      <c r="C26" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="79"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="110"/>
+      <c r="J26" s="101"/>
       <c r="K26" s="64"/>
-      <c r="L26" s="116"/>
+      <c r="L26" s="107"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
+      <c r="C27" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3147,18 +3127,18 @@
       <c r="B28" s="47">
         <v>0</v>
       </c>
-      <c r="C28" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="92"/>
+      <c r="C28" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="85"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="110"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="64"/>
-      <c r="L28" s="116"/>
+      <c r="L28" s="107"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3167,10 +3147,10 @@
       <c r="B29" s="47">
         <v>0</v>
       </c>
-      <c r="C29" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="94"/>
+      <c r="C29" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="87"/>
       <c r="E29" s="47"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
@@ -3178,7 +3158,7 @@
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
       <c r="K29" s="64"/>
-      <c r="L29" s="116"/>
+      <c r="L29" s="107"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3187,22 +3167,22 @@
       <c r="B30" s="47">
         <v>0</v>
       </c>
-      <c r="C30" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="94" t="s">
+      <c r="C30" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="94" t="s">
+      <c r="D30" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="95" t="s">
+      <c r="E30" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="94"/>
-      <c r="J30" s="119"/>
+      <c r="F30" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="87"/>
+      <c r="J30" s="110"/>
       <c r="K30" s="64"/>
-      <c r="L30" s="116"/>
+      <c r="L30" s="107"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3212,24 +3192,24 @@
         <v>1</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
+      <c r="K31" s="107"/>
+      <c r="L31" s="107"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3239,26 +3219,26 @@
         <v>1</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="J32" s="120"/>
-      <c r="K32" s="116"/>
-      <c r="L32" s="116"/>
+        <v>57</v>
+      </c>
+      <c r="J32" s="111"/>
+      <c r="K32" s="107"/>
+      <c r="L32" s="107"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3268,83 +3248,83 @@
         <v>1</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H33" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J33" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
+        <v>65</v>
+      </c>
+      <c r="K33" s="107"/>
+      <c r="L33" s="107"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="96" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="97">
+      <c r="A34" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="90">
         <v>1</v>
       </c>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="97"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="90"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
       <c r="N34" s="47"/>
     </row>
     <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="99">
+      <c r="A35" s="72">
         <v>1</v>
       </c>
-      <c r="B35" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="101"/>
+      <c r="B35" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="110"/>
+      <c r="J35" s="101"/>
       <c r="K35" s="68"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
       <c r="A36" s="69">
         <v>1</v>
       </c>
-      <c r="B36" s="102" t="s">
-        <v>41</v>
+      <c r="B36" s="93" t="s">
+        <v>42</v>
       </c>
       <c r="C36" s="69" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D36" s="71" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E36" s="71"/>
       <c r="F36" s="71"/>
@@ -3369,11 +3349,11 @@
     </row>
     <row r="38" ht="16.5" spans="1:11">
       <c r="A38" s="68"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
       <c r="G38" s="68"/>
       <c r="H38" s="68"/>
       <c r="I38" s="47"/>
@@ -3382,13 +3362,13 @@
     </row>
     <row r="39" ht="16.5" spans="1:11">
       <c r="A39" s="68"/>
-      <c r="C39" s="99" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="C39" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="92"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H39" s="68"/>
       <c r="I39" s="68"/>
@@ -3396,36 +3376,36 @@
       <c r="K39" s="68"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
-      <c r="A40" s="83"/>
-      <c r="B40" s="84" t="s">
-        <v>70</v>
+      <c r="A40" s="76"/>
+      <c r="B40" s="77" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="104" t="s">
+      <c r="F40" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="H40" s="105">
+      <c r="G40" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="96">
         <v>20</v>
       </c>
-      <c r="I40" s="131" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" s="121"/>
-      <c r="K40" s="121"/>
+      <c r="I40" s="122" t="s">
+        <v>77</v>
+      </c>
+      <c r="J40" s="112"/>
+      <c r="K40" s="112"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
-      <c r="A41" s="83"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="46">
         <v>25</v>
       </c>
@@ -3438,23 +3418,23 @@
       <c r="E41" s="64">
         <v>1.5</v>
       </c>
-      <c r="F41" s="106">
+      <c r="F41" s="97">
         <v>12</v>
       </c>
       <c r="G41" s="68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H41" s="68">
         <v>4</v>
       </c>
-      <c r="I41" s="132" t="s">
-        <v>78</v>
+      <c r="I41" s="123" t="s">
+        <v>79</v>
       </c>
       <c r="J41" s="47"/>
       <c r="K41" s="68"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
-      <c r="A42" s="83"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="46">
         <v>50</v>
       </c>
@@ -3467,11 +3447,11 @@
       <c r="E42" s="64">
         <v>2.5</v>
       </c>
-      <c r="F42" s="106">
+      <c r="F42" s="97">
         <v>12</v>
       </c>
       <c r="G42" s="68" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H42" s="68">
         <v>10</v>
@@ -3481,7 +3461,7 @@
       <c r="K42" s="68"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="83"/>
+      <c r="A43" s="76"/>
       <c r="B43" s="46">
         <v>75</v>
       </c>
@@ -3492,13 +3472,13 @@
         <v>4</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="106">
+        <v>81</v>
+      </c>
+      <c r="F43" s="97">
         <v>12</v>
       </c>
       <c r="G43" s="68" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H43" s="68">
         <v>12</v>
@@ -3508,10 +3488,10 @@
       <c r="K43" s="68"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
-      <c r="A44" s="83" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="107">
+      <c r="A44" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="98">
         <v>100</v>
       </c>
       <c r="C44" s="64">
@@ -3520,10 +3500,10 @@
       <c r="D44" s="64">
         <v>4</v>
       </c>
-      <c r="E44" s="103">
+      <c r="E44" s="94">
         <v>4.5</v>
       </c>
-      <c r="F44" s="106">
+      <c r="F44" s="97">
         <v>12</v>
       </c>
       <c r="G44" s="68"/>
@@ -3533,10 +3513,10 @@
       <c r="K44" s="68"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
-      <c r="A45" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="108">
+      <c r="A45" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="99">
         <v>125</v>
       </c>
       <c r="C45" s="64">
@@ -3545,10 +3525,10 @@
       <c r="D45" s="64">
         <v>4</v>
       </c>
-      <c r="E45" s="103" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" s="106">
+      <c r="E45" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="97">
         <v>12</v>
       </c>
       <c r="G45" s="68"/>
@@ -3558,10 +3538,10 @@
       <c r="K45" s="68"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
-      <c r="A46" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="108">
+      <c r="A46" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="99">
         <v>150</v>
       </c>
       <c r="C46" s="64">
@@ -3570,10 +3550,10 @@
       <c r="D46" s="64">
         <v>4</v>
       </c>
-      <c r="E46" s="103" t="s">
-        <v>86</v>
-      </c>
-      <c r="F46" s="106">
+      <c r="E46" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="97">
         <v>12</v>
       </c>
       <c r="G46" s="68"/>
@@ -3583,10 +3563,10 @@
       <c r="K46" s="68"/>
     </row>
     <row r="47" ht="15.75" spans="1:11">
-      <c r="A47" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="108">
+      <c r="A47" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="99">
         <v>175</v>
       </c>
       <c r="C47" s="64">
@@ -3595,10 +3575,10 @@
       <c r="D47" s="64">
         <v>4</v>
       </c>
-      <c r="E47" s="103" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" s="106">
+      <c r="E47" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="97">
         <v>12</v>
       </c>
       <c r="G47" s="68"/>
@@ -3608,10 +3588,10 @@
       <c r="K47" s="68"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
-      <c r="A48" s="83" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48" s="108">
+      <c r="A48" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="99">
         <v>200</v>
       </c>
       <c r="C48" s="64">
@@ -3621,13 +3601,13 @@
         <v>5</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" s="106">
+        <v>91</v>
+      </c>
+      <c r="F48" s="97">
         <v>13</v>
       </c>
       <c r="G48" s="68" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
@@ -3635,10 +3615,10 @@
       <c r="K48" s="68"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
-      <c r="A49" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="107">
+      <c r="A49" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="98">
         <v>225</v>
       </c>
       <c r="C49" s="64">
@@ -3650,7 +3630,7 @@
       <c r="E49" s="64">
         <v>8.25</v>
       </c>
-      <c r="F49" s="106">
+      <c r="F49" s="97">
         <v>13</v>
       </c>
       <c r="G49" s="68"/>
@@ -3660,8 +3640,8 @@
       <c r="K49" s="68"/>
     </row>
     <row r="50" ht="15.75" spans="1:11">
-      <c r="A50" s="83" t="s">
-        <v>93</v>
+      <c r="A50" s="76" t="s">
+        <v>94</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
@@ -3678,15 +3658,15 @@
       <c r="F50" s="48">
         <v>13</v>
       </c>
-      <c r="G50" s="103"/>
+      <c r="G50" s="94"/>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
       <c r="J50" s="47"/>
       <c r="K50" s="68"/>
     </row>
     <row r="51" ht="15.75" spans="1:11">
-      <c r="A51" s="83" t="s">
-        <v>94</v>
+      <c r="A51" s="76" t="s">
+        <v>95</v>
       </c>
       <c r="B51" s="46">
         <v>275</v>
@@ -3710,8 +3690,8 @@
       <c r="K51" s="68"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="83" t="s">
-        <v>95</v>
+      <c r="A52" s="76" t="s">
+        <v>96</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -3733,13 +3713,13 @@
       </c>
       <c r="H52" s="68"/>
       <c r="I52" s="68"/>
-      <c r="J52" s="77"/>
-      <c r="K52" s="77"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
       <c r="M52" s="68"/>
     </row>
     <row r="53" ht="16.5" spans="1:13">
-      <c r="A53" s="83" t="s">
-        <v>96</v>
+      <c r="A53" s="76" t="s">
+        <v>97</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -3762,7 +3742,7 @@
       <c r="M53" s="68"/>
     </row>
     <row r="54" ht="15.75" spans="2:13">
-      <c r="B54" s="109">
+      <c r="B54" s="100">
         <v>350</v>
       </c>
       <c r="C54" s="58">
@@ -3774,7 +3754,7 @@
       <c r="E54" s="58">
         <v>11.5</v>
       </c>
-      <c r="F54" s="110">
+      <c r="F54" s="101">
         <v>14</v>
       </c>
       <c r="G54" s="47"/>
@@ -3783,7 +3763,7 @@
       <c r="M54" s="68"/>
     </row>
     <row r="55" ht="15.75" spans="2:9">
-      <c r="B55" s="107">
+      <c r="B55" s="98">
         <v>375</v>
       </c>
       <c r="C55" s="47">
@@ -3819,7 +3799,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
@@ -3865,7 +3845,7 @@
       <c r="I58" s="47"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="108">
+      <c r="B59" s="99">
         <v>475</v>
       </c>
       <c r="C59" s="47">
@@ -3881,13 +3861,13 @@
         <v>14</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
     </row>
     <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="111">
+      <c r="B60" s="102">
         <v>500</v>
       </c>
       <c r="C60" s="52">
@@ -3936,8 +3916,8 @@
       <c r="E64" s="47">
         <v>10</v>
       </c>
-      <c r="F64" s="112" t="s">
-        <v>99</v>
+      <c r="F64" s="103" t="s">
+        <v>100</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
@@ -3973,7 +3953,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -3982,8 +3962,8 @@
       <c r="I69" s="47"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="122" t="s">
-        <v>101</v>
+      <c r="C70" s="113" t="s">
+        <v>102</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -3999,13 +3979,13 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="123"/>
-      <c r="B72" s="104"/>
-      <c r="C72" s="124"/>
-      <c r="D72" s="124"/>
+      <c r="A72" s="114"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="115"/>
       <c r="E72" s="68"/>
       <c r="F72" s="68" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G72" s="68"/>
       <c r="H72" s="68"/>
@@ -4033,13 +4013,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4060,7 +4040,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4082,11 +4062,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4107,12 +4087,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="133" t="s">
-        <v>109</v>
+      <c r="D77" s="124" t="s">
+        <v>110</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4125,7 +4105,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="123"/>
+      <c r="A78" s="114"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4133,18 +4113,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" s="125"/>
+        <v>112</v>
+      </c>
+      <c r="E78" s="116"/>
       <c r="F78" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="G78" s="125"/>
-      <c r="H78" s="125"/>
-      <c r="I78" s="125"/>
-      <c r="J78" s="125"/>
-      <c r="K78" s="125"/>
-      <c r="L78" s="125"/>
+        <v>113</v>
+      </c>
+      <c r="G78" s="116"/>
+      <c r="H78" s="116"/>
+      <c r="I78" s="116"/>
+      <c r="J78" s="116"/>
+      <c r="K78" s="116"/>
+      <c r="L78" s="116"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4157,7 +4137,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4178,11 +4158,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4201,8 +4181,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="133" t="s">
-        <v>109</v>
+      <c r="D81" s="124" t="s">
+        <v>110</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4224,7 +4204,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4243,7 +4223,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4262,7 +4242,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4277,7 +4257,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4474,8 +4454,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="126"/>
-      <c r="F103" s="126"/>
+      <c r="E103" s="117"/>
+      <c r="F103" s="117"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4579,31 +4559,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4611,28 +4591,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>128</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4640,28 +4620,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>131</v>
-      </c>
       <c r="E3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4669,28 +4649,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>135</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4698,28 +4678,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4727,28 +4707,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4756,28 +4736,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4785,28 +4765,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4814,28 +4794,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4843,28 +4823,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4872,28 +4852,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4901,28 +4881,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4930,28 +4910,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -4959,33 +4939,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>202</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5017,34 +4997,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5052,31 +5032,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5084,31 +5064,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>221</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>222</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5116,31 +5096,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>226</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G21" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5148,31 +5128,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G22" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5180,31 +5160,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>235</v>
-      </c>
       <c r="E23" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5212,31 +5192,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F24" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>241</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5244,31 +5224,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>246</v>
-      </c>
       <c r="I25" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5276,31 +5256,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5308,31 +5288,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5340,31 +5320,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="E28" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5372,31 +5352,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5404,31 +5384,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5436,63 +5416,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardized the language among all documents: No more Cooldown-based (only Insight-based), no more Advanced/Basic Spells (only Insight/Mana Spells), no more Charges (only Mana), no more Prepared (only Know/Learn), no more Slot (only Insight), no more Saves (only Checks). Separated feats from Abilities and cleaned up the python script for database generation. Created a Trello board for keeping track of tasks.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="319">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -137,7 +137,184 @@
     <t>Save or half (50% chance) (+35%)</t>
   </si>
   <si>
-    <t>4d4 + Main Stat</t>
+    <r>
+      <t xml:space="preserve">8.5 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 6.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   4 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.5 |    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 13 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 9.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   8 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 11 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 8.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">17 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">16.5 | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AoE 12.5</t>
+    </r>
   </si>
   <si>
     <t>Pet Attack</t>
@@ -951,12 +1128,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1136,36 +1313,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1181,9 +1328,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1194,13 +1370,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1229,7 +1398,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1237,7 +1406,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1252,7 +1435,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1266,17 +1449,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1295,7 +1479,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,55 +1569,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1367,37 +1641,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1409,73 +1659,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1658,20 +1842,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1700,17 +1881,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1760,7 +1944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1778,134 +1962,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="26" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2110,9 +2294,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2120,6 +2310,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2610,8 +2806,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2643,13 +2839,13 @@
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
-      <c r="L3" s="75" t="s">
+      <c r="L3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="68" t="s">
+      <c r="M3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="75"/>
+      <c r="N3" s="79"/>
     </row>
     <row r="4" ht="15.75" spans="2:14">
       <c r="B4" s="29" t="s">
@@ -2664,13 +2860,13 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="75"/>
+      <c r="N4" s="79"/>
     </row>
     <row r="5" ht="15.75" spans="2:14">
       <c r="B5" s="32" t="s">
@@ -2685,13 +2881,13 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="33"/>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="68"/>
+      <c r="N5" s="69"/>
     </row>
     <row r="6" ht="16.5" spans="2:14">
       <c r="B6" s="34" t="s">
@@ -2704,25 +2900,25 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="L6" s="75" t="s">
+      <c r="L6" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="68" t="s">
+      <c r="M6" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="68"/>
+      <c r="N6" s="69"/>
     </row>
     <row r="7" ht="16.5" spans="5:14">
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="104" t="s">
+      <c r="L7" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="68" t="s">
+      <c r="M7" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="68"/>
+      <c r="N7" s="69"/>
     </row>
     <row r="8" ht="16.5" spans="3:14">
       <c r="C8" s="37" t="s">
@@ -2732,11 +2928,11 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="104"/>
-      <c r="N8" s="75"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="79"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="41" t="s">
@@ -2768,13 +2964,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="118" t="s">
+      <c r="A10" s="122" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -2786,24 +2982,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="119" t="s">
+      <c r="G10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="105">
+      <c r="I10" s="109">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="122" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -2815,24 +3011,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="119" t="s">
+      <c r="G11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="105">
+      <c r="I11" s="109">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="124" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -2844,13 +3040,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="121" t="s">
+      <c r="G12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="106">
+      <c r="I12" s="110">
         <v>11.5</v>
       </c>
     </row>
@@ -2916,21 +3112,21 @@
       <c r="B18" s="62">
         <v>0</v>
       </c>
-      <c r="C18" s="66">
-        <v>8.5</v>
-      </c>
-      <c r="D18" s="67">
-        <v>4</v>
+      <c r="C18" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>41</v>
       </c>
       <c r="E18" s="64">
         <v>0</v>
       </c>
-      <c r="F18" s="65">
-        <v>5.5</v>
+      <c r="F18" s="68" t="s">
+        <v>42</v>
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="66"/>
-      <c r="K18" s="75"/>
+      <c r="K18" s="79"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">
       <c r="A19" s="61">
@@ -2939,23 +3135,21 @@
       <c r="B19" s="62">
         <v>0</v>
       </c>
-      <c r="C19" s="68">
-        <v>13</v>
-      </c>
-      <c r="D19" s="67">
-        <v>8</v>
+      <c r="C19" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>44</v>
       </c>
       <c r="E19" s="64">
         <v>0</v>
       </c>
-      <c r="F19" s="65">
-        <v>11</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="68"/>
-      <c r="K19" s="75"/>
+      <c r="F19" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="47"/>
+      <c r="H19" s="69"/>
+      <c r="K19" s="79"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
       <c r="A20" s="61">
@@ -2964,21 +3158,21 @@
       <c r="B20" s="62">
         <v>1</v>
       </c>
-      <c r="C20" s="66">
-        <v>8.5</v>
-      </c>
-      <c r="D20" s="67">
-        <v>4</v>
-      </c>
-      <c r="E20" s="64">
-        <v>4</v>
-      </c>
-      <c r="F20" s="65">
-        <v>5.5</v>
+      <c r="C20" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="66"/>
-      <c r="K20" s="75"/>
+      <c r="K20" s="79"/>
     </row>
     <row r="21" ht="15.75" spans="1:11">
       <c r="A21" s="61">
@@ -2987,56 +3181,56 @@
       <c r="B21" s="62">
         <v>1</v>
       </c>
-      <c r="C21" s="68">
-        <v>13</v>
-      </c>
-      <c r="D21" s="67">
-        <v>8</v>
-      </c>
-      <c r="E21" s="64">
+      <c r="C21" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="47"/>
+      <c r="H21" s="69"/>
+      <c r="K21" s="79"/>
+    </row>
+    <row r="22" ht="16.5" spans="1:11">
+      <c r="A22" s="71">
+        <v>1</v>
+      </c>
+      <c r="B22" s="72">
+        <v>1</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="47"/>
+      <c r="H22" s="69"/>
+      <c r="K22" s="79"/>
+    </row>
+    <row r="23" ht="15.75" spans="1:11">
+      <c r="A23" s="76">
+        <v>1</v>
+      </c>
+      <c r="B23" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="78">
         <v>6</v>
       </c>
-      <c r="F21" s="65">
-        <v>11</v>
-      </c>
-      <c r="G21" s="47"/>
-      <c r="H21" s="68"/>
-      <c r="K21" s="75"/>
-    </row>
-    <row r="22" ht="16.5" spans="1:11">
-      <c r="A22" s="69">
-        <v>1</v>
-      </c>
-      <c r="B22" s="70">
-        <v>1</v>
-      </c>
-      <c r="C22" s="71">
-        <v>17</v>
-      </c>
-      <c r="D22" s="70">
-        <v>12</v>
-      </c>
-      <c r="E22" s="52">
-        <v>8</v>
-      </c>
-      <c r="F22" s="50">
-        <v>16.5</v>
-      </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="68"/>
-      <c r="K22" s="75"/>
-    </row>
-    <row r="23" ht="15.75" spans="1:11">
-      <c r="A23" s="72">
-        <v>1</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="74">
-        <v>6</v>
-      </c>
-      <c r="D23" s="73">
+      <c r="D23" s="77">
         <v>2</v>
       </c>
       <c r="E23" s="58"/>
@@ -3044,22 +3238,22 @@
         <v>3</v>
       </c>
       <c r="G23" s="47"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
     </row>
     <row r="24" ht="16.5" spans="1:11">
-      <c r="A24" s="69">
+      <c r="A24" s="71">
         <v>1</v>
       </c>
-      <c r="B24" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="71">
+      <c r="B24" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="73">
         <v>8</v>
       </c>
-      <c r="D24" s="70">
+      <c r="D24" s="72">
         <v>4</v>
       </c>
       <c r="E24" s="52"/>
@@ -3067,58 +3261,58 @@
         <v>5.5</v>
       </c>
       <c r="G24" s="47"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
     </row>
     <row r="25" ht="16.5" spans="1:11">
-      <c r="A25" s="76"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
     </row>
     <row r="26" ht="15.75" spans="1:12">
-      <c r="A26" s="77"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="58"/>
-      <c r="C26" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="79"/>
+      <c r="C26" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="83"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="101"/>
+      <c r="J26" s="105"/>
       <c r="K26" s="64"/>
-      <c r="L26" s="107"/>
+      <c r="L26" s="111"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="82" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
+      <c r="C27" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3127,18 +3321,18 @@
       <c r="B28" s="47">
         <v>0</v>
       </c>
-      <c r="C28" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="85"/>
+      <c r="C28" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="89"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="101"/>
+      <c r="J28" s="105"/>
       <c r="K28" s="64"/>
-      <c r="L28" s="107"/>
+      <c r="L28" s="111"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3147,10 +3341,10 @@
       <c r="B29" s="47">
         <v>0</v>
       </c>
-      <c r="C29" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="87"/>
+      <c r="C29" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="91"/>
       <c r="E29" s="47"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
@@ -3158,7 +3352,7 @@
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
       <c r="K29" s="64"/>
-      <c r="L29" s="107"/>
+      <c r="L29" s="111"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3167,22 +3361,22 @@
       <c r="B30" s="47">
         <v>0</v>
       </c>
-      <c r="C30" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="87" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" s="88" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="87"/>
-      <c r="J30" s="110"/>
+      <c r="C30" s="90" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="91"/>
+      <c r="J30" s="114"/>
       <c r="K30" s="64"/>
-      <c r="L30" s="107"/>
+      <c r="L30" s="111"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3192,24 +3386,24 @@
         <v>1</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="111"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3219,26 +3413,26 @@
         <v>1</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="111"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
+        <v>68</v>
+      </c>
+      <c r="J32" s="115"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="111"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3248,164 +3442,164 @@
         <v>1</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="H33" s="52" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="J33" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
+        <v>76</v>
+      </c>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="89" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="90">
+      <c r="A34" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="94">
         <v>1</v>
       </c>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="90"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="94"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
       <c r="N34" s="47"/>
     </row>
     <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="72">
+      <c r="A35" s="76">
         <v>1</v>
       </c>
-      <c r="B35" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
+      <c r="B35" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="68"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="69"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
-      <c r="A36" s="69">
+      <c r="A36" s="71">
         <v>1</v>
       </c>
-      <c r="B36" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="71"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="71"/>
+      <c r="B36" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="71" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
       <c r="I36" s="52"/>
       <c r="J36" s="53"/>
-      <c r="K36" s="68"/>
+      <c r="K36" s="69"/>
     </row>
     <row r="37" ht="15.75" spans="1:11">
-      <c r="A37" s="68"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
-      <c r="K37" s="68"/>
+      <c r="K37" s="69"/>
     </row>
     <row r="38" ht="16.5" spans="1:11">
-      <c r="A38" s="68"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
-      <c r="K38" s="68"/>
+      <c r="K38" s="69"/>
     </row>
     <row r="39" ht="16.5" spans="1:11">
-      <c r="A39" s="68"/>
-      <c r="C39" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="92"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
+      <c r="A39" s="69"/>
+      <c r="C39" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="96"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
       <c r="J39" s="47"/>
-      <c r="K39" s="68"/>
+      <c r="K39" s="69"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
-      <c r="A40" s="76"/>
-      <c r="B40" s="77" t="s">
-        <v>71</v>
+      <c r="A40" s="80"/>
+      <c r="B40" s="81" t="s">
+        <v>82</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="95" t="s">
-        <v>76</v>
-      </c>
-      <c r="H40" s="96">
+        <v>85</v>
+      </c>
+      <c r="F40" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="100">
         <v>20</v>
       </c>
-      <c r="I40" s="122" t="s">
-        <v>77</v>
-      </c>
-      <c r="J40" s="112"/>
-      <c r="K40" s="112"/>
+      <c r="I40" s="126" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" s="116"/>
+      <c r="K40" s="116"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
-      <c r="A41" s="76"/>
+      <c r="A41" s="80"/>
       <c r="B41" s="46">
         <v>25</v>
       </c>
@@ -3418,23 +3612,23 @@
       <c r="E41" s="64">
         <v>1.5</v>
       </c>
-      <c r="F41" s="97">
+      <c r="F41" s="101">
         <v>12</v>
       </c>
-      <c r="G41" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="H41" s="68">
+      <c r="G41" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" s="69">
         <v>4</v>
       </c>
-      <c r="I41" s="123" t="s">
-        <v>79</v>
+      <c r="I41" s="127" t="s">
+        <v>90</v>
       </c>
       <c r="J41" s="47"/>
-      <c r="K41" s="68"/>
+      <c r="K41" s="69"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
-      <c r="A42" s="76"/>
+      <c r="A42" s="80"/>
       <c r="B42" s="46">
         <v>50</v>
       </c>
@@ -3447,21 +3641,21 @@
       <c r="E42" s="64">
         <v>2.5</v>
       </c>
-      <c r="F42" s="97">
+      <c r="F42" s="101">
         <v>12</v>
       </c>
-      <c r="G42" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="H42" s="68">
+      <c r="G42" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="69">
         <v>10</v>
       </c>
-      <c r="I42" s="68"/>
+      <c r="I42" s="69"/>
       <c r="J42" s="47"/>
-      <c r="K42" s="68"/>
+      <c r="K42" s="69"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="76"/>
+      <c r="A43" s="80"/>
       <c r="B43" s="46">
         <v>75</v>
       </c>
@@ -3472,26 +3666,26 @@
         <v>4</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="97">
+        <v>92</v>
+      </c>
+      <c r="F43" s="101">
         <v>12</v>
       </c>
-      <c r="G43" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="H43" s="68">
+      <c r="G43" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="H43" s="69">
         <v>12</v>
       </c>
-      <c r="I43" s="68"/>
+      <c r="I43" s="69"/>
       <c r="J43" s="47"/>
-      <c r="K43" s="68"/>
+      <c r="K43" s="69"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
-      <c r="A44" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="98">
+      <c r="A44" s="80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="102">
         <v>100</v>
       </c>
       <c r="C44" s="64">
@@ -3500,23 +3694,23 @@
       <c r="D44" s="64">
         <v>4</v>
       </c>
-      <c r="E44" s="94">
+      <c r="E44" s="98">
         <v>4.5</v>
       </c>
-      <c r="F44" s="97">
+      <c r="F44" s="101">
         <v>12</v>
       </c>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
       <c r="I44" s="47"/>
       <c r="J44" s="47"/>
-      <c r="K44" s="68"/>
+      <c r="K44" s="69"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
-      <c r="A45" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="99">
+      <c r="A45" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="103">
         <v>125</v>
       </c>
       <c r="C45" s="64">
@@ -3525,23 +3719,23 @@
       <c r="D45" s="64">
         <v>4</v>
       </c>
-      <c r="E45" s="94" t="s">
-        <v>85</v>
-      </c>
-      <c r="F45" s="97">
+      <c r="E45" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="101">
         <v>12</v>
       </c>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
       <c r="I45" s="47"/>
       <c r="J45" s="47"/>
-      <c r="K45" s="68"/>
+      <c r="K45" s="69"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
-      <c r="A46" s="76" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="99">
+      <c r="A46" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="103">
         <v>150</v>
       </c>
       <c r="C46" s="64">
@@ -3550,23 +3744,23 @@
       <c r="D46" s="64">
         <v>4</v>
       </c>
-      <c r="E46" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="F46" s="97">
+      <c r="E46" s="98" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="101">
         <v>12</v>
       </c>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
       <c r="I46" s="47"/>
       <c r="J46" s="47"/>
-      <c r="K46" s="68"/>
+      <c r="K46" s="69"/>
     </row>
     <row r="47" ht="15.75" spans="1:11">
-      <c r="A47" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="99">
+      <c r="A47" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="103">
         <v>175</v>
       </c>
       <c r="C47" s="64">
@@ -3575,23 +3769,23 @@
       <c r="D47" s="64">
         <v>4</v>
       </c>
-      <c r="E47" s="94" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="97">
+      <c r="E47" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="101">
         <v>12</v>
       </c>
-      <c r="G47" s="68"/>
+      <c r="G47" s="69"/>
       <c r="H47" s="47"/>
       <c r="I47" s="47"/>
       <c r="J47" s="47"/>
-      <c r="K47" s="68"/>
+      <c r="K47" s="69"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
-      <c r="A48" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="99">
+      <c r="A48" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="103">
         <v>200</v>
       </c>
       <c r="C48" s="64">
@@ -3601,24 +3795,24 @@
         <v>5</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="F48" s="97">
+        <v>102</v>
+      </c>
+      <c r="F48" s="101">
         <v>13</v>
       </c>
-      <c r="G48" s="68" t="s">
-        <v>92</v>
+      <c r="G48" s="69" t="s">
+        <v>103</v>
       </c>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="68"/>
+      <c r="K48" s="69"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
-      <c r="A49" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="98">
+      <c r="A49" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="102">
         <v>225</v>
       </c>
       <c r="C49" s="64">
@@ -3630,18 +3824,18 @@
       <c r="E49" s="64">
         <v>8.25</v>
       </c>
-      <c r="F49" s="97">
+      <c r="F49" s="101">
         <v>13</v>
       </c>
-      <c r="G49" s="68"/>
+      <c r="G49" s="69"/>
       <c r="H49" s="47"/>
       <c r="I49" s="47"/>
       <c r="J49" s="47"/>
-      <c r="K49" s="68"/>
+      <c r="K49" s="69"/>
     </row>
     <row r="50" ht="15.75" spans="1:11">
-      <c r="A50" s="76" t="s">
-        <v>94</v>
+      <c r="A50" s="80" t="s">
+        <v>105</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
@@ -3658,15 +3852,15 @@
       <c r="F50" s="48">
         <v>13</v>
       </c>
-      <c r="G50" s="94"/>
+      <c r="G50" s="98"/>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
       <c r="J50" s="47"/>
-      <c r="K50" s="68"/>
+      <c r="K50" s="69"/>
     </row>
     <row r="51" ht="15.75" spans="1:11">
-      <c r="A51" s="76" t="s">
-        <v>95</v>
+      <c r="A51" s="80" t="s">
+        <v>106</v>
       </c>
       <c r="B51" s="46">
         <v>275</v>
@@ -3683,15 +3877,15 @@
       <c r="F51" s="48">
         <v>13</v>
       </c>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
       <c r="I51" s="47"/>
       <c r="J51" s="47"/>
-      <c r="K51" s="68"/>
+      <c r="K51" s="69"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="76" t="s">
-        <v>96</v>
+      <c r="A52" s="80" t="s">
+        <v>107</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -3711,15 +3905,15 @@
       <c r="G52" s="47">
         <v>13</v>
       </c>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="75"/>
-      <c r="M52" s="68"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="69"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="M52" s="69"/>
     </row>
     <row r="53" ht="16.5" spans="1:13">
-      <c r="A53" s="76" t="s">
-        <v>97</v>
+      <c r="A53" s="80" t="s">
+        <v>108</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -3739,10 +3933,10 @@
       <c r="G53" s="47"/>
       <c r="H53" s="47"/>
       <c r="I53" s="47"/>
-      <c r="M53" s="68"/>
+      <c r="M53" s="69"/>
     </row>
     <row r="54" ht="15.75" spans="2:13">
-      <c r="B54" s="100">
+      <c r="B54" s="104">
         <v>350</v>
       </c>
       <c r="C54" s="58">
@@ -3754,16 +3948,16 @@
       <c r="E54" s="58">
         <v>11.5</v>
       </c>
-      <c r="F54" s="101">
+      <c r="F54" s="105">
         <v>14</v>
       </c>
       <c r="G54" s="47"/>
       <c r="H54" s="47"/>
       <c r="I54" s="47"/>
-      <c r="M54" s="68"/>
+      <c r="M54" s="69"/>
     </row>
     <row r="55" ht="15.75" spans="2:9">
-      <c r="B55" s="98">
+      <c r="B55" s="102">
         <v>375</v>
       </c>
       <c r="C55" s="47">
@@ -3799,7 +3993,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
@@ -3845,7 +4039,7 @@
       <c r="I58" s="47"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="99">
+      <c r="B59" s="103">
         <v>475</v>
       </c>
       <c r="C59" s="47">
@@ -3861,13 +4055,13 @@
         <v>14</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
     </row>
     <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="102">
+      <c r="B60" s="106">
         <v>500</v>
       </c>
       <c r="C60" s="52">
@@ -3916,8 +4110,8 @@
       <c r="E64" s="47">
         <v>10</v>
       </c>
-      <c r="F64" s="103" t="s">
-        <v>100</v>
+      <c r="F64" s="107" t="s">
+        <v>111</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
@@ -3953,7 +4147,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -3962,8 +4156,8 @@
       <c r="I69" s="47"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="113" t="s">
-        <v>102</v>
+      <c r="C70" s="117" t="s">
+        <v>113</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -3979,19 +4173,19 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="114"/>
-      <c r="B72" s="95"/>
-      <c r="C72" s="115"/>
-      <c r="D72" s="115"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68" t="s">
-        <v>103</v>
-      </c>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
-      <c r="I72" s="68"/>
-      <c r="J72" s="68"/>
-      <c r="K72" s="68"/>
+      <c r="A72" s="118"/>
+      <c r="B72" s="99"/>
+      <c r="C72" s="119"/>
+      <c r="D72" s="119"/>
+      <c r="E72" s="69"/>
+      <c r="F72" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="69"/>
+      <c r="J72" s="69"/>
+      <c r="K72" s="69"/>
       <c r="M72" s="47"/>
       <c r="N72" s="47"/>
     </row>
@@ -4013,13 +4207,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4040,7 +4234,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4062,11 +4256,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4087,12 +4281,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="124" t="s">
-        <v>110</v>
+      <c r="D77" s="128" t="s">
+        <v>121</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4105,7 +4299,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="114"/>
+      <c r="A78" s="118"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4113,18 +4307,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="E78" s="116"/>
+        <v>123</v>
+      </c>
+      <c r="E78" s="120"/>
       <c r="F78" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="G78" s="116"/>
-      <c r="H78" s="116"/>
-      <c r="I78" s="116"/>
-      <c r="J78" s="116"/>
-      <c r="K78" s="116"/>
-      <c r="L78" s="116"/>
+        <v>124</v>
+      </c>
+      <c r="G78" s="120"/>
+      <c r="H78" s="120"/>
+      <c r="I78" s="120"/>
+      <c r="J78" s="120"/>
+      <c r="K78" s="120"/>
+      <c r="L78" s="120"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4137,7 +4331,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4158,11 +4352,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4181,8 +4375,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="124" t="s">
-        <v>110</v>
+      <c r="D81" s="128" t="s">
+        <v>121</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4204,7 +4398,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4223,7 +4417,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4242,7 +4436,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4257,7 +4451,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4454,8 +4648,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="117"/>
-      <c r="F103" s="117"/>
+      <c r="E103" s="121"/>
+      <c r="F103" s="121"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4559,31 +4753,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4591,28 +4785,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4620,28 +4814,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4649,28 +4843,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4678,28 +4872,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4707,28 +4901,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4736,28 +4930,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4765,28 +4959,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4794,28 +4988,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4823,28 +5017,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4852,28 +5046,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4881,28 +5075,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4910,28 +5104,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -4939,33 +5133,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="H14" s="9" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -4997,34 +5191,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5032,31 +5226,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5064,31 +5258,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5096,31 +5290,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5128,31 +5322,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5160,31 +5354,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5192,31 +5386,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5224,31 +5418,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5256,31 +5450,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5288,31 +5482,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5320,31 +5514,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5352,31 +5546,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5384,31 +5578,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5416,63 +5610,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made lots of changes and addiitons.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23295" windowHeight="13095"/>
+    <workbookView windowWidth="27195" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="321">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">8.5 | </t>
     </r>
     <r>
@@ -153,6 +159,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">   4 | </t>
     </r>
     <r>
@@ -168,6 +180,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">5.5 |    </t>
     </r>
     <r>
@@ -183,6 +202,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> 13 | </t>
     </r>
     <r>
@@ -198,6 +224,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">   8 | </t>
     </r>
     <r>
@@ -213,6 +245,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> 11 | </t>
     </r>
     <r>
@@ -227,7 +266,17 @@
     </r>
   </si>
   <si>
+    <t>3d6 + Main Stat</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">4 | </t>
     </r>
     <r>
@@ -243,6 +292,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">6 | </t>
     </r>
     <r>
@@ -257,7 +313,17 @@
     </r>
   </si>
   <si>
+    <t>3d4 + 3 = 8</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">17 | </t>
     </r>
     <r>
@@ -273,6 +339,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">12 | </t>
     </r>
     <r>
@@ -288,6 +361,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">8 | </t>
     </r>
     <r>
@@ -303,6 +383,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">16.5 | </t>
     </r>
     <r>
@@ -1128,10 +1215,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="44">
     <font>
@@ -1313,6 +1400,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1329,14 +1431,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1350,8 +1445,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1365,11 +1461,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1390,13 +1507,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1405,22 +1515,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1433,25 +1537,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1479,7 +1566,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,7 +1578,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1503,13 +1650,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1521,145 +1740,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,17 +1929,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1872,11 +1979,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1900,21 +2013,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1928,23 +2026,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1962,130 +2049,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2807,7 +2894,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3147,8 +3234,12 @@
       <c r="F19" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="69"/>
+      <c r="G19" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="69">
+        <v>2</v>
+      </c>
       <c r="K19" s="79"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
@@ -3165,7 +3256,7 @@
         <v>41</v>
       </c>
       <c r="E20" s="70" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" s="68" t="s">
         <v>42</v>
@@ -3188,12 +3279,14 @@
         <v>44</v>
       </c>
       <c r="E21" s="70" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="47"/>
+      <c r="G21" s="47" t="s">
+        <v>49</v>
+      </c>
       <c r="H21" s="69"/>
       <c r="K21" s="79"/>
     </row>
@@ -3205,16 +3298,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D22" s="72" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E22" s="74" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F22" s="75" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G22" s="47"/>
       <c r="H22" s="69"/>
@@ -3225,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C23" s="78">
         <v>6</v>
@@ -3248,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="72" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="73">
         <v>8</v>
@@ -3282,7 +3375,7 @@
       <c r="A26" s="81"/>
       <c r="B26" s="58"/>
       <c r="C26" s="82" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D26" s="83"/>
       <c r="E26" s="58"/>
@@ -3302,7 +3395,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="86" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D27" s="87"/>
       <c r="E27" s="87"/>
@@ -3322,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="88" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D28" s="89"/>
       <c r="E28" s="58"/>
@@ -3342,7 +3435,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="90" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" s="91"/>
       <c r="E29" s="47"/>
@@ -3362,16 +3455,16 @@
         <v>0</v>
       </c>
       <c r="C30" s="90" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" s="91" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E30" s="91" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F30" s="92" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H30" s="91"/>
       <c r="J30" s="114"/>
@@ -3386,19 +3479,19 @@
         <v>1</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
@@ -3413,22 +3506,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J32" s="115"/>
       <c r="K32" s="111"/>
@@ -3442,35 +3535,35 @@
         <v>1</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H33" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J33" s="53" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K33" s="111"/>
       <c r="L33" s="111"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
       <c r="A34" s="93" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B34" s="94">
         <v>1</v>
@@ -3493,10 +3586,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="96" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C35" s="81" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="78"/>
       <c r="E35" s="78"/>
@@ -3512,13 +3605,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="97" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D36" s="73" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E36" s="73"/>
       <c r="F36" s="73"/>
@@ -3557,12 +3650,12 @@
     <row r="39" ht="16.5" spans="1:11">
       <c r="A39" s="69"/>
       <c r="C39" s="76" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D39" s="96"/>
       <c r="F39" s="69"/>
       <c r="G39" s="69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H39" s="69"/>
       <c r="I39" s="69"/>
@@ -3572,28 +3665,28 @@
     <row r="40" ht="15.75" spans="1:11">
       <c r="A40" s="80"/>
       <c r="B40" s="81" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F40" s="96" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G40" s="99" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H40" s="100">
         <v>20</v>
       </c>
       <c r="I40" s="126" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J40" s="116"/>
       <c r="K40" s="116"/>
@@ -3616,13 +3709,13 @@
         <v>12</v>
       </c>
       <c r="G41" s="69" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H41" s="69">
         <v>4</v>
       </c>
       <c r="I41" s="127" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J41" s="47"/>
       <c r="K41" s="69"/>
@@ -3645,7 +3738,7 @@
         <v>12</v>
       </c>
       <c r="G42" s="69" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H42" s="69">
         <v>10</v>
@@ -3666,13 +3759,13 @@
         <v>4</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F43" s="101">
         <v>12</v>
       </c>
       <c r="G43" s="69" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H43" s="69">
         <v>12</v>
@@ -3683,7 +3776,7 @@
     </row>
     <row r="44" ht="15.75" spans="1:11">
       <c r="A44" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B44" s="102">
         <v>100</v>
@@ -3708,7 +3801,7 @@
     </row>
     <row r="45" ht="15.75" spans="1:11">
       <c r="A45" s="80" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B45" s="103">
         <v>125</v>
@@ -3720,7 +3813,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="98" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F45" s="101">
         <v>12</v>
@@ -3733,7 +3826,7 @@
     </row>
     <row r="46" ht="15.75" spans="1:11">
       <c r="A46" s="80" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B46" s="103">
         <v>150</v>
@@ -3745,7 +3838,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="98" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F46" s="101">
         <v>12</v>
@@ -3758,7 +3851,7 @@
     </row>
     <row r="47" ht="15.75" spans="1:11">
       <c r="A47" s="80" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B47" s="103">
         <v>175</v>
@@ -3770,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="98" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F47" s="101">
         <v>12</v>
@@ -3783,7 +3876,7 @@
     </row>
     <row r="48" ht="15.75" spans="1:11">
       <c r="A48" s="80" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B48" s="103">
         <v>200</v>
@@ -3795,13 +3888,13 @@
         <v>5</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F48" s="101">
         <v>13</v>
       </c>
       <c r="G48" s="69" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
@@ -3810,7 +3903,7 @@
     </row>
     <row r="49" ht="15.75" spans="1:11">
       <c r="A49" s="80" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B49" s="102">
         <v>225</v>
@@ -3835,7 +3928,7 @@
     </row>
     <row r="50" ht="15.75" spans="1:11">
       <c r="A50" s="80" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
@@ -3860,7 +3953,7 @@
     </row>
     <row r="51" ht="15.75" spans="1:11">
       <c r="A51" s="80" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B51" s="46">
         <v>275</v>
@@ -3885,7 +3978,7 @@
     </row>
     <row r="52" ht="15.75" spans="1:13">
       <c r="A52" s="80" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -3913,7 +4006,7 @@
     </row>
     <row r="53" ht="16.5" spans="1:13">
       <c r="A53" s="80" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -3993,7 +4086,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
@@ -4055,7 +4148,7 @@
         <v>14</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
@@ -4111,7 +4204,7 @@
         <v>10</v>
       </c>
       <c r="F64" s="107" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
@@ -4147,7 +4240,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4157,7 +4250,7 @@
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
       <c r="C70" s="117" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4179,7 +4272,7 @@
       <c r="D72" s="119"/>
       <c r="E72" s="69"/>
       <c r="F72" s="69" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G72" s="69"/>
       <c r="H72" s="69"/>
@@ -4207,13 +4300,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4234,7 +4327,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4256,11 +4349,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4282,11 +4375,11 @@
         <v>30</v>
       </c>
       <c r="D77" s="128" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4307,11 +4400,11 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E78" s="120"/>
       <c r="F78" s="47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G78" s="120"/>
       <c r="H78" s="120"/>
@@ -4331,7 +4424,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4352,11 +4445,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4376,7 +4469,7 @@
         <v>50</v>
       </c>
       <c r="D81" s="128" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4398,7 +4491,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4417,7 +4510,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4436,7 +4529,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4451,7 +4544,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4734,7 +4827,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4753,31 +4846,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4785,28 +4878,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4814,28 +4907,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4843,28 +4936,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4872,28 +4965,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4901,28 +4994,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>156</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4930,28 +5023,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4959,28 +5052,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4988,28 +5081,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5017,28 +5110,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5046,28 +5139,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5075,28 +5168,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5104,28 +5197,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5133,33 +5226,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>216</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5191,34 +5284,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5226,31 +5319,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5258,31 +5351,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5290,31 +5383,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5322,31 +5415,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5354,31 +5447,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5386,31 +5479,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G24" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>253</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5418,31 +5511,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F25" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="I25" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5450,31 +5543,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5482,31 +5575,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5514,31 +5607,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5546,31 +5639,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5578,31 +5671,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5610,63 +5703,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed a lot of things design-wise. Refer to the trello board for the changes.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="322">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -551,6 +551,9 @@
     <t>(10.75) 6.75</t>
   </si>
   <si>
+    <t>1d6 + 2 = 6.5 - 3 = 3.5</t>
+  </si>
+  <si>
     <t>Level 5</t>
   </si>
   <si>
@@ -1215,9 +1218,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="44">
@@ -1407,11 +1410,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1424,14 +1426,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1447,7 +1442,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1461,32 +1456,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1507,14 +1481,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1524,14 +1490,51 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1572,25 +1575,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1602,7 +1623,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1614,7 +1635,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1632,7 +1665,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1644,13 +1695,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1662,67 +1713,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1741,12 +1750,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1929,11 +1932,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1964,36 +2021,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2002,44 +2029,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2052,127 +2055,127 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2893,8 +2896,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3354,7 +3357,9 @@
         <v>5.5</v>
       </c>
       <c r="G24" s="47"/>
-      <c r="H24" s="79"/>
+      <c r="H24" s="79">
+        <v>17.5</v>
+      </c>
       <c r="I24" s="79"/>
       <c r="J24" s="79"/>
       <c r="K24" s="79"/>
@@ -3726,7 +3731,7 @@
         <v>50</v>
       </c>
       <c r="C42" s="64">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D42" s="64">
         <v>4</v>
@@ -3753,7 +3758,7 @@
         <v>75</v>
       </c>
       <c r="C43" s="64">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D43" s="64">
         <v>4</v>
@@ -3782,7 +3787,7 @@
         <v>100</v>
       </c>
       <c r="C44" s="64">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D44" s="64">
         <v>4</v>
@@ -3807,7 +3812,7 @@
         <v>125</v>
       </c>
       <c r="C45" s="64">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D45" s="64">
         <v>4</v>
@@ -3832,7 +3837,7 @@
         <v>150</v>
       </c>
       <c r="C46" s="64">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D46" s="64">
         <v>4</v>
@@ -3857,7 +3862,7 @@
         <v>175</v>
       </c>
       <c r="C47" s="64">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D47" s="64">
         <v>4</v>
@@ -3869,32 +3874,34 @@
         <v>12</v>
       </c>
       <c r="G47" s="69"/>
-      <c r="H47" s="47"/>
+      <c r="H47" s="47" t="s">
+        <v>103</v>
+      </c>
       <c r="I47" s="47"/>
       <c r="J47" s="47"/>
       <c r="K47" s="69"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
       <c r="A48" s="80" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B48" s="103">
         <v>200</v>
       </c>
       <c r="C48" s="64">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D48" s="64">
         <v>5</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F48" s="101">
         <v>13</v>
       </c>
       <c r="G48" s="69" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
@@ -3903,13 +3910,13 @@
     </row>
     <row r="49" ht="15.75" spans="1:11">
       <c r="A49" s="80" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B49" s="102">
         <v>225</v>
       </c>
       <c r="C49" s="64">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D49" s="64">
         <v>5</v>
@@ -3928,13 +3935,13 @@
     </row>
     <row r="50" ht="15.75" spans="1:11">
       <c r="A50" s="80" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
       </c>
       <c r="C50" s="47">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D50" s="47">
         <v>5</v>
@@ -3953,13 +3960,13 @@
     </row>
     <row r="51" ht="15.75" spans="1:11">
       <c r="A51" s="80" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B51" s="46">
         <v>275</v>
       </c>
       <c r="C51" s="47">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D51" s="47">
         <v>5</v>
@@ -3978,13 +3985,13 @@
     </row>
     <row r="52" ht="15.75" spans="1:13">
       <c r="A52" s="80" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
       </c>
       <c r="C52" s="47">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D52" s="47">
         <v>5</v>
@@ -4006,13 +4013,13 @@
     </row>
     <row r="53" ht="16.5" spans="1:13">
       <c r="A53" s="80" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
       </c>
       <c r="C53" s="52">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D53" s="52">
         <v>5</v>
@@ -4033,7 +4040,7 @@
         <v>350</v>
       </c>
       <c r="C54" s="58">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D54" s="58">
         <v>5</v>
@@ -4054,7 +4061,7 @@
         <v>375</v>
       </c>
       <c r="C55" s="47">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D55" s="64">
         <v>5</v>
@@ -4074,7 +4081,7 @@
         <v>400</v>
       </c>
       <c r="C56" s="47">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D56" s="64">
         <v>5</v>
@@ -4086,7 +4093,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
@@ -4096,7 +4103,7 @@
         <v>425</v>
       </c>
       <c r="C57" s="47">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D57" s="64">
         <v>5</v>
@@ -4116,7 +4123,7 @@
         <v>450</v>
       </c>
       <c r="C58" s="47">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D58" s="64">
         <v>5</v>
@@ -4136,7 +4143,7 @@
         <v>475</v>
       </c>
       <c r="C59" s="47">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D59" s="64">
         <v>5</v>
@@ -4148,7 +4155,7 @@
         <v>14</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
@@ -4158,7 +4165,7 @@
         <v>500</v>
       </c>
       <c r="C60" s="52">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D60" s="52">
         <v>5</v>
@@ -4204,7 +4211,7 @@
         <v>10</v>
       </c>
       <c r="F64" s="107" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="47"/>
@@ -4240,7 +4247,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4250,7 +4257,7 @@
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
       <c r="C70" s="117" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4272,7 +4279,7 @@
       <c r="D72" s="119"/>
       <c r="E72" s="69"/>
       <c r="F72" s="69" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G72" s="69"/>
       <c r="H72" s="69"/>
@@ -4300,13 +4307,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4327,7 +4334,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4349,11 +4356,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4375,11 +4382,11 @@
         <v>30</v>
       </c>
       <c r="D77" s="128" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4400,11 +4407,11 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E78" s="120"/>
       <c r="F78" s="47" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G78" s="120"/>
       <c r="H78" s="120"/>
@@ -4424,7 +4431,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4445,11 +4452,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4469,7 +4476,7 @@
         <v>50</v>
       </c>
       <c r="D81" s="128" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4491,7 +4498,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4510,7 +4517,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4529,7 +4536,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4544,7 +4551,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4827,7 +4834,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4846,31 +4853,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4878,28 +4885,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4907,28 +4914,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="E3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4936,28 +4943,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>149</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4965,28 +4972,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>153</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4994,28 +5001,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5023,28 +5030,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>165</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5052,28 +5059,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5081,28 +5088,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5110,28 +5117,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5139,28 +5146,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5168,28 +5175,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5197,28 +5204,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5226,33 +5233,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>216</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5284,34 +5291,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5319,31 +5326,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>232</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5351,31 +5358,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>235</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5383,31 +5390,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G21" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5415,31 +5422,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G22" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5447,31 +5454,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>249</v>
-      </c>
       <c r="E23" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5479,31 +5486,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>255</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5511,31 +5518,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="I25" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5543,31 +5550,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5575,31 +5582,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5607,31 +5614,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>162</v>
-      </c>
       <c r="E28" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5639,31 +5646,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5671,31 +5678,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5703,63 +5710,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2023-03-04: Davels, Nature and Cover
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="311">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -128,13 +128,16 @@
     <t>Damage With Armor</t>
   </si>
   <si>
-    <t>Damage (5 Armor)</t>
+    <t>Damage (3.5 Armor)</t>
   </si>
   <si>
     <t>Heal</t>
   </si>
   <si>
-    <t>Save or half (50% chance) (+35%)</t>
+    <t>Save or half (70% chance) (+15%)</t>
+  </si>
+  <si>
+    <t>Ranged Penalty</t>
   </si>
   <si>
     <r>
@@ -159,13 +162,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   4 | </t>
+      <t xml:space="preserve">   5 | </t>
     </r>
     <r>
       <rPr>
@@ -175,19 +172,12 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AoE 3</t>
+      <t>AoE 3.5</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">5.5 |    </t>
+      <t xml:space="preserve">5.75 |    </t>
     </r>
     <r>
       <rPr>
@@ -202,14 +192,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 13 | </t>
+      <t xml:space="preserve"> 13.5 | </t>
     </r>
     <r>
       <rPr>
@@ -224,13 +207,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   8 | </t>
+      <t xml:space="preserve">   10 | </t>
     </r>
     <r>
       <rPr>
@@ -240,19 +217,12 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AoE 6</t>
+      <t>AoE 7</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 11 | </t>
+      <t xml:space="preserve"> 11.5 | </t>
     </r>
     <r>
       <rPr>
@@ -264,9 +234,6 @@
       </rPr>
       <t>AoE 8.5</t>
     </r>
-  </si>
-  <si>
-    <t>3d6 + Main Stat</t>
   </si>
   <si>
     <r>
@@ -313,18 +280,8 @@
     </r>
   </si>
   <si>
-    <t>3d4 + 3 = 8</t>
-  </si>
-  <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">17 | </t>
+      <t xml:space="preserve">18.5 | </t>
     </r>
     <r>
       <rPr>
@@ -339,14 +296,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">12 | </t>
+      <t xml:space="preserve">15 | </t>
     </r>
     <r>
       <rPr>
@@ -356,7 +306,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AoE 9</t>
+      <t>AoE 10.5</t>
     </r>
   </si>
   <si>
@@ -383,14 +333,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">16.5 | </t>
+      <t xml:space="preserve">17.5 | </t>
     </r>
     <r>
       <rPr>
@@ -491,9 +434,6 @@
     <t>Monster Stats By Rating</t>
   </si>
   <si>
-    <t>[Player]</t>
-  </si>
-  <si>
     <t>Experience</t>
   </si>
   <si>
@@ -503,42 +443,27 @@
     <t>Defense</t>
   </si>
   <si>
+    <t>Player Defense</t>
+  </si>
+  <si>
     <t>Effective Damage / round</t>
   </si>
   <si>
     <t>Save DC</t>
   </si>
   <si>
-    <t>Health:</t>
-  </si>
-  <si>
     <t>+5 per level</t>
   </si>
   <si>
-    <t>Armor:</t>
-  </si>
-  <si>
     <t>+1 at level 6</t>
   </si>
   <si>
-    <t xml:space="preserve">True Damage (per round): </t>
-  </si>
-  <si>
-    <t>(7.5) 3.5</t>
-  </si>
-  <si>
-    <t>Save DC:</t>
-  </si>
-  <si>
     <t>Level 1</t>
   </si>
   <si>
     <t>Level 2</t>
   </si>
   <si>
-    <t>(9) 5.25</t>
-  </si>
-  <si>
     <t>Level 3</t>
   </si>
   <si>
@@ -551,18 +476,12 @@
     <t>(10.75) 6.75</t>
   </si>
   <si>
-    <t>1d6 + 2 = 6.5 - 3 = 3.5</t>
-  </si>
-  <si>
     <t>Level 5</t>
   </si>
   <si>
     <t>(11.5) 7.5</t>
   </si>
   <si>
-    <t>8.5 x2</t>
-  </si>
-  <si>
     <t>Level 6</t>
   </si>
   <si>
@@ -576,15 +495,6 @@
   </si>
   <si>
     <t>Level 10</t>
-  </si>
-  <si>
-    <t>9 + 9</t>
-  </si>
-  <si>
-    <t>1d12 + 2</t>
-  </si>
-  <si>
-    <t>1d6 + 3</t>
   </si>
   <si>
     <t>XP Rules</t>
@@ -653,6 +563,9 @@
   </si>
   <si>
     <t>1-Handed (+3)</t>
+  </si>
+  <si>
+    <t>1d12 + 2</t>
   </si>
   <si>
     <t>d6 + 5</t>
@@ -1219,8 +1132,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="44">
@@ -1404,6 +1317,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1411,7 +1331,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1425,13 +1345,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1440,9 +1353,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1465,6 +1377,21 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1481,7 +1408,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1490,21 +1417,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1513,14 +1434,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1569,13 +1482,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,19 +1524,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1617,30 +1566,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1648,36 +1573,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1707,7 +1602,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1719,7 +1632,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1731,25 +1662,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1933,16 +1846,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1995,21 +1908,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2017,6 +1915,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2034,15 +1947,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2052,134 +1965,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2360,6 +2273,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2378,6 +2294,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2406,6 +2325,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2477,9 +2399,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2499,9 +2418,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2535,6 +2451,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2896,8 +2815,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:G3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2929,13 +2848,13 @@
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
-      <c r="L3" s="79" t="s">
+      <c r="L3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="69" t="s">
+      <c r="M3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="79"/>
+      <c r="N3" s="82"/>
     </row>
     <row r="4" ht="15.75" spans="2:14">
       <c r="B4" s="29" t="s">
@@ -2950,13 +2869,13 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="L4" s="79" t="s">
+      <c r="L4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="79"/>
+      <c r="N4" s="82"/>
     </row>
     <row r="5" ht="15.75" spans="2:14">
       <c r="B5" s="32" t="s">
@@ -2971,13 +2890,13 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="33"/>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="69" t="s">
+      <c r="M5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="69"/>
+      <c r="N5" s="71"/>
     </row>
     <row r="6" ht="16.5" spans="2:14">
       <c r="B6" s="34" t="s">
@@ -2990,25 +2909,25 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="L6" s="79" t="s">
+      <c r="L6" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="69" t="s">
+      <c r="M6" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="69"/>
+      <c r="N6" s="71"/>
     </row>
     <row r="7" ht="16.5" spans="5:14">
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="69" t="s">
+      <c r="M7" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="69"/>
+      <c r="N7" s="71"/>
     </row>
     <row r="8" ht="16.5" spans="3:14">
       <c r="C8" s="37" t="s">
@@ -3018,11 +2937,11 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="108" t="s">
+      <c r="L8" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="108"/>
-      <c r="N8" s="79"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="82"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="41" t="s">
@@ -3054,13 +2973,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="124" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="125" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -3072,24 +2991,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="123" t="s">
+      <c r="G10" s="125" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="109">
+      <c r="I10" s="110">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="124" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="125" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -3101,24 +3020,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="123" t="s">
+      <c r="G11" s="125" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="109">
+      <c r="I11" s="110">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="126" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="127" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -3130,13 +3049,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="127" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="110">
+      <c r="I12" s="111">
         <v>11.5</v>
       </c>
     </row>
@@ -3145,7 +3064,7 @@
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
     </row>
-    <row r="15" ht="15.75" spans="2:6">
+    <row r="15" spans="2:6">
       <c r="B15" s="47"/>
       <c r="D15" s="47"/>
       <c r="E15" s="47"/>
@@ -3170,163 +3089,171 @@
       <c r="F16" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="60"/>
+      <c r="G16" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="61"/>
     </row>
     <row r="17" ht="15.75" spans="1:8">
-      <c r="A17" s="61">
+      <c r="A17" s="62">
         <v>0</v>
       </c>
-      <c r="B17" s="62">
+      <c r="B17" s="63">
         <v>0</v>
       </c>
       <c r="C17" s="47">
         <v>0</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="64">
         <v>0</v>
       </c>
-      <c r="E17" s="64">
+      <c r="E17" s="65">
         <v>0</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="66">
         <v>0</v>
       </c>
-      <c r="G17" s="47"/>
+      <c r="G17" s="67">
+        <v>0</v>
+      </c>
       <c r="H17" s="47"/>
     </row>
     <row r="18" ht="15.75" spans="1:11">
-      <c r="A18" s="61">
+      <c r="A18" s="62">
         <v>0.5</v>
       </c>
-      <c r="B18" s="62">
+      <c r="B18" s="63">
         <v>0</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="67" t="s">
+      <c r="C18" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="64">
+      <c r="D18" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="65">
         <v>0</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="67">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="K18" s="82"/>
+    </row>
+    <row r="19" ht="15.75" spans="1:11">
+      <c r="A19" s="62">
+        <v>1</v>
+      </c>
+      <c r="B19" s="63">
+        <v>0</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="65">
+        <v>0</v>
+      </c>
+      <c r="F19" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="67">
+        <v>-2</v>
+      </c>
+      <c r="H19" s="71"/>
+      <c r="K19" s="82"/>
+    </row>
+    <row r="20" ht="15.75" spans="1:11">
+      <c r="A20" s="62">
+        <v>0</v>
+      </c>
+      <c r="B20" s="63">
+        <v>1</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="66"/>
-      <c r="K18" s="79"/>
-    </row>
-    <row r="19" ht="15.75" spans="1:11">
-      <c r="A19" s="61">
+      <c r="E20" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="67">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="68"/>
+      <c r="K20" s="82"/>
+    </row>
+    <row r="21" ht="15.75" spans="1:11">
+      <c r="A21" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="B21" s="63">
         <v>1</v>
       </c>
-      <c r="B19" s="62">
-        <v>0</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="67" t="s">
+      <c r="C21" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="64">
-        <v>0</v>
-      </c>
-      <c r="F19" s="68" t="s">
+      <c r="D21" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="47" t="s">
+      <c r="E21" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="69">
-        <v>2</v>
-      </c>
-      <c r="K19" s="79"/>
-    </row>
-    <row r="20" ht="15.75" spans="1:11">
-      <c r="A20" s="61">
-        <v>0</v>
-      </c>
-      <c r="B20" s="62">
+      <c r="G21" s="67">
+        <v>-2</v>
+      </c>
+      <c r="H21" s="71"/>
+      <c r="K21" s="82"/>
+    </row>
+    <row r="22" ht="16.5" spans="1:11">
+      <c r="A22" s="73">
         <v>1</v>
       </c>
-      <c r="C20" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="47"/>
-      <c r="H20" s="66"/>
-      <c r="K20" s="79"/>
-    </row>
-    <row r="21" ht="15.75" spans="1:11">
-      <c r="A21" s="61">
-        <v>0.5</v>
-      </c>
-      <c r="B21" s="62">
+      <c r="B22" s="74">
         <v>1</v>
       </c>
-      <c r="C21" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="47" t="s">
+      <c r="C22" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="69"/>
-      <c r="K21" s="79"/>
-    </row>
-    <row r="22" ht="16.5" spans="1:11">
-      <c r="A22" s="71">
+      <c r="D22" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="78">
+        <v>-3</v>
+      </c>
+      <c r="H22" s="71"/>
+      <c r="K22" s="82"/>
+    </row>
+    <row r="23" ht="15.75" spans="1:11">
+      <c r="A23" s="79">
         <v>1</v>
       </c>
-      <c r="B22" s="72">
-        <v>1</v>
-      </c>
-      <c r="C22" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="75" t="s">
+      <c r="B23" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="69"/>
-      <c r="K22" s="79"/>
-    </row>
-    <row r="23" ht="15.75" spans="1:11">
-      <c r="A23" s="76">
-        <v>1</v>
-      </c>
-      <c r="B23" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="78">
+      <c r="C23" s="81">
         <v>6</v>
       </c>
-      <c r="D23" s="77">
+      <c r="D23" s="80">
         <v>2</v>
       </c>
       <c r="E23" s="58"/>
@@ -3334,22 +3261,22 @@
         <v>3</v>
       </c>
       <c r="G23" s="47"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
     </row>
     <row r="24" ht="16.5" spans="1:11">
-      <c r="A24" s="71">
+      <c r="A24" s="73">
         <v>1</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="73">
+      <c r="B24" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="75">
         <v>8</v>
       </c>
-      <c r="D24" s="72">
+      <c r="D24" s="74">
         <v>4</v>
       </c>
       <c r="E24" s="52"/>
@@ -3357,60 +3284,60 @@
         <v>5.5</v>
       </c>
       <c r="G24" s="47"/>
-      <c r="H24" s="79">
+      <c r="H24" s="82">
         <v>17.5</v>
       </c>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
     </row>
     <row r="25" ht="16.5" spans="1:11">
-      <c r="A25" s="80"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
     </row>
     <row r="26" ht="15.75" spans="1:12">
-      <c r="A26" s="81"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="58"/>
-      <c r="C26" s="82" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="83"/>
+      <c r="C26" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="86"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="111"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="112"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="84" t="s">
+      <c r="A27" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="113"/>
-      <c r="L27" s="113"/>
+      <c r="C27" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3419,18 +3346,18 @@
       <c r="B28" s="47">
         <v>0</v>
       </c>
-      <c r="C28" s="88" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="89"/>
+      <c r="C28" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="92"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="111"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="112"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3439,18 +3366,18 @@
       <c r="B29" s="47">
         <v>0</v>
       </c>
-      <c r="C29" s="90" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="91"/>
+      <c r="C29" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="94"/>
       <c r="E29" s="47"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
       <c r="H29" s="47"/>
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="111"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="112"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3459,22 +3386,22 @@
       <c r="B30" s="47">
         <v>0</v>
       </c>
-      <c r="C30" s="90" t="s">
+      <c r="C30" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="E30" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="91" t="s">
+      <c r="F30" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="91"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="111"/>
+      <c r="H30" s="94"/>
+      <c r="J30" s="115"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="112"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3484,24 +3411,24 @@
         <v>1</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="F31" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="47" t="s">
+      <c r="G31" s="47" t="s">
         <v>66</v>
-      </c>
-      <c r="G31" s="47" t="s">
-        <v>67</v>
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="111"/>
-      <c r="L31" s="111"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="112"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3511,26 +3438,26 @@
         <v>1</v>
       </c>
       <c r="C32" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="E32" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="47" t="s">
-        <v>62</v>
-      </c>
       <c r="F32" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="47" t="s">
+      <c r="H32" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="J32" s="115"/>
-      <c r="K32" s="111"/>
-      <c r="L32" s="111"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="112"/>
+      <c r="L32" s="112"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3540,402 +3467,400 @@
         <v>1</v>
       </c>
       <c r="C33" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="E33" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="52" t="s">
+      <c r="F33" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="52" t="s">
+      <c r="G33" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="52" t="s">
+      <c r="H33" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="H33" s="52" t="s">
+      <c r="I33" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="I33" s="52" t="s">
+      <c r="J33" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="J33" s="53" t="s">
+      <c r="K33" s="112"/>
+      <c r="L33" s="112"/>
+    </row>
+    <row r="34" ht="15.75" spans="1:14">
+      <c r="A34" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="K33" s="111"/>
-      <c r="L33" s="111"/>
-    </row>
-    <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="94">
+      <c r="B34" s="97">
         <v>1</v>
       </c>
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="94"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="97"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
       <c r="N34" s="47"/>
     </row>
     <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="76">
+      <c r="A35" s="79">
         <v>1</v>
       </c>
-      <c r="B35" s="96" t="s">
+      <c r="B35" s="99" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="71"/>
+    </row>
+    <row r="36" ht="16.5" spans="1:11">
+      <c r="A36" s="73">
+        <v>1</v>
+      </c>
+      <c r="B36" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="69"/>
-    </row>
-    <row r="36" ht="16.5" spans="1:11">
-      <c r="A36" s="71">
-        <v>1</v>
-      </c>
-      <c r="B36" s="97" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="71" t="s">
+      <c r="C36" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="52"/>
       <c r="J36" s="53"/>
-      <c r="K36" s="69"/>
+      <c r="K36" s="71"/>
     </row>
     <row r="37" ht="15.75" spans="1:11">
-      <c r="A37" s="69"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
+      <c r="A37" s="71"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
-      <c r="K37" s="69"/>
+      <c r="K37" s="71"/>
     </row>
     <row r="38" ht="16.5" spans="1:11">
-      <c r="A38" s="69"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
-      <c r="K38" s="69"/>
+      <c r="K38" s="71"/>
     </row>
     <row r="39" ht="16.5" spans="1:11">
-      <c r="A39" s="69"/>
-      <c r="C39" s="76" t="s">
+      <c r="A39" s="71"/>
+      <c r="C39" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="99"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="71"/>
+    </row>
+    <row r="40" ht="15.75" spans="1:11">
+      <c r="A40" s="83"/>
+      <c r="B40" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="96"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69" t="s">
+      <c r="C40" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="69"/>
-    </row>
-    <row r="40" ht="15.75" spans="1:11">
-      <c r="A40" s="80"/>
-      <c r="B40" s="81" t="s">
+      <c r="D40" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="E40" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="F40" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="58" t="s">
+      <c r="G40" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="F40" s="96" t="s">
+      <c r="H40" s="102"/>
+      <c r="I40" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="H40" s="100">
-        <v>20</v>
-      </c>
-      <c r="I40" s="126" t="s">
-        <v>90</v>
-      </c>
-      <c r="J40" s="116"/>
-      <c r="K40" s="116"/>
+      <c r="J40" s="117"/>
+      <c r="K40" s="117"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
-      <c r="A41" s="80"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="46">
         <v>25</v>
       </c>
-      <c r="C41" s="64">
+      <c r="C41" s="65">
         <v>6</v>
       </c>
-      <c r="D41" s="64">
-        <v>4</v>
-      </c>
-      <c r="E41" s="64">
+      <c r="D41" s="65">
+        <v>3</v>
+      </c>
+      <c r="E41" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F41" s="65">
         <v>1.5</v>
       </c>
-      <c r="F41" s="101">
-        <v>12</v>
-      </c>
-      <c r="G41" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" s="69">
-        <v>4</v>
-      </c>
-      <c r="I41" s="127" t="s">
-        <v>92</v>
+      <c r="G41" s="103">
+        <v>9</v>
+      </c>
+      <c r="H41" s="71"/>
+      <c r="I41" s="129" t="s">
+        <v>89</v>
       </c>
       <c r="J41" s="47"/>
-      <c r="K41" s="69"/>
+      <c r="K41" s="71"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
-      <c r="A42" s="80"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="46">
         <v>50</v>
       </c>
-      <c r="C42" s="64">
+      <c r="C42" s="65">
         <v>10</v>
       </c>
-      <c r="D42" s="64">
-        <v>4</v>
-      </c>
-      <c r="E42" s="64">
+      <c r="D42" s="65">
+        <v>3</v>
+      </c>
+      <c r="E42" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F42" s="65">
         <v>2.5</v>
       </c>
-      <c r="F42" s="101">
-        <v>12</v>
-      </c>
-      <c r="G42" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="H42" s="69">
-        <v>10</v>
-      </c>
-      <c r="I42" s="69"/>
+      <c r="G42" s="103">
+        <v>9</v>
+      </c>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
       <c r="J42" s="47"/>
-      <c r="K42" s="69"/>
+      <c r="K42" s="71"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="80"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="46">
         <v>75</v>
       </c>
-      <c r="C43" s="64">
+      <c r="C43" s="65">
         <v>15</v>
       </c>
-      <c r="D43" s="64">
-        <v>4</v>
-      </c>
-      <c r="E43" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="101">
-        <v>12</v>
-      </c>
-      <c r="G43" s="69" t="s">
-        <v>95</v>
-      </c>
-      <c r="H43" s="69">
-        <v>12</v>
-      </c>
-      <c r="I43" s="69"/>
+      <c r="D43" s="65">
+        <v>3</v>
+      </c>
+      <c r="E43" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F43" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="G43" s="103">
+        <v>9</v>
+      </c>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
       <c r="J43" s="47"/>
-      <c r="K43" s="69"/>
+      <c r="K43" s="71"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
-      <c r="A44" s="80" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="102">
+      <c r="A44" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="104">
         <v>100</v>
       </c>
-      <c r="C44" s="64">
+      <c r="C44" s="65">
         <v>20</v>
       </c>
-      <c r="D44" s="64">
-        <v>4</v>
-      </c>
-      <c r="E44" s="98">
+      <c r="D44" s="65">
+        <v>3</v>
+      </c>
+      <c r="E44" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F44" s="101">
         <v>4.5</v>
       </c>
-      <c r="F44" s="101">
-        <v>12</v>
-      </c>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
+      <c r="G44" s="103">
+        <v>9</v>
+      </c>
+      <c r="H44" s="71"/>
       <c r="I44" s="47"/>
       <c r="J44" s="47"/>
-      <c r="K44" s="69"/>
+      <c r="K44" s="71"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
-      <c r="A45" s="80" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="103">
+      <c r="A45" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="105">
         <v>125</v>
       </c>
-      <c r="C45" s="64">
+      <c r="C45" s="65">
         <v>24</v>
       </c>
-      <c r="D45" s="64">
-        <v>4</v>
-      </c>
-      <c r="E45" s="98" t="s">
-        <v>98</v>
+      <c r="D45" s="65">
+        <v>3</v>
+      </c>
+      <c r="E45" s="65">
+        <v>3.5</v>
       </c>
       <c r="F45" s="101">
-        <v>12</v>
-      </c>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
+        <v>5.25</v>
+      </c>
+      <c r="G45" s="103">
+        <v>9</v>
+      </c>
+      <c r="H45" s="71"/>
       <c r="I45" s="47"/>
       <c r="J45" s="47"/>
-      <c r="K45" s="69"/>
+      <c r="K45" s="71"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
-      <c r="A46" s="80" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="103">
+      <c r="A46" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="105">
         <v>150</v>
       </c>
-      <c r="C46" s="64">
+      <c r="C46" s="65">
         <v>28</v>
       </c>
-      <c r="D46" s="64">
-        <v>4</v>
-      </c>
-      <c r="E46" s="98" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="101">
-        <v>12</v>
-      </c>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
+      <c r="D46" s="65">
+        <v>3</v>
+      </c>
+      <c r="E46" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F46" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" s="103">
+        <v>9</v>
+      </c>
+      <c r="H46" s="71"/>
       <c r="I46" s="47"/>
       <c r="J46" s="47"/>
-      <c r="K46" s="69"/>
+      <c r="K46" s="71"/>
     </row>
     <row r="47" ht="15.75" spans="1:11">
-      <c r="A47" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="103">
+      <c r="A47" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="105">
         <v>175</v>
       </c>
-      <c r="C47" s="64">
+      <c r="C47" s="65">
         <v>32</v>
       </c>
-      <c r="D47" s="64">
-        <v>4</v>
-      </c>
-      <c r="E47" s="98" t="s">
-        <v>102</v>
-      </c>
-      <c r="F47" s="101">
-        <v>12</v>
-      </c>
-      <c r="G47" s="69"/>
-      <c r="H47" s="47" t="s">
-        <v>103</v>
-      </c>
+      <c r="D47" s="65">
+        <v>3</v>
+      </c>
+      <c r="E47" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F47" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47" s="103">
+        <v>9</v>
+      </c>
+      <c r="H47" s="47"/>
       <c r="I47" s="47"/>
       <c r="J47" s="47"/>
-      <c r="K47" s="69"/>
+      <c r="K47" s="71"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
-      <c r="A48" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="103">
+      <c r="A48" s="83" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="105">
         <v>200</v>
       </c>
-      <c r="C48" s="64">
+      <c r="C48" s="65">
         <v>37</v>
       </c>
-      <c r="D48" s="64">
-        <v>5</v>
-      </c>
-      <c r="E48" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" s="101">
-        <v>13</v>
-      </c>
-      <c r="G48" s="69" t="s">
-        <v>106</v>
+      <c r="D48" s="65">
+        <v>4</v>
+      </c>
+      <c r="E48" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F48" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="103">
+        <v>10</v>
       </c>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="69"/>
+      <c r="K48" s="71"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
-      <c r="A49" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="102">
+      <c r="A49" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="104">
         <v>225</v>
       </c>
-      <c r="C49" s="64">
+      <c r="C49" s="65">
         <v>44</v>
       </c>
-      <c r="D49" s="64">
-        <v>5</v>
-      </c>
-      <c r="E49" s="64">
+      <c r="D49" s="65">
+        <v>4</v>
+      </c>
+      <c r="E49" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F49" s="65">
         <v>8.25</v>
       </c>
-      <c r="F49" s="101">
-        <v>13</v>
-      </c>
-      <c r="G49" s="69"/>
+      <c r="G49" s="103">
+        <v>10</v>
+      </c>
       <c r="H49" s="47"/>
       <c r="I49" s="47"/>
       <c r="J49" s="47"/>
-      <c r="K49" s="69"/>
+      <c r="K49" s="71"/>
     </row>
     <row r="50" ht="15.75" spans="1:11">
-      <c r="A50" s="80" t="s">
-        <v>108</v>
+      <c r="A50" s="83" t="s">
+        <v>99</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
@@ -3943,24 +3868,26 @@
       <c r="C50" s="47">
         <v>50</v>
       </c>
-      <c r="D50" s="47">
-        <v>5</v>
-      </c>
-      <c r="E50" s="47">
+      <c r="D50" s="65">
+        <v>4</v>
+      </c>
+      <c r="E50" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F50" s="47">
         <v>9</v>
       </c>
-      <c r="F50" s="48">
-        <v>13</v>
-      </c>
-      <c r="G50" s="98"/>
+      <c r="G50" s="103">
+        <v>10</v>
+      </c>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
       <c r="J50" s="47"/>
-      <c r="K50" s="69"/>
+      <c r="K50" s="71"/>
     </row>
     <row r="51" ht="15.75" spans="1:11">
-      <c r="A51" s="80" t="s">
-        <v>109</v>
+      <c r="A51" s="83" t="s">
+        <v>100</v>
       </c>
       <c r="B51" s="46">
         <v>275</v>
@@ -3968,24 +3895,26 @@
       <c r="C51" s="47">
         <v>56</v>
       </c>
-      <c r="D51" s="47">
-        <v>5</v>
-      </c>
-      <c r="E51" s="47">
+      <c r="D51" s="65">
+        <v>4</v>
+      </c>
+      <c r="E51" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F51" s="47">
         <v>9.5</v>
       </c>
-      <c r="F51" s="48">
-        <v>13</v>
-      </c>
-      <c r="G51" s="69"/>
-      <c r="H51" s="69"/>
+      <c r="G51" s="103">
+        <v>10</v>
+      </c>
+      <c r="H51" s="71"/>
       <c r="I51" s="47"/>
       <c r="J51" s="47"/>
-      <c r="K51" s="69"/>
+      <c r="K51" s="71"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="80" t="s">
-        <v>110</v>
+      <c r="A52" s="83" t="s">
+        <v>101</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -3993,27 +3922,27 @@
       <c r="C52" s="47">
         <v>63</v>
       </c>
-      <c r="D52" s="47">
-        <v>5</v>
-      </c>
-      <c r="E52" s="47">
+      <c r="D52" s="65">
+        <v>4</v>
+      </c>
+      <c r="E52" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="F52" s="47">
         <v>10</v>
       </c>
-      <c r="F52" s="48">
-        <v>14</v>
-      </c>
-      <c r="G52" s="47">
-        <v>13</v>
-      </c>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="79"/>
-      <c r="K52" s="79"/>
-      <c r="M52" s="69"/>
+      <c r="G52" s="48">
+        <v>11</v>
+      </c>
+      <c r="H52" s="71"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="82"/>
+      <c r="K52" s="82"/>
+      <c r="M52" s="71"/>
     </row>
     <row r="53" ht="16.5" spans="1:13">
-      <c r="A53" s="80" t="s">
-        <v>111</v>
+      <c r="A53" s="83" t="s">
+        <v>102</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -4022,21 +3951,23 @@
         <v>75</v>
       </c>
       <c r="D53" s="52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" s="52">
+        <v>3.5</v>
+      </c>
+      <c r="F53" s="52">
         <v>10.75</v>
       </c>
-      <c r="F53" s="53">
-        <v>14</v>
-      </c>
-      <c r="G53" s="47"/>
+      <c r="G53" s="53">
+        <v>11</v>
+      </c>
       <c r="H53" s="47"/>
       <c r="I53" s="47"/>
-      <c r="M53" s="69"/>
+      <c r="M53" s="71"/>
     </row>
     <row r="54" ht="15.75" spans="2:13">
-      <c r="B54" s="104">
+      <c r="B54" s="106">
         <v>350</v>
       </c>
       <c r="C54" s="58">
@@ -4046,33 +3977,37 @@
         <v>5</v>
       </c>
       <c r="E54" s="58">
+        <v>4.5</v>
+      </c>
+      <c r="F54" s="58">
         <v>11.5</v>
       </c>
-      <c r="F54" s="105">
-        <v>14</v>
-      </c>
-      <c r="G54" s="47"/>
+      <c r="G54" s="107">
+        <v>11</v>
+      </c>
       <c r="H54" s="47"/>
       <c r="I54" s="47"/>
-      <c r="M54" s="69"/>
+      <c r="M54" s="71"/>
     </row>
     <row r="55" ht="15.75" spans="2:9">
-      <c r="B55" s="102">
+      <c r="B55" s="104">
         <v>375</v>
       </c>
       <c r="C55" s="47">
         <v>58</v>
       </c>
-      <c r="D55" s="64">
-        <v>5</v>
+      <c r="D55" s="65">
+        <v>4</v>
       </c>
       <c r="E55" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="F55" s="47">
         <v>12.25</v>
       </c>
-      <c r="F55" s="48">
-        <v>14</v>
-      </c>
-      <c r="G55" s="47"/>
+      <c r="G55" s="48">
+        <v>11</v>
+      </c>
       <c r="H55" s="47"/>
       <c r="I55" s="47"/>
     </row>
@@ -4083,17 +4018,17 @@
       <c r="C56" s="47">
         <v>63</v>
       </c>
-      <c r="D56" s="64">
-        <v>5</v>
+      <c r="D56" s="65">
+        <v>4</v>
       </c>
       <c r="E56" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="F56" s="47">
         <v>13</v>
       </c>
-      <c r="F56" s="48">
-        <v>14</v>
-      </c>
-      <c r="G56" s="47" t="s">
-        <v>112</v>
+      <c r="G56" s="48">
+        <v>11</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="47"/>
@@ -4105,16 +4040,18 @@
       <c r="C57" s="47">
         <v>69</v>
       </c>
-      <c r="D57" s="64">
-        <v>5</v>
+      <c r="D57" s="65">
+        <v>4</v>
       </c>
       <c r="E57" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="F57" s="47">
         <v>13.5</v>
       </c>
-      <c r="F57" s="48">
-        <v>14</v>
-      </c>
-      <c r="G57" s="47"/>
+      <c r="G57" s="48">
+        <v>11</v>
+      </c>
       <c r="H57" s="47"/>
       <c r="I57" s="47"/>
     </row>
@@ -4125,58 +4062,62 @@
       <c r="C58" s="47">
         <v>75</v>
       </c>
-      <c r="D58" s="64">
-        <v>5</v>
+      <c r="D58" s="65">
+        <v>4</v>
       </c>
       <c r="E58" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="F58" s="47">
         <v>14</v>
       </c>
-      <c r="F58" s="48">
-        <v>14</v>
-      </c>
-      <c r="G58" s="47"/>
+      <c r="G58" s="48">
+        <v>11</v>
+      </c>
       <c r="H58" s="47"/>
       <c r="I58" s="47"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="103">
+      <c r="B59" s="105">
         <v>475</v>
       </c>
       <c r="C59" s="47">
         <v>81</v>
       </c>
-      <c r="D59" s="64">
-        <v>5</v>
+      <c r="D59" s="65">
+        <v>4</v>
       </c>
       <c r="E59" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="F59" s="47">
         <v>14.5</v>
       </c>
-      <c r="F59" s="48">
-        <v>14</v>
-      </c>
-      <c r="G59" s="47" t="s">
-        <v>113</v>
+      <c r="G59" s="48">
+        <v>11</v>
       </c>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
     </row>
     <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="106">
+      <c r="B60" s="108">
         <v>500</v>
       </c>
       <c r="C60" s="52">
         <v>87</v>
       </c>
       <c r="D60" s="52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E60" s="52">
+        <v>4.5</v>
+      </c>
+      <c r="F60" s="52">
         <v>15.25</v>
       </c>
-      <c r="F60" s="53">
-        <v>14</v>
-      </c>
-      <c r="G60" s="47"/>
+      <c r="G60" s="53">
+        <v>11</v>
+      </c>
       <c r="H60" s="47"/>
       <c r="I60" s="47"/>
     </row>
@@ -4198,22 +4139,17 @@
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47">
-        <v>13.5</v>
+        <v>10</v>
       </c>
       <c r="H63" s="47"/>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="4:9">
-      <c r="D64">
-        <v>13</v>
-      </c>
-      <c r="E64" s="47">
+    <row r="64" spans="5:9">
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47">
         <v>10</v>
       </c>
-      <c r="F64" s="107" t="s">
-        <v>114</v>
-      </c>
-      <c r="G64" s="47"/>
       <c r="H64" s="47"/>
       <c r="I64" s="47"/>
     </row>
@@ -4247,7 +4183,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4256,8 +4192,8 @@
       <c r="I69" s="47"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="117" t="s">
-        <v>116</v>
+      <c r="C70" s="118" t="s">
+        <v>104</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4273,19 +4209,19 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="118"/>
-      <c r="B72" s="99"/>
-      <c r="C72" s="119"/>
-      <c r="D72" s="119"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="G72" s="69"/>
-      <c r="H72" s="69"/>
-      <c r="I72" s="69"/>
-      <c r="J72" s="69"/>
-      <c r="K72" s="69"/>
+      <c r="A72" s="119"/>
+      <c r="B72" s="120"/>
+      <c r="C72" s="121"/>
+      <c r="D72" s="121"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="71"/>
+      <c r="J72" s="71"/>
+      <c r="K72" s="71"/>
       <c r="M72" s="47"/>
       <c r="N72" s="47"/>
     </row>
@@ -4307,13 +4243,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4334,7 +4270,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4356,11 +4292,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4381,12 +4317,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="128" t="s">
-        <v>124</v>
+      <c r="D77" s="130" t="s">
+        <v>112</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4399,7 +4335,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="118"/>
+      <c r="A78" s="119"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4407,18 +4343,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="E78" s="120"/>
+        <v>114</v>
+      </c>
+      <c r="E78" s="122"/>
       <c r="F78" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G78" s="120"/>
-      <c r="H78" s="120"/>
-      <c r="I78" s="120"/>
-      <c r="J78" s="120"/>
-      <c r="K78" s="120"/>
-      <c r="L78" s="120"/>
+        <v>115</v>
+      </c>
+      <c r="G78" s="122"/>
+      <c r="H78" s="122"/>
+      <c r="I78" s="122"/>
+      <c r="J78" s="122"/>
+      <c r="K78" s="122"/>
+      <c r="L78" s="122"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4431,7 +4367,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4452,11 +4388,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4475,8 +4411,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="128" t="s">
-        <v>124</v>
+      <c r="D81" s="130" t="s">
+        <v>112</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4498,7 +4434,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4517,7 +4453,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4536,7 +4472,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4551,7 +4487,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4748,8 +4684,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="121"/>
-      <c r="F103" s="121"/>
+      <c r="E103" s="123"/>
+      <c r="F103" s="123"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4834,7 +4770,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4853,31 +4789,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4885,28 +4821,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4914,28 +4850,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4943,28 +4879,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4972,28 +4908,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5001,28 +4937,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5030,28 +4966,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5059,28 +4995,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5088,28 +5024,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5117,28 +5053,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5146,28 +5082,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5175,28 +5111,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5204,28 +5140,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5233,33 +5169,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>220</v>
-      </c>
       <c r="G14" s="9" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5291,34 +5227,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5326,31 +5262,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5358,31 +5294,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5390,31 +5326,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5422,31 +5358,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5454,31 +5390,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5486,31 +5422,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5518,31 +5454,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5550,31 +5486,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5582,31 +5518,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5614,31 +5550,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5646,31 +5582,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5678,31 +5614,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5710,63 +5646,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sense and GM QoL Update
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="347">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">   5 | </t>
     </r>
     <r>
@@ -177,6 +183,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">5.75 |    </t>
     </r>
     <r>
@@ -192,6 +205,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> 13.5 | </t>
     </r>
     <r>
@@ -207,6 +227,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">   10 | </t>
     </r>
     <r>
@@ -222,6 +248,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> 11.5 | </t>
     </r>
     <r>
@@ -281,6 +314,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">18.5 | </t>
     </r>
     <r>
@@ -296,6 +336,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">15 | </t>
     </r>
     <r>
@@ -333,6 +380,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">17.5 | </t>
     </r>
     <r>
@@ -443,58 +497,171 @@
     <t>Defense</t>
   </si>
   <si>
-    <t>Player Defense</t>
-  </si>
-  <si>
-    <t>Effective Damage / round</t>
-  </si>
-  <si>
-    <t>Save DC</t>
+    <t>Direct Damage / round</t>
+  </si>
+  <si>
+    <t>Attack Damage / round
+assuming 3 Defense</t>
+  </si>
+  <si>
+    <t>Check Grade</t>
   </si>
   <si>
     <t>+5 per level</t>
   </si>
   <si>
+    <t>0.5 (1d4 - 2)</t>
+  </si>
+  <si>
+    <t>3.5 (1d6)</t>
+  </si>
+  <si>
     <t>+1 at level 6</t>
   </si>
   <si>
+    <t>1.5 (1d4 - 1)</t>
+  </si>
+  <si>
+    <t>4.5 (1d6 + 1)</t>
+  </si>
+  <si>
+    <t>2.5 (1d4)</t>
+  </si>
+  <si>
+    <t>5.5 (1d6 + 2)</t>
+  </si>
+  <si>
     <t>Level 1</t>
   </si>
   <si>
+    <t>6.5 (1d6 + 3)</t>
+  </si>
+  <si>
     <t>Level 2</t>
   </si>
   <si>
+    <t>4.5 (1d8)</t>
+  </si>
+  <si>
+    <t>7.5 (1d6 + 4)</t>
+  </si>
+  <si>
     <t>Level 3</t>
   </si>
   <si>
-    <t>(10) 6</t>
+    <t>5 (2d4)</t>
+  </si>
+  <si>
+    <t>8 (2d4 + 3)</t>
+  </si>
+  <si>
+    <t>1.5 + 3</t>
+  </si>
+  <si>
+    <t>6 (2d4 + 1)</t>
+  </si>
+  <si>
+    <t>9 (2d4 + 4)</t>
   </si>
   <si>
     <t>Level 4</t>
   </si>
   <si>
-    <t>(10.75) 6.75</t>
+    <t>9.5 (1d6 + 5)</t>
   </si>
   <si>
     <t>Level 5</t>
   </si>
   <si>
-    <t>(11.5) 7.5</t>
+    <t>7 (2d4 + 2)</t>
+  </si>
+  <si>
+    <t>10 (2d4 + 5)</t>
   </si>
   <si>
     <t>Level 6</t>
   </si>
   <si>
+    <t>10.5  (1d6 + 6)</t>
+  </si>
+  <si>
+    <t>11 (2d4 + 7)</t>
+  </si>
+  <si>
     <t>Level 7</t>
   </si>
   <si>
+    <t>8.5 (1d6 + 4)</t>
+  </si>
+  <si>
+    <t>11.5 (1d6 + 7)</t>
+  </si>
+  <si>
     <t>Level 8</t>
   </si>
   <si>
+    <t>9 (2d6 + 2)</t>
+  </si>
+  <si>
+    <t>12 (2d6 + 5)</t>
+  </si>
+  <si>
     <t>Level 9</t>
   </si>
   <si>
+    <t>10 (2d6 + 3)</t>
+  </si>
+  <si>
+    <t>13 (2d6 + 6)</t>
+  </si>
+  <si>
+    <t>10.75 (3d4 + 3)</t>
+  </si>
+  <si>
+    <t>13.75 (3d4 + 6)</t>
+  </si>
+  <si>
     <t>Level 10</t>
+  </si>
+  <si>
+    <t>11.5 (5d4 - 1)</t>
+  </si>
+  <si>
+    <t>14.5 (1d8 + 10)</t>
+  </si>
+  <si>
+    <t>12 (4d4 + 2)</t>
+  </si>
+  <si>
+    <t>15 (2d6 + 8)</t>
+  </si>
+  <si>
+    <t>12.5 (3d6 + 2)</t>
+  </si>
+  <si>
+    <t>15.5 (1d8 + 11)</t>
+  </si>
+  <si>
+    <t>13 (4d4 + 3)</t>
+  </si>
+  <si>
+    <t>16  (2d6 + 9)</t>
+  </si>
+  <si>
+    <t>13.5 (3d6 + 3)</t>
+  </si>
+  <si>
+    <t>16.5  (1d8 + 12)</t>
+  </si>
+  <si>
+    <t>The double of another column
+should be 120% of its half
+E.g. 400XP HP = 1.2 * 2 * 200XP HP</t>
+  </si>
+  <si>
+    <t>The double of another column
+should be ~80% of its half
+E.g. 400XP dmg = 0.8 * 2 * 200XP dmg</t>
   </si>
   <si>
     <t>XP Rules</t>
@@ -1131,12 +1298,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1294,14 +1461,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color rgb="FFCB5D13"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1317,6 +1476,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1324,16 +1490,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1354,7 +1521,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1369,7 +1536,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1378,21 +1545,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1415,9 +1567,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1440,21 +1605,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1482,7 +1641,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1494,175 +1815,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,36 +2004,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1899,6 +2028,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1908,13 +2052,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1936,9 +2093,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1947,15 +2106,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1968,131 +2127,131 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2273,9 +2432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2294,9 +2450,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2325,9 +2478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2399,7 +2549,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2411,14 +2564,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2429,6 +2582,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2444,19 +2600,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2477,7 +2630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
@@ -2815,8 +2968,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2826,7 +2979,7 @@
     <col min="3" max="3" width="24.4666666666667" customWidth="1"/>
     <col min="4" max="4" width="25.9619047619048" customWidth="1"/>
     <col min="5" max="5" width="30.8" customWidth="1"/>
-    <col min="6" max="6" width="33.5428571428571" customWidth="1"/>
+    <col min="6" max="6" width="33.9047619047619" customWidth="1"/>
     <col min="7" max="7" width="27.952380952381" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="10" width="17.4285714285714" customWidth="1"/>
@@ -2848,13 +3001,13 @@
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
-      <c r="L3" s="82" t="s">
+      <c r="L3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="82"/>
+      <c r="N3" s="79"/>
     </row>
     <row r="4" ht="15.75" spans="2:14">
       <c r="B4" s="29" t="s">
@@ -2869,13 +3022,13 @@
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="L4" s="82" t="s">
+      <c r="L4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="71" t="s">
+      <c r="M4" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="82"/>
+      <c r="N4" s="79"/>
     </row>
     <row r="5" ht="15.75" spans="2:14">
       <c r="B5" s="32" t="s">
@@ -2890,13 +3043,13 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="33"/>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="71" t="s">
+      <c r="M5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="71"/>
+      <c r="N5" s="69"/>
     </row>
     <row r="6" ht="16.5" spans="2:14">
       <c r="B6" s="34" t="s">
@@ -2909,25 +3062,25 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="L6" s="82" t="s">
+      <c r="L6" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="71" t="s">
+      <c r="M6" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="71"/>
+      <c r="N6" s="69"/>
     </row>
     <row r="7" ht="16.5" spans="5:14">
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="109" t="s">
+      <c r="L7" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="71" t="s">
+      <c r="M7" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="71"/>
+      <c r="N7" s="69"/>
     </row>
     <row r="8" ht="16.5" spans="3:14">
       <c r="C8" s="37" t="s">
@@ -2937,11 +3090,11 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="109" t="s">
+      <c r="L8" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="109"/>
-      <c r="N8" s="82"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="79"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="41" t="s">
@@ -2973,13 +3126,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="122" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -2991,24 +3144,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="125" t="s">
+      <c r="G10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="110">
+      <c r="I10" s="108">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="122" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -3020,24 +3173,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="125" t="s">
+      <c r="G11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="110">
+      <c r="I11" s="108">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="126" t="s">
+      <c r="A12" s="124" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="127" t="s">
+      <c r="C12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -3049,13 +3202,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="127" t="s">
+      <c r="G12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="111">
+      <c r="I12" s="109">
         <v>11.5</v>
       </c>
     </row>
@@ -3064,7 +3217,7 @@
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" ht="15.75" spans="2:6">
       <c r="B15" s="47"/>
       <c r="D15" s="47"/>
       <c r="E15" s="47"/>
@@ -3089,171 +3242,171 @@
       <c r="F16" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="60" t="s">
+      <c r="G16" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="61"/>
+      <c r="H16" s="60"/>
     </row>
     <row r="17" ht="15.75" spans="1:8">
-      <c r="A17" s="62">
+      <c r="A17" s="61">
         <v>0</v>
       </c>
-      <c r="B17" s="63">
+      <c r="B17" s="62">
         <v>0</v>
       </c>
       <c r="C17" s="47">
         <v>0</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="63">
         <v>0</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="64">
         <v>0</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F17" s="65">
         <v>0</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="65">
         <v>0</v>
       </c>
       <c r="H17" s="47"/>
     </row>
     <row r="18" ht="15.75" spans="1:11">
-      <c r="A18" s="62">
+      <c r="A18" s="61">
         <v>0.5</v>
       </c>
-      <c r="B18" s="63">
+      <c r="B18" s="62">
         <v>0</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="64">
         <v>0</v>
       </c>
-      <c r="F18" s="70" t="s">
+      <c r="F18" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="65">
         <v>-1</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="K18" s="82"/>
+      <c r="H18" s="66"/>
+      <c r="K18" s="79"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">
-      <c r="A19" s="62">
+      <c r="A19" s="61">
         <v>1</v>
       </c>
-      <c r="B19" s="63">
+      <c r="B19" s="62">
         <v>0</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="64">
         <v>0</v>
       </c>
-      <c r="F19" s="70" t="s">
+      <c r="F19" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="65">
         <v>-2</v>
       </c>
-      <c r="H19" s="71"/>
-      <c r="K19" s="82"/>
+      <c r="H19" s="69"/>
+      <c r="K19" s="79"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
-      <c r="A20" s="62">
+      <c r="A20" s="61">
         <v>0</v>
       </c>
-      <c r="B20" s="63">
+      <c r="B20" s="62">
         <v>1</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="72" t="s">
+      <c r="E20" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="70" t="s">
+      <c r="F20" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="67">
+      <c r="G20" s="65">
         <v>-1</v>
       </c>
-      <c r="H20" s="68"/>
-      <c r="K20" s="82"/>
+      <c r="H20" s="66"/>
+      <c r="K20" s="79"/>
     </row>
     <row r="21" ht="15.75" spans="1:11">
-      <c r="A21" s="62">
+      <c r="A21" s="61">
         <v>0.5</v>
       </c>
-      <c r="B21" s="63">
+      <c r="B21" s="62">
         <v>1</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="D21" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="70" t="s">
+      <c r="F21" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="67">
+      <c r="G21" s="65">
         <v>-2</v>
       </c>
-      <c r="H21" s="71"/>
-      <c r="K21" s="82"/>
+      <c r="H21" s="69"/>
+      <c r="K21" s="79"/>
     </row>
     <row r="22" ht="16.5" spans="1:11">
-      <c r="A22" s="73">
+      <c r="A22" s="71">
         <v>1</v>
       </c>
-      <c r="B22" s="74">
+      <c r="B22" s="72">
         <v>1</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="77" t="s">
+      <c r="F22" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="78">
+      <c r="G22" s="50">
         <v>-3</v>
       </c>
-      <c r="H22" s="71"/>
-      <c r="K22" s="82"/>
+      <c r="H22" s="69"/>
+      <c r="K22" s="79"/>
     </row>
     <row r="23" ht="15.75" spans="1:11">
-      <c r="A23" s="79">
+      <c r="A23" s="76">
         <v>1</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="81">
+      <c r="C23" s="78">
         <v>6</v>
       </c>
-      <c r="D23" s="80">
+      <c r="D23" s="77">
         <v>2</v>
       </c>
       <c r="E23" s="58"/>
@@ -3261,22 +3414,22 @@
         <v>3</v>
       </c>
       <c r="G23" s="47"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
     </row>
     <row r="24" ht="16.5" spans="1:11">
-      <c r="A24" s="73">
+      <c r="A24" s="71">
         <v>1</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="75">
+      <c r="C24" s="73">
         <v>8</v>
       </c>
-      <c r="D24" s="74">
+      <c r="D24" s="72">
         <v>4</v>
       </c>
       <c r="E24" s="52"/>
@@ -3284,60 +3437,60 @@
         <v>5.5</v>
       </c>
       <c r="G24" s="47"/>
-      <c r="H24" s="82">
+      <c r="H24" s="79">
         <v>17.5</v>
       </c>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
     </row>
     <row r="25" ht="16.5" spans="1:11">
-      <c r="A25" s="83"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
     </row>
     <row r="26" ht="15.75" spans="1:12">
-      <c r="A26" s="84"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="58"/>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="86"/>
+      <c r="D26" s="83"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="112"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="111"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3346,18 +3499,18 @@
       <c r="B28" s="47">
         <v>0</v>
       </c>
-      <c r="C28" s="91" t="s">
+      <c r="C28" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="92"/>
+      <c r="D28" s="89"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="112"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="111"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3366,18 +3519,18 @@
       <c r="B29" s="47">
         <v>0</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="C29" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="94"/>
+      <c r="D29" s="91"/>
       <c r="E29" s="47"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
       <c r="H29" s="47"/>
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="112"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="111"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3386,22 +3539,22 @@
       <c r="B30" s="47">
         <v>0</v>
       </c>
-      <c r="C30" s="93" t="s">
+      <c r="C30" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="94" t="s">
+      <c r="E30" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="94"/>
-      <c r="J30" s="115"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="112"/>
+      <c r="H30" s="91"/>
+      <c r="J30" s="114"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="111"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3427,8 +3580,8 @@
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="112"/>
-      <c r="L31" s="112"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="111"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3455,9 +3608,9 @@
       <c r="H32" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="J32" s="116"/>
-      <c r="K32" s="112"/>
-      <c r="L32" s="112"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="111"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3490,111 +3643,111 @@
       <c r="J33" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="K33" s="112"/>
-      <c r="L33" s="112"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="97">
+      <c r="B34" s="94">
         <v>1</v>
       </c>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="97"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="94"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
       <c r="N34" s="47"/>
     </row>
     <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="79">
+      <c r="A35" s="76">
         <v>1</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="107"/>
-      <c r="K35" s="71"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="69"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
-      <c r="A36" s="73">
+      <c r="A36" s="71">
         <v>1</v>
       </c>
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="75" t="s">
+      <c r="D36" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
       <c r="I36" s="52"/>
       <c r="J36" s="53"/>
-      <c r="K36" s="71"/>
+      <c r="K36" s="69"/>
     </row>
     <row r="37" ht="15.75" spans="1:11">
-      <c r="A37" s="71"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
-      <c r="K37" s="71"/>
+      <c r="K37" s="69"/>
     </row>
     <row r="38" ht="16.5" spans="1:11">
-      <c r="A38" s="71"/>
-      <c r="B38" s="101"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
-      <c r="K38" s="71"/>
+      <c r="K38" s="69"/>
     </row>
     <row r="39" ht="16.5" spans="1:11">
-      <c r="A39" s="71"/>
-      <c r="C39" s="79" t="s">
+      <c r="A39" s="69"/>
+      <c r="C39" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="99"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
+      <c r="D39" s="96"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
       <c r="J39" s="47"/>
-      <c r="K39" s="71"/>
-    </row>
-    <row r="40" ht="15.75" spans="1:11">
-      <c r="A40" s="83"/>
-      <c r="B40" s="84" t="s">
+      <c r="K39" s="69"/>
+    </row>
+    <row r="40" ht="30" spans="1:11">
+      <c r="A40" s="80"/>
+      <c r="B40" s="81" t="s">
         <v>82</v>
       </c>
       <c r="C40" s="58" t="s">
@@ -3606,431 +3759,417 @@
       <c r="E40" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="58" t="s">
+      <c r="F40" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="99" t="s">
+      <c r="G40" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="102"/>
-      <c r="I40" s="128" t="s">
+      <c r="I40" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="J40" s="117"/>
-      <c r="K40" s="117"/>
+      <c r="J40" s="116"/>
+      <c r="K40" s="116"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
-      <c r="A41" s="83"/>
+      <c r="A41" s="80"/>
       <c r="B41" s="46">
         <v>25</v>
       </c>
-      <c r="C41" s="65">
-        <v>6</v>
-      </c>
-      <c r="D41" s="65">
+      <c r="C41" s="64">
+        <v>5</v>
+      </c>
+      <c r="D41" s="64">
         <v>3</v>
       </c>
-      <c r="E41" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F41" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="G41" s="103">
-        <v>9</v>
-      </c>
-      <c r="H41" s="71"/>
-      <c r="I41" s="129" t="s">
+      <c r="E41" s="64" t="s">
         <v>89</v>
       </c>
+      <c r="F41" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="101">
+        <v>10</v>
+      </c>
+      <c r="I41" s="127" t="s">
+        <v>91</v>
+      </c>
       <c r="J41" s="47"/>
-      <c r="K41" s="71"/>
+      <c r="K41" s="69"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
-      <c r="A42" s="83"/>
+      <c r="A42" s="80"/>
       <c r="B42" s="46">
         <v>50</v>
       </c>
-      <c r="C42" s="65">
+      <c r="C42" s="64">
         <v>10</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="64">
         <v>3</v>
       </c>
-      <c r="E42" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F42" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="G42" s="103">
-        <v>9</v>
-      </c>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
+      <c r="E42" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="101">
+        <v>10</v>
+      </c>
+      <c r="I42" s="69"/>
       <c r="J42" s="47"/>
-      <c r="K42" s="71"/>
+      <c r="K42" s="69"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="83"/>
+      <c r="A43" s="80"/>
       <c r="B43" s="46">
         <v>75</v>
       </c>
-      <c r="C43" s="65">
+      <c r="C43" s="64">
         <v>15</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="64">
         <v>3</v>
       </c>
-      <c r="E43" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F43" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="G43" s="103">
-        <v>9</v>
-      </c>
-      <c r="H43" s="71"/>
-      <c r="I43" s="71"/>
+      <c r="E43" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="G43" s="101">
+        <v>10</v>
+      </c>
+      <c r="I43" s="69"/>
       <c r="J43" s="47"/>
-      <c r="K43" s="71"/>
+      <c r="K43" s="69"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
-      <c r="A44" s="83" t="s">
+      <c r="A44" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="102">
+        <v>100</v>
+      </c>
+      <c r="C44" s="64">
+        <v>20</v>
+      </c>
+      <c r="D44" s="64">
+        <v>3</v>
+      </c>
+      <c r="E44" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="104">
-        <v>100</v>
-      </c>
-      <c r="C44" s="65">
-        <v>20</v>
-      </c>
-      <c r="D44" s="65">
-        <v>3</v>
-      </c>
-      <c r="E44" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F44" s="101">
-        <v>4.5</v>
-      </c>
-      <c r="G44" s="103">
-        <v>9</v>
-      </c>
-      <c r="H44" s="71"/>
+      <c r="F44" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="101">
+        <v>10</v>
+      </c>
       <c r="I44" s="47"/>
       <c r="J44" s="47"/>
-      <c r="K44" s="71"/>
+      <c r="K44" s="69"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
-      <c r="A45" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="105">
+      <c r="A45" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="103">
         <v>125</v>
       </c>
-      <c r="C45" s="65">
-        <v>24</v>
-      </c>
-      <c r="D45" s="65">
+      <c r="C45" s="64">
+        <v>27</v>
+      </c>
+      <c r="D45" s="64">
         <v>3</v>
       </c>
-      <c r="E45" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F45" s="101">
-        <v>5.25</v>
-      </c>
-      <c r="G45" s="103">
-        <v>9</v>
-      </c>
-      <c r="H45" s="71"/>
+      <c r="E45" s="98" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="101">
+        <v>10</v>
+      </c>
       <c r="I45" s="47"/>
       <c r="J45" s="47"/>
-      <c r="K45" s="71"/>
+      <c r="K45" s="69"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
-      <c r="A46" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="105">
+      <c r="A46" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="103">
         <v>150</v>
       </c>
-      <c r="C46" s="65">
-        <v>28</v>
-      </c>
-      <c r="D46" s="65">
+      <c r="C46" s="64">
+        <v>33</v>
+      </c>
+      <c r="D46" s="64">
         <v>3</v>
       </c>
-      <c r="E46" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F46" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="G46" s="103">
-        <v>9</v>
-      </c>
-      <c r="H46" s="71"/>
+      <c r="E46" s="98" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" s="100" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" s="101">
+        <v>10</v>
+      </c>
+      <c r="H46" t="s">
+        <v>104</v>
+      </c>
       <c r="I46" s="47"/>
       <c r="J46" s="47"/>
-      <c r="K46" s="71"/>
-    </row>
-    <row r="47" ht="15.75" spans="1:11">
-      <c r="A47" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="105">
+      <c r="K46" s="69"/>
+    </row>
+    <row r="47" ht="15.75" spans="2:11">
+      <c r="B47" s="103">
         <v>175</v>
       </c>
-      <c r="C47" s="65">
-        <v>32</v>
-      </c>
-      <c r="D47" s="65">
+      <c r="C47" s="64">
+        <v>39</v>
+      </c>
+      <c r="D47" s="64">
         <v>3</v>
       </c>
-      <c r="E47" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F47" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="103">
-        <v>9</v>
-      </c>
-      <c r="H47" s="47"/>
+      <c r="E47" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="101">
+        <v>10</v>
+      </c>
       <c r="I47" s="47"/>
       <c r="J47" s="47"/>
-      <c r="K47" s="71"/>
+      <c r="K47" s="69"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
-      <c r="A48" s="83" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="105">
+      <c r="A48" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="103">
         <v>200</v>
       </c>
-      <c r="C48" s="65">
-        <v>37</v>
-      </c>
-      <c r="D48" s="65">
+      <c r="C48" s="64">
+        <v>47</v>
+      </c>
+      <c r="D48" s="64">
         <v>4</v>
       </c>
-      <c r="E48" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F48" s="65" t="s">
+      <c r="E48" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="G48" s="103">
-        <v>10</v>
-      </c>
-      <c r="H48" s="47"/>
+      <c r="F48" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="101">
+        <v>11</v>
+      </c>
       <c r="I48" s="47"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="71"/>
+      <c r="K48" s="69"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
-      <c r="A49" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="104">
+      <c r="A49" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="102">
         <v>225</v>
       </c>
-      <c r="C49" s="65">
-        <v>44</v>
-      </c>
-      <c r="D49" s="65">
+      <c r="C49" s="64">
+        <v>54</v>
+      </c>
+      <c r="D49" s="64">
         <v>4</v>
       </c>
-      <c r="E49" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F49" s="65">
-        <v>8.25</v>
-      </c>
-      <c r="G49" s="103">
-        <v>10</v>
-      </c>
-      <c r="H49" s="47"/>
+      <c r="E49" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" s="101">
+        <v>11</v>
+      </c>
       <c r="I49" s="47"/>
       <c r="J49" s="47"/>
-      <c r="K49" s="71"/>
+      <c r="K49" s="69"/>
     </row>
     <row r="50" ht="15.75" spans="1:11">
-      <c r="A50" s="83" t="s">
-        <v>99</v>
+      <c r="A50" s="80" t="s">
+        <v>112</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
       </c>
       <c r="C50" s="47">
-        <v>50</v>
-      </c>
-      <c r="D50" s="65">
+        <v>65</v>
+      </c>
+      <c r="D50" s="64">
         <v>4</v>
       </c>
-      <c r="E50" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F50" s="47">
-        <v>9</v>
-      </c>
-      <c r="G50" s="103">
-        <v>10</v>
-      </c>
-      <c r="H50" s="47"/>
+      <c r="E50" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="100" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="101">
+        <v>11</v>
+      </c>
       <c r="I50" s="47"/>
       <c r="J50" s="47"/>
-      <c r="K50" s="71"/>
-    </row>
-    <row r="51" ht="15.75" spans="1:11">
-      <c r="A51" s="83" t="s">
-        <v>100</v>
-      </c>
+      <c r="K50" s="69"/>
+    </row>
+    <row r="51" ht="15.75" spans="2:11">
       <c r="B51" s="46">
         <v>275</v>
       </c>
       <c r="C51" s="47">
-        <v>56</v>
-      </c>
-      <c r="D51" s="65">
+        <v>73</v>
+      </c>
+      <c r="D51" s="64">
         <v>4</v>
       </c>
-      <c r="E51" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F51" s="47">
-        <v>9.5</v>
-      </c>
-      <c r="G51" s="103">
-        <v>10</v>
-      </c>
-      <c r="H51" s="71"/>
+      <c r="E51" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="100" t="s">
+        <v>114</v>
+      </c>
+      <c r="G51" s="101">
+        <v>11</v>
+      </c>
       <c r="I51" s="47"/>
       <c r="J51" s="47"/>
-      <c r="K51" s="71"/>
+      <c r="K51" s="69"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="83" t="s">
-        <v>101</v>
+      <c r="A52" s="80" t="s">
+        <v>115</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
       </c>
       <c r="C52" s="47">
-        <v>63</v>
-      </c>
-      <c r="D52" s="65">
+        <v>80</v>
+      </c>
+      <c r="D52" s="64">
         <v>4</v>
       </c>
-      <c r="E52" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F52" s="47">
-        <v>10</v>
+      <c r="E52" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="100" t="s">
+        <v>117</v>
       </c>
       <c r="G52" s="48">
-        <v>11</v>
-      </c>
-      <c r="H52" s="71"/>
-      <c r="I52" s="71"/>
-      <c r="J52" s="82"/>
-      <c r="K52" s="82"/>
-      <c r="M52" s="71"/>
+        <v>12</v>
+      </c>
+      <c r="I52" s="69"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="M52" s="69"/>
     </row>
     <row r="53" ht="16.5" spans="1:13">
-      <c r="A53" s="83" t="s">
-        <v>102</v>
+      <c r="A53" s="80" t="s">
+        <v>118</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
       </c>
       <c r="C53" s="52">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D53" s="52">
-        <v>4</v>
-      </c>
-      <c r="E53" s="52">
-        <v>3.5</v>
-      </c>
-      <c r="F53" s="52">
-        <v>10.75</v>
+        <v>5</v>
+      </c>
+      <c r="E53" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="F53" s="104" t="s">
+        <v>120</v>
       </c>
       <c r="G53" s="53">
-        <v>11</v>
-      </c>
-      <c r="H53" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I53" s="47"/>
-      <c r="M53" s="71"/>
-    </row>
-    <row r="54" ht="15.75" spans="2:13">
-      <c r="B54" s="106">
+      <c r="M53" s="69"/>
+    </row>
+    <row r="54" ht="15.75" spans="1:13">
+      <c r="A54" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="103">
         <v>350</v>
       </c>
-      <c r="C54" s="58">
-        <v>54</v>
-      </c>
-      <c r="D54" s="58">
+      <c r="C54" s="64">
+        <v>93</v>
+      </c>
+      <c r="D54" s="64">
         <v>5</v>
       </c>
-      <c r="E54" s="58">
-        <v>4.5</v>
-      </c>
-      <c r="F54" s="58">
-        <v>11.5</v>
-      </c>
-      <c r="G54" s="107">
-        <v>11</v>
-      </c>
-      <c r="H54" s="47"/>
+      <c r="E54" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="F54" s="100" t="s">
+        <v>123</v>
+      </c>
+      <c r="G54" s="48">
+        <v>12</v>
+      </c>
       <c r="I54" s="47"/>
-      <c r="M54" s="71"/>
+      <c r="M54" s="69"/>
     </row>
     <row r="55" ht="15.75" spans="2:9">
-      <c r="B55" s="104">
+      <c r="B55" s="102">
         <v>375</v>
       </c>
       <c r="C55" s="47">
-        <v>58</v>
-      </c>
-      <c r="D55" s="65">
-        <v>4</v>
-      </c>
-      <c r="E55" s="47">
-        <v>4.5</v>
-      </c>
-      <c r="F55" s="47">
-        <v>12.25</v>
+        <v>99</v>
+      </c>
+      <c r="D55" s="64">
+        <v>5</v>
+      </c>
+      <c r="E55" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F55" s="100" t="s">
+        <v>125</v>
       </c>
       <c r="G55" s="48">
-        <v>11</v>
-      </c>
-      <c r="H55" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I55" s="47"/>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" ht="15.75" spans="1:9">
+      <c r="A56" s="80" t="s">
+        <v>126</v>
+      </c>
       <c r="B56" s="46">
         <v>400</v>
       </c>
       <c r="C56" s="47">
-        <v>63</v>
-      </c>
-      <c r="D56" s="65">
-        <v>4</v>
-      </c>
-      <c r="E56" s="47">
-        <v>4.5</v>
-      </c>
-      <c r="F56" s="47">
-        <v>13</v>
+        <v>105</v>
+      </c>
+      <c r="D56" s="64">
+        <v>5</v>
+      </c>
+      <c r="E56" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="100" t="s">
+        <v>128</v>
       </c>
       <c r="G56" s="48">
-        <v>11</v>
-      </c>
-      <c r="H56" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I56" s="47"/>
     </row>
     <row r="57" spans="2:9">
@@ -4038,21 +4177,20 @@
         <v>425</v>
       </c>
       <c r="C57" s="47">
-        <v>69</v>
-      </c>
-      <c r="D57" s="65">
-        <v>4</v>
-      </c>
-      <c r="E57" s="47">
-        <v>4.5</v>
-      </c>
-      <c r="F57" s="47">
-        <v>13.5</v>
+        <v>118</v>
+      </c>
+      <c r="D57" s="64">
+        <v>5</v>
+      </c>
+      <c r="E57" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="F57" s="100" t="s">
+        <v>130</v>
       </c>
       <c r="G57" s="48">
-        <v>11</v>
-      </c>
-      <c r="H57" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I57" s="47"/>
     </row>
     <row r="58" spans="2:9">
@@ -4060,65 +4198,62 @@
         <v>450</v>
       </c>
       <c r="C58" s="47">
-        <v>75</v>
-      </c>
-      <c r="D58" s="65">
-        <v>4</v>
-      </c>
-      <c r="E58" s="47">
-        <v>4.5</v>
-      </c>
-      <c r="F58" s="47">
-        <v>14</v>
+        <v>130</v>
+      </c>
+      <c r="D58" s="64">
+        <v>5</v>
+      </c>
+      <c r="E58" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" s="100" t="s">
+        <v>132</v>
       </c>
       <c r="G58" s="48">
-        <v>11</v>
-      </c>
-      <c r="H58" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I58" s="47"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="105">
+      <c r="B59" s="103">
         <v>475</v>
       </c>
       <c r="C59" s="47">
-        <v>81</v>
-      </c>
-      <c r="D59" s="65">
-        <v>4</v>
-      </c>
-      <c r="E59" s="47">
-        <v>4.5</v>
-      </c>
-      <c r="F59" s="47">
-        <v>14.5</v>
+        <v>143</v>
+      </c>
+      <c r="D59" s="64">
+        <v>5</v>
+      </c>
+      <c r="E59" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="F59" s="100" t="s">
+        <v>134</v>
       </c>
       <c r="G59" s="48">
-        <v>11</v>
-      </c>
-      <c r="H59" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I59" s="47"/>
     </row>
     <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="108">
+      <c r="B60" s="105">
         <v>500</v>
       </c>
       <c r="C60" s="52">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="D60" s="52">
-        <v>4</v>
-      </c>
-      <c r="E60" s="52">
-        <v>4.5</v>
-      </c>
-      <c r="F60" s="52">
-        <v>15.25</v>
+        <v>5</v>
+      </c>
+      <c r="E60" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="F60" s="104" t="s">
+        <v>136</v>
       </c>
       <c r="G60" s="53">
-        <v>11</v>
-      </c>
-      <c r="H60" s="47"/>
+        <v>12</v>
+      </c>
       <c r="I60" s="47"/>
     </row>
     <row r="61" spans="5:9">
@@ -4128,9 +4263,14 @@
       <c r="H61" s="47"/>
       <c r="I61" s="47"/>
     </row>
-    <row r="62" spans="5:9">
+    <row r="62" ht="75" spans="3:9">
+      <c r="C62" s="106" t="s">
+        <v>137</v>
+      </c>
       <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
+      <c r="F62" s="106" t="s">
+        <v>138</v>
+      </c>
       <c r="G62" s="47"/>
       <c r="H62" s="47"/>
       <c r="I62" s="47"/>
@@ -4183,7 +4323,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4192,8 +4332,8 @@
       <c r="I69" s="47"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="118" t="s">
-        <v>104</v>
+      <c r="C70" s="106" t="s">
+        <v>140</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4209,19 +4349,19 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="119"/>
-      <c r="B72" s="120"/>
-      <c r="C72" s="121"/>
-      <c r="D72" s="121"/>
-      <c r="E72" s="71"/>
-      <c r="F72" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="71"/>
-      <c r="J72" s="71"/>
-      <c r="K72" s="71"/>
+      <c r="A72" s="117"/>
+      <c r="B72" s="118"/>
+      <c r="C72" s="119"/>
+      <c r="D72" s="119"/>
+      <c r="E72" s="69"/>
+      <c r="F72" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="69"/>
+      <c r="J72" s="69"/>
+      <c r="K72" s="69"/>
       <c r="M72" s="47"/>
       <c r="N72" s="47"/>
     </row>
@@ -4243,13 +4383,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4270,7 +4410,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4292,11 +4432,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4317,12 +4457,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="130" t="s">
-        <v>112</v>
+      <c r="D77" s="128" t="s">
+        <v>148</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4335,7 +4475,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="119"/>
+      <c r="A78" s="117"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4343,18 +4483,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="E78" s="122"/>
+        <v>150</v>
+      </c>
+      <c r="E78" s="120"/>
       <c r="F78" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="G78" s="122"/>
-      <c r="H78" s="122"/>
-      <c r="I78" s="122"/>
-      <c r="J78" s="122"/>
-      <c r="K78" s="122"/>
-      <c r="L78" s="122"/>
+        <v>151</v>
+      </c>
+      <c r="G78" s="120"/>
+      <c r="H78" s="120"/>
+      <c r="I78" s="120"/>
+      <c r="J78" s="120"/>
+      <c r="K78" s="120"/>
+      <c r="L78" s="120"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4367,7 +4507,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4388,11 +4528,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4411,8 +4551,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="130" t="s">
-        <v>112</v>
+      <c r="D81" s="128" t="s">
+        <v>148</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4434,7 +4574,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4453,7 +4593,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4472,7 +4612,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4487,7 +4627,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4684,8 +4824,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="123"/>
-      <c r="F103" s="123"/>
+      <c r="E103" s="121"/>
+      <c r="F103" s="121"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4789,31 +4929,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4821,28 +4961,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4850,28 +4990,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4879,28 +5019,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4908,28 +5048,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4937,28 +5077,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4966,28 +5106,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>160</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4995,28 +5135,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5024,28 +5164,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>175</v>
+        <v>211</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5053,28 +5193,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5082,28 +5222,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5111,28 +5251,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5140,28 +5280,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>202</v>
+        <v>238</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5169,33 +5309,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5227,34 +5367,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5262,31 +5402,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5294,31 +5434,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5326,31 +5466,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5358,31 +5498,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5390,31 +5530,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5422,31 +5562,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>247</v>
+        <v>283</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5454,31 +5594,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>251</v>
+        <v>287</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>255</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5486,31 +5626,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>257</v>
+        <v>293</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>259</v>
+        <v>295</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>262</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5518,31 +5658,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>270</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5550,31 +5690,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>271</v>
+        <v>307</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>275</v>
+        <v>311</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>276</v>
+        <v>312</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5582,31 +5722,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>279</v>
+        <v>315</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>280</v>
+        <v>316</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>281</v>
+        <v>317</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>284</v>
+        <v>320</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5614,31 +5754,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>287</v>
+        <v>323</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>288</v>
+        <v>324</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>289</v>
+        <v>325</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>290</v>
+        <v>326</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>292</v>
+        <v>328</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>293</v>
+        <v>329</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>294</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5646,63 +5786,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>295</v>
+        <v>331</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>296</v>
+        <v>332</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>297</v>
+        <v>333</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>301</v>
+        <v>337</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>302</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>306</v>
+        <v>342</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>309</v>
+        <v>345</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>310</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Massive update to Cleric, Rogue and Hunter + other changes
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="348">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -269,6 +269,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">9 + </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1298,10 +1301,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1475,6 +1478,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1482,31 +1493,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1536,24 +1540,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1567,15 +1562,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1604,16 +1600,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1641,7 +1644,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1659,91 +1734,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1755,13 +1752,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1779,7 +1770,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1791,13 +1782,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1809,19 +1812,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2013,6 +2016,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2024,21 +2042,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2063,15 +2066,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2101,20 +2095,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2124,134 +2127,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2552,9 +2555,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2562,9 +2562,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2968,8 +2965,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3074,7 +3071,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="107" t="s">
+      <c r="L7" s="105" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="69" t="s">
@@ -3090,10 +3087,10 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="107" t="s">
+      <c r="L8" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="107"/>
+      <c r="M8" s="105"/>
       <c r="N8" s="79"/>
     </row>
     <row r="9" spans="1:9">
@@ -3126,13 +3123,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="120" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="121" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -3144,24 +3141,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="123" t="s">
+      <c r="G10" s="121" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="108">
+      <c r="I10" s="106">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="120" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="121" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -3173,24 +3170,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="123" t="s">
+      <c r="G11" s="121" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="108">
+      <c r="I11" s="106">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="122" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="123" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -3202,13 +3199,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="123" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="109">
+      <c r="I12" s="107">
         <v>11.5</v>
       </c>
     </row>
@@ -3293,7 +3290,9 @@
       <c r="G18" s="65">
         <v>-1</v>
       </c>
-      <c r="H18" s="66"/>
+      <c r="H18" s="66">
+        <v>14.5</v>
+      </c>
       <c r="K18" s="79"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">
@@ -3318,7 +3317,9 @@
       <c r="G19" s="65">
         <v>-2</v>
       </c>
-      <c r="H19" s="69"/>
+      <c r="H19" s="69" t="s">
+        <v>47</v>
+      </c>
       <c r="K19" s="79"/>
     </row>
     <row r="20" ht="15.75" spans="1:11">
@@ -3335,7 +3336,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="70" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" s="68" t="s">
         <v>43</v>
@@ -3360,7 +3361,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="70" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F21" s="68" t="s">
         <v>46</v>
@@ -3379,16 +3380,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="74" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F22" s="75" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G22" s="50">
         <v>-3</v>
@@ -3401,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="78">
         <v>6</v>
@@ -3424,7 +3425,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="72" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="73">
         <v>8</v>
@@ -3460,7 +3461,7 @@
       <c r="A26" s="81"/>
       <c r="B26" s="58"/>
       <c r="C26" s="82" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="83"/>
       <c r="E26" s="58"/>
@@ -3468,9 +3469,9 @@
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="110"/>
+      <c r="J26" s="108"/>
       <c r="K26" s="64"/>
-      <c r="L26" s="111"/>
+      <c r="L26" s="109"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
       <c r="A27" s="84" t="s">
@@ -3480,7 +3481,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="86" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="87"/>
       <c r="E27" s="87"/>
@@ -3488,9 +3489,9 @@
       <c r="G27" s="87"/>
       <c r="H27" s="87"/>
       <c r="I27" s="87"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="113"/>
-      <c r="L27" s="113"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="111"/>
+      <c r="L27" s="111"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3500,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="88" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="89"/>
       <c r="E28" s="58"/>
@@ -3508,9 +3509,9 @@
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="110"/>
+      <c r="J28" s="108"/>
       <c r="K28" s="64"/>
-      <c r="L28" s="111"/>
+      <c r="L28" s="109"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3520,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="90" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29" s="91"/>
       <c r="E29" s="47"/>
@@ -3530,7 +3531,7 @@
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
       <c r="K29" s="64"/>
-      <c r="L29" s="111"/>
+      <c r="L29" s="109"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3540,21 +3541,21 @@
         <v>0</v>
       </c>
       <c r="C30" s="90" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="91" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="91" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F30" s="92" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H30" s="91"/>
-      <c r="J30" s="114"/>
+      <c r="J30" s="112"/>
       <c r="K30" s="64"/>
-      <c r="L30" s="111"/>
+      <c r="L30" s="109"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3564,24 +3565,24 @@
         <v>1</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="111"/>
-      <c r="L31" s="111"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="109"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3591,26 +3592,26 @@
         <v>1</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="J32" s="115"/>
-      <c r="K32" s="111"/>
-      <c r="L32" s="111"/>
+        <v>70</v>
+      </c>
+      <c r="J32" s="113"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3620,35 +3621,35 @@
         <v>1</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H33" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J33" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="K33" s="111"/>
-      <c r="L33" s="111"/>
+        <v>78</v>
+      </c>
+      <c r="K33" s="109"/>
+      <c r="L33" s="109"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
       <c r="A34" s="93" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="94">
         <v>1</v>
@@ -3671,10 +3672,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="96" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C35" s="81" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D35" s="78"/>
       <c r="E35" s="78"/>
@@ -3682,7 +3683,7 @@
       <c r="G35" s="78"/>
       <c r="H35" s="78"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="110"/>
+      <c r="J35" s="108"/>
       <c r="K35" s="69"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
@@ -3690,13 +3691,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="97" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D36" s="73" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E36" s="73"/>
       <c r="F36" s="73"/>
@@ -3735,7 +3736,7 @@
     <row r="39" ht="16.5" spans="1:11">
       <c r="A39" s="69"/>
       <c r="C39" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D39" s="96"/>
       <c r="F39" s="69"/>
@@ -3748,28 +3749,28 @@
     <row r="40" ht="30" spans="1:11">
       <c r="A40" s="80"/>
       <c r="B40" s="81" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F40" s="99" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G40" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="J40" s="116"/>
-      <c r="K40" s="116"/>
+      <c r="I40" s="124" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" s="114"/>
+      <c r="K40" s="114"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="80"/>
@@ -3783,16 +3784,16 @@
         <v>3</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="101">
+      <c r="F41" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="100">
         <v>10</v>
       </c>
-      <c r="I41" s="127" t="s">
-        <v>91</v>
+      <c r="I41" s="125" t="s">
+        <v>92</v>
       </c>
       <c r="J41" s="47"/>
       <c r="K41" s="69"/>
@@ -3809,12 +3810,12 @@
         <v>3</v>
       </c>
       <c r="E42" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="G42" s="101">
+      <c r="F42" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="100">
         <v>10</v>
       </c>
       <c r="I42" s="69"/>
@@ -3833,12 +3834,12 @@
         <v>3</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="G43" s="101">
+      <c r="F43" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="100">
         <v>10</v>
       </c>
       <c r="I43" s="69"/>
@@ -3847,9 +3848,9 @@
     </row>
     <row r="44" ht="15.75" spans="1:11">
       <c r="A44" s="80" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="102">
+        <v>97</v>
+      </c>
+      <c r="B44" s="101">
         <v>100</v>
       </c>
       <c r="C44" s="64">
@@ -3859,12 +3860,12 @@
         <v>3</v>
       </c>
       <c r="E44" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="G44" s="101">
+        <v>91</v>
+      </c>
+      <c r="F44" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" s="100">
         <v>10</v>
       </c>
       <c r="I44" s="47"/>
@@ -3873,9 +3874,9 @@
     </row>
     <row r="45" ht="15.75" spans="1:11">
       <c r="A45" s="80" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="103">
+        <v>99</v>
+      </c>
+      <c r="B45" s="102">
         <v>125</v>
       </c>
       <c r="C45" s="64">
@@ -3885,12 +3886,12 @@
         <v>3</v>
       </c>
       <c r="E45" s="98" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="G45" s="101">
+      <c r="F45" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="100">
         <v>10</v>
       </c>
       <c r="I45" s="47"/>
@@ -3899,9 +3900,9 @@
     </row>
     <row r="46" ht="15.75" spans="1:11">
       <c r="A46" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="B46" s="103">
+        <v>102</v>
+      </c>
+      <c r="B46" s="102">
         <v>150</v>
       </c>
       <c r="C46" s="64">
@@ -3911,23 +3912,23 @@
         <v>3</v>
       </c>
       <c r="E46" s="98" t="s">
-        <v>102</v>
-      </c>
-      <c r="F46" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="G46" s="101">
+      <c r="F46" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="100">
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I46" s="47"/>
       <c r="J46" s="47"/>
       <c r="K46" s="69"/>
     </row>
     <row r="47" ht="15.75" spans="2:11">
-      <c r="B47" s="103">
+      <c r="B47" s="102">
         <v>175</v>
       </c>
       <c r="C47" s="64">
@@ -3937,12 +3938,12 @@
         <v>3</v>
       </c>
       <c r="E47" s="98" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="101">
+      <c r="F47" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" s="100">
         <v>10</v>
       </c>
       <c r="I47" s="47"/>
@@ -3951,9 +3952,9 @@
     </row>
     <row r="48" ht="15.75" spans="1:11">
       <c r="A48" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="B48" s="103">
+        <v>108</v>
+      </c>
+      <c r="B48" s="102">
         <v>200</v>
       </c>
       <c r="C48" s="64">
@@ -3963,12 +3964,12 @@
         <v>4</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="100" t="s">
-        <v>108</v>
-      </c>
-      <c r="G48" s="101">
+        <v>98</v>
+      </c>
+      <c r="F48" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="100">
         <v>11</v>
       </c>
       <c r="I48" s="47"/>
@@ -3977,9 +3978,9 @@
     </row>
     <row r="49" ht="15.75" spans="1:11">
       <c r="A49" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" s="102">
+        <v>110</v>
+      </c>
+      <c r="B49" s="101">
         <v>225</v>
       </c>
       <c r="C49" s="64">
@@ -3989,12 +3990,12 @@
         <v>4</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="G49" s="101">
+      <c r="F49" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" s="100">
         <v>11</v>
       </c>
       <c r="I49" s="47"/>
@@ -4003,7 +4004,7 @@
     </row>
     <row r="50" ht="15.75" spans="1:11">
       <c r="A50" s="80" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B50" s="46">
         <v>250</v>
@@ -4015,12 +4016,12 @@
         <v>4</v>
       </c>
       <c r="E50" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="F50" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="G50" s="101">
+        <v>101</v>
+      </c>
+      <c r="F50" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="100">
         <v>11</v>
       </c>
       <c r="I50" s="47"/>
@@ -4038,12 +4039,12 @@
         <v>4</v>
       </c>
       <c r="E51" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="100" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="101">
+        <v>104</v>
+      </c>
+      <c r="F51" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="G51" s="100">
         <v>11</v>
       </c>
       <c r="I51" s="47"/>
@@ -4052,7 +4053,7 @@
     </row>
     <row r="52" ht="15.75" spans="1:13">
       <c r="A52" s="80" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -4064,10 +4065,10 @@
         <v>4</v>
       </c>
       <c r="E52" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F52" s="100" t="s">
         <v>117</v>
+      </c>
+      <c r="F52" s="47" t="s">
+        <v>118</v>
       </c>
       <c r="G52" s="48">
         <v>12</v>
@@ -4079,7 +4080,7 @@
     </row>
     <row r="53" ht="16.5" spans="1:13">
       <c r="A53" s="80" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -4091,10 +4092,10 @@
         <v>5</v>
       </c>
       <c r="E53" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="F53" s="104" t="s">
         <v>120</v>
+      </c>
+      <c r="F53" s="52" t="s">
+        <v>121</v>
       </c>
       <c r="G53" s="53">
         <v>12</v>
@@ -4104,9 +4105,9 @@
     </row>
     <row r="54" ht="15.75" spans="1:13">
       <c r="A54" s="80" t="s">
-        <v>121</v>
-      </c>
-      <c r="B54" s="103">
+        <v>122</v>
+      </c>
+      <c r="B54" s="102">
         <v>350</v>
       </c>
       <c r="C54" s="64">
@@ -4116,10 +4117,10 @@
         <v>5</v>
       </c>
       <c r="E54" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="F54" s="100" t="s">
         <v>123</v>
+      </c>
+      <c r="F54" s="47" t="s">
+        <v>124</v>
       </c>
       <c r="G54" s="48">
         <v>12</v>
@@ -4128,7 +4129,7 @@
       <c r="M54" s="69"/>
     </row>
     <row r="55" ht="15.75" spans="2:9">
-      <c r="B55" s="102">
+      <c r="B55" s="101">
         <v>375</v>
       </c>
       <c r="C55" s="47">
@@ -4138,10 +4139,10 @@
         <v>5</v>
       </c>
       <c r="E55" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="100" t="s">
         <v>125</v>
+      </c>
+      <c r="F55" s="47" t="s">
+        <v>126</v>
       </c>
       <c r="G55" s="48">
         <v>12</v>
@@ -4150,7 +4151,7 @@
     </row>
     <row r="56" ht="15.75" spans="1:9">
       <c r="A56" s="80" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B56" s="46">
         <v>400</v>
@@ -4162,10 +4163,10 @@
         <v>5</v>
       </c>
       <c r="E56" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="F56" s="100" t="s">
         <v>128</v>
+      </c>
+      <c r="F56" s="47" t="s">
+        <v>129</v>
       </c>
       <c r="G56" s="48">
         <v>12</v>
@@ -4183,10 +4184,10 @@
         <v>5</v>
       </c>
       <c r="E57" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="F57" s="100" t="s">
         <v>130</v>
+      </c>
+      <c r="F57" s="47" t="s">
+        <v>131</v>
       </c>
       <c r="G57" s="48">
         <v>12</v>
@@ -4204,10 +4205,10 @@
         <v>5</v>
       </c>
       <c r="E58" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="F58" s="100" t="s">
         <v>132</v>
+      </c>
+      <c r="F58" s="47" t="s">
+        <v>133</v>
       </c>
       <c r="G58" s="48">
         <v>12</v>
@@ -4215,7 +4216,7 @@
       <c r="I58" s="47"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="103">
+      <c r="B59" s="102">
         <v>475</v>
       </c>
       <c r="C59" s="47">
@@ -4225,10 +4226,10 @@
         <v>5</v>
       </c>
       <c r="E59" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" s="100" t="s">
         <v>134</v>
+      </c>
+      <c r="F59" s="47" t="s">
+        <v>135</v>
       </c>
       <c r="G59" s="48">
         <v>12</v>
@@ -4236,7 +4237,7 @@
       <c r="I59" s="47"/>
     </row>
     <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="105">
+      <c r="B60" s="103">
         <v>500</v>
       </c>
       <c r="C60" s="52">
@@ -4246,10 +4247,10 @@
         <v>5</v>
       </c>
       <c r="E60" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F60" s="104" t="s">
         <v>136</v>
+      </c>
+      <c r="F60" s="52" t="s">
+        <v>137</v>
       </c>
       <c r="G60" s="53">
         <v>12</v>
@@ -4264,12 +4265,12 @@
       <c r="I61" s="47"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="106" t="s">
-        <v>137</v>
+      <c r="C62" s="104" t="s">
+        <v>138</v>
       </c>
       <c r="E62" s="47"/>
-      <c r="F62" s="106" t="s">
-        <v>138</v>
+      <c r="F62" s="104" t="s">
+        <v>139</v>
       </c>
       <c r="G62" s="47"/>
       <c r="H62" s="47"/>
@@ -4323,7 +4324,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4332,8 +4333,8 @@
       <c r="I69" s="47"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="106" t="s">
-        <v>140</v>
+      <c r="C70" s="104" t="s">
+        <v>141</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4349,13 +4350,13 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="117"/>
-      <c r="B72" s="118"/>
-      <c r="C72" s="119"/>
-      <c r="D72" s="119"/>
+      <c r="A72" s="115"/>
+      <c r="B72" s="116"/>
+      <c r="C72" s="117"/>
+      <c r="D72" s="117"/>
       <c r="E72" s="69"/>
       <c r="F72" s="69" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G72" s="69"/>
       <c r="H72" s="69"/>
@@ -4383,13 +4384,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4410,7 +4411,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4432,11 +4433,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4457,12 +4458,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="128" t="s">
-        <v>148</v>
+      <c r="D77" s="126" t="s">
+        <v>149</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4475,7 +4476,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="117"/>
+      <c r="A78" s="115"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4483,18 +4484,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="E78" s="120"/>
+        <v>151</v>
+      </c>
+      <c r="E78" s="118"/>
       <c r="F78" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="G78" s="120"/>
-      <c r="H78" s="120"/>
-      <c r="I78" s="120"/>
-      <c r="J78" s="120"/>
-      <c r="K78" s="120"/>
-      <c r="L78" s="120"/>
+        <v>152</v>
+      </c>
+      <c r="G78" s="118"/>
+      <c r="H78" s="118"/>
+      <c r="I78" s="118"/>
+      <c r="J78" s="118"/>
+      <c r="K78" s="118"/>
+      <c r="L78" s="118"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4507,7 +4508,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4528,11 +4529,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4551,8 +4552,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="128" t="s">
-        <v>148</v>
+      <c r="D81" s="126" t="s">
+        <v>149</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4574,7 +4575,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4593,7 +4594,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4612,7 +4613,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4627,7 +4628,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4824,8 +4825,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="121"/>
-      <c r="F103" s="121"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="119"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4929,31 +4930,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4961,28 +4962,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>168</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4990,28 +4991,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="E3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5019,28 +5020,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>175</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5048,28 +5049,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>179</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5077,28 +5078,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5106,28 +5107,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5135,28 +5136,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5164,28 +5165,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5193,28 +5194,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5222,28 +5223,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5251,28 +5252,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5280,28 +5281,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5309,33 +5310,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>242</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5367,34 +5368,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5402,31 +5403,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5434,31 +5435,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>261</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5466,31 +5467,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>266</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G21" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5498,31 +5499,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>270</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G22" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>271</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5530,31 +5531,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>275</v>
-      </c>
       <c r="E23" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5562,31 +5563,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F24" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5594,31 +5595,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>286</v>
-      </c>
       <c r="I25" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5626,31 +5627,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5658,31 +5659,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5690,31 +5691,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="E28" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5722,31 +5723,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5754,31 +5755,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5786,63 +5787,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Long Rest -> Adventure Update 2023-04-26
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="349">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -561,21 +561,21 @@
     <t>1.5 + 3</t>
   </si>
   <si>
+    <t>Level 4</t>
+  </si>
+  <si>
     <t>6 (2d4 + 1)</t>
   </si>
   <si>
     <t>9 (2d4 + 4)</t>
   </si>
   <si>
-    <t>Level 4</t>
+    <t>Level 5</t>
   </si>
   <si>
     <t>9.5 (1d6 + 5)</t>
   </si>
   <si>
-    <t>Level 5</t>
-  </si>
-  <si>
     <t>7 (2d4 + 2)</t>
   </si>
   <si>
@@ -588,10 +588,13 @@
     <t>10.5  (1d6 + 6)</t>
   </si>
   <si>
+    <t>Level 7</t>
+  </si>
+  <si>
     <t>11 (2d4 + 7)</t>
   </si>
   <si>
-    <t>Level 7</t>
+    <t>Level 8</t>
   </si>
   <si>
     <t>8.5 (1d6 + 4)</t>
@@ -600,7 +603,7 @@
     <t>11.5 (1d6 + 7)</t>
   </si>
   <si>
-    <t>Level 8</t>
+    <t>Level 9</t>
   </si>
   <si>
     <t>9 (2d6 + 2)</t>
@@ -609,7 +612,7 @@
     <t>12 (2d6 + 5)</t>
   </si>
   <si>
-    <t>Level 9</t>
+    <t>Level 10</t>
   </si>
   <si>
     <t>10 (2d6 + 3)</t>
@@ -622,9 +625,6 @@
   </si>
   <si>
     <t>13.75 (3d4 + 6)</t>
-  </si>
-  <si>
-    <t>Level 10</t>
   </si>
   <si>
     <t>11.5 (5d4 - 1)</t>
@@ -665,6 +665,9 @@
     <t>The double of another column
 should be ~80% of its half
 E.g. 400XP dmg = 0.8 * 2 * 200XP dmg</t>
+  </si>
+  <si>
+    <t>6.5 -- 6.5</t>
   </si>
   <si>
     <t>XP Rules</t>
@@ -1301,10 +1304,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1487,22 +1490,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1510,7 +1512,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1525,7 +1527,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1555,14 +1557,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1570,8 +1564,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1609,13 +1619,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1644,7 +1647,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1656,109 +1773,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1782,25 +1809,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1812,19 +1821,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2011,7 +2014,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2027,6 +2045,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2049,23 +2076,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2095,166 +2107,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2569,6 +2572,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2965,8 +2971,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3071,7 +3077,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="L7" s="105" t="s">
+      <c r="L7" s="106" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="69" t="s">
@@ -3087,10 +3093,10 @@
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
-      <c r="L8" s="105" t="s">
+      <c r="L8" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="105"/>
+      <c r="M8" s="106"/>
       <c r="N8" s="79"/>
     </row>
     <row r="9" spans="1:9">
@@ -3123,13 +3129,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="121" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="46">
         <v>5.5</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="47">
@@ -3141,24 +3147,24 @@
       <c r="F10" s="49">
         <v>10.5</v>
       </c>
-      <c r="G10" s="121" t="s">
+      <c r="G10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="47">
         <v>-4</v>
       </c>
-      <c r="I10" s="106">
+      <c r="I10" s="107">
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="121" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="46">
         <v>5.5</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="47">
@@ -3170,24 +3176,24 @@
       <c r="F11" s="49">
         <v>10.5</v>
       </c>
-      <c r="G11" s="121" t="s">
+      <c r="G11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="47">
         <v>-4</v>
       </c>
-      <c r="I11" s="106">
+      <c r="I11" s="107">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="123" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="51">
         <v>5.5</v>
       </c>
-      <c r="C12" s="123" t="s">
+      <c r="C12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="52">
@@ -3199,13 +3205,13 @@
       <c r="F12" s="54">
         <v>10.5</v>
       </c>
-      <c r="G12" s="123" t="s">
+      <c r="G12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="52">
         <v>-5</v>
       </c>
-      <c r="I12" s="107">
+      <c r="I12" s="108">
         <v>11.5</v>
       </c>
     </row>
@@ -3469,9 +3475,9 @@
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
-      <c r="J26" s="108"/>
+      <c r="J26" s="109"/>
       <c r="K26" s="64"/>
-      <c r="L26" s="109"/>
+      <c r="L26" s="110"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
       <c r="A27" s="84" t="s">
@@ -3489,9 +3495,9 @@
       <c r="G27" s="87"/>
       <c r="H27" s="87"/>
       <c r="I27" s="87"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="46">
@@ -3509,9 +3515,9 @@
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
-      <c r="J28" s="108"/>
+      <c r="J28" s="109"/>
       <c r="K28" s="64"/>
-      <c r="L28" s="109"/>
+      <c r="L28" s="110"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="46">
@@ -3531,7 +3537,7 @@
       <c r="I29" s="47"/>
       <c r="J29" s="48"/>
       <c r="K29" s="64"/>
-      <c r="L29" s="109"/>
+      <c r="L29" s="110"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="46">
@@ -3553,9 +3559,9 @@
         <v>63</v>
       </c>
       <c r="H30" s="91"/>
-      <c r="J30" s="112"/>
+      <c r="J30" s="113"/>
       <c r="K30" s="64"/>
-      <c r="L30" s="109"/>
+      <c r="L30" s="110"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="46">
@@ -3581,8 +3587,8 @@
       </c>
       <c r="H31" s="47"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="109"/>
+      <c r="K31" s="110"/>
+      <c r="L31" s="110"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="46">
@@ -3609,9 +3615,9 @@
       <c r="H32" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="113"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
     </row>
     <row r="33" ht="15.75" spans="1:12">
       <c r="A33" s="51">
@@ -3644,8 +3650,8 @@
       <c r="J33" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="K33" s="109"/>
-      <c r="L33" s="109"/>
+      <c r="K33" s="110"/>
+      <c r="L33" s="110"/>
     </row>
     <row r="34" ht="15.75" spans="1:14">
       <c r="A34" s="93" t="s">
@@ -3683,7 +3689,7 @@
       <c r="G35" s="78"/>
       <c r="H35" s="78"/>
       <c r="I35" s="58"/>
-      <c r="J35" s="108"/>
+      <c r="J35" s="109"/>
       <c r="K35" s="69"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
@@ -3766,11 +3772,11 @@
       <c r="G40" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="124" t="s">
+      <c r="I40" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="114"/>
-      <c r="K40" s="114"/>
+      <c r="J40" s="115"/>
+      <c r="K40" s="115"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="80"/>
@@ -3792,7 +3798,7 @@
       <c r="G41" s="100">
         <v>10</v>
       </c>
-      <c r="I41" s="125" t="s">
+      <c r="I41" s="126" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="47"/>
@@ -3927,7 +3933,10 @@
       <c r="J46" s="47"/>
       <c r="K46" s="69"/>
     </row>
-    <row r="47" ht="15.75" spans="2:11">
+    <row r="47" ht="15.75" spans="1:11">
+      <c r="A47" s="80" t="s">
+        <v>106</v>
+      </c>
       <c r="B47" s="102">
         <v>175</v>
       </c>
@@ -3938,10 +3947,10 @@
         <v>3</v>
       </c>
       <c r="E47" s="98" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G47" s="100">
         <v>10</v>
@@ -3952,7 +3961,7 @@
     </row>
     <row r="48" ht="15.75" spans="1:11">
       <c r="A48" s="80" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B48" s="102">
         <v>200</v>
@@ -3967,7 +3976,7 @@
         <v>98</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G48" s="100">
         <v>11</v>
@@ -3976,10 +3985,7 @@
       <c r="J48" s="47"/>
       <c r="K48" s="69"/>
     </row>
-    <row r="49" ht="15.75" spans="1:11">
-      <c r="A49" s="80" t="s">
-        <v>110</v>
-      </c>
+    <row r="49" ht="15.75" spans="2:11">
       <c r="B49" s="101">
         <v>225</v>
       </c>
@@ -4028,7 +4034,10 @@
       <c r="J50" s="47"/>
       <c r="K50" s="69"/>
     </row>
-    <row r="51" ht="15.75" spans="2:11">
+    <row r="51" ht="15.75" spans="1:11">
+      <c r="A51" s="80" t="s">
+        <v>115</v>
+      </c>
       <c r="B51" s="46">
         <v>275</v>
       </c>
@@ -4042,7 +4051,7 @@
         <v>104</v>
       </c>
       <c r="F51" s="47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G51" s="100">
         <v>11</v>
@@ -4053,7 +4062,7 @@
     </row>
     <row r="52" ht="15.75" spans="1:13">
       <c r="A52" s="80" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B52" s="46">
         <v>300</v>
@@ -4065,10 +4074,10 @@
         <v>4</v>
       </c>
       <c r="E52" s="47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F52" s="47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G52" s="48">
         <v>12</v>
@@ -4080,7 +4089,7 @@
     </row>
     <row r="53" ht="16.5" spans="1:13">
       <c r="A53" s="80" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B53" s="51">
         <v>325</v>
@@ -4092,10 +4101,10 @@
         <v>5</v>
       </c>
       <c r="E53" s="52" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G53" s="53">
         <v>12</v>
@@ -4105,7 +4114,7 @@
     </row>
     <row r="54" ht="15.75" spans="1:13">
       <c r="A54" s="80" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B54" s="102">
         <v>350</v>
@@ -4117,10 +4126,10 @@
         <v>5</v>
       </c>
       <c r="E54" s="64" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F54" s="47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G54" s="48">
         <v>12</v>
@@ -4139,20 +4148,17 @@
         <v>5</v>
       </c>
       <c r="E55" s="47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F55" s="47" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G55" s="48">
         <v>12</v>
       </c>
       <c r="I55" s="47"/>
     </row>
-    <row r="56" ht="15.75" spans="1:9">
-      <c r="A56" s="80" t="s">
-        <v>127</v>
-      </c>
+    <row r="56" spans="2:9">
       <c r="B56" s="46">
         <v>400</v>
       </c>
@@ -4279,18 +4285,20 @@
     <row r="63" spans="5:9">
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
-      <c r="G63" s="47">
-        <v>10</v>
-      </c>
+      <c r="G63" s="47"/>
       <c r="H63" s="47"/>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="5:9">
-      <c r="E64" s="47"/>
+    <row r="64" spans="4:9">
+      <c r="D64">
+        <f>20+6*9</f>
+        <v>74</v>
+      </c>
+      <c r="E64" s="105" t="s">
+        <v>140</v>
+      </c>
       <c r="F64" s="47"/>
-      <c r="G64" s="47">
-        <v>10</v>
-      </c>
+      <c r="G64" s="47"/>
       <c r="H64" s="47"/>
       <c r="I64" s="47"/>
     </row>
@@ -4324,7 +4332,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
@@ -4334,7 +4342,7 @@
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
       <c r="C70" s="104" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E70" s="47"/>
       <c r="F70" s="47"/>
@@ -4350,13 +4358,13 @@
       <c r="I71" s="47"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="115"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="117"/>
-      <c r="D72" s="117"/>
+      <c r="A72" s="116"/>
+      <c r="B72" s="117"/>
+      <c r="C72" s="118"/>
+      <c r="D72" s="118"/>
       <c r="E72" s="69"/>
       <c r="F72" s="69" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G72" s="69"/>
       <c r="H72" s="69"/>
@@ -4384,13 +4392,13 @@
     <row r="74" spans="1:14">
       <c r="A74" s="47"/>
       <c r="B74" s="47" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D74" s="47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
@@ -4411,7 +4419,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="47" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E75" s="47"/>
       <c r="F75" s="47"/>
@@ -4433,11 +4441,11 @@
         <v>25</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E76" s="47"/>
       <c r="F76" s="47" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G76" s="47">
         <v>3.5</v>
@@ -4458,12 +4466,12 @@
       <c r="C77" s="47">
         <v>30</v>
       </c>
-      <c r="D77" s="126" t="s">
-        <v>149</v>
+      <c r="D77" s="127" t="s">
+        <v>150</v>
       </c>
       <c r="E77" s="47"/>
       <c r="F77" s="47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G77" s="47">
         <v>9</v>
@@ -4476,7 +4484,7 @@
       <c r="N77" s="47"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="115"/>
+      <c r="A78" s="116"/>
       <c r="B78" s="47">
         <v>4</v>
       </c>
@@ -4484,18 +4492,18 @@
         <v>35</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="E78" s="118"/>
+        <v>152</v>
+      </c>
+      <c r="E78" s="119"/>
       <c r="F78" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="G78" s="118"/>
-      <c r="H78" s="118"/>
-      <c r="I78" s="118"/>
-      <c r="J78" s="118"/>
-      <c r="K78" s="118"/>
-      <c r="L78" s="118"/>
+        <v>153</v>
+      </c>
+      <c r="G78" s="119"/>
+      <c r="H78" s="119"/>
+      <c r="I78" s="119"/>
+      <c r="J78" s="119"/>
+      <c r="K78" s="119"/>
+      <c r="L78" s="119"/>
       <c r="M78" s="47"/>
       <c r="N78" s="47"/>
     </row>
@@ -4508,7 +4516,7 @@
         <v>40</v>
       </c>
       <c r="D79" s="47" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E79" s="47"/>
       <c r="F79" s="47"/>
@@ -4529,11 +4537,11 @@
         <v>45</v>
       </c>
       <c r="D80" s="47" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E80" s="47"/>
       <c r="F80" s="47" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G80" s="47"/>
       <c r="H80" s="47"/>
@@ -4552,8 +4560,8 @@
       <c r="C81" s="47">
         <v>50</v>
       </c>
-      <c r="D81" s="126" t="s">
-        <v>149</v>
+      <c r="D81" s="127" t="s">
+        <v>150</v>
       </c>
       <c r="E81" s="47"/>
       <c r="F81" s="47"/>
@@ -4575,7 +4583,7 @@
         <v>55</v>
       </c>
       <c r="D82" s="47" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -4594,7 +4602,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="47" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E83" s="47"/>
       <c r="F83" s="47"/>
@@ -4613,7 +4621,7 @@
         <v>65</v>
       </c>
       <c r="D84" s="47" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E84" s="47"/>
       <c r="F84" s="47"/>
@@ -4628,7 +4636,7 @@
       <c r="B85" s="47"/>
       <c r="C85" s="47"/>
       <c r="D85" s="47" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
@@ -4825,8 +4833,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="47"/>
       <c r="D103" s="47"/>
-      <c r="E103" s="119"/>
-      <c r="F103" s="119"/>
+      <c r="E103" s="120"/>
+      <c r="F103" s="120"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="47"/>
@@ -4911,7 +4919,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75"/>
@@ -4930,31 +4938,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4962,28 +4970,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4991,28 +4999,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="E3" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5020,28 +5028,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5049,28 +5057,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5078,28 +5086,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5107,28 +5115,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>192</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5136,28 +5144,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5165,28 +5173,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5194,28 +5202,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5223,28 +5231,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5252,28 +5260,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5281,28 +5289,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -5310,33 +5318,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>243</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
@@ -5368,34 +5376,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5403,31 +5411,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>259</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5435,31 +5443,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>263</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5467,31 +5475,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G21" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>268</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5499,31 +5507,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>271</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G22" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>272</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5531,31 +5539,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>276</v>
-      </c>
       <c r="E23" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5563,31 +5571,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F24" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>282</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5595,31 +5603,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>287</v>
-      </c>
       <c r="I25" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5627,31 +5635,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5659,31 +5667,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5691,31 +5699,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>189</v>
-      </c>
       <c r="E28" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -5723,31 +5731,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5755,31 +5763,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -5787,63 +5795,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Basic Abilities to the new levels secategorisation
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -1570,8 +1570,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="44">
     <font>
@@ -1752,18 +1752,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1774,16 +1767,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1792,6 +1777,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1806,22 +1798,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1842,8 +1835,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1858,30 +1874,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1890,7 +1890,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1903,7 +1903,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1924,7 +1924,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1936,13 +1990,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1954,49 +2086,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2008,103 +2098,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2287,30 +2281,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2326,6 +2296,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2337,6 +2325,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2362,25 +2365,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2389,15 +2383,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2407,130 +2401,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5141,7 +5135,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5464,7 +5458,9 @@
       <c r="F18" s="55">
         <v>-1</v>
       </c>
-      <c r="H18" s="57"/>
+      <c r="H18" s="57">
+        <v>12</v>
+      </c>
       <c r="K18" s="69"/>
     </row>
     <row r="19" ht="15.75" spans="1:11">

</xml_diff>

<commit_message>
Almost finished classes; still on Shaman and it's the last one.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27195" windowHeight="13095" activeTab="1"/>
+    <workbookView windowWidth="27015" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1566,12 +1566,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="44">
     <font>
@@ -1760,15 +1760,79 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1789,9 +1853,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1804,37 +1868,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -1842,55 +1875,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1924,7 +1924,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1936,31 +2062,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1972,115 +2080,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2092,13 +2092,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2281,39 +2281,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2329,27 +2296,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2378,153 +2328,203 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2874,52 +2874,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -5135,7 +5135,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5458,8 +5458,13 @@
       <c r="F18" s="55">
         <v>-1</v>
       </c>
+      <c r="G18">
+        <f>4*8+8</f>
+        <v>40</v>
+      </c>
       <c r="H18" s="57">
-        <v>12</v>
+        <f>10+24</f>
+        <v>34</v>
       </c>
       <c r="K18" s="69"/>
     </row>
@@ -5482,6 +5487,10 @@
       <c r="F19" s="55">
         <v>-2</v>
       </c>
+      <c r="G19">
+        <f>40/6.5</f>
+        <v>6.15384615384615</v>
+      </c>
       <c r="H19" s="58"/>
       <c r="K19" s="69"/>
     </row>
@@ -5504,6 +5513,10 @@
       <c r="F20" s="63">
         <v>-1</v>
       </c>
+      <c r="G20">
+        <f>6*6.5</f>
+        <v>39</v>
+      </c>
       <c r="H20" s="57"/>
       <c r="K20" s="69"/>
     </row>
@@ -5526,6 +5539,7 @@
       <c r="F21" s="55">
         <v>-2</v>
       </c>
+      <c r="G21"/>
       <c r="H21" s="58"/>
       <c r="K21" s="69"/>
     </row>

</xml_diff>

<commit_message>
Added magic items page and reworked other pages. Some magic items have icons.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12330" activeTab="1"/>
+    <workbookView windowWidth="27015" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="364">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -844,6 +844,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">6 | </t>
     </r>
     <r>
@@ -902,6 +909,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">8 | </t>
     </r>
     <r>
@@ -983,6 +997,14 @@
   </si>
   <si>
     <t>New Health</t>
+  </si>
+  <si>
+    <t>16.5  (1d8 + 13)</t>
+  </si>
+  <si>
+    <t>The double of another column
+should be ~85% of its half
+E.g. 400XP dmg = 0.85 * 2 * 200XP dmg</t>
   </si>
   <si>
     <t>1-Handed (+3)</t>
@@ -2514,7 +2536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2797,41 +2819,53 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3349,13 +3383,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="112" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="113" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3367,7 +3401,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="113" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3378,13 +3412,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="112" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="113" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3396,7 +3430,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="109" t="s">
+      <c r="G11" s="113" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3407,13 +3441,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="114" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="115" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3425,7 +3459,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="111" t="s">
+      <c r="G12" s="115" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3977,7 +4011,7 @@
       <c r="G40" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="112" t="s">
+      <c r="I40" s="116" t="s">
         <v>89</v>
       </c>
       <c r="J40" s="102"/>
@@ -4003,7 +4037,7 @@
       <c r="G41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="113" t="s">
+      <c r="I41" s="117" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4476,11 +4510,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="94" t="s">
+      <c r="C62" s="109" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="94" t="s">
+      <c r="F62" s="109" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4499,7 +4533,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="95" t="s">
+      <c r="E64" s="105" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4546,7 +4580,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="94" t="s">
+      <c r="C70" s="109" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4563,10 +4597,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="103"/>
-      <c r="B72" s="104"/>
-      <c r="C72" s="105"/>
-      <c r="D72" s="105"/>
+      <c r="A72" s="106"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4671,7 +4705,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="114" t="s">
+      <c r="D77" s="118" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4689,7 +4723,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="103"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4699,16 +4733,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="106"/>
+      <c r="E78" s="110"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="106"/>
-      <c r="H78" s="106"/>
-      <c r="I78" s="106"/>
-      <c r="J78" s="106"/>
-      <c r="K78" s="106"/>
-      <c r="L78" s="106"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
+      <c r="I78" s="110"/>
+      <c r="J78" s="110"/>
+      <c r="K78" s="110"/>
+      <c r="L78" s="110"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4765,7 +4799,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="114" t="s">
+      <c r="D81" s="118" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5038,8 +5072,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="107"/>
-      <c r="F103" s="107"/>
+      <c r="E103" s="111"/>
+      <c r="F103" s="111"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5123,8 +5157,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5281,13 +5315,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="112" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="113" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5299,7 +5333,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="113" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5310,13 +5344,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="112" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="113" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5328,7 +5362,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="109" t="s">
+      <c r="G11" s="113" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5339,13 +5373,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="114" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="115" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5357,7 +5391,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="111" t="s">
+      <c r="G12" s="115" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5448,8 +5482,8 @@
         <v>-1</v>
       </c>
       <c r="G18">
-        <f>7*3.5</f>
-        <v>24.5</v>
+        <f>2*5.5</f>
+        <v>11</v>
       </c>
       <c r="H18" s="57"/>
       <c r="K18" s="70"/>
@@ -5473,10 +5507,7 @@
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="G19">
-        <f>6.5+4*4.5</f>
-        <v>24.5</v>
-      </c>
+      <c r="G19"/>
       <c r="H19" s="58"/>
       <c r="K19" s="70"/>
     </row>
@@ -5499,7 +5530,6 @@
       <c r="F20" s="63">
         <v>-1</v>
       </c>
-      <c r="G20"/>
       <c r="H20" s="57"/>
       <c r="K20" s="70"/>
     </row>
@@ -5904,7 +5934,7 @@
       <c r="G40" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="112" t="s">
+      <c r="I40" s="116" t="s">
         <v>89</v>
       </c>
       <c r="J40" s="102"/>
@@ -5931,7 +5961,7 @@
       <c r="G41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="113" t="s">
+      <c r="I41" s="117" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -5971,7 +6001,7 @@
         <v>21</v>
       </c>
       <c r="D43" s="40">
-        <f t="shared" ref="D43:D60" si="0">FLOOR(C43*1.32,1)</f>
+        <f t="shared" ref="D43:D61" si="0">FLOOR(C43*1.32,1)</f>
         <v>27</v>
       </c>
       <c r="E43" s="40" t="s">
@@ -6205,10 +6235,10 @@
       <c r="K51" s="58"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="72" t="s">
+      <c r="A52" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="39">
+      <c r="B52" s="95">
         <v>300</v>
       </c>
       <c r="C52" s="40">
@@ -6232,27 +6262,27 @@
       <c r="K52" s="70"/>
       <c r="M52" s="58"/>
     </row>
-    <row r="53" ht="16.5" spans="1:13">
-      <c r="A53" s="72" t="s">
+    <row r="53" ht="15.75" spans="1:13">
+      <c r="A53" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="44">
+      <c r="B53" s="95">
         <v>325</v>
       </c>
-      <c r="C53" s="45">
+      <c r="C53" s="95">
         <v>120</v>
       </c>
-      <c r="D53" s="45">
+      <c r="D53" s="95">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E53" s="45" t="s">
+      <c r="E53" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="45" t="s">
+      <c r="F53" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="G53" s="46">
+      <c r="G53" s="41">
         <v>12</v>
       </c>
       <c r="I53" s="40"/>
@@ -6284,30 +6314,35 @@
       <c r="I54" s="40"/>
       <c r="M54" s="58"/>
     </row>
-    <row r="55" ht="15.75" spans="1:9">
+    <row r="55" ht="16.5" spans="1:9">
       <c r="A55" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="B55" s="52">
+      <c r="B55" s="65">
         <v>375</v>
       </c>
-      <c r="C55" s="40">
+      <c r="C55" s="45">
         <v>140</v>
       </c>
-      <c r="D55" s="40">
+      <c r="D55" s="45">
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="G55" s="41">
+      <c r="G55" s="46">
         <v>12</v>
       </c>
-      <c r="I55" s="40"/>
+      <c r="H55">
+        <v>7</v>
+      </c>
+      <c r="I55" s="40">
+        <v>300</v>
+      </c>
     </row>
     <row r="56" spans="2:9">
       <c r="B56" s="39">
@@ -6329,7 +6364,12 @@
       <c r="G56" s="41">
         <v>12</v>
       </c>
-      <c r="I56" s="40"/>
+      <c r="H56">
+        <v>6.5</v>
+      </c>
+      <c r="I56" s="40">
+        <v>275</v>
+      </c>
     </row>
     <row r="57" spans="2:9">
       <c r="B57" s="39">
@@ -6351,7 +6391,12 @@
       <c r="G57" s="41">
         <v>12</v>
       </c>
-      <c r="I57" s="40"/>
+      <c r="H57">
+        <v>6.5</v>
+      </c>
+      <c r="I57" s="40">
+        <v>275</v>
+      </c>
     </row>
     <row r="58" spans="2:9">
       <c r="B58" s="39">
@@ -6373,7 +6418,12 @@
       <c r="G58" s="41">
         <v>12</v>
       </c>
-      <c r="I58" s="40"/>
+      <c r="H58">
+        <v>5.5</v>
+      </c>
+      <c r="I58" s="40">
+        <v>250</v>
+      </c>
     </row>
     <row r="59" spans="2:9">
       <c r="B59" s="39">
@@ -6395,80 +6445,129 @@
       <c r="G59" s="41">
         <v>12</v>
       </c>
-      <c r="I59" s="40"/>
-    </row>
-    <row r="60" ht="16.5" spans="2:9">
-      <c r="B60" s="65">
+      <c r="H59">
+        <v>6.5</v>
+      </c>
+      <c r="I59" s="40">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" spans="2:9">
+      <c r="B60" s="52">
         <v>500</v>
       </c>
-      <c r="C60" s="45">
+      <c r="C60" s="95">
         <v>218</v>
       </c>
-      <c r="D60" s="45">
+      <c r="D60" s="95">
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-      <c r="E60" s="45" t="s">
+      <c r="E60" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F60" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="G60" s="46">
+      <c r="G60" s="41">
         <v>12</v>
       </c>
-      <c r="I60" s="40"/>
-    </row>
-    <row r="61" spans="5:9">
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-    </row>
-    <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="94" t="s">
-        <v>138</v>
-      </c>
-      <c r="E62" s="40"/>
-      <c r="F62" s="94" t="s">
-        <v>139</v>
-      </c>
-      <c r="G62" s="40"/>
+      <c r="H60">
+        <v>5.5</v>
+      </c>
+      <c r="I60" s="40">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" spans="2:9">
+      <c r="B61" s="52">
+        <v>600</v>
+      </c>
+      <c r="C61" s="95"/>
+      <c r="D61" s="95">
+        <v>350</v>
+      </c>
+      <c r="E61" s="95">
+        <v>14.5</v>
+      </c>
+      <c r="F61" s="95"/>
+      <c r="G61" s="41">
+        <v>13</v>
+      </c>
+      <c r="H61" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="I61" s="40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" spans="2:9">
+      <c r="B62" s="52">
+        <v>750</v>
+      </c>
+      <c r="C62" s="95"/>
+      <c r="D62" s="95">
+        <v>441</v>
+      </c>
+      <c r="E62" s="95">
+        <v>17.25</v>
+      </c>
+      <c r="F62" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="G62" s="41">
+        <v>13</v>
+      </c>
       <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-    </row>
-    <row r="63" spans="5:9">
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
+      <c r="I62" s="103">
+        <f>SUM(I55:I61)</f>
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="63" ht="16.5" spans="2:9">
+      <c r="B63" s="65">
+        <v>1000</v>
+      </c>
+      <c r="C63" s="45"/>
+      <c r="D63" s="45">
+        <v>688</v>
+      </c>
+      <c r="E63" s="45">
+        <v>21.5</v>
+      </c>
+      <c r="F63" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="G63" s="46">
+        <v>13</v>
+      </c>
       <c r="H63" s="40"/>
       <c r="I63" s="40"/>
     </row>
-    <row r="64" spans="4:9">
-      <c r="D64">
-        <f>20+6*9</f>
-        <v>74</v>
-      </c>
-      <c r="E64" s="95" t="s">
-        <v>140</v>
-      </c>
-      <c r="F64" s="40"/>
+    <row r="64" spans="7:9">
       <c r="G64" s="40"/>
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
     </row>
-    <row r="65" spans="5:9">
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
+    <row r="65" ht="15.75" spans="7:9">
       <c r="G65" s="40"/>
       <c r="H65" s="40"/>
       <c r="I65" s="40"/>
     </row>
-    <row r="66" spans="5:9">
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
+    <row r="66" ht="75.75" spans="3:9">
+      <c r="C66" s="104" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="104" t="s">
+        <v>142</v>
+      </c>
+      <c r="E66" s="104" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="40">
+        <f>350*4*0.8</f>
+        <v>1120</v>
+      </c>
       <c r="H66" s="40"/>
       <c r="I66" s="40"/>
     </row>
@@ -6480,26 +6579,21 @@
       <c r="I67" s="40"/>
     </row>
     <row r="68" spans="5:9">
-      <c r="E68" s="40"/>
+      <c r="E68" s="105"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
       <c r="I68" s="40"/>
     </row>
     <row r="69" spans="3:9">
-      <c r="C69" s="40" t="s">
-        <v>141</v>
-      </c>
+      <c r="C69" s="40"/>
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
       <c r="G69" s="40"/>
       <c r="H69" s="40"/>
       <c r="I69" s="40"/>
     </row>
-    <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="94" t="s">
-        <v>142</v>
-      </c>
+    <row r="70" ht="13" customHeight="1" spans="5:9">
       <c r="E70" s="40"/>
       <c r="F70" s="40"/>
       <c r="G70" s="40"/>
@@ -6514,10 +6608,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="103"/>
-      <c r="B72" s="104"/>
-      <c r="C72" s="105"/>
-      <c r="D72" s="105"/>
+      <c r="A72" s="106"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -6622,7 +6716,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="114" t="s">
+      <c r="D77" s="118" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -6640,7 +6734,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="103"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -6650,16 +6744,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="106"/>
+      <c r="E78" s="110"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="106"/>
-      <c r="H78" s="106"/>
-      <c r="I78" s="106"/>
-      <c r="J78" s="106"/>
-      <c r="K78" s="106"/>
-      <c r="L78" s="106"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
+      <c r="I78" s="110"/>
+      <c r="J78" s="110"/>
+      <c r="K78" s="110"/>
+      <c r="L78" s="110"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -6716,7 +6810,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="114" t="s">
+      <c r="D81" s="118" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -6989,8 +7083,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="107"/>
-      <c r="F103" s="107"/>
+      <c r="E103" s="111"/>
+      <c r="F103" s="111"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -7094,31 +7188,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7126,28 +7220,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7155,28 +7249,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7184,28 +7278,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7213,28 +7307,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7242,28 +7336,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>199</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7271,28 +7365,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7300,28 +7394,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7329,28 +7423,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7358,28 +7452,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7387,28 +7481,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7416,28 +7510,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7445,28 +7539,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7474,33 +7568,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7532,34 +7626,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7567,31 +7661,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7599,31 +7693,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7631,31 +7725,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7663,31 +7757,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7695,31 +7789,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7727,31 +7821,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G24" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="H24" s="14" t="s">
-        <v>296</v>
-      </c>
       <c r="I24" s="13" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7759,31 +7853,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>301</v>
-      </c>
       <c r="I25" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7791,31 +7885,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7823,31 +7917,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7855,31 +7949,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7887,31 +7981,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -7919,31 +8013,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -7951,63 +8045,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Reserve Health to Health Regen.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27015" windowHeight="12930" activeTab="1"/>
+    <workbookView windowWidth="27015" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="395">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -736,6 +736,18 @@
     <t>XP Reward per Difficulty</t>
   </si>
   <si>
+    <t>Race Start</t>
+  </si>
+  <si>
+    <t>Average Might</t>
+  </si>
+  <si>
+    <t>Extra Class Start</t>
+  </si>
+  <si>
+    <t>Per Level</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1005,6 +1017,87 @@
     <t>The double of another column
 should be ~85% of its half
 E.g. 400XP dmg = 0.85 * 2 * 200XP dmg</t>
+  </si>
+  <si>
+    <t>For 2...</t>
+  </si>
+  <si>
+    <t>...gain 1</t>
+  </si>
+  <si>
+    <t>18.5 + Might + Other</t>
+  </si>
+  <si>
+    <t>6 + Level</t>
+  </si>
+  <si>
+    <t>HP Regen</t>
+  </si>
+  <si>
+    <t>Reserve HP</t>
+  </si>
+  <si>
+    <t>Health Regen (6 + Level)</t>
+  </si>
+  <si>
+    <t>Bertle</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Davel</t>
+  </si>
+  <si>
+    <t>Low-Medium</t>
+  </si>
+  <si>
+    <t>Medium-High</t>
+  </si>
+  <si>
+    <t>Dragonborn</t>
+  </si>
+  <si>
+    <t>Dwarf</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Elf</t>
+  </si>
+  <si>
+    <t>Gnome</t>
+  </si>
+  <si>
+    <t>Very Low</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Hollow</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Orc</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>Enemy HP</t>
+  </si>
+  <si>
+    <t>Bork (12 hits) (100 armor (50%))</t>
+  </si>
+  <si>
+    <t>Kraken (12 hits)</t>
   </si>
   <si>
     <t>1-Handed (+3)</t>
@@ -2536,7 +2629,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2756,6 +2849,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2828,6 +2924,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2864,14 +2963,38 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3331,7 +3454,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="97" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3347,10 +3470,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="96" t="s">
+      <c r="L8" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="96"/>
+      <c r="M8" s="97"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3383,13 +3506,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="122" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3401,7 +3524,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="113" t="s">
+      <c r="G10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3412,13 +3535,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="122" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3430,7 +3553,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="113" t="s">
+      <c r="G11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3441,13 +3564,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="124" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3459,7 +3582,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="115" t="s">
+      <c r="G12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3634,7 +3757,7 @@
       <c r="B22" s="66">
         <v>1</v>
       </c>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="92" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="66" t="s">
@@ -3659,7 +3782,7 @@
       <c r="B23" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="89">
+      <c r="C23" s="90">
         <v>6</v>
       </c>
       <c r="D23" s="68">
@@ -3682,7 +3805,7 @@
       <c r="B24" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="91">
+      <c r="C24" s="92">
         <v>8</v>
       </c>
       <c r="D24" s="66">
@@ -3713,39 +3836,39 @@
       <c r="K25" s="70"/>
     </row>
     <row r="26" ht="15.75" spans="1:11">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="51"/>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="75"/>
+      <c r="D26" s="76"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="97"/>
+      <c r="J26" s="99"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3754,16 +3877,16 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="81"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="97"/>
+      <c r="J28" s="99"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -3773,10 +3896,10 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="84"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -3792,20 +3915,20 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="82" t="s">
+      <c r="C30" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="83" t="s">
+      <c r="D30" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="84" t="s">
+      <c r="F30" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="83"/>
-      <c r="J30" s="100"/>
+      <c r="H30" s="84"/>
+      <c r="J30" s="102"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -3858,7 +3981,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="101"/>
+      <c r="J32" s="103"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -3893,20 +4016,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="86">
+      <c r="B34" s="87">
         <v>1</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="86"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="87"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -3916,38 +4039,38 @@
       <c r="A35" s="67">
         <v>1</v>
       </c>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="97"/>
+      <c r="J35" s="99"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
       <c r="A36" s="65">
         <v>1</v>
       </c>
-      <c r="B36" s="90" t="s">
+      <c r="B36" s="91" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="92"/>
       <c r="I36" s="45"/>
       <c r="J36" s="46"/>
       <c r="K36" s="58"/>
@@ -3983,7 +4106,7 @@
       <c r="C39" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="88"/>
+      <c r="D39" s="89"/>
       <c r="F39" s="58"/>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
@@ -3993,7 +4116,7 @@
     </row>
     <row r="40" ht="30" spans="1:11">
       <c r="A40" s="72"/>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="74" t="s">
         <v>83</v>
       </c>
       <c r="C40" s="51" t="s">
@@ -4005,17 +4128,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="92" t="s">
+      <c r="F40" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="88" t="s">
+      <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="116" t="s">
+      <c r="I40" s="126" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4034,10 +4157,10 @@
       <c r="F41" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="93">
+      <c r="G41" s="94">
         <v>10</v>
       </c>
-      <c r="I41" s="117" t="s">
+      <c r="I41" s="127" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4060,7 +4183,7 @@
       <c r="F42" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="93">
+      <c r="G42" s="94">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -4084,7 +4207,7 @@
       <c r="F43" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="93">
+      <c r="G43" s="94">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -4110,7 +4233,7 @@
       <c r="F44" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="93">
+      <c r="G44" s="94">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -4136,7 +4259,7 @@
       <c r="F45" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="93">
+      <c r="G45" s="94">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -4162,7 +4285,7 @@
       <c r="F46" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="93">
+      <c r="G46" s="94">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -4191,7 +4314,7 @@
       <c r="F47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="93">
+      <c r="G47" s="94">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -4217,7 +4340,7 @@
       <c r="F48" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="93">
+      <c r="G48" s="94">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -4240,7 +4363,7 @@
       <c r="F49" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="93">
+      <c r="G49" s="94">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -4266,7 +4389,7 @@
       <c r="F50" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="93">
+      <c r="G50" s="94">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -4292,7 +4415,7 @@
       <c r="F51" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="93">
+      <c r="G51" s="94">
         <v>11</v>
       </c>
       <c r="I51" s="40"/>
@@ -4510,11 +4633,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="109" t="s">
+      <c r="C62" s="121" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="109" t="s">
+      <c r="F62" s="121" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4533,7 +4656,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="105" t="s">
+      <c r="E64" s="107" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4580,7 +4703,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="109" t="s">
+      <c r="C70" s="121" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4597,10 +4720,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="106"/>
-      <c r="B72" s="107"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="110"/>
+      <c r="D72" s="110"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4705,7 +4828,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="118" t="s">
+      <c r="D77" s="128" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4723,7 +4846,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="106"/>
+      <c r="A78" s="108"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4733,16 +4856,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="110"/>
+      <c r="E78" s="120"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="110"/>
-      <c r="H78" s="110"/>
-      <c r="I78" s="110"/>
-      <c r="J78" s="110"/>
-      <c r="K78" s="110"/>
-      <c r="L78" s="110"/>
+      <c r="G78" s="120"/>
+      <c r="H78" s="120"/>
+      <c r="I78" s="120"/>
+      <c r="J78" s="120"/>
+      <c r="K78" s="120"/>
+      <c r="L78" s="120"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4799,7 +4922,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="118" t="s">
+      <c r="D81" s="128" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5072,8 +5195,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="111"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="119"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5157,8 +5280,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5263,7 +5386,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="97" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5279,10 +5402,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="96" t="s">
+      <c r="L8" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="96"/>
+      <c r="M8" s="97"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5315,13 +5438,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="122" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5333,7 +5456,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="113" t="s">
+      <c r="G10" s="123" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5344,13 +5467,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="122" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5362,7 +5485,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="113" t="s">
+      <c r="G11" s="123" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5373,13 +5496,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="124" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5391,7 +5514,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="115" t="s">
+      <c r="G12" s="125" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5414,13 +5537,25 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="2:6">
+    <row r="15" ht="15.75" spans="2:10">
       <c r="B15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-    </row>
-    <row r="16" ht="15.75" spans="1:8">
+      <c r="G15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I15" t="s">
+        <v>163</v>
+      </c>
+      <c r="J15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:11">
       <c r="A16" s="48" t="s">
         <v>34</v>
       </c>
@@ -5439,9 +5574,20 @@
       <c r="F16" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" ht="15.75" spans="1:8">
+      <c r="G16">
+        <v>16</v>
+      </c>
+      <c r="H16" s="40">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="1:11">
       <c r="A17" s="52">
         <v>0</v>
       </c>
@@ -5460,7 +5606,16 @@
       <c r="F17" s="55">
         <v>0</v>
       </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
       <c r="H17" s="40"/>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" ht="15.75" spans="1:11">
       <c r="A18" s="52">
@@ -5470,23 +5625,24 @@
         <v>0</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D18" s="40">
         <v>0</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F18" s="55">
         <v>-1</v>
       </c>
       <c r="G18">
-        <f>2*5.5</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H18" s="57"/>
-      <c r="K18" s="70"/>
+      <c r="K18" s="70">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" ht="15.75" spans="1:11">
       <c r="A19" s="52">
@@ -5496,20 +5652,24 @@
         <v>0</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D19" s="40">
         <v>0</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="G19"/>
+      <c r="G19">
+        <v>19</v>
+      </c>
       <c r="H19" s="58"/>
-      <c r="K19" s="70"/>
+      <c r="K19" s="70">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" ht="15.75" spans="1:11">
       <c r="A20" s="59">
@@ -5519,19 +5679,24 @@
         <v>1</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F20" s="63">
         <v>-1</v>
       </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
       <c r="H20" s="57"/>
-      <c r="K20" s="70"/>
+      <c r="K20" s="70">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" ht="15.75" spans="1:11">
       <c r="A21" s="52">
@@ -5541,19 +5706,24 @@
         <v>1</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F21" s="55">
         <v>-2</v>
       </c>
+      <c r="G21">
+        <v>16</v>
+      </c>
       <c r="H21" s="58"/>
-      <c r="K21" s="70"/>
+      <c r="K21" s="70">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" ht="16.5" spans="1:11">
       <c r="A22" s="65">
@@ -5566,16 +5736,21 @@
         <v>50</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F22" s="43">
         <v>-3</v>
       </c>
+      <c r="G22">
+        <v>15</v>
+      </c>
       <c r="H22" s="58"/>
-      <c r="K22" s="70"/>
+      <c r="K22" s="70">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" ht="15.75" spans="1:11">
       <c r="A23" s="67">
@@ -5594,11 +5769,15 @@
       <c r="F23" s="50">
         <v>3</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="40">
+        <v>16</v>
+      </c>
       <c r="H23" s="70"/>
       <c r="I23" s="70"/>
       <c r="J23" s="70"/>
-      <c r="K23" s="70"/>
+      <c r="K23" s="70">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" ht="16.5" spans="1:11">
       <c r="A24" s="65">
@@ -5617,11 +5796,15 @@
       <c r="F24" s="43">
         <v>5.5</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="40">
+        <v>18</v>
+      </c>
       <c r="H24" s="70"/>
       <c r="I24" s="70"/>
       <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
+      <c r="K24" s="70">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" ht="16.5" spans="1:11">
       <c r="A25" s="72"/>
@@ -5630,45 +5813,55 @@
       <c r="D25" s="58"/>
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
+      <c r="G25" s="73">
+        <v>16.5</v>
+      </c>
+      <c r="H25" s="40">
+        <v>2</v>
+      </c>
+      <c r="I25" s="70">
+        <v>1.5</v>
+      </c>
       <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
+      <c r="K25" s="98">
+        <f>46/9</f>
+        <v>5.11111111111111</v>
+      </c>
     </row>
     <row r="26" ht="15.75" spans="1:11">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="51"/>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="75"/>
+      <c r="D26" s="76"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="97"/>
+      <c r="J26" s="99"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -5677,16 +5870,16 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="81"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="97"/>
+      <c r="J28" s="99"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -5696,10 +5889,10 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="84"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -5715,20 +5908,20 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="82" t="s">
+      <c r="C30" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="83" t="s">
+      <c r="D30" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="84" t="s">
+      <c r="F30" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="83"/>
-      <c r="J30" s="100"/>
+      <c r="H30" s="84"/>
+      <c r="J30" s="102"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -5781,7 +5974,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="101"/>
+      <c r="J32" s="103"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -5816,20 +6009,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="86">
+      <c r="B34" s="87">
         <v>1</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="86"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="87"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -5839,38 +6032,38 @@
       <c r="A35" s="67">
         <v>1</v>
       </c>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="97"/>
+      <c r="J35" s="99"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
       <c r="A36" s="65">
         <v>1</v>
       </c>
-      <c r="B36" s="90" t="s">
+      <c r="B36" s="91" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="92"/>
       <c r="I36" s="45"/>
       <c r="J36" s="46"/>
       <c r="K36" s="58"/>
@@ -5906,7 +6099,7 @@
       <c r="C39" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="88"/>
+      <c r="D39" s="89"/>
       <c r="F39" s="58"/>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
@@ -5916,29 +6109,29 @@
     </row>
     <row r="40" ht="30" spans="1:11">
       <c r="A40" s="72"/>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="74" t="s">
         <v>83</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="92" t="s">
+      <c r="F40" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="88" t="s">
+      <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="116" t="s">
+      <c r="I40" s="126" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -5958,10 +6151,10 @@
       <c r="F41" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="93">
+      <c r="G41" s="94">
         <v>10</v>
       </c>
-      <c r="I41" s="117" t="s">
+      <c r="I41" s="127" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -5985,7 +6178,7 @@
       <c r="F42" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="93">
+      <c r="G42" s="94">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -6010,7 +6203,7 @@
       <c r="F43" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="93">
+      <c r="G43" s="94">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -6037,7 +6230,7 @@
       <c r="F44" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="93">
+      <c r="G44" s="94">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -6064,7 +6257,7 @@
       <c r="F45" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="93">
+      <c r="G45" s="94">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -6091,7 +6284,7 @@
       <c r="F46" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="93">
+      <c r="G46" s="94">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -6121,7 +6314,7 @@
       <c r="F47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="93">
+      <c r="G47" s="94">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -6145,7 +6338,7 @@
       <c r="F48" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="93">
+      <c r="G48" s="94">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -6172,7 +6365,7 @@
       <c r="F49" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="93">
+      <c r="G49" s="94">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -6199,7 +6392,7 @@
       <c r="F50" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="93">
+      <c r="G50" s="94">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -6223,7 +6416,7 @@
       <c r="F51" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="93">
+      <c r="G51" s="94">
         <v>11</v>
       </c>
       <c r="H51">
@@ -6235,10 +6428,10 @@
       <c r="K51" s="58"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="95">
+      <c r="B52" s="96">
         <v>300</v>
       </c>
       <c r="C52" s="40">
@@ -6263,23 +6456,23 @@
       <c r="M52" s="58"/>
     </row>
     <row r="53" ht="15.75" spans="1:13">
-      <c r="A53" s="94" t="s">
+      <c r="A53" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="95">
+      <c r="B53" s="96">
         <v>325</v>
       </c>
-      <c r="C53" s="95">
+      <c r="C53" s="96">
         <v>120</v>
       </c>
-      <c r="D53" s="95">
+      <c r="D53" s="96">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E53" s="95" t="s">
+      <c r="E53" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="95" t="s">
+      <c r="F53" s="96" t="s">
         <v>122</v>
       </c>
       <c r="G53" s="41">
@@ -6456,17 +6649,17 @@
       <c r="B60" s="52">
         <v>500</v>
       </c>
-      <c r="C60" s="95">
+      <c r="C60" s="96">
         <v>218</v>
       </c>
-      <c r="D60" s="95">
+      <c r="D60" s="96">
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-      <c r="E60" s="95" t="s">
+      <c r="E60" s="96" t="s">
         <v>136</v>
       </c>
-      <c r="F60" s="95" t="s">
+      <c r="F60" s="96" t="s">
         <v>137</v>
       </c>
       <c r="G60" s="41">
@@ -6483,14 +6676,14 @@
       <c r="B61" s="52">
         <v>600</v>
       </c>
-      <c r="C61" s="95"/>
-      <c r="D61" s="95">
+      <c r="C61" s="96"/>
+      <c r="D61" s="96">
         <v>350</v>
       </c>
-      <c r="E61" s="95">
+      <c r="E61" s="96">
         <v>14.5</v>
       </c>
-      <c r="F61" s="95"/>
+      <c r="F61" s="96"/>
       <c r="G61" s="41">
         <v>13</v>
       </c>
@@ -6505,21 +6698,21 @@
       <c r="B62" s="52">
         <v>750</v>
       </c>
-      <c r="C62" s="95"/>
-      <c r="D62" s="95">
+      <c r="C62" s="96"/>
+      <c r="D62" s="96">
         <v>441</v>
       </c>
-      <c r="E62" s="95">
+      <c r="E62" s="96">
         <v>17.25</v>
       </c>
-      <c r="F62" s="95" t="s">
-        <v>174</v>
+      <c r="F62" s="96" t="s">
+        <v>178</v>
       </c>
       <c r="G62" s="41">
         <v>13</v>
       </c>
       <c r="H62" s="40"/>
-      <c r="I62" s="103">
+      <c r="I62" s="105">
         <f>SUM(I55:I61)</f>
         <v>1825</v>
       </c>
@@ -6551,18 +6744,21 @@
     </row>
     <row r="65" ht="15.75" spans="7:9">
       <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
+      <c r="H65" s="40">
+        <f>4*3.5</f>
+        <v>14</v>
+      </c>
       <c r="I65" s="40"/>
     </row>
     <row r="66" ht="75.75" spans="3:9">
-      <c r="C66" s="104" t="s">
+      <c r="C66" s="106" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="104" t="s">
+      <c r="D66" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="E66" s="104" t="s">
-        <v>175</v>
+      <c r="E66" s="106" t="s">
+        <v>179</v>
       </c>
       <c r="G66" s="40">
         <f>350*4*0.8</f>
@@ -6579,7 +6775,7 @@
       <c r="I67" s="40"/>
     </row>
     <row r="68" spans="5:9">
-      <c r="E68" s="105"/>
+      <c r="E68" s="107"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
@@ -6608,32 +6804,42 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="106"/>
-      <c r="B72" s="107"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="110"/>
+      <c r="D72" s="110"/>
       <c r="E72" s="58"/>
-      <c r="F72" s="58" t="s">
-        <v>143</v>
-      </c>
+      <c r="F72" s="58"/>
       <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
+      <c r="H72" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="I72" s="58" t="s">
+        <v>181</v>
+      </c>
       <c r="J72" s="58"/>
       <c r="K72" s="58"/>
       <c r="M72" s="40"/>
       <c r="N72" s="40"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" ht="15.75" spans="1:14">
       <c r="A73" s="40"/>
       <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
+      <c r="C73" s="40" t="s">
+        <v>182</v>
+      </c>
       <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
+      <c r="E73" s="40" t="s">
+        <v>183</v>
+      </c>
       <c r="F73" s="40"/>
       <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
+      <c r="H73" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="I73" s="40" t="s">
+        <v>184</v>
+      </c>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
       <c r="M73" s="40"/>
@@ -6641,20 +6847,28 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="40"/>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="111" t="s">
         <v>144</v>
       </c>
-      <c r="C74" s="40" t="s">
+      <c r="C74" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E74" s="40"/>
+      <c r="D74" s="112" t="s">
+        <v>185</v>
+      </c>
+      <c r="E74" s="112" t="s">
+        <v>186</v>
+      </c>
       <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
+      <c r="G74" s="113" t="s">
+        <v>187</v>
+      </c>
+      <c r="H74" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="I74" s="113" t="s">
+        <v>189</v>
+      </c>
       <c r="J74" s="40"/>
       <c r="K74" s="40"/>
       <c r="M74" s="40"/>
@@ -6662,20 +6876,28 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="40"/>
-      <c r="B75" s="40">
+      <c r="B75" s="114">
         <v>1</v>
       </c>
-      <c r="C75" s="40">
-        <v>20</v>
-      </c>
-      <c r="D75" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="E75" s="40"/>
+      <c r="C75" s="115">
+        <v>22</v>
+      </c>
+      <c r="D75" s="115">
+        <v>10</v>
+      </c>
+      <c r="E75" s="115">
+        <v>7</v>
+      </c>
       <c r="F75" s="40"/>
-      <c r="G75" s="40"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="40"/>
+      <c r="G75" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="H75" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="I75" s="40" t="s">
+        <v>192</v>
+      </c>
       <c r="J75" s="40"/>
       <c r="K75" s="40"/>
       <c r="L75" s="40"/>
@@ -6684,95 +6906,121 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="40"/>
-      <c r="B76" s="40">
+      <c r="B76" s="114">
         <v>2</v>
       </c>
-      <c r="C76" s="40">
-        <v>25</v>
-      </c>
-      <c r="D76" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="E76" s="40"/>
-      <c r="F76" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="G76" s="40">
-        <v>3.5</v>
-      </c>
-      <c r="H76" s="40"/>
-      <c r="I76" s="40"/>
+      <c r="C76" s="115">
+        <v>27</v>
+      </c>
+      <c r="D76" s="115">
+        <f>FLOOR(C76/2,1)</f>
+        <v>13</v>
+      </c>
+      <c r="E76" s="115">
+        <v>8</v>
+      </c>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="H76" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="I76" s="40" t="s">
+        <v>191</v>
+      </c>
       <c r="J76" s="40"/>
       <c r="K76" s="40"/>
       <c r="L76" s="40"/>
       <c r="M76" s="40"/>
       <c r="N76" s="40"/>
     </row>
-    <row r="77" ht="45" spans="1:14">
+    <row r="77" spans="1:14">
       <c r="A77" s="40"/>
-      <c r="B77" s="40">
+      <c r="B77" s="114">
         <v>3</v>
       </c>
-      <c r="C77" s="40">
-        <v>30</v>
-      </c>
-      <c r="D77" s="118" t="s">
-        <v>150</v>
-      </c>
-      <c r="E77" s="40"/>
-      <c r="F77" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="G77" s="40">
+      <c r="C77" s="115">
+        <v>32</v>
+      </c>
+      <c r="D77" s="115">
+        <f t="shared" ref="D77:D84" si="1">FLOOR(C77/2,1)</f>
+        <v>16</v>
+      </c>
+      <c r="E77" s="115">
         <v>9</v>
       </c>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="H77" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="I77" s="40" t="s">
+        <v>189</v>
+      </c>
       <c r="J77" s="40"/>
       <c r="K77" s="40"/>
       <c r="M77" s="40"/>
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="106"/>
-      <c r="B78" s="40">
+      <c r="A78" s="108"/>
+      <c r="B78" s="114">
         <v>4</v>
       </c>
-      <c r="C78" s="40">
-        <v>35</v>
-      </c>
-      <c r="D78" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="E78" s="110"/>
-      <c r="F78" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="G78" s="110"/>
-      <c r="H78" s="110"/>
-      <c r="I78" s="110"/>
-      <c r="J78" s="110"/>
-      <c r="K78" s="110"/>
-      <c r="L78" s="110"/>
+      <c r="C78" s="115">
+        <v>37</v>
+      </c>
+      <c r="D78" s="115">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E78" s="115">
+        <v>10</v>
+      </c>
+      <c r="F78" s="40"/>
+      <c r="G78" s="116" t="s">
+        <v>196</v>
+      </c>
+      <c r="H78" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="I78" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="J78" s="120"/>
+      <c r="K78" s="120"/>
+      <c r="L78" s="120"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="40"/>
-      <c r="B79" s="40">
+      <c r="B79" s="114">
         <v>5</v>
       </c>
-      <c r="C79" s="40">
-        <v>40</v>
-      </c>
-      <c r="D79" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="E79" s="40"/>
+      <c r="C79" s="115">
+        <v>42</v>
+      </c>
+      <c r="D79" s="115">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="E79" s="115">
+        <v>11</v>
+      </c>
       <c r="F79" s="40"/>
-      <c r="G79" s="40"/>
-      <c r="H79" s="40"/>
-      <c r="I79" s="40"/>
+      <c r="G79" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="H79" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="I79" s="40" t="s">
+        <v>199</v>
+      </c>
       <c r="J79" s="40"/>
       <c r="K79" s="40"/>
       <c r="M79" s="40"/>
@@ -6780,44 +7028,60 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="40"/>
-      <c r="B80" s="40">
+      <c r="B80" s="114">
         <v>6</v>
       </c>
-      <c r="C80" s="40">
-        <v>45</v>
-      </c>
-      <c r="D80" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E80" s="40"/>
-      <c r="F80" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="G80" s="40"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="40"/>
+      <c r="C80" s="115">
+        <v>47</v>
+      </c>
+      <c r="D80" s="115">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E80" s="115">
+        <v>12</v>
+      </c>
+      <c r="F80" s="40"/>
+      <c r="G80" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="H80" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="I80" s="40" t="s">
+        <v>198</v>
+      </c>
       <c r="J80" s="40"/>
       <c r="K80" s="40"/>
       <c r="L80" s="40"/>
       <c r="M80" s="40"/>
       <c r="N80" s="40"/>
     </row>
-    <row r="81" ht="45" spans="1:14">
+    <row r="81" spans="1:14">
       <c r="A81" s="40"/>
-      <c r="B81" s="40">
+      <c r="B81" s="114">
         <v>7</v>
       </c>
-      <c r="C81" s="40">
-        <v>50</v>
-      </c>
-      <c r="D81" s="118" t="s">
-        <v>150</v>
-      </c>
-      <c r="E81" s="40"/>
+      <c r="C81" s="115">
+        <v>52</v>
+      </c>
+      <c r="D81" s="115">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E81" s="115">
+        <v>13</v>
+      </c>
       <c r="F81" s="40"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="40"/>
-      <c r="I81" s="40"/>
+      <c r="G81" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="H81" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="I81" s="40" t="s">
+        <v>189</v>
+      </c>
       <c r="J81" s="40"/>
       <c r="K81" s="40"/>
       <c r="L81" s="40"/>
@@ -6826,35 +7090,47 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="40"/>
-      <c r="B82" s="40">
+      <c r="B82" s="114">
         <v>8</v>
       </c>
-      <c r="C82" s="40">
-        <v>55</v>
-      </c>
-      <c r="D82" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E82" s="40"/>
+      <c r="C82" s="115">
+        <v>57</v>
+      </c>
+      <c r="D82" s="115">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E82" s="115">
+        <v>14</v>
+      </c>
       <c r="F82" s="40"/>
-      <c r="G82" s="40"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="40"/>
+      <c r="G82" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H82" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="I82" s="40" t="s">
+        <v>188</v>
+      </c>
       <c r="J82" s="40"/>
       <c r="K82" s="40"/>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="40"/>
-      <c r="B83" s="40">
+      <c r="B83" s="114">
         <v>9</v>
       </c>
-      <c r="C83" s="40">
-        <v>60</v>
-      </c>
-      <c r="D83" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="E83" s="40"/>
+      <c r="C83" s="115">
+        <v>62</v>
+      </c>
+      <c r="D83" s="115">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="E83" s="115">
+        <v>15</v>
+      </c>
       <c r="F83" s="40"/>
       <c r="G83" s="40"/>
       <c r="H83" s="40"/>
@@ -6862,18 +7138,21 @@
       <c r="J83" s="40"/>
       <c r="K83" s="40"/>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" ht="15.75" spans="1:11">
       <c r="A84" s="40"/>
-      <c r="B84" s="40">
+      <c r="B84" s="117">
         <v>10</v>
       </c>
-      <c r="C84" s="40">
-        <v>65</v>
-      </c>
-      <c r="D84" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="E84" s="40"/>
+      <c r="C84" s="118">
+        <v>67</v>
+      </c>
+      <c r="D84" s="118">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="E84" s="118">
+        <v>16</v>
+      </c>
       <c r="F84" s="40"/>
       <c r="G84" s="40"/>
       <c r="H84" s="40"/>
@@ -6885,14 +7164,16 @@
       <c r="A85" s="40"/>
       <c r="B85" s="40"/>
       <c r="C85" s="40"/>
-      <c r="D85" s="40" t="s">
-        <v>160</v>
-      </c>
+      <c r="D85" s="40"/>
       <c r="E85" s="40"/>
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
-      <c r="H85" s="40"/>
-      <c r="I85" s="40"/>
+      <c r="H85" s="40">
+        <v>5</v>
+      </c>
+      <c r="I85" s="40">
+        <v>3</v>
+      </c>
       <c r="J85" s="40"/>
       <c r="K85" s="40"/>
     </row>
@@ -6903,7 +7184,7 @@
       <c r="E86" s="40"/>
       <c r="F86" s="40"/>
       <c r="G86" s="40"/>
-      <c r="H86" s="40"/>
+      <c r="H86" s="107"/>
       <c r="I86" s="40"/>
       <c r="J86" s="40"/>
       <c r="K86" s="40"/>
@@ -6933,35 +7214,67 @@
       <c r="K88" s="40"/>
     </row>
     <row r="89" spans="2:11">
-      <c r="B89" s="40"/>
-      <c r="C89" s="40"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="40"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="40"/>
+      <c r="B89" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C89" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="D89" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="E89" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="F89" s="40" t="s">
+        <v>206</v>
+      </c>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
       <c r="J89" s="40"/>
       <c r="K89" s="40"/>
     </row>
     <row r="90" spans="2:11">
-      <c r="B90" s="40"/>
-      <c r="C90" s="40"/>
-      <c r="D90" s="40"/>
-      <c r="E90" s="40"/>
-      <c r="F90" s="40"/>
-      <c r="G90" s="40"/>
+      <c r="B90" s="40">
+        <v>10</v>
+      </c>
+      <c r="C90" s="40">
+        <v>200</v>
+      </c>
+      <c r="D90" s="40">
+        <v>2000</v>
+      </c>
+      <c r="E90" s="40">
+        <f>12*200+936+70</f>
+        <v>3406</v>
+      </c>
+      <c r="F90" s="40">
+        <f>(55+130)*4+12*200*1.2*1.05</f>
+        <v>3764</v>
+      </c>
       <c r="H90" s="40"/>
       <c r="I90" s="40"/>
       <c r="J90" s="40"/>
       <c r="K90" s="40"/>
     </row>
     <row r="91" spans="2:11">
-      <c r="B91" s="40"/>
-      <c r="C91" s="40"/>
-      <c r="D91" s="40"/>
-      <c r="E91" s="40"/>
-      <c r="F91" s="40"/>
+      <c r="B91" s="40">
+        <v>10</v>
+      </c>
+      <c r="C91" s="40">
+        <v>200</v>
+      </c>
+      <c r="D91" s="40">
+        <v>3000</v>
+      </c>
+      <c r="E91" s="40">
+        <f>12*200+936*1.5+70</f>
+        <v>3874</v>
+      </c>
+      <c r="F91" s="40">
+        <f>(55+130)*4+12*200*1.2*1.05</f>
+        <v>3764</v>
+      </c>
       <c r="G91" s="40"/>
       <c r="H91" s="40"/>
       <c r="I91" s="40"/>
@@ -7009,7 +7322,7 @@
       <c r="C95" s="40"/>
       <c r="D95" s="40"/>
       <c r="E95" s="40"/>
-      <c r="F95" s="40"/>
+      <c r="F95" s="105"/>
       <c r="G95" s="40"/>
       <c r="H95" s="40"/>
       <c r="I95" s="40"/>
@@ -7028,7 +7341,8 @@
       <c r="J96" s="40"/>
       <c r="K96" s="40"/>
     </row>
-    <row r="97" spans="9:11">
+    <row r="97" spans="5:11">
+      <c r="E97" s="40"/>
       <c r="I97" s="40"/>
       <c r="J97" s="40"/>
       <c r="K97" s="40"/>
@@ -7039,7 +7353,7 @@
       <c r="C98" s="40"/>
       <c r="D98" s="40"/>
       <c r="E98" s="40"/>
-      <c r="F98" s="40"/>
+      <c r="F98" s="105"/>
       <c r="G98" s="40"/>
       <c r="H98" s="40"/>
       <c r="I98" s="40"/>
@@ -7083,8 +7397,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="111"/>
+      <c r="E103" s="40"/>
+      <c r="F103" s="119"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -7188,31 +7502,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7220,28 +7534,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7249,28 +7563,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7278,28 +7592,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7307,28 +7621,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>198</v>
+        <v>229</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7336,28 +7650,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7365,28 +7679,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7394,28 +7708,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7423,28 +7737,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7452,28 +7766,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7481,28 +7795,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>238</v>
+        <v>269</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>244</v>
+        <v>275</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7510,28 +7824,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>253</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7539,28 +7853,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7568,33 +7882,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>260</v>
+        <v>291</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7626,34 +7940,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>273</v>
+        <v>304</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7661,31 +7975,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>277</v>
+        <v>308</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>277</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7693,31 +8007,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>279</v>
+        <v>310</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>279</v>
+        <v>310</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7725,31 +8039,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>285</v>
+        <v>316</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7757,31 +8071,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>289</v>
+        <v>320</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>291</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7789,31 +8103,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>293</v>
+        <v>324</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>294</v>
+        <v>325</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>295</v>
+        <v>326</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>296</v>
+        <v>327</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>297</v>
+        <v>328</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7821,31 +8135,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>298</v>
+        <v>329</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>299</v>
+        <v>330</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>300</v>
+        <v>331</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>298</v>
+        <v>329</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>302</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7853,31 +8167,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>303</v>
+        <v>334</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>304</v>
+        <v>335</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>305</v>
+        <v>336</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>303</v>
+        <v>334</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>307</v>
+        <v>338</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>308</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7885,31 +8199,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>312</v>
+        <v>343</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>313</v>
+        <v>344</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>314</v>
+        <v>345</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>315</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7917,31 +8231,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>316</v>
+        <v>347</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>317</v>
+        <v>348</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>318</v>
+        <v>349</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>319</v>
+        <v>350</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>320</v>
+        <v>351</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>323</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7949,31 +8263,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>325</v>
+        <v>356</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>327</v>
+        <v>358</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7981,31 +8295,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>331</v>
+        <v>362</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>332</v>
+        <v>363</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>333</v>
+        <v>364</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>337</v>
+        <v>368</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>338</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8013,31 +8327,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>339</v>
+        <v>370</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>340</v>
+        <v>371</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>341</v>
+        <v>372</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>343</v>
+        <v>374</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>344</v>
+        <v>375</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>345</v>
+        <v>376</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>346</v>
+        <v>377</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>347</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8045,63 +8359,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>349</v>
+        <v>380</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>350</v>
+        <v>381</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>351</v>
+        <v>382</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>352</v>
+        <v>383</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>353</v>
+        <v>384</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>354</v>
+        <v>385</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>357</v>
+        <v>388</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>359</v>
+        <v>390</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>360</v>
+        <v>391</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>361</v>
+        <v>392</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>362</v>
+        <v>393</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>363</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded changes to new repo folder on my local machine. Old repo folder .git was corrupted.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="392">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -734,15 +734,6 @@
   </si>
   <si>
     <t>XP Reward per Difficulty</t>
-  </si>
-  <si>
-    <t>Race Start</t>
-  </si>
-  <si>
-    <t>Average Might</t>
-  </si>
-  <si>
-    <t>Extra Class Start</t>
   </si>
   <si>
     <t>Per Level</t>
@@ -2629,7 +2620,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2963,28 +2954,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3349,7 +3322,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -3506,13 +3479,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="116" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="117" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3524,7 +3497,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="123" t="s">
+      <c r="G10" s="117" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3535,13 +3508,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="116" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="117" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3553,7 +3526,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="123" t="s">
+      <c r="G11" s="117" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3564,13 +3537,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="118" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="119" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3582,7 +3555,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="119" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -4134,7 +4107,7 @@
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="126" t="s">
+      <c r="I40" s="120" t="s">
         <v>89</v>
       </c>
       <c r="J40" s="104"/>
@@ -4160,7 +4133,7 @@
       <c r="G41" s="94">
         <v>10</v>
       </c>
-      <c r="I41" s="127" t="s">
+      <c r="I41" s="121" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4633,11 +4606,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="121" t="s">
+      <c r="C62" s="115" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="121" t="s">
+      <c r="F62" s="115" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4703,7 +4676,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="121" t="s">
+      <c r="C70" s="115" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4828,7 +4801,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="128" t="s">
+      <c r="D77" s="122" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4856,16 +4829,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="120"/>
+      <c r="E78" s="114"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="120"/>
-      <c r="H78" s="120"/>
-      <c r="I78" s="120"/>
-      <c r="J78" s="120"/>
-      <c r="K78" s="120"/>
-      <c r="L78" s="120"/>
+      <c r="G78" s="114"/>
+      <c r="H78" s="114"/>
+      <c r="I78" s="114"/>
+      <c r="J78" s="114"/>
+      <c r="K78" s="114"/>
+      <c r="L78" s="114"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4922,7 +4895,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="128" t="s">
+      <c r="D81" s="122" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5195,8 +5168,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="119"/>
-      <c r="F103" s="119"/>
+      <c r="E103" s="113"/>
+      <c r="F103" s="113"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5280,8 +5253,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5438,13 +5411,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="116" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="117" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5456,7 +5429,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="123" t="s">
+      <c r="G10" s="117" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5467,13 +5440,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="116" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="117" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5485,7 +5458,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="123" t="s">
+      <c r="G11" s="117" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5496,13 +5469,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="118" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="119" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5514,7 +5487,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="119" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5537,22 +5510,16 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="2:10">
+    <row r="15" spans="2:10">
       <c r="B15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-      <c r="G15" t="s">
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15" t="s">
         <v>161</v>
-      </c>
-      <c r="H15" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" t="s">
-        <v>163</v>
-      </c>
-      <c r="J15" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:11">
@@ -5574,15 +5541,9 @@
       <c r="F16" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G16">
-        <v>16</v>
-      </c>
-      <c r="H16" s="40">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
+      <c r="G16"/>
+      <c r="H16" s="40"/>
+      <c r="I16"/>
       <c r="K16">
         <v>5</v>
       </c>
@@ -5606,13 +5567,9 @@
       <c r="F17" s="55">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>16</v>
-      </c>
+      <c r="G17"/>
       <c r="H17" s="40"/>
-      <c r="I17">
-        <v>3</v>
-      </c>
+      <c r="I17"/>
       <c r="K17">
         <v>6</v>
       </c>
@@ -5625,20 +5582,18 @@
         <v>0</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D18" s="40">
         <v>0</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F18" s="55">
         <v>-1</v>
       </c>
-      <c r="G18">
-        <v>17</v>
-      </c>
+      <c r="G18"/>
       <c r="H18" s="57"/>
       <c r="K18" s="70">
         <v>4</v>
@@ -5652,20 +5607,18 @@
         <v>0</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D19" s="40">
         <v>0</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="G19">
-        <v>19</v>
-      </c>
+      <c r="G19"/>
       <c r="H19" s="58"/>
       <c r="K19" s="70">
         <v>5</v>
@@ -5679,20 +5632,18 @@
         <v>1</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F20" s="63">
         <v>-1</v>
       </c>
-      <c r="G20">
-        <v>17</v>
-      </c>
+      <c r="G20"/>
       <c r="H20" s="57"/>
       <c r="K20" s="70">
         <v>6</v>
@@ -5706,20 +5657,18 @@
         <v>1</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F21" s="55">
         <v>-2</v>
       </c>
-      <c r="G21">
-        <v>16</v>
-      </c>
+      <c r="G21"/>
       <c r="H21" s="58"/>
       <c r="K21" s="70">
         <v>4</v>
@@ -5736,17 +5685,15 @@
         <v>50</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F22" s="43">
         <v>-3</v>
       </c>
-      <c r="G22">
-        <v>15</v>
-      </c>
+      <c r="G22"/>
       <c r="H22" s="58"/>
       <c r="K22" s="70">
         <v>5</v>
@@ -5769,9 +5716,7 @@
       <c r="F23" s="50">
         <v>3</v>
       </c>
-      <c r="G23" s="40">
-        <v>16</v>
-      </c>
+      <c r="G23" s="40"/>
       <c r="H23" s="70"/>
       <c r="I23" s="70"/>
       <c r="J23" s="70"/>
@@ -5796,9 +5741,7 @@
       <c r="F24" s="43">
         <v>5.5</v>
       </c>
-      <c r="G24" s="40">
-        <v>18</v>
-      </c>
+      <c r="G24" s="40"/>
       <c r="H24" s="70"/>
       <c r="I24" s="70"/>
       <c r="J24" s="70"/>
@@ -5813,15 +5756,9 @@
       <c r="D25" s="58"/>
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
-      <c r="G25" s="73">
-        <v>16.5</v>
-      </c>
-      <c r="H25" s="40">
-        <v>2</v>
-      </c>
-      <c r="I25" s="70">
-        <v>1.5</v>
-      </c>
+      <c r="G25" s="73"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="70"/>
       <c r="J25" s="70"/>
       <c r="K25" s="98">
         <f>46/9</f>
@@ -6116,7 +6053,7 @@
         <v>84</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E40" s="51" t="s">
         <v>86</v>
@@ -6127,7 +6064,7 @@
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="126" t="s">
+      <c r="I40" s="120" t="s">
         <v>89</v>
       </c>
       <c r="J40" s="104"/>
@@ -6154,7 +6091,7 @@
       <c r="G41" s="94">
         <v>10</v>
       </c>
-      <c r="I41" s="127" t="s">
+      <c r="I41" s="121" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -6706,7 +6643,7 @@
         <v>17.25</v>
       </c>
       <c r="F62" s="96" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G62" s="41">
         <v>13</v>
@@ -6758,7 +6695,7 @@
         <v>142</v>
       </c>
       <c r="E66" s="106" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G66" s="40">
         <f>350*4*0.8</f>
@@ -6812,10 +6749,10 @@
       <c r="F72" s="58"/>
       <c r="G72" s="58"/>
       <c r="H72" s="58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J72" s="58"/>
       <c r="K72" s="58"/>
@@ -6826,11 +6763,11 @@
       <c r="A73" s="40"/>
       <c r="B73" s="40"/>
       <c r="C73" s="40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D73" s="40"/>
       <c r="E73" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F73" s="40"/>
       <c r="G73" s="40"/>
@@ -6838,7 +6775,7 @@
         <v>145</v>
       </c>
       <c r="I73" s="40" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
@@ -6847,27 +6784,27 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="40"/>
-      <c r="B74" s="111" t="s">
+      <c r="B74" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="C74" s="112" t="s">
+      <c r="C74" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="112" t="s">
+      <c r="D74" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="F74" s="40"/>
+      <c r="G74" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="H74" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E74" s="112" t="s">
+      <c r="I74" s="111" t="s">
         <v>186</v>
-      </c>
-      <c r="F74" s="40"/>
-      <c r="G74" s="113" t="s">
-        <v>187</v>
-      </c>
-      <c r="H74" s="113" t="s">
-        <v>188</v>
-      </c>
-      <c r="I74" s="113" t="s">
-        <v>189</v>
       </c>
       <c r="J74" s="40"/>
       <c r="K74" s="40"/>
@@ -6876,27 +6813,27 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="40"/>
-      <c r="B75" s="114">
+      <c r="B75" s="39">
         <v>1</v>
       </c>
-      <c r="C75" s="115">
+      <c r="C75" s="55">
         <v>22</v>
       </c>
-      <c r="D75" s="115">
+      <c r="D75" s="55">
         <v>10</v>
       </c>
-      <c r="E75" s="115">
+      <c r="E75" s="55">
         <v>7</v>
       </c>
       <c r="F75" s="40"/>
       <c r="G75" s="40" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I75" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J75" s="40"/>
       <c r="K75" s="40"/>
@@ -6906,28 +6843,28 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="40"/>
-      <c r="B76" s="114">
+      <c r="B76" s="39">
         <v>2</v>
       </c>
-      <c r="C76" s="115">
+      <c r="C76" s="55">
         <v>27</v>
       </c>
-      <c r="D76" s="115">
+      <c r="D76" s="55">
         <f>FLOOR(C76/2,1)</f>
         <v>13</v>
       </c>
-      <c r="E76" s="115">
+      <c r="E76" s="55">
         <v>8</v>
       </c>
       <c r="F76" s="40"/>
       <c r="G76" s="40" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J76" s="40"/>
       <c r="K76" s="40"/>
@@ -6937,28 +6874,28 @@
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="40"/>
-      <c r="B77" s="114">
+      <c r="B77" s="39">
         <v>3</v>
       </c>
-      <c r="C77" s="115">
+      <c r="C77" s="55">
         <v>32</v>
       </c>
-      <c r="D77" s="115">
+      <c r="D77" s="55">
         <f t="shared" ref="D77:D84" si="1">FLOOR(C77/2,1)</f>
         <v>16</v>
       </c>
-      <c r="E77" s="115">
+      <c r="E77" s="55">
         <v>9</v>
       </c>
       <c r="F77" s="40"/>
       <c r="G77" s="40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I77" s="40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J77" s="40"/>
       <c r="K77" s="40"/>
@@ -6967,59 +6904,59 @@
     </row>
     <row r="78" ht="15.75" spans="1:14">
       <c r="A78" s="108"/>
-      <c r="B78" s="114">
+      <c r="B78" s="39">
         <v>4</v>
       </c>
-      <c r="C78" s="115">
+      <c r="C78" s="55">
         <v>37</v>
       </c>
-      <c r="D78" s="115">
+      <c r="D78" s="55">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E78" s="115">
+      <c r="E78" s="55">
         <v>10</v>
       </c>
       <c r="F78" s="40"/>
-      <c r="G78" s="116" t="s">
-        <v>196</v>
-      </c>
-      <c r="H78" s="116" t="s">
-        <v>189</v>
-      </c>
-      <c r="I78" s="116" t="s">
-        <v>189</v>
-      </c>
-      <c r="J78" s="120"/>
-      <c r="K78" s="120"/>
-      <c r="L78" s="120"/>
+      <c r="G78" s="112" t="s">
+        <v>193</v>
+      </c>
+      <c r="H78" s="112" t="s">
+        <v>186</v>
+      </c>
+      <c r="I78" s="112" t="s">
+        <v>186</v>
+      </c>
+      <c r="J78" s="114"/>
+      <c r="K78" s="114"/>
+      <c r="L78" s="114"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="40"/>
-      <c r="B79" s="114">
+      <c r="B79" s="39">
         <v>5</v>
       </c>
-      <c r="C79" s="115">
+      <c r="C79" s="55">
         <v>42</v>
       </c>
-      <c r="D79" s="115">
+      <c r="D79" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E79" s="115">
+      <c r="E79" s="55">
         <v>11</v>
       </c>
       <c r="F79" s="40"/>
       <c r="G79" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I79" s="40" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J79" s="40"/>
       <c r="K79" s="40"/>
@@ -7028,28 +6965,28 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="40"/>
-      <c r="B80" s="114">
+      <c r="B80" s="39">
         <v>6</v>
       </c>
-      <c r="C80" s="115">
+      <c r="C80" s="55">
         <v>47</v>
       </c>
-      <c r="D80" s="115">
+      <c r="D80" s="55">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="E80" s="115">
+      <c r="E80" s="55">
         <v>12</v>
       </c>
       <c r="F80" s="40"/>
       <c r="G80" s="40" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H80" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="I80" s="40" t="s">
         <v>195</v>
-      </c>
-      <c r="I80" s="40" t="s">
-        <v>198</v>
       </c>
       <c r="J80" s="40"/>
       <c r="K80" s="40"/>
@@ -7059,28 +6996,28 @@
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="40"/>
-      <c r="B81" s="114">
+      <c r="B81" s="39">
         <v>7</v>
       </c>
-      <c r="C81" s="115">
+      <c r="C81" s="55">
         <v>52</v>
       </c>
-      <c r="D81" s="115">
+      <c r="D81" s="55">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E81" s="115">
+      <c r="E81" s="55">
         <v>13</v>
       </c>
       <c r="F81" s="40"/>
       <c r="G81" s="40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I81" s="40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J81" s="40"/>
       <c r="K81" s="40"/>
@@ -7090,45 +7027,45 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="40"/>
-      <c r="B82" s="114">
+      <c r="B82" s="39">
         <v>8</v>
       </c>
-      <c r="C82" s="115">
+      <c r="C82" s="55">
         <v>57</v>
       </c>
-      <c r="D82" s="115">
+      <c r="D82" s="55">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="E82" s="115">
+      <c r="E82" s="55">
         <v>14</v>
       </c>
       <c r="F82" s="40"/>
       <c r="G82" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I82" s="40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J82" s="40"/>
       <c r="K82" s="40"/>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="40"/>
-      <c r="B83" s="114">
+      <c r="B83" s="39">
         <v>9</v>
       </c>
-      <c r="C83" s="115">
+      <c r="C83" s="55">
         <v>62</v>
       </c>
-      <c r="D83" s="115">
+      <c r="D83" s="55">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="E83" s="115">
+      <c r="E83" s="55">
         <v>15</v>
       </c>
       <c r="F83" s="40"/>
@@ -7140,17 +7077,17 @@
     </row>
     <row r="84" ht="15.75" spans="1:11">
       <c r="A84" s="40"/>
-      <c r="B84" s="117">
+      <c r="B84" s="44">
         <v>10</v>
       </c>
-      <c r="C84" s="118">
+      <c r="C84" s="43">
         <v>67</v>
       </c>
-      <c r="D84" s="118">
+      <c r="D84" s="43">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="E84" s="118">
+      <c r="E84" s="43">
         <v>16</v>
       </c>
       <c r="F84" s="40"/>
@@ -7218,16 +7155,16 @@
         <v>144</v>
       </c>
       <c r="C89" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D89" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="E89" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="F89" s="40" t="s">
         <v>203</v>
-      </c>
-      <c r="D89" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="E89" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="F89" s="40" t="s">
-        <v>206</v>
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
@@ -7398,7 +7335,7 @@
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
       <c r="E103" s="40"/>
-      <c r="F103" s="119"/>
+      <c r="F103" s="113"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -7483,7 +7420,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="18.75"/>
@@ -7502,31 +7439,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="16" t="s">
         <v>212</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7534,28 +7471,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7563,28 +7500,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7592,28 +7529,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7621,28 +7558,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7650,28 +7587,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7679,28 +7616,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="G7" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7708,28 +7645,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7737,28 +7674,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7766,28 +7703,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7795,28 +7732,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7824,28 +7761,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7853,28 +7790,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="G13" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="I13" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7882,33 +7819,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>294</v>
-      </c>
       <c r="I14" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7940,34 +7877,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7975,31 +7912,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -8007,31 +7944,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="J20" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -8039,31 +7976,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8071,31 +8008,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="J22" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -8103,31 +8040,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="H23" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>328</v>
-      </c>
       <c r="J23" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -8135,31 +8072,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="F24" s="13" t="s">
+      <c r="J24" s="14" t="s">
         <v>330</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8167,31 +8104,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="H25" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="J25" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8199,31 +8136,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="J26" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8231,31 +8168,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="G27" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="J27" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8263,31 +8200,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="J28" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8295,31 +8232,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="G29" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="J29" s="6" t="s">
         <v>366</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8327,31 +8264,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="G30" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="J30" s="6" t="s">
         <v>375</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8359,63 +8296,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="G31" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="I31" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="J31" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="F32" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="G32" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the new update
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,19 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27015" windowHeight="12480" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Alternative" sheetId="3" r:id="rId2"/>
     <sheet name="OLD Weapon Calculations" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="394">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -1006,6 +1019,18 @@
   </si>
   <si>
     <t>The double of another column
+should be 120% of that column
+E.g. 400XP HP = 1.2 * 2 * 200XP HP</t>
+  </si>
+  <si>
+    <t>Epic HP multpliers are:
+x2: 0.8
+x3: 0.75
+x4: 0.7
+x5: 0.65</t>
+  </si>
+  <si>
+    <t>The double of another column
 should be ~85% of its half
 E.g. 400XP dmg = 0.85 * 2 * 200XP dmg</t>
   </si>
@@ -1658,14 +1683,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1823,6 +1848,13 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2490,137 +2522,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2900,72 +2932,87 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2981,7 +3028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
@@ -3322,7 +3369,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -3427,7 +3474,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="101" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3443,10 +3490,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="97" t="s">
+      <c r="L8" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="97"/>
+      <c r="M8" s="101"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3479,13 +3526,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="121" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3497,7 +3544,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3508,13 +3555,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="121" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3526,7 +3573,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="117" t="s">
+      <c r="G11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3537,13 +3584,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="123" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3555,7 +3602,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="119" t="s">
+      <c r="G12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3820,7 +3867,7 @@
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="99"/>
+      <c r="J26" s="103"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
@@ -3839,9 +3886,9 @@
       <c r="G27" s="80"/>
       <c r="H27" s="80"/>
       <c r="I27" s="80"/>
-      <c r="J27" s="100"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3859,7 +3906,7 @@
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="99"/>
+      <c r="J28" s="103"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -3901,7 +3948,7 @@
         <v>63</v>
       </c>
       <c r="H30" s="84"/>
-      <c r="J30" s="102"/>
+      <c r="J30" s="106"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -3954,7 +4001,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="103"/>
+      <c r="J32" s="107"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -4024,7 +4071,7 @@
       <c r="G35" s="90"/>
       <c r="H35" s="90"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="99"/>
+      <c r="J35" s="103"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
@@ -4101,17 +4148,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="93" t="s">
+      <c r="F40" s="119" t="s">
         <v>87</v>
       </c>
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="120" t="s">
+      <c r="I40" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="108"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4130,10 +4177,10 @@
       <c r="F41" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="94">
+      <c r="G41" s="95">
         <v>10</v>
       </c>
-      <c r="I41" s="121" t="s">
+      <c r="I41" s="126" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4156,7 +4203,7 @@
       <c r="F42" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="94">
+      <c r="G42" s="95">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -4180,7 +4227,7 @@
       <c r="F43" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="94">
+      <c r="G43" s="95">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -4206,7 +4253,7 @@
       <c r="F44" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="94">
+      <c r="G44" s="95">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -4232,7 +4279,7 @@
       <c r="F45" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="94">
+      <c r="G45" s="95">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -4258,7 +4305,7 @@
       <c r="F46" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="94">
+      <c r="G46" s="95">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -4287,7 +4334,7 @@
       <c r="F47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="94">
+      <c r="G47" s="95">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -4313,7 +4360,7 @@
       <c r="F48" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="94">
+      <c r="G48" s="95">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -4336,7 +4383,7 @@
       <c r="F49" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="94">
+      <c r="G49" s="95">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -4362,7 +4409,7 @@
       <c r="F50" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="94">
+      <c r="G50" s="95">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -4388,7 +4435,7 @@
       <c r="F51" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="94">
+      <c r="G51" s="95">
         <v>11</v>
       </c>
       <c r="I51" s="40"/>
@@ -4606,11 +4653,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="115" t="s">
+      <c r="C62" s="120" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="115" t="s">
+      <c r="F62" s="120" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4629,7 +4676,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="107" t="s">
+      <c r="E64" s="111" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4676,7 +4723,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="115" t="s">
+      <c r="C70" s="120" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4693,10 +4740,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="108"/>
-      <c r="B72" s="109"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="110"/>
+      <c r="A72" s="112"/>
+      <c r="B72" s="113"/>
+      <c r="C72" s="114"/>
+      <c r="D72" s="114"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4801,7 +4848,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="122" t="s">
+      <c r="D77" s="127" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4819,7 +4866,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="108"/>
+      <c r="A78" s="112"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4829,16 +4876,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="114"/>
+      <c r="E78" s="118"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="114"/>
-      <c r="H78" s="114"/>
-      <c r="I78" s="114"/>
-      <c r="J78" s="114"/>
-      <c r="K78" s="114"/>
-      <c r="L78" s="114"/>
+      <c r="G78" s="118"/>
+      <c r="H78" s="118"/>
+      <c r="I78" s="118"/>
+      <c r="J78" s="118"/>
+      <c r="K78" s="118"/>
+      <c r="L78" s="118"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4895,7 +4942,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="122" t="s">
+      <c r="D81" s="127" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5168,8 +5215,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="113"/>
-      <c r="F103" s="113"/>
+      <c r="E103" s="117"/>
+      <c r="F103" s="117"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5253,8 +5300,8 @@
   <sheetPr/>
   <dimension ref="A2:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5359,7 +5406,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="101" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5375,10 +5422,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="97" t="s">
+      <c r="L8" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="97"/>
+      <c r="M8" s="101"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5411,13 +5458,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="121" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5429,7 +5476,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5440,13 +5487,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="121" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5458,7 +5505,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="117" t="s">
+      <c r="G11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5469,13 +5516,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="123" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5487,7 +5534,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="119" t="s">
+      <c r="G12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5510,14 +5557,11 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" ht="15.75" spans="2:10">
       <c r="B15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
       <c r="J15" t="s">
         <v>161</v>
       </c>
@@ -5541,9 +5585,7 @@
       <c r="F16" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G16"/>
       <c r="H16" s="40"/>
-      <c r="I16"/>
       <c r="K16">
         <v>5</v>
       </c>
@@ -5567,9 +5609,7 @@
       <c r="F17" s="55">
         <v>0</v>
       </c>
-      <c r="G17"/>
       <c r="H17" s="40"/>
-      <c r="I17"/>
       <c r="K17">
         <v>6</v>
       </c>
@@ -5593,7 +5633,6 @@
       <c r="F18" s="55">
         <v>-1</v>
       </c>
-      <c r="G18"/>
       <c r="H18" s="57"/>
       <c r="K18" s="70">
         <v>4</v>
@@ -5618,7 +5657,6 @@
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="G19"/>
       <c r="H19" s="58"/>
       <c r="K19" s="70">
         <v>5</v>
@@ -5643,7 +5681,6 @@
       <c r="F20" s="63">
         <v>-1</v>
       </c>
-      <c r="G20"/>
       <c r="H20" s="57"/>
       <c r="K20" s="70">
         <v>6</v>
@@ -5668,7 +5705,6 @@
       <c r="F21" s="55">
         <v>-2</v>
       </c>
-      <c r="G21"/>
       <c r="H21" s="58"/>
       <c r="K21" s="70">
         <v>4</v>
@@ -5693,7 +5729,6 @@
       <c r="F22" s="43">
         <v>-3</v>
       </c>
-      <c r="G22"/>
       <c r="H22" s="58"/>
       <c r="K22" s="70">
         <v>5</v>
@@ -5760,7 +5795,7 @@
       <c r="H25" s="40"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
-      <c r="K25" s="98">
+      <c r="K25" s="102">
         <f>46/9</f>
         <v>5.11111111111111</v>
       </c>
@@ -5777,7 +5812,7 @@
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="99"/>
+      <c r="J26" s="103"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
@@ -5796,9 +5831,9 @@
       <c r="G27" s="80"/>
       <c r="H27" s="80"/>
       <c r="I27" s="80"/>
-      <c r="J27" s="100"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -5816,7 +5851,7 @@
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="99"/>
+      <c r="J28" s="103"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -5858,7 +5893,7 @@
         <v>63</v>
       </c>
       <c r="H30" s="84"/>
-      <c r="J30" s="102"/>
+      <c r="J30" s="106"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -5911,7 +5946,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="103"/>
+      <c r="J32" s="107"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -5981,7 +6016,7 @@
       <c r="G35" s="90"/>
       <c r="H35" s="90"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="99"/>
+      <c r="J35" s="103"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
@@ -6064,11 +6099,11 @@
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="120" t="s">
+      <c r="I40" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="108"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -6085,13 +6120,13 @@
       <c r="E41" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="94">
+      <c r="G41" s="95">
         <v>10</v>
       </c>
-      <c r="I41" s="121" t="s">
+      <c r="I41" s="126" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -6112,10 +6147,10 @@
       <c r="E42" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="94">
+      <c r="G42" s="95">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -6137,10 +6172,10 @@
       <c r="E43" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="40" t="s">
+      <c r="F43" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="94">
+      <c r="G43" s="95">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -6164,10 +6199,10 @@
       <c r="E44" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="94" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="94">
+      <c r="G44" s="95">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -6191,10 +6226,10 @@
       <c r="E45" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="40" t="s">
+      <c r="F45" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="94">
+      <c r="G45" s="95">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -6218,10 +6253,10 @@
       <c r="E46" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F46" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="94">
+      <c r="G46" s="95">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -6248,10 +6283,10 @@
       <c r="E47" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="F47" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="94">
+      <c r="G47" s="95">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -6272,10 +6307,10 @@
       <c r="E48" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F48" s="40" t="s">
+      <c r="F48" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="94">
+      <c r="G48" s="95">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -6299,10 +6334,10 @@
       <c r="E49" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="F49" s="40" t="s">
+      <c r="F49" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="94">
+      <c r="G49" s="95">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -6326,10 +6361,10 @@
       <c r="E50" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="40" t="s">
+      <c r="F50" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="94">
+      <c r="G50" s="95">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -6350,10 +6385,10 @@
       <c r="E51" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="94">
+      <c r="G51" s="95">
         <v>11</v>
       </c>
       <c r="H51">
@@ -6365,10 +6400,10 @@
       <c r="K51" s="58"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="95" t="s">
+      <c r="A52" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="96">
+      <c r="B52" s="97">
         <v>300</v>
       </c>
       <c r="C52" s="40">
@@ -6381,7 +6416,7 @@
       <c r="E52" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="94" t="s">
         <v>119</v>
       </c>
       <c r="G52" s="41">
@@ -6393,23 +6428,23 @@
       <c r="M52" s="58"/>
     </row>
     <row r="53" ht="15.75" spans="1:13">
-      <c r="A53" s="95" t="s">
+      <c r="A53" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="96">
+      <c r="B53" s="97">
         <v>325</v>
       </c>
-      <c r="C53" s="96">
+      <c r="C53" s="97">
         <v>120</v>
       </c>
-      <c r="D53" s="96">
+      <c r="D53" s="97">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E53" s="96" t="s">
+      <c r="E53" s="97" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="96" t="s">
+      <c r="F53" s="98" t="s">
         <v>122</v>
       </c>
       <c r="G53" s="41">
@@ -6435,7 +6470,7 @@
       <c r="E54" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="94" t="s">
         <v>125</v>
       </c>
       <c r="G54" s="41">
@@ -6461,7 +6496,7 @@
       <c r="E55" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="F55" s="45" t="s">
+      <c r="F55" s="99" t="s">
         <v>127</v>
       </c>
       <c r="G55" s="46">
@@ -6488,7 +6523,7 @@
       <c r="E56" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="F56" s="40" t="s">
+      <c r="F56" s="94" t="s">
         <v>129</v>
       </c>
       <c r="G56" s="41">
@@ -6515,7 +6550,7 @@
       <c r="E57" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F57" s="40" t="s">
+      <c r="F57" s="94" t="s">
         <v>131</v>
       </c>
       <c r="G57" s="41">
@@ -6542,7 +6577,7 @@
       <c r="E58" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="94" t="s">
         <v>133</v>
       </c>
       <c r="G58" s="41">
@@ -6569,7 +6604,7 @@
       <c r="E59" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="F59" s="40" t="s">
+      <c r="F59" s="94" t="s">
         <v>135</v>
       </c>
       <c r="G59" s="41">
@@ -6586,17 +6621,17 @@
       <c r="B60" s="52">
         <v>500</v>
       </c>
-      <c r="C60" s="96">
+      <c r="C60" s="97">
         <v>218</v>
       </c>
-      <c r="D60" s="96">
+      <c r="D60" s="97">
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-      <c r="E60" s="96" t="s">
+      <c r="E60" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="F60" s="96" t="s">
+      <c r="F60" s="98" t="s">
         <v>137</v>
       </c>
       <c r="G60" s="41">
@@ -6613,14 +6648,14 @@
       <c r="B61" s="52">
         <v>600</v>
       </c>
-      <c r="C61" s="96"/>
-      <c r="D61" s="96">
+      <c r="C61" s="97"/>
+      <c r="D61" s="97">
         <v>350</v>
       </c>
-      <c r="E61" s="96">
+      <c r="E61" s="97">
         <v>14.5</v>
       </c>
-      <c r="F61" s="96"/>
+      <c r="F61" s="100"/>
       <c r="G61" s="41">
         <v>13</v>
       </c>
@@ -6635,21 +6670,21 @@
       <c r="B62" s="52">
         <v>750</v>
       </c>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96">
+      <c r="C62" s="97"/>
+      <c r="D62" s="97">
         <v>441</v>
       </c>
-      <c r="E62" s="96">
+      <c r="E62" s="97">
         <v>17.25</v>
       </c>
-      <c r="F62" s="96" t="s">
+      <c r="F62" s="98" t="s">
         <v>175</v>
       </c>
       <c r="G62" s="41">
         <v>13</v>
       </c>
       <c r="H62" s="40"/>
-      <c r="I62" s="105">
+      <c r="I62" s="109">
         <f>SUM(I55:I61)</f>
         <v>1825</v>
       </c>
@@ -6665,7 +6700,7 @@
       <c r="E63" s="45">
         <v>21.5</v>
       </c>
-      <c r="F63" s="45" t="s">
+      <c r="F63" s="99" t="s">
         <v>137</v>
       </c>
       <c r="G63" s="46">
@@ -6687,15 +6722,19 @@
       </c>
       <c r="I65" s="40"/>
     </row>
-    <row r="66" ht="75.75" spans="3:9">
-      <c r="C66" s="106" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="106" t="s">
-        <v>142</v>
-      </c>
-      <c r="E66" s="106" t="s">
+    <row r="66" ht="90.75" spans="1:9">
+      <c r="A66">
+        <f>147*2*0.8</f>
+        <v>235.2</v>
+      </c>
+      <c r="C66" s="110" t="s">
         <v>176</v>
+      </c>
+      <c r="D66" s="110" t="s">
+        <v>177</v>
+      </c>
+      <c r="E66" s="110" t="s">
+        <v>178</v>
       </c>
       <c r="G66" s="40">
         <f>350*4*0.8</f>
@@ -6712,7 +6751,7 @@
       <c r="I67" s="40"/>
     </row>
     <row r="68" spans="5:9">
-      <c r="E68" s="107"/>
+      <c r="E68" s="111"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
@@ -6741,18 +6780,18 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="108"/>
-      <c r="B72" s="109"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="110"/>
+      <c r="A72" s="112"/>
+      <c r="B72" s="113"/>
+      <c r="C72" s="114"/>
+      <c r="D72" s="114"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58"/>
       <c r="G72" s="58"/>
       <c r="H72" s="58" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J72" s="58"/>
       <c r="K72" s="58"/>
@@ -6763,11 +6802,11 @@
       <c r="A73" s="40"/>
       <c r="B73" s="40"/>
       <c r="C73" s="40" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D73" s="40"/>
       <c r="E73" s="40" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F73" s="40"/>
       <c r="G73" s="40"/>
@@ -6775,7 +6814,7 @@
         <v>145</v>
       </c>
       <c r="I73" s="40" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
@@ -6791,20 +6830,20 @@
         <v>145</v>
       </c>
       <c r="D74" s="50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F74" s="40"/>
-      <c r="G74" s="111" t="s">
-        <v>184</v>
-      </c>
-      <c r="H74" s="111" t="s">
-        <v>185</v>
-      </c>
-      <c r="I74" s="111" t="s">
+      <c r="G74" s="115" t="s">
         <v>186</v>
+      </c>
+      <c r="H74" s="115" t="s">
+        <v>187</v>
+      </c>
+      <c r="I74" s="115" t="s">
+        <v>188</v>
       </c>
       <c r="J74" s="40"/>
       <c r="K74" s="40"/>
@@ -6827,13 +6866,13 @@
       </c>
       <c r="F75" s="40"/>
       <c r="G75" s="40" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I75" s="40" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J75" s="40"/>
       <c r="K75" s="40"/>
@@ -6858,13 +6897,13 @@
       </c>
       <c r="F76" s="40"/>
       <c r="G76" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H76" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="I76" s="40" t="s">
         <v>190</v>
-      </c>
-      <c r="H76" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="I76" s="40" t="s">
-        <v>188</v>
       </c>
       <c r="J76" s="40"/>
       <c r="K76" s="40"/>
@@ -6889,13 +6928,13 @@
       </c>
       <c r="F77" s="40"/>
       <c r="G77" s="40" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I77" s="40" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J77" s="40"/>
       <c r="K77" s="40"/>
@@ -6903,7 +6942,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="108"/>
+      <c r="A78" s="112"/>
       <c r="B78" s="39">
         <v>4</v>
       </c>
@@ -6918,18 +6957,18 @@
         <v>10</v>
       </c>
       <c r="F78" s="40"/>
-      <c r="G78" s="112" t="s">
-        <v>193</v>
-      </c>
-      <c r="H78" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="I78" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="J78" s="114"/>
-      <c r="K78" s="114"/>
-      <c r="L78" s="114"/>
+      <c r="G78" s="116" t="s">
+        <v>195</v>
+      </c>
+      <c r="H78" s="116" t="s">
+        <v>188</v>
+      </c>
+      <c r="I78" s="116" t="s">
+        <v>188</v>
+      </c>
+      <c r="J78" s="118"/>
+      <c r="K78" s="118"/>
+      <c r="L78" s="118"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -6950,13 +6989,13 @@
       </c>
       <c r="F79" s="40"/>
       <c r="G79" s="40" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I79" s="40" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J79" s="40"/>
       <c r="K79" s="40"/>
@@ -6980,13 +7019,13 @@
       </c>
       <c r="F80" s="40"/>
       <c r="G80" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="H80" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="I80" s="40" t="s">
         <v>197</v>
-      </c>
-      <c r="H80" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="I80" s="40" t="s">
-        <v>195</v>
       </c>
       <c r="J80" s="40"/>
       <c r="K80" s="40"/>
@@ -7011,13 +7050,13 @@
       </c>
       <c r="F81" s="40"/>
       <c r="G81" s="40" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="I81" s="40" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J81" s="40"/>
       <c r="K81" s="40"/>
@@ -7042,13 +7081,13 @@
       </c>
       <c r="F82" s="40"/>
       <c r="G82" s="40" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I82" s="40" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J82" s="40"/>
       <c r="K82" s="40"/>
@@ -7121,7 +7160,7 @@
       <c r="E86" s="40"/>
       <c r="F86" s="40"/>
       <c r="G86" s="40"/>
-      <c r="H86" s="107"/>
+      <c r="H86" s="111"/>
       <c r="I86" s="40"/>
       <c r="J86" s="40"/>
       <c r="K86" s="40"/>
@@ -7155,16 +7194,16 @@
         <v>144</v>
       </c>
       <c r="C89" s="40" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E89" s="40" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F89" s="40" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
@@ -7259,7 +7298,7 @@
       <c r="C95" s="40"/>
       <c r="D95" s="40"/>
       <c r="E95" s="40"/>
-      <c r="F95" s="105"/>
+      <c r="F95" s="109"/>
       <c r="G95" s="40"/>
       <c r="H95" s="40"/>
       <c r="I95" s="40"/>
@@ -7290,7 +7329,7 @@
       <c r="C98" s="40"/>
       <c r="D98" s="40"/>
       <c r="E98" s="40"/>
-      <c r="F98" s="105"/>
+      <c r="F98" s="109"/>
       <c r="G98" s="40"/>
       <c r="H98" s="40"/>
       <c r="I98" s="40"/>
@@ -7335,7 +7374,7 @@
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
       <c r="E103" s="40"/>
-      <c r="F103" s="113"/>
+      <c r="F103" s="117"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -7420,7 +7459,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="18.75"/>
@@ -7439,31 +7478,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7471,28 +7510,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7500,28 +7539,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7529,28 +7568,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7558,28 +7597,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7587,28 +7626,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7616,28 +7655,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>236</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7645,28 +7684,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7674,28 +7713,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7703,28 +7742,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7732,28 +7771,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7761,28 +7800,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7790,28 +7829,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7819,33 +7858,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7877,34 +7916,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7912,31 +7951,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7944,31 +7983,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7976,31 +8015,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8008,31 +8047,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -8040,31 +8079,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -8072,31 +8111,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G24" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="H24" s="14" t="s">
-        <v>326</v>
-      </c>
       <c r="I24" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8104,31 +8143,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>331</v>
-      </c>
       <c r="I25" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8136,31 +8175,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8168,31 +8207,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8200,31 +8239,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8232,31 +8271,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8264,31 +8303,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8296,63 +8335,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working and mostly finished the Level Up update.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="399">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -1012,10 +1012,28 @@
     </r>
   </si>
   <si>
+    <t>Slow (as extra)</t>
+  </si>
+  <si>
+    <t>Fumbling (as extra)</t>
+  </si>
+  <si>
+    <t>Rooted</t>
+  </si>
+  <si>
+    <t>Charm</t>
+  </si>
+  <si>
+    <t>Daze (+extra)</t>
+  </si>
+  <si>
+    <t>Blind</t>
+  </si>
+  <si>
+    <t>Feared</t>
+  </si>
+  <si>
     <t>New Health</t>
-  </si>
-  <si>
-    <t>16.5  (1d8 + 13)</t>
   </si>
   <si>
     <t>The double of another column
@@ -1044,16 +1062,13 @@
     <t>18.5 + Might + Other</t>
   </si>
   <si>
-    <t>6 + Level</t>
-  </si>
-  <si>
     <t>HP Regen</t>
   </si>
   <si>
     <t>Reserve HP</t>
   </si>
   <si>
-    <t>Health Regen (6 + Level)</t>
+    <t>Health Regen (6 - 2 + 2*Level)</t>
   </si>
   <si>
     <t>Bertle</t>
@@ -1690,7 +1705,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1840,13 +1855,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="4"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1854,7 +1862,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.25"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2522,137 +2530,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2884,6 +2892,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2896,10 +2907,13 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2908,16 +2922,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2930,12 +2947,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2947,75 +2958,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3028,7 +3054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
@@ -3474,7 +3500,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="101" t="s">
+      <c r="L7" s="99" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3490,10 +3516,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="101" t="s">
+      <c r="L8" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="101"/>
+      <c r="M8" s="99"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3526,13 +3552,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="127" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3544,7 +3570,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="122" t="s">
+      <c r="G10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3555,13 +3581,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="127" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3573,7 +3599,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="122" t="s">
+      <c r="G11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3584,13 +3610,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="129" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3602,7 +3628,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="124" t="s">
+      <c r="G12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3777,7 +3803,7 @@
       <c r="B22" s="66">
         <v>1</v>
       </c>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="95" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="66" t="s">
@@ -3802,7 +3828,7 @@
       <c r="B23" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="90">
+      <c r="C23" s="93">
         <v>6</v>
       </c>
       <c r="D23" s="68">
@@ -3825,7 +3851,7 @@
       <c r="B24" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="92">
+      <c r="C24" s="95">
         <v>8</v>
       </c>
       <c r="D24" s="66">
@@ -3858,37 +3884,37 @@
     <row r="26" ht="15.75" spans="1:11">
       <c r="A26" s="74"/>
       <c r="B26" s="51"/>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="76"/>
+      <c r="D26" s="114"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="103"/>
+      <c r="J26" s="84"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C27" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="105"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="124"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3897,16 +3923,16 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="82"/>
+      <c r="D28" s="118"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="103"/>
+      <c r="J28" s="84"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -3916,10 +3942,10 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="84"/>
+      <c r="D29" s="89"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -3935,20 +3961,20 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="84" t="s">
+      <c r="D30" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="84" t="s">
+      <c r="E30" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="85" t="s">
+      <c r="F30" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="84"/>
-      <c r="J30" s="106"/>
+      <c r="H30" s="89"/>
+      <c r="J30" s="125"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -4001,7 +4027,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="107"/>
+      <c r="J32" s="126"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -4036,20 +4062,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="87">
+      <c r="B34" s="120">
         <v>1</v>
       </c>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="87"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="121"/>
+      <c r="H34" s="121"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="120"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -4059,38 +4085,38 @@
       <c r="A35" s="67">
         <v>1</v>
       </c>
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="92" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="103"/>
+      <c r="J35" s="84"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
       <c r="A36" s="65">
         <v>1</v>
       </c>
-      <c r="B36" s="91" t="s">
+      <c r="B36" s="94" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="92" t="s">
+      <c r="D36" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="95"/>
       <c r="I36" s="45"/>
       <c r="J36" s="46"/>
       <c r="K36" s="58"/>
@@ -4126,7 +4152,7 @@
       <c r="C39" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="89"/>
+      <c r="D39" s="92"/>
       <c r="F39" s="58"/>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
@@ -4148,17 +4174,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="119" t="s">
+      <c r="F40" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="89" t="s">
+      <c r="G40" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="125" t="s">
+      <c r="I40" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="108"/>
-      <c r="K40" s="108"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="102"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4177,10 +4203,10 @@
       <c r="F41" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="95">
+      <c r="G41" s="96">
         <v>10</v>
       </c>
-      <c r="I41" s="126" t="s">
+      <c r="I41" s="132" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4203,7 +4229,7 @@
       <c r="F42" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="95">
+      <c r="G42" s="96">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -4227,7 +4253,7 @@
       <c r="F43" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="95">
+      <c r="G43" s="96">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -4253,7 +4279,7 @@
       <c r="F44" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="95">
+      <c r="G44" s="96">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -4279,7 +4305,7 @@
       <c r="F45" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="95">
+      <c r="G45" s="96">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -4305,7 +4331,7 @@
       <c r="F46" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="95">
+      <c r="G46" s="96">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -4334,7 +4360,7 @@
       <c r="F47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="95">
+      <c r="G47" s="96">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -4360,7 +4386,7 @@
       <c r="F48" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="95">
+      <c r="G48" s="96">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -4383,7 +4409,7 @@
       <c r="F49" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="95">
+      <c r="G49" s="96">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -4409,7 +4435,7 @@
       <c r="F50" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="95">
+      <c r="G50" s="96">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -4435,7 +4461,7 @@
       <c r="F51" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="95">
+      <c r="G51" s="96">
         <v>11</v>
       </c>
       <c r="I51" s="40"/>
@@ -4653,11 +4679,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="120" t="s">
+      <c r="C62" s="123" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="120" t="s">
+      <c r="F62" s="123" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4676,7 +4702,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="111" t="s">
+      <c r="E64" s="105" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4723,7 +4749,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="120" t="s">
+      <c r="C70" s="123" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4740,10 +4766,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="112"/>
-      <c r="B72" s="113"/>
-      <c r="C72" s="114"/>
-      <c r="D72" s="114"/>
+      <c r="A72" s="106"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4848,7 +4874,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="127" t="s">
+      <c r="D77" s="133" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4866,7 +4892,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="112"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4876,16 +4902,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="118"/>
+      <c r="E78" s="112"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="118"/>
-      <c r="H78" s="118"/>
-      <c r="I78" s="118"/>
-      <c r="J78" s="118"/>
-      <c r="K78" s="118"/>
-      <c r="L78" s="118"/>
+      <c r="G78" s="112"/>
+      <c r="H78" s="112"/>
+      <c r="I78" s="112"/>
+      <c r="J78" s="112"/>
+      <c r="K78" s="112"/>
+      <c r="L78" s="112"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4942,7 +4968,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="127" t="s">
+      <c r="D81" s="133" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5215,8 +5241,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="117"/>
-      <c r="F103" s="117"/>
+      <c r="E103" s="111"/>
+      <c r="F103" s="111"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5298,10 +5324,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:N112"/>
+  <dimension ref="A2:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5406,7 +5432,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="101" t="s">
+      <c r="L7" s="99" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5422,10 +5448,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="101" t="s">
+      <c r="L8" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="101"/>
+      <c r="M8" s="99"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5458,13 +5484,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="127" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5476,7 +5502,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="122" t="s">
+      <c r="G10" s="128" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5487,13 +5513,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="127" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5505,7 +5531,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="122" t="s">
+      <c r="G11" s="128" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5516,13 +5542,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="129" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5534,7 +5560,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="124" t="s">
+      <c r="G12" s="130" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5633,7 +5659,10 @@
       <c r="F18" s="55">
         <v>-1</v>
       </c>
-      <c r="H18" s="57"/>
+      <c r="H18" s="57">
+        <f>6.5+9</f>
+        <v>15.5</v>
+      </c>
       <c r="K18" s="70">
         <v>4</v>
       </c>
@@ -5795,45 +5824,45 @@
       <c r="H25" s="40"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
-      <c r="K25" s="102">
+      <c r="K25" s="100">
         <f>46/9</f>
         <v>5.11111111111111</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="1:11">
+    <row r="26" spans="1:11">
       <c r="A26" s="74"/>
       <c r="B26" s="51"/>
       <c r="C26" s="75" t="s">
         <v>56</v>
       </c>
       <c r="D26" s="76"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="103"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C27" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="105"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -5842,16 +5871,18 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="82"/>
+      <c r="C28" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>175</v>
+      </c>
       <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="103"/>
+      <c r="F28" s="84"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -5861,16 +5892,18 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="83" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="84"/>
+      <c r="C29" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="D29" s="86" t="s">
+        <v>177</v>
+      </c>
       <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
+      <c r="F29" s="87"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
       <c r="K29" s="40"/>
     </row>
     <row r="30" spans="1:11">
@@ -5880,167 +5913,114 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="84"/>
-      <c r="J30" s="106"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="90"/>
       <c r="K30" s="40"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:6">
       <c r="A31" s="39">
         <v>0</v>
       </c>
       <c r="B31" s="40">
         <v>1</v>
       </c>
-      <c r="C31" s="39" t="s">
-        <v>59</v>
+      <c r="C31" s="91" t="s">
+        <v>178</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="40"/>
-      <c r="J31" s="41"/>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="F31" s="87" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="39">
         <v>0.5</v>
       </c>
       <c r="B32" s="40">
         <v>1</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>60</v>
+      <c r="C32" s="83" t="s">
+        <v>62</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="J32" s="107"/>
-    </row>
-    <row r="33" ht="15.75" spans="1:10">
+        <v>67</v>
+      </c>
+      <c r="E32" s="40"/>
+      <c r="F32" s="87"/>
+    </row>
+    <row r="33" ht="15.75" spans="1:6">
       <c r="A33" s="44">
         <v>1</v>
       </c>
       <c r="B33" s="45">
         <v>1</v>
       </c>
-      <c r="C33" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="86" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="87">
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
+    </row>
+    <row r="34" ht="15.75" spans="1:11">
+      <c r="A34" s="67">
         <v>1</v>
       </c>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="87"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-    </row>
-    <row r="35" ht="15.75" spans="1:11">
-      <c r="A35" s="67">
+      <c r="B34" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="92"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34" s="58"/>
+    </row>
+    <row r="35" ht="16.5" spans="1:11">
+      <c r="A35" s="65">
         <v>1</v>
       </c>
-      <c r="B35" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="103"/>
+      <c r="B35" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="95" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="95"/>
+      <c r="F35" s="94"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
       <c r="K35" s="58"/>
     </row>
-    <row r="36" ht="16.5" spans="1:11">
-      <c r="A36" s="65">
-        <v>1</v>
-      </c>
-      <c r="B36" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="92" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="46"/>
+    <row r="36" ht="15.75" spans="1:11">
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
       <c r="K36" s="58"/>
     </row>
-    <row r="37" ht="15.75" spans="1:11">
+    <row r="37" ht="16.5" spans="1:11">
       <c r="A37" s="58"/>
       <c r="B37" s="58"/>
       <c r="C37" s="58"/>
@@ -6055,102 +6035,98 @@
     </row>
     <row r="38" ht="16.5" spans="1:11">
       <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
+      <c r="C38" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="92"/>
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
-      <c r="I38" s="40"/>
+      <c r="I38" s="58"/>
       <c r="J38" s="40"/>
       <c r="K38" s="58"/>
     </row>
-    <row r="39" ht="16.5" spans="1:11">
-      <c r="A39" s="58"/>
-      <c r="C39" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="89"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="58"/>
-    </row>
-    <row r="40" ht="30" spans="1:11">
+    <row r="39" ht="15.75" spans="1:11">
+      <c r="A39" s="72"/>
+      <c r="B39" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="I39" s="102"/>
+      <c r="J39" s="102"/>
+      <c r="K39" s="102"/>
+    </row>
+    <row r="40" ht="15.75" spans="1:11">
       <c r="A40" s="72"/>
-      <c r="B40" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="F40" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="89" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="125" t="s">
-        <v>89</v>
-      </c>
-      <c r="J40" s="108"/>
-      <c r="K40" s="108"/>
+      <c r="B40" s="39">
+        <v>25</v>
+      </c>
+      <c r="C40" s="40">
+        <v>7</v>
+      </c>
+      <c r="D40" s="40">
+        <f>FLOOR(C40*1.32,1)</f>
+        <v>9</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="96">
+        <v>10</v>
+      </c>
+      <c r="I40" s="58"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="58"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
       <c r="B41" s="39">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C41" s="40">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D41" s="40">
         <f>FLOOR(C41*1.32,1)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E41" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="94" t="s">
-        <v>91</v>
-      </c>
-      <c r="G41" s="95">
+        <v>93</v>
+      </c>
+      <c r="F41" s="96">
         <v>10</v>
       </c>
-      <c r="I41" s="126" t="s">
-        <v>92</v>
-      </c>
+      <c r="I41" s="58"/>
       <c r="J41" s="40"/>
       <c r="K41" s="58"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
       <c r="A42" s="72"/>
       <c r="B42" s="39">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C42" s="40">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D42" s="40">
-        <f>FLOOR(C42*1.32,1)</f>
-        <v>18</v>
+        <f t="shared" ref="D42:D60" si="0">FLOOR(C42*1.32,1)</f>
+        <v>27</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="94" t="s">
-        <v>94</v>
-      </c>
-      <c r="G42" s="95">
+        <v>95</v>
+      </c>
+      <c r="F42" s="96">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -6158,554 +6134,456 @@
       <c r="K42" s="58"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
-      <c r="A43" s="72"/>
-      <c r="B43" s="39">
-        <v>75</v>
+      <c r="A43" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="52">
+        <v>100</v>
       </c>
       <c r="C43" s="40">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D43" s="40">
-        <f t="shared" ref="D43:D61" si="0">FLOOR(C43*1.32,1)</f>
-        <v>27</v>
-      </c>
-      <c r="E43" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="94" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" s="95">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E43" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="96">
         <v>10</v>
       </c>
-      <c r="I43" s="58"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43" s="40"/>
       <c r="J43" s="40"/>
       <c r="K43" s="58"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
       <c r="A44" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="52">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="B44" s="39">
+        <v>125</v>
       </c>
       <c r="C44" s="40">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D44" s="40">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" s="94" t="s">
-        <v>98</v>
-      </c>
-      <c r="G44" s="95">
+        <v>100</v>
+      </c>
+      <c r="F44" s="96">
         <v>10</v>
       </c>
+      <c r="G44"/>
+      <c r="H44"/>
       <c r="I44" s="40"/>
       <c r="J44" s="40"/>
       <c r="K44" s="58"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
       <c r="A45" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B45" s="39">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C45" s="40">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D45" s="40">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="95">
+        <v>103</v>
+      </c>
+      <c r="F45" s="96">
         <v>10</v>
       </c>
+      <c r="G45"/>
+      <c r="H45"/>
       <c r="I45" s="40"/>
       <c r="J45" s="40"/>
       <c r="K45" s="58"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
       <c r="A46" s="72" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B46" s="39">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="C46" s="40">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D46" s="40">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" s="94" t="s">
-        <v>104</v>
-      </c>
-      <c r="G46" s="95">
+        <v>107</v>
+      </c>
+      <c r="F46" s="96">
         <v>10</v>
       </c>
-      <c r="H46" t="s">
-        <v>105</v>
-      </c>
+      <c r="G46"/>
+      <c r="H46"/>
       <c r="I46" s="40"/>
       <c r="J46" s="40"/>
       <c r="K46" s="58"/>
     </row>
-    <row r="47" ht="15.75" spans="1:11">
-      <c r="A47" s="72" t="s">
-        <v>106</v>
-      </c>
+    <row r="47" ht="15.75" spans="2:11">
       <c r="B47" s="39">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="C47" s="40">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D47" s="40">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="E47" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="G47" s="95">
-        <v>10</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="96">
+        <v>11</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
       <c r="I47" s="40"/>
       <c r="J47" s="40"/>
       <c r="K47" s="58"/>
     </row>
-    <row r="48" ht="15.75" spans="2:11">
-      <c r="B48" s="39">
-        <v>200</v>
+    <row r="48" ht="15.75" spans="1:11">
+      <c r="A48" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="52">
+        <v>225</v>
       </c>
       <c r="C48" s="40">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D48" s="40">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="94" t="s">
-        <v>110</v>
-      </c>
-      <c r="G48" s="95">
+        <v>111</v>
+      </c>
+      <c r="F48" s="96">
         <v>11</v>
       </c>
+      <c r="G48"/>
+      <c r="H48"/>
       <c r="I48" s="40"/>
       <c r="J48" s="40"/>
       <c r="K48" s="58"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
       <c r="A49" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" s="52">
-        <v>225</v>
+        <v>113</v>
+      </c>
+      <c r="B49" s="39">
+        <v>250</v>
       </c>
       <c r="C49" s="40">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D49" s="40">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="E49" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="F49" s="94" t="s">
-        <v>112</v>
-      </c>
-      <c r="G49" s="95">
+        <v>101</v>
+      </c>
+      <c r="F49" s="96">
         <v>11</v>
       </c>
+      <c r="G49"/>
+      <c r="H49"/>
       <c r="I49" s="40"/>
       <c r="J49" s="40"/>
       <c r="K49" s="58"/>
     </row>
-    <row r="50" ht="15.75" spans="1:11">
-      <c r="A50" s="72" t="s">
-        <v>113</v>
-      </c>
+    <row r="50" ht="15.75" spans="2:11">
       <c r="B50" s="39">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="C50" s="40">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D50" s="40">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="E50" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="F50" s="94" t="s">
-        <v>114</v>
-      </c>
-      <c r="G50" s="95">
+        <v>104</v>
+      </c>
+      <c r="F50" s="96">
         <v>11</v>
       </c>
+      <c r="G50"/>
+      <c r="H50"/>
       <c r="I50" s="40"/>
       <c r="J50" s="40"/>
       <c r="K50" s="58"/>
     </row>
-    <row r="51" ht="15.75" spans="2:11">
-      <c r="B51" s="39">
-        <v>275</v>
+    <row r="51" ht="15.75" spans="1:13">
+      <c r="A51" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="98">
+        <v>300</v>
       </c>
       <c r="C51" s="40">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D51" s="40">
         <f t="shared" si="0"/>
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="E51" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="G51" s="95">
-        <v>11</v>
-      </c>
-      <c r="H51">
-        <f>7*250</f>
-        <v>1750</v>
-      </c>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="58"/>
+        <v>118</v>
+      </c>
+      <c r="F51" s="41">
+        <v>12</v>
+      </c>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70"/>
+      <c r="M51" s="58"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="96" t="s">
-        <v>115</v>
-      </c>
-      <c r="B52" s="97">
-        <v>300</v>
-      </c>
-      <c r="C52" s="40">
-        <v>112</v>
-      </c>
-      <c r="D52" s="40">
-        <f t="shared" si="0"/>
-        <v>147</v>
-      </c>
-      <c r="E52" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="94" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="41">
-        <v>12</v>
-      </c>
-      <c r="I52" s="58"/>
-      <c r="J52" s="70"/>
-      <c r="K52" s="70"/>
-      <c r="M52" s="58"/>
-    </row>
-    <row r="53" ht="15.75" spans="1:13">
-      <c r="A53" s="96" t="s">
+      <c r="A52" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="97">
+      <c r="B52" s="98">
         <v>325</v>
       </c>
-      <c r="C53" s="97">
+      <c r="C52" s="98">
         <v>120</v>
       </c>
-      <c r="D53" s="97">
+      <c r="D52" s="98">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E53" s="97" t="s">
+      <c r="E52" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="98" t="s">
-        <v>122</v>
-      </c>
-      <c r="G53" s="41">
+      <c r="F52" s="41">
         <v>12</v>
       </c>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52" s="40"/>
+      <c r="M52" s="58"/>
+    </row>
+    <row r="53" ht="15.75" spans="1:13">
+      <c r="A53" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="39">
+        <v>350</v>
+      </c>
+      <c r="C53" s="40">
+        <v>130</v>
+      </c>
+      <c r="D53" s="40">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="41">
+        <v>12</v>
+      </c>
+      <c r="G53"/>
+      <c r="H53"/>
       <c r="I53" s="40"/>
       <c r="M53" s="58"/>
     </row>
-    <row r="54" ht="15.75" spans="1:13">
+    <row r="54" ht="16.5" spans="1:9">
       <c r="A54" s="72" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" s="39">
-        <v>350</v>
-      </c>
-      <c r="C54" s="40">
-        <v>130</v>
-      </c>
-      <c r="D54" s="40">
-        <f t="shared" si="0"/>
-        <v>171</v>
-      </c>
-      <c r="E54" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F54" s="94" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" s="41">
-        <v>12</v>
-      </c>
-      <c r="I54" s="40"/>
-      <c r="M54" s="58"/>
-    </row>
-    <row r="55" ht="16.5" spans="1:9">
-      <c r="A55" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="B55" s="65">
+      <c r="B54" s="65">
         <v>375</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C54" s="45">
         <v>140</v>
       </c>
-      <c r="D55" s="45">
+      <c r="D54" s="45">
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="E55" s="45" t="s">
+      <c r="E54" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="F55" s="99" t="s">
-        <v>127</v>
-      </c>
-      <c r="G55" s="46">
+      <c r="F54" s="46">
         <v>12</v>
       </c>
-      <c r="H55">
-        <v>7</v>
-      </c>
-      <c r="I55" s="40">
-        <v>300</v>
-      </c>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54" s="40"/>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="39">
+        <v>400</v>
+      </c>
+      <c r="C55" s="40">
+        <v>147</v>
+      </c>
+      <c r="D55" s="40">
+        <f t="shared" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="41">
+        <v>12</v>
+      </c>
+      <c r="I55" s="40"/>
     </row>
     <row r="56" spans="2:9">
       <c r="B56" s="39">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="C56" s="40">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="D56" s="40">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="E56" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="F56" s="94" t="s">
-        <v>129</v>
-      </c>
-      <c r="G56" s="41">
+        <v>130</v>
+      </c>
+      <c r="F56" s="41">
         <v>12</v>
       </c>
-      <c r="H56">
-        <v>6.5</v>
-      </c>
-      <c r="I56" s="40">
-        <v>275</v>
-      </c>
+      <c r="I56" s="40"/>
     </row>
     <row r="57" spans="2:9">
       <c r="B57" s="39">
-        <v>425</v>
+        <v>450</v>
       </c>
       <c r="C57" s="40">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D57" s="40">
         <f t="shared" si="0"/>
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="E57" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="F57" s="94" t="s">
-        <v>131</v>
-      </c>
-      <c r="G57" s="41">
+        <v>132</v>
+      </c>
+      <c r="F57" s="41">
         <v>12</v>
       </c>
-      <c r="H57">
-        <v>6.5</v>
-      </c>
-      <c r="I57" s="40">
-        <v>275</v>
-      </c>
+      <c r="I57" s="40"/>
     </row>
     <row r="58" spans="2:9">
       <c r="B58" s="39">
-        <v>450</v>
+        <v>475</v>
       </c>
       <c r="C58" s="40">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="D58" s="40">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="E58" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="F58" s="94" t="s">
-        <v>133</v>
-      </c>
-      <c r="G58" s="41">
+        <v>134</v>
+      </c>
+      <c r="F58" s="41">
         <v>12</v>
       </c>
-      <c r="H58">
-        <v>5.5</v>
-      </c>
-      <c r="I58" s="40">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9">
-      <c r="B59" s="39">
-        <v>475</v>
-      </c>
-      <c r="C59" s="40">
-        <v>200</v>
-      </c>
-      <c r="D59" s="40">
+      <c r="I58" s="40"/>
+    </row>
+    <row r="59" ht="15.75" spans="2:9">
+      <c r="B59" s="52">
+        <v>500</v>
+      </c>
+      <c r="C59" s="98">
+        <v>218</v>
+      </c>
+      <c r="D59" s="98">
         <f t="shared" si="0"/>
-        <v>264</v>
-      </c>
-      <c r="E59" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="F59" s="94" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="41">
+        <v>287</v>
+      </c>
+      <c r="E59" s="98" t="s">
+        <v>136</v>
+      </c>
+      <c r="F59" s="41">
         <v>12</v>
       </c>
-      <c r="H59">
-        <v>6.5</v>
-      </c>
-      <c r="I59" s="40">
-        <v>275</v>
-      </c>
+      <c r="I59" s="40"/>
     </row>
     <row r="60" ht="15.75" spans="2:9">
       <c r="B60" s="52">
-        <v>500</v>
-      </c>
-      <c r="C60" s="97">
-        <v>218</v>
-      </c>
-      <c r="D60" s="97">
-        <f t="shared" si="0"/>
-        <v>287</v>
-      </c>
-      <c r="E60" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="F60" s="98" t="s">
-        <v>137</v>
-      </c>
-      <c r="G60" s="41">
-        <v>12</v>
-      </c>
-      <c r="H60">
-        <v>5.5</v>
-      </c>
-      <c r="I60" s="40">
-        <v>250</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="C60" s="98"/>
+      <c r="D60" s="98">
+        <v>350</v>
+      </c>
+      <c r="E60" s="98">
+        <v>14.5</v>
+      </c>
+      <c r="F60" s="41">
+        <v>13</v>
+      </c>
+      <c r="H60" s="40"/>
+      <c r="I60" s="40"/>
     </row>
     <row r="61" ht="15.75" spans="2:9">
       <c r="B61" s="52">
-        <v>600</v>
-      </c>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97">
-        <v>350</v>
-      </c>
-      <c r="E61" s="97">
-        <v>14.5</v>
-      </c>
-      <c r="F61" s="100"/>
-      <c r="G61" s="41">
+        <v>750</v>
+      </c>
+      <c r="C61" s="98"/>
+      <c r="D61" s="98">
+        <v>441</v>
+      </c>
+      <c r="E61" s="98">
+        <v>17.25</v>
+      </c>
+      <c r="F61" s="41">
         <v>13</v>
       </c>
-      <c r="H61" s="40">
-        <v>4.5</v>
-      </c>
-      <c r="I61" s="40">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" spans="2:9">
-      <c r="B62" s="52">
-        <v>750</v>
-      </c>
-      <c r="C62" s="97"/>
-      <c r="D62" s="97">
-        <v>441</v>
-      </c>
-      <c r="E62" s="97">
-        <v>17.25</v>
-      </c>
-      <c r="F62" s="98" t="s">
-        <v>175</v>
-      </c>
-      <c r="G62" s="41">
+      <c r="H61" s="40"/>
+      <c r="I61" s="103"/>
+    </row>
+    <row r="62" ht="16.5" spans="2:9">
+      <c r="B62" s="65">
+        <v>1000</v>
+      </c>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45">
+        <v>688</v>
+      </c>
+      <c r="E62" s="45">
+        <v>21.5</v>
+      </c>
+      <c r="F62" s="46">
         <v>13</v>
       </c>
       <c r="H62" s="40"/>
-      <c r="I62" s="109">
-        <f>SUM(I55:I61)</f>
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="63" ht="16.5" spans="2:9">
-      <c r="B63" s="65">
-        <v>1000</v>
-      </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45">
-        <v>688</v>
-      </c>
-      <c r="E63" s="45">
-        <v>21.5</v>
-      </c>
-      <c r="F63" s="99" t="s">
-        <v>137</v>
-      </c>
-      <c r="G63" s="46">
-        <v>13</v>
-      </c>
+      <c r="I62" s="40"/>
+    </row>
+    <row r="63" spans="7:9">
+      <c r="G63" s="40"/>
       <c r="H63" s="40"/>
       <c r="I63" s="40"/>
     </row>
@@ -6714,107 +6592,126 @@
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
     </row>
-    <row r="65" ht="15.75" spans="7:9">
-      <c r="G65" s="40"/>
-      <c r="H65" s="40">
-        <f>4*3.5</f>
-        <v>14</v>
-      </c>
-      <c r="I65" s="40"/>
-    </row>
-    <row r="66" ht="90.75" spans="1:9">
-      <c r="A66">
+    <row r="65" ht="90.75" spans="1:9">
+      <c r="A65">
         <f>147*2*0.8</f>
         <v>235.2</v>
       </c>
-      <c r="C66" s="110" t="s">
-        <v>176</v>
-      </c>
-      <c r="D66" s="110" t="s">
-        <v>177</v>
-      </c>
-      <c r="E66" s="110" t="s">
-        <v>178</v>
-      </c>
-      <c r="G66" s="40">
+      <c r="C65" s="104" t="s">
+        <v>182</v>
+      </c>
+      <c r="D65" s="104" t="s">
+        <v>183</v>
+      </c>
+      <c r="E65" s="104" t="s">
+        <v>184</v>
+      </c>
+      <c r="G65" s="40">
         <f>350*4*0.8</f>
         <v>1120</v>
       </c>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+    </row>
+    <row r="66" spans="5:9">
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
       <c r="H66" s="40"/>
       <c r="I66" s="40"/>
     </row>
     <row r="67" spans="5:9">
-      <c r="E67" s="40"/>
+      <c r="E67" s="105"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
       <c r="I67" s="40"/>
     </row>
-    <row r="68" spans="5:9">
-      <c r="E68" s="111"/>
+    <row r="68" spans="3:9">
+      <c r="C68" s="40"/>
+      <c r="E68" s="40"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
       <c r="I68" s="40"/>
     </row>
-    <row r="69" spans="3:9">
-      <c r="C69" s="40"/>
+    <row r="69" ht="13" customHeight="1" spans="5:9">
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
       <c r="G69" s="40"/>
       <c r="H69" s="40"/>
       <c r="I69" s="40"/>
     </row>
-    <row r="70" ht="13" customHeight="1" spans="5:9">
+    <row r="70" spans="5:9">
       <c r="E70" s="40"/>
       <c r="F70" s="40"/>
       <c r="G70" s="40"/>
       <c r="H70" s="40"/>
       <c r="I70" s="40"/>
     </row>
-    <row r="71" spans="5:9">
-      <c r="E71" s="40"/>
-      <c r="F71" s="40"/>
-      <c r="G71" s="40"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="40"/>
+    <row r="71" ht="15.75" spans="1:14">
+      <c r="A71" s="106"/>
+      <c r="B71" s="107"/>
+      <c r="C71" s="108"/>
+      <c r="D71" s="108"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58" t="s">
+        <v>185</v>
+      </c>
+      <c r="I71" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="J71" s="58"/>
+      <c r="K71" s="58"/>
+      <c r="M71" s="40"/>
+      <c r="N71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="112"/>
-      <c r="B72" s="113"/>
-      <c r="C72" s="114"/>
-      <c r="D72" s="114"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58" t="s">
-        <v>179</v>
-      </c>
-      <c r="I72" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="J72" s="58"/>
-      <c r="K72" s="58"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="40"/>
+      <c r="H72" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="I72" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="J72" s="40"/>
+      <c r="K72" s="40"/>
       <c r="M72" s="40"/>
       <c r="N72" s="40"/>
     </row>
-    <row r="73" ht="15.75" spans="1:14">
+    <row r="73" spans="1:14">
       <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40" t="s">
-        <v>182</v>
+      <c r="B73" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="50" t="s">
+        <v>190</v>
       </c>
       <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="I73" s="40" t="s">
-        <v>183</v>
+      <c r="G73" s="109" t="s">
+        <v>191</v>
+      </c>
+      <c r="H73" s="109" t="s">
+        <v>192</v>
+      </c>
+      <c r="I73" s="109" t="s">
+        <v>193</v>
       </c>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
@@ -6823,56 +6720,58 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="40"/>
-      <c r="B74" s="74" t="s">
-        <v>144</v>
-      </c>
-      <c r="C74" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="D74" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="E74" s="50" t="s">
-        <v>185</v>
+      <c r="B74" s="39">
+        <v>1</v>
+      </c>
+      <c r="C74" s="55">
+        <v>22</v>
+      </c>
+      <c r="D74" s="55">
+        <v>10</v>
+      </c>
+      <c r="E74" s="55">
+        <v>6</v>
       </c>
       <c r="F74" s="40"/>
-      <c r="G74" s="115" t="s">
-        <v>186</v>
-      </c>
-      <c r="H74" s="115" t="s">
-        <v>187</v>
-      </c>
-      <c r="I74" s="115" t="s">
-        <v>188</v>
+      <c r="G74" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="H74" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="I74" s="40" t="s">
+        <v>196</v>
       </c>
       <c r="J74" s="40"/>
       <c r="K74" s="40"/>
+      <c r="L74" s="40"/>
       <c r="M74" s="40"/>
       <c r="N74" s="40"/>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="40"/>
       <c r="B75" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C75" s="55">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D75" s="55">
-        <v>10</v>
+        <f>FLOOR(C75/2,1)</f>
+        <v>13</v>
       </c>
       <c r="E75" s="55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F75" s="40"/>
       <c r="G75" s="40" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="I75" s="40" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="J75" s="40"/>
       <c r="K75" s="40"/>
@@ -6883,149 +6782,149 @@
     <row r="76" spans="1:14">
       <c r="A76" s="40"/>
       <c r="B76" s="39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C76" s="55">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D76" s="55">
-        <f>FLOOR(C76/2,1)</f>
-        <v>13</v>
+        <f t="shared" ref="D76:D83" si="1">FLOOR(C76/2,1)</f>
+        <v>16</v>
       </c>
       <c r="E76" s="55">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F76" s="40"/>
       <c r="G76" s="40" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J76" s="40"/>
       <c r="K76" s="40"/>
-      <c r="L76" s="40"/>
       <c r="M76" s="40"/>
       <c r="N76" s="40"/>
     </row>
-    <row r="77" spans="1:14">
-      <c r="A77" s="40"/>
+    <row r="77" ht="15.75" spans="1:14">
+      <c r="A77" s="106"/>
       <c r="B77" s="39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C77" s="55">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D77" s="55">
-        <f t="shared" ref="D77:D84" si="1">FLOOR(C77/2,1)</f>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="E77" s="55">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F77" s="40"/>
-      <c r="G77" s="40" t="s">
+      <c r="G77" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="H77" s="110" t="s">
         <v>193</v>
       </c>
-      <c r="H77" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="I77" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="J77" s="40"/>
-      <c r="K77" s="40"/>
+      <c r="I77" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="J77" s="112"/>
+      <c r="K77" s="112"/>
+      <c r="L77" s="112"/>
       <c r="M77" s="40"/>
       <c r="N77" s="40"/>
     </row>
-    <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="112"/>
+    <row r="78" spans="1:14">
+      <c r="A78" s="40"/>
       <c r="B78" s="39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C78" s="55">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D78" s="55">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E78" s="55">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F78" s="40"/>
-      <c r="G78" s="116" t="s">
-        <v>195</v>
-      </c>
-      <c r="H78" s="116" t="s">
-        <v>188</v>
-      </c>
-      <c r="I78" s="116" t="s">
-        <v>188</v>
-      </c>
-      <c r="J78" s="118"/>
-      <c r="K78" s="118"/>
-      <c r="L78" s="118"/>
+      <c r="G78" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="H78" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I78" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="J78" s="40"/>
+      <c r="K78" s="40"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="40"/>
       <c r="B79" s="39">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C79" s="55">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D79" s="55">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E79" s="55">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F79" s="40"/>
       <c r="G79" s="40" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I79" s="40" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="J79" s="40"/>
       <c r="K79" s="40"/>
+      <c r="L79" s="40"/>
       <c r="M79" s="40"/>
       <c r="N79" s="40"/>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="40"/>
       <c r="B80" s="39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C80" s="55">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D80" s="55">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E80" s="55">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F80" s="40"/>
       <c r="G80" s="40" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I80" s="40" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J80" s="40"/>
       <c r="K80" s="40"/>
@@ -7033,79 +6932,70 @@
       <c r="M80" s="40"/>
       <c r="N80" s="40"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:11">
       <c r="A81" s="40"/>
       <c r="B81" s="39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C81" s="55">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D81" s="55">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E81" s="55">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F81" s="40"/>
       <c r="G81" s="40" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="I81" s="40" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="J81" s="40"/>
       <c r="K81" s="40"/>
-      <c r="L81" s="40"/>
-      <c r="M81" s="40"/>
-      <c r="N81" s="40"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="40"/>
       <c r="B82" s="39">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C82" s="55">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D82" s="55">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E82" s="55">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F82" s="40"/>
-      <c r="G82" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="H82" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="I82" s="40" t="s">
-        <v>187</v>
-      </c>
+      <c r="G82" s="40"/>
+      <c r="H82" s="40"/>
+      <c r="I82" s="40"/>
       <c r="J82" s="40"/>
       <c r="K82" s="40"/>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" ht="15.75" spans="1:11">
       <c r="A83" s="40"/>
-      <c r="B83" s="39">
-        <v>9</v>
-      </c>
-      <c r="C83" s="55">
-        <v>62</v>
-      </c>
-      <c r="D83" s="55">
+      <c r="B83" s="44">
+        <v>10</v>
+      </c>
+      <c r="C83" s="43">
+        <v>67</v>
+      </c>
+      <c r="D83" s="43">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="E83" s="55">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="E83" s="43">
+        <v>24</v>
       </c>
       <c r="F83" s="40"/>
       <c r="G83" s="40"/>
@@ -7114,42 +7004,32 @@
       <c r="J83" s="40"/>
       <c r="K83" s="40"/>
     </row>
-    <row r="84" ht="15.75" spans="1:11">
+    <row r="84" spans="1:11">
       <c r="A84" s="40"/>
-      <c r="B84" s="44">
-        <v>10</v>
-      </c>
-      <c r="C84" s="43">
-        <v>67</v>
-      </c>
-      <c r="D84" s="43">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="E84" s="43">
-        <v>16</v>
-      </c>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="40"/>
       <c r="F84" s="40"/>
       <c r="G84" s="40"/>
-      <c r="H84" s="40"/>
-      <c r="I84" s="40"/>
+      <c r="H84" s="40">
+        <v>5</v>
+      </c>
+      <c r="I84" s="40">
+        <v>3</v>
+      </c>
       <c r="J84" s="40"/>
       <c r="K84" s="40"/>
     </row>
-    <row r="85" spans="1:11">
-      <c r="A85" s="40"/>
+    <row r="85" spans="2:11">
       <c r="B85" s="40"/>
       <c r="C85" s="40"/>
       <c r="D85" s="40"/>
       <c r="E85" s="40"/>
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
-      <c r="H85" s="40">
-        <v>5</v>
-      </c>
-      <c r="I85" s="40">
-        <v>3</v>
-      </c>
+      <c r="H85" s="105"/>
+      <c r="I85" s="40"/>
       <c r="J85" s="40"/>
       <c r="K85" s="40"/>
     </row>
@@ -7160,7 +7040,7 @@
       <c r="E86" s="40"/>
       <c r="F86" s="40"/>
       <c r="G86" s="40"/>
-      <c r="H86" s="111"/>
+      <c r="H86" s="40"/>
       <c r="I86" s="40"/>
       <c r="J86" s="40"/>
       <c r="K86" s="40"/>
@@ -7178,32 +7058,43 @@
       <c r="K87" s="40"/>
     </row>
     <row r="88" spans="2:11">
-      <c r="B88" s="40"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="40"/>
-      <c r="F88" s="40"/>
-      <c r="G88" s="40"/>
+      <c r="B88" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D88" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="E88" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="F88" s="40" t="s">
+        <v>210</v>
+      </c>
       <c r="H88" s="40"/>
       <c r="I88" s="40"/>
       <c r="J88" s="40"/>
       <c r="K88" s="40"/>
     </row>
     <row r="89" spans="2:11">
-      <c r="B89" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="C89" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="D89" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="E89" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="F89" s="40" t="s">
-        <v>205</v>
+      <c r="B89" s="40">
+        <v>10</v>
+      </c>
+      <c r="C89" s="40">
+        <v>200</v>
+      </c>
+      <c r="D89" s="40">
+        <v>2000</v>
+      </c>
+      <c r="E89" s="40">
+        <f>12*200+936+70</f>
+        <v>3406</v>
+      </c>
+      <c r="F89" s="40">
+        <f>(55+130)*4+12*200*1.2*1.05</f>
+        <v>3764</v>
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
@@ -7218,39 +7109,28 @@
         <v>200</v>
       </c>
       <c r="D90" s="40">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E90" s="40">
-        <f>12*200+936+70</f>
-        <v>3406</v>
+        <f>12*200+936*1.5+70</f>
+        <v>3874</v>
       </c>
       <c r="F90" s="40">
         <f>(55+130)*4+12*200*1.2*1.05</f>
         <v>3764</v>
       </c>
+      <c r="G90" s="40"/>
       <c r="H90" s="40"/>
       <c r="I90" s="40"/>
       <c r="J90" s="40"/>
       <c r="K90" s="40"/>
     </row>
     <row r="91" spans="2:11">
-      <c r="B91" s="40">
-        <v>10</v>
-      </c>
-      <c r="C91" s="40">
-        <v>200</v>
-      </c>
-      <c r="D91" s="40">
-        <v>3000</v>
-      </c>
-      <c r="E91" s="40">
-        <f>12*200+936*1.5+70</f>
-        <v>3874</v>
-      </c>
-      <c r="F91" s="40">
-        <f>(55+130)*4+12*200*1.2*1.05</f>
-        <v>3764</v>
-      </c>
+      <c r="B91" s="40"/>
+      <c r="C91" s="40"/>
+      <c r="D91" s="40"/>
+      <c r="E91" s="40"/>
+      <c r="F91" s="40"/>
       <c r="G91" s="40"/>
       <c r="H91" s="40"/>
       <c r="I91" s="40"/>
@@ -7286,7 +7166,7 @@
       <c r="C94" s="40"/>
       <c r="D94" s="40"/>
       <c r="E94" s="40"/>
-      <c r="F94" s="40"/>
+      <c r="F94" s="103"/>
       <c r="G94" s="40"/>
       <c r="H94" s="40"/>
       <c r="I94" s="40"/>
@@ -7298,27 +7178,28 @@
       <c r="C95" s="40"/>
       <c r="D95" s="40"/>
       <c r="E95" s="40"/>
-      <c r="F95" s="109"/>
+      <c r="F95" s="40"/>
       <c r="G95" s="40"/>
       <c r="H95" s="40"/>
       <c r="I95" s="40"/>
       <c r="J95" s="40"/>
       <c r="K95" s="40"/>
     </row>
-    <row r="96" spans="2:11">
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
+    <row r="96" spans="5:11">
       <c r="E96" s="40"/>
-      <c r="F96" s="40"/>
-      <c r="G96" s="40"/>
-      <c r="H96" s="40"/>
       <c r="I96" s="40"/>
       <c r="J96" s="40"/>
       <c r="K96" s="40"/>
     </row>
-    <row r="97" spans="5:11">
+    <row r="97" spans="1:11">
+      <c r="A97" s="40"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
+      <c r="D97" s="40"/>
       <c r="E97" s="40"/>
+      <c r="F97" s="103"/>
+      <c r="G97" s="40"/>
+      <c r="H97" s="40"/>
       <c r="I97" s="40"/>
       <c r="J97" s="40"/>
       <c r="K97" s="40"/>
@@ -7329,36 +7210,29 @@
       <c r="C98" s="40"/>
       <c r="D98" s="40"/>
       <c r="E98" s="40"/>
-      <c r="F98" s="109"/>
+      <c r="F98" s="40"/>
       <c r="G98" s="40"/>
       <c r="H98" s="40"/>
       <c r="I98" s="40"/>
       <c r="J98" s="40"/>
       <c r="K98" s="40"/>
     </row>
-    <row r="99" spans="1:11">
-      <c r="A99" s="40"/>
+    <row r="99" spans="2:6">
       <c r="B99" s="40"/>
       <c r="C99" s="40"/>
       <c r="D99" s="40"/>
       <c r="E99" s="40"/>
       <c r="F99" s="40"/>
-      <c r="G99" s="40"/>
-      <c r="H99" s="40"/>
-      <c r="I99" s="40"/>
-      <c r="J99" s="40"/>
-      <c r="K99" s="40"/>
-    </row>
-    <row r="100" spans="2:6">
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="40"/>
       <c r="B100" s="40"/>
       <c r="C100" s="40"/>
       <c r="D100" s="40"/>
       <c r="E100" s="40"/>
       <c r="F100" s="40"/>
     </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="40"/>
-      <c r="B101" s="40"/>
+    <row r="101" spans="3:6">
       <c r="C101" s="40"/>
       <c r="D101" s="40"/>
       <c r="E101" s="40"/>
@@ -7368,13 +7242,13 @@
       <c r="C102" s="40"/>
       <c r="D102" s="40"/>
       <c r="E102" s="40"/>
-      <c r="F102" s="40"/>
+      <c r="F102" s="111"/>
     </row>
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
       <c r="E103" s="40"/>
-      <c r="F103" s="117"/>
+      <c r="F103" s="40"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -7424,14 +7298,8 @@
       <c r="E111" s="40"/>
       <c r="F111" s="40"/>
     </row>
-    <row r="112" spans="3:6">
-      <c r="C112" s="40"/>
-      <c r="D112" s="40"/>
-      <c r="E112" s="40"/>
-      <c r="F112" s="40"/>
-    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="M3:N3"/>
@@ -7440,13 +7308,14 @@
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="K74:L74"/>
     <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -7478,31 +7347,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7510,28 +7379,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7539,28 +7408,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7568,28 +7437,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7597,28 +7466,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7626,28 +7495,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7655,28 +7524,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7684,28 +7553,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7713,28 +7582,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7742,28 +7611,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7771,28 +7640,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7800,28 +7669,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7829,28 +7698,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>281</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7858,33 +7727,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7916,34 +7785,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7951,31 +7820,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7983,31 +7852,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -8015,31 +7884,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8047,31 +7916,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -8079,31 +7948,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -8111,31 +7980,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8143,31 +8012,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8175,31 +8044,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8207,31 +8076,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8239,31 +8108,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8271,31 +8140,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8303,31 +8172,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8335,63 +8204,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished changing and updating weapons. Update still WIP.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="387">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -1036,6 +1036,12 @@
     <t>New Health</t>
   </si>
   <si>
+    <t>4 (2d4 - 1)</t>
+  </si>
+  <si>
+    <t>5 (1d8)</t>
+  </si>
+  <si>
     <t>The double of another column
 should be 120% of that column
 E.g. 400XP HP = 1.2 * 2 * 200XP HP</t>
@@ -1053,18 +1059,9 @@
 E.g. 400XP dmg = 0.85 * 2 * 200XP dmg</t>
   </si>
   <si>
-    <t>For 2...</t>
-  </si>
-  <si>
-    <t>...gain 1</t>
-  </si>
-  <si>
     <t>18.5 + Might + Other</t>
   </si>
   <si>
-    <t>HP Regen</t>
-  </si>
-  <si>
     <t>Reserve HP</t>
   </si>
   <si>
@@ -1074,42 +1071,21 @@
     <t>Bertle</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>Davel</t>
   </si>
   <si>
-    <t>Low-Medium</t>
-  </si>
-  <si>
-    <t>Medium-High</t>
-  </si>
-  <si>
     <t>Dragonborn</t>
   </si>
   <si>
     <t>Dwarf</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Elf</t>
   </si>
   <si>
     <t>Gnome</t>
   </si>
   <si>
-    <t>Very Low</t>
-  </si>
-  <si>
-    <t>Very High</t>
-  </si>
-  <si>
     <t>Hollow</t>
   </si>
   <si>
@@ -1117,18 +1093,6 @@
   </si>
   <si>
     <t>Orc</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>Enemy HP</t>
-  </si>
-  <si>
-    <t>Bork (12 hits) (100 armor (50%))</t>
-  </si>
-  <si>
-    <t>Kraken (12 hits)</t>
   </si>
   <si>
     <t>1-Handed (+3)</t>
@@ -2660,7 +2624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2910,9 +2874,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2922,9 +2883,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2932,9 +2890,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2995,21 +2950,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3032,12 +2978,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -3500,7 +3440,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="99" t="s">
+      <c r="L7" s="96" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3516,10 +3456,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="99" t="s">
+      <c r="L8" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="99"/>
+      <c r="M8" s="96"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3552,13 +3492,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="119" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="120" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3570,7 +3510,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="128" t="s">
+      <c r="G10" s="120" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3581,13 +3521,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="119" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3599,7 +3539,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="128" t="s">
+      <c r="G11" s="120" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3610,13 +3550,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="121" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="122" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3628,7 +3568,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="130" t="s">
+      <c r="G12" s="122" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3803,7 +3743,7 @@
       <c r="B22" s="66">
         <v>1</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="92" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="66" t="s">
@@ -3828,7 +3768,7 @@
       <c r="B23" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="93">
+      <c r="C23" s="90">
         <v>6</v>
       </c>
       <c r="D23" s="68">
@@ -3851,7 +3791,7 @@
       <c r="B24" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="95">
+      <c r="C24" s="92">
         <v>8</v>
       </c>
       <c r="D24" s="66">
@@ -3884,16 +3824,16 @@
     <row r="26" ht="15.75" spans="1:11">
       <c r="A26" s="74"/>
       <c r="B26" s="51"/>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="114"/>
+      <c r="D26" s="76"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="84"/>
+      <c r="J26" s="83"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
@@ -3903,18 +3843,18 @@
       <c r="B27" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="115" t="s">
+      <c r="C27" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="124"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3923,16 +3863,16 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="118"/>
+      <c r="D28" s="112"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="51"/>
-      <c r="J28" s="84"/>
+      <c r="J28" s="83"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -3942,10 +3882,10 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="89"/>
+      <c r="D29" s="87"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -3961,20 +3901,20 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="89" t="s">
+      <c r="D30" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="89" t="s">
+      <c r="E30" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="86" t="s">
+      <c r="F30" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="89"/>
-      <c r="J30" s="125"/>
+      <c r="H30" s="87"/>
+      <c r="J30" s="88"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:10">
@@ -4027,7 +3967,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="126"/>
+      <c r="J32" s="118"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -4062,20 +4002,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="120">
+      <c r="B34" s="114">
         <v>1</v>
       </c>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="120"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="114"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -4085,38 +4025,38 @@
       <c r="A35" s="67">
         <v>1</v>
       </c>
-      <c r="B35" s="92" t="s">
+      <c r="B35" s="89" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="84"/>
+      <c r="J35" s="83"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="16.5" spans="1:11">
       <c r="A36" s="65">
         <v>1</v>
       </c>
-      <c r="B36" s="94" t="s">
+      <c r="B36" s="91" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="92"/>
       <c r="I36" s="45"/>
       <c r="J36" s="46"/>
       <c r="K36" s="58"/>
@@ -4152,7 +4092,7 @@
       <c r="C39" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="92"/>
+      <c r="D39" s="89"/>
       <c r="F39" s="58"/>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
@@ -4174,17 +4114,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="122" t="s">
+      <c r="F40" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="92" t="s">
+      <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="131" t="s">
+      <c r="I40" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
+      <c r="J40" s="99"/>
+      <c r="K40" s="99"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4203,10 +4143,10 @@
       <c r="F41" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="96">
+      <c r="G41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="132" t="s">
+      <c r="I41" s="124" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4229,7 +4169,7 @@
       <c r="F42" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="96">
+      <c r="G42" s="93">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -4253,7 +4193,7 @@
       <c r="F43" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="96">
+      <c r="G43" s="93">
         <v>10</v>
       </c>
       <c r="I43" s="58"/>
@@ -4279,7 +4219,7 @@
       <c r="F44" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="96">
+      <c r="G44" s="93">
         <v>10</v>
       </c>
       <c r="I44" s="40"/>
@@ -4305,7 +4245,7 @@
       <c r="F45" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="96">
+      <c r="G45" s="93">
         <v>10</v>
       </c>
       <c r="I45" s="40"/>
@@ -4331,7 +4271,7 @@
       <c r="F46" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="96">
+      <c r="G46" s="93">
         <v>10</v>
       </c>
       <c r="H46" t="s">
@@ -4360,7 +4300,7 @@
       <c r="F47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="96">
+      <c r="G47" s="93">
         <v>10</v>
       </c>
       <c r="I47" s="40"/>
@@ -4386,7 +4326,7 @@
       <c r="F48" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="96">
+      <c r="G48" s="93">
         <v>11</v>
       </c>
       <c r="I48" s="40"/>
@@ -4409,7 +4349,7 @@
       <c r="F49" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="96">
+      <c r="G49" s="93">
         <v>11</v>
       </c>
       <c r="I49" s="40"/>
@@ -4435,7 +4375,7 @@
       <c r="F50" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="96">
+      <c r="G50" s="93">
         <v>11</v>
       </c>
       <c r="I50" s="40"/>
@@ -4461,7 +4401,7 @@
       <c r="F51" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="96">
+      <c r="G51" s="93">
         <v>11</v>
       </c>
       <c r="I51" s="40"/>
@@ -4679,11 +4619,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="123" t="s">
+      <c r="C62" s="117" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="123" t="s">
+      <c r="F62" s="117" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4702,7 +4642,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="105" t="s">
+      <c r="E64" s="102" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4749,7 +4689,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="123" t="s">
+      <c r="C70" s="117" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4766,10 +4706,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="106"/>
-      <c r="B72" s="107"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
+      <c r="A72" s="103"/>
+      <c r="B72" s="104"/>
+      <c r="C72" s="105"/>
+      <c r="D72" s="105"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4874,7 +4814,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="133" t="s">
+      <c r="D77" s="125" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4892,7 +4832,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="106"/>
+      <c r="A78" s="103"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4902,16 +4842,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="112"/>
+      <c r="E78" s="110"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="112"/>
-      <c r="H78" s="112"/>
-      <c r="I78" s="112"/>
-      <c r="J78" s="112"/>
-      <c r="K78" s="112"/>
-      <c r="L78" s="112"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
+      <c r="I78" s="110"/>
+      <c r="J78" s="110"/>
+      <c r="K78" s="110"/>
+      <c r="L78" s="110"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4968,7 +4908,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="133" t="s">
+      <c r="D81" s="125" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5241,8 +5181,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="111"/>
+      <c r="E103" s="109"/>
+      <c r="F103" s="109"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5326,8 +5266,8 @@
   <sheetPr/>
   <dimension ref="A2:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5432,7 +5372,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="99" t="s">
+      <c r="L7" s="96" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5448,10 +5388,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="99" t="s">
+      <c r="L8" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="99"/>
+      <c r="M8" s="96"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5484,13 +5424,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="119" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="120" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5502,7 +5442,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="128" t="s">
+      <c r="G10" s="120" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5513,13 +5453,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="119" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5531,7 +5471,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="128" t="s">
+      <c r="G11" s="120" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5542,13 +5482,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="121" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="122" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5560,7 +5500,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="130" t="s">
+      <c r="G12" s="122" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5660,8 +5600,8 @@
         <v>-1</v>
       </c>
       <c r="H18" s="57">
-        <f>6.5+9</f>
-        <v>15.5</v>
+        <f>6.5*2</f>
+        <v>13</v>
       </c>
       <c r="K18" s="70">
         <v>4</v>
@@ -5686,7 +5626,10 @@
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="58">
+        <f>(14-5)*2</f>
+        <v>18</v>
+      </c>
       <c r="K19" s="70">
         <v>5</v>
       </c>
@@ -5824,12 +5767,12 @@
       <c r="H25" s="40"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
-      <c r="K25" s="100">
+      <c r="K25" s="97">
         <f>46/9</f>
         <v>5.11111111111111</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" ht="15.75" spans="1:11">
       <c r="A26" s="74"/>
       <c r="B26" s="51"/>
       <c r="C26" s="75" t="s">
@@ -5838,10 +5781,6 @@
       <c r="D26" s="76"/>
       <c r="E26" s="76"/>
       <c r="F26" s="77"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" ht="16.5" spans="1:12">
@@ -5857,12 +5796,8 @@
       <c r="D27" s="81"/>
       <c r="E27" s="81"/>
       <c r="F27" s="82"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -5871,18 +5806,14 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="39" t="s">
         <v>174</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E28" s="51"/>
-      <c r="F28" s="84"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
+      <c r="F28" s="83"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11">
@@ -5892,18 +5823,14 @@
       <c r="B29" s="40">
         <v>0</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="85" t="s">
         <v>177</v>
       </c>
       <c r="E29" s="40"/>
-      <c r="F29" s="87"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
+      <c r="F29" s="41"/>
       <c r="K29" s="40"/>
     </row>
     <row r="30" spans="1:11">
@@ -5913,10 +5840,10 @@
       <c r="B30" s="40">
         <v>0</v>
       </c>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="88"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:6">
@@ -5926,7 +5853,7 @@
       <c r="B31" s="40">
         <v>1</v>
       </c>
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="39" t="s">
         <v>178</v>
       </c>
       <c r="D31" s="40" t="s">
@@ -5935,7 +5862,7 @@
       <c r="E31" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="87" t="s">
+      <c r="F31" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5946,14 +5873,14 @@
       <c r="B32" s="40">
         <v>1</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="39" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="40" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="40"/>
-      <c r="F32" s="87"/>
+      <c r="F32" s="41"/>
     </row>
     <row r="33" ht="15.75" spans="1:6">
       <c r="A33" s="44">
@@ -5971,40 +5898,32 @@
       <c r="A34" s="67">
         <v>1</v>
       </c>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="89" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="92"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="89"/>
       <c r="K34" s="58"/>
     </row>
     <row r="35" ht="16.5" spans="1:11">
       <c r="A35" s="65">
         <v>1</v>
       </c>
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="91" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="95"/>
-      <c r="F35" s="94"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="91"/>
       <c r="K35" s="58"/>
     </row>
     <row r="36" ht="15.75" spans="1:11">
@@ -6038,7 +5957,7 @@
       <c r="C38" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="92"/>
+      <c r="D38" s="89"/>
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
@@ -6060,12 +5979,12 @@
       <c r="E39" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="92" t="s">
+      <c r="F39" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I39" s="102"/>
-      <c r="J39" s="102"/>
-      <c r="K39" s="102"/>
+      <c r="I39" s="99"/>
+      <c r="J39" s="99"/>
+      <c r="K39" s="99"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
       <c r="A40" s="72"/>
@@ -6080,9 +5999,9 @@
         <v>9</v>
       </c>
       <c r="E40" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" s="96">
+        <v>93</v>
+      </c>
+      <c r="F40" s="93">
         <v>10</v>
       </c>
       <c r="I40" s="58"/>
@@ -6102,9 +6021,9 @@
         <v>18</v>
       </c>
       <c r="E41" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" s="96">
+        <v>95</v>
+      </c>
+      <c r="F41" s="93">
         <v>10</v>
       </c>
       <c r="I41" s="58"/>
@@ -6124,9 +6043,9 @@
         <v>27</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="96">
+        <v>91</v>
+      </c>
+      <c r="F42" s="93">
         <v>10</v>
       </c>
       <c r="I42" s="58"/>
@@ -6148,13 +6067,11 @@
         <v>36</v>
       </c>
       <c r="E43" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="F43" s="96">
+        <v>182</v>
+      </c>
+      <c r="F43" s="93">
         <v>10</v>
       </c>
-      <c r="G43"/>
-      <c r="H43"/>
       <c r="I43" s="40"/>
       <c r="J43" s="40"/>
       <c r="K43" s="58"/>
@@ -6174,13 +6091,11 @@
         <v>48</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="F44" s="96">
+        <v>183</v>
+      </c>
+      <c r="F44" s="93">
         <v>10</v>
       </c>
-      <c r="G44"/>
-      <c r="H44"/>
       <c r="I44" s="40"/>
       <c r="J44" s="40"/>
       <c r="K44" s="58"/>
@@ -6200,13 +6115,11 @@
         <v>60</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="96">
+        <v>96</v>
+      </c>
+      <c r="F45" s="93">
         <v>10</v>
       </c>
-      <c r="G45"/>
-      <c r="H45"/>
       <c r="I45" s="40"/>
       <c r="J45" s="40"/>
       <c r="K45" s="58"/>
@@ -6228,11 +6141,9 @@
       <c r="E46" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="96">
+      <c r="F46" s="93">
         <v>10</v>
       </c>
-      <c r="G46"/>
-      <c r="H46"/>
       <c r="I46" s="40"/>
       <c r="J46" s="40"/>
       <c r="K46" s="58"/>
@@ -6251,11 +6162,9 @@
       <c r="E47" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="96">
+      <c r="F47" s="93">
         <v>11</v>
       </c>
-      <c r="G47"/>
-      <c r="H47"/>
       <c r="I47" s="40"/>
       <c r="J47" s="40"/>
       <c r="K47" s="58"/>
@@ -6277,11 +6186,9 @@
       <c r="E48" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="96">
+      <c r="F48" s="93">
         <v>11</v>
       </c>
-      <c r="G48"/>
-      <c r="H48"/>
       <c r="I48" s="40"/>
       <c r="J48" s="40"/>
       <c r="K48" s="58"/>
@@ -6303,11 +6210,9 @@
       <c r="E49" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="F49" s="96">
+      <c r="F49" s="93">
         <v>11</v>
       </c>
-      <c r="G49"/>
-      <c r="H49"/>
       <c r="I49" s="40"/>
       <c r="J49" s="40"/>
       <c r="K49" s="58"/>
@@ -6326,20 +6231,18 @@
       <c r="E50" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F50" s="96">
+      <c r="F50" s="93">
         <v>11</v>
       </c>
-      <c r="G50"/>
-      <c r="H50"/>
       <c r="I50" s="40"/>
       <c r="J50" s="40"/>
       <c r="K50" s="58"/>
     </row>
     <row r="51" ht="15.75" spans="1:13">
-      <c r="A51" s="97" t="s">
+      <c r="A51" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="98">
+      <c r="B51" s="95">
         <v>300</v>
       </c>
       <c r="C51" s="40">
@@ -6355,35 +6258,31 @@
       <c r="F51" s="41">
         <v>12</v>
       </c>
-      <c r="G51"/>
-      <c r="H51"/>
       <c r="I51" s="58"/>
       <c r="J51" s="70"/>
       <c r="K51" s="70"/>
       <c r="M51" s="58"/>
     </row>
     <row r="52" ht="15.75" spans="1:13">
-      <c r="A52" s="97" t="s">
+      <c r="A52" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="98">
+      <c r="B52" s="95">
         <v>325</v>
       </c>
-      <c r="C52" s="98">
+      <c r="C52" s="95">
         <v>120</v>
       </c>
-      <c r="D52" s="98">
+      <c r="D52" s="95">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="E52" s="98" t="s">
+      <c r="E52" s="95" t="s">
         <v>121</v>
       </c>
       <c r="F52" s="41">
         <v>12</v>
       </c>
-      <c r="G52"/>
-      <c r="H52"/>
       <c r="I52" s="40"/>
       <c r="M52" s="58"/>
     </row>
@@ -6407,8 +6306,6 @@
       <c r="F53" s="41">
         <v>12</v>
       </c>
-      <c r="G53"/>
-      <c r="H53"/>
       <c r="I53" s="40"/>
       <c r="M53" s="58"/>
     </row>
@@ -6432,8 +6329,6 @@
       <c r="F54" s="46">
         <v>12</v>
       </c>
-      <c r="G54"/>
-      <c r="H54"/>
       <c r="I54" s="40"/>
     </row>
     <row r="55" spans="2:9">
@@ -6516,14 +6411,14 @@
       <c r="B59" s="52">
         <v>500</v>
       </c>
-      <c r="C59" s="98">
+      <c r="C59" s="95">
         <v>218</v>
       </c>
-      <c r="D59" s="98">
+      <c r="D59" s="95">
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-      <c r="E59" s="98" t="s">
+      <c r="E59" s="95" t="s">
         <v>136</v>
       </c>
       <c r="F59" s="41">
@@ -6535,11 +6430,11 @@
       <c r="B60" s="52">
         <v>600</v>
       </c>
-      <c r="C60" s="98"/>
-      <c r="D60" s="98">
+      <c r="C60" s="95"/>
+      <c r="D60" s="95">
         <v>350</v>
       </c>
-      <c r="E60" s="98">
+      <c r="E60" s="95">
         <v>14.5</v>
       </c>
       <c r="F60" s="41">
@@ -6552,18 +6447,18 @@
       <c r="B61" s="52">
         <v>750</v>
       </c>
-      <c r="C61" s="98"/>
-      <c r="D61" s="98">
+      <c r="C61" s="95"/>
+      <c r="D61" s="95">
         <v>441</v>
       </c>
-      <c r="E61" s="98">
+      <c r="E61" s="95">
         <v>17.25</v>
       </c>
       <c r="F61" s="41">
         <v>13</v>
       </c>
       <c r="H61" s="40"/>
-      <c r="I61" s="103"/>
+      <c r="I61" s="100"/>
     </row>
     <row r="62" ht="16.5" spans="2:9">
       <c r="B62" s="65">
@@ -6587,7 +6482,7 @@
       <c r="H63" s="40"/>
       <c r="I63" s="40"/>
     </row>
-    <row r="64" spans="7:9">
+    <row r="64" ht="15.75" spans="7:9">
       <c r="G64" s="40"/>
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
@@ -6597,14 +6492,14 @@
         <f>147*2*0.8</f>
         <v>235.2</v>
       </c>
-      <c r="C65" s="104" t="s">
-        <v>182</v>
-      </c>
-      <c r="D65" s="104" t="s">
-        <v>183</v>
-      </c>
-      <c r="E65" s="104" t="s">
+      <c r="C65" s="101" t="s">
         <v>184</v>
+      </c>
+      <c r="D65" s="101" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" s="101" t="s">
+        <v>186</v>
       </c>
       <c r="G65" s="40">
         <f>350*4*0.8</f>
@@ -6621,7 +6516,7 @@
       <c r="I66" s="40"/>
     </row>
     <row r="67" spans="5:9">
-      <c r="E67" s="105"/>
+      <c r="E67" s="102"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
@@ -6650,25 +6545,21 @@
       <c r="I70" s="40"/>
     </row>
     <row r="71" ht="15.75" spans="1:14">
-      <c r="A71" s="106"/>
-      <c r="B71" s="107"/>
-      <c r="C71" s="108"/>
-      <c r="D71" s="108"/>
+      <c r="A71" s="103"/>
+      <c r="B71" s="104"/>
+      <c r="C71" s="105"/>
+      <c r="D71" s="105"/>
       <c r="E71" s="58"/>
       <c r="F71" s="58"/>
       <c r="G71" s="58"/>
-      <c r="H71" s="58" t="s">
-        <v>185</v>
-      </c>
-      <c r="I71" s="58" t="s">
-        <v>186</v>
-      </c>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
       <c r="J71" s="58"/>
       <c r="K71" s="58"/>
       <c r="M71" s="40"/>
       <c r="N71" s="40"/>
     </row>
-    <row r="72" ht="15.75" spans="1:14">
+    <row r="72" spans="1:14">
       <c r="A72" s="40"/>
       <c r="B72" s="40"/>
       <c r="C72" s="40" t="s">
@@ -6678,12 +6569,8 @@
       <c r="E72" s="40"/>
       <c r="F72" s="40"/>
       <c r="G72" s="40"/>
-      <c r="H72" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="I72" s="40" t="s">
-        <v>188</v>
-      </c>
+      <c r="H72" s="40"/>
+      <c r="I72" s="40"/>
       <c r="J72" s="40"/>
       <c r="K72" s="40"/>
       <c r="M72" s="40"/>
@@ -6698,21 +6585,17 @@
         <v>145</v>
       </c>
       <c r="D73" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="E73" s="50" t="s">
+      <c r="F73" s="40"/>
+      <c r="G73" s="106" t="s">
         <v>190</v>
       </c>
-      <c r="F73" s="40"/>
-      <c r="G73" s="109" t="s">
-        <v>191</v>
-      </c>
-      <c r="H73" s="109" t="s">
-        <v>192</v>
-      </c>
-      <c r="I73" s="109" t="s">
-        <v>193</v>
-      </c>
+      <c r="H73" s="106"/>
+      <c r="I73" s="106"/>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
       <c r="M73" s="40"/>
@@ -6734,14 +6617,10 @@
       </c>
       <c r="F74" s="40"/>
       <c r="G74" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="H74" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="I74" s="40" t="s">
-        <v>196</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H74" s="40"/>
+      <c r="I74" s="40"/>
       <c r="J74" s="40"/>
       <c r="K74" s="40"/>
       <c r="L74" s="40"/>
@@ -6765,14 +6644,10 @@
       </c>
       <c r="F75" s="40"/>
       <c r="G75" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="H75" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="I75" s="40" t="s">
-        <v>195</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="H75" s="40"/>
+      <c r="I75" s="40"/>
       <c r="J75" s="40"/>
       <c r="K75" s="40"/>
       <c r="L75" s="40"/>
@@ -6796,21 +6671,17 @@
       </c>
       <c r="F76" s="40"/>
       <c r="G76" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="H76" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="I76" s="40" t="s">
         <v>193</v>
       </c>
+      <c r="H76" s="40"/>
+      <c r="I76" s="40"/>
       <c r="J76" s="40"/>
       <c r="K76" s="40"/>
       <c r="M76" s="40"/>
       <c r="N76" s="40"/>
     </row>
     <row r="77" ht="15.75" spans="1:14">
-      <c r="A77" s="106"/>
+      <c r="A77" s="103"/>
       <c r="B77" s="39">
         <v>4</v>
       </c>
@@ -6825,18 +6696,14 @@
         <v>12</v>
       </c>
       <c r="F77" s="40"/>
-      <c r="G77" s="110" t="s">
-        <v>200</v>
-      </c>
-      <c r="H77" s="110" t="s">
-        <v>193</v>
-      </c>
-      <c r="I77" s="110" t="s">
-        <v>193</v>
-      </c>
-      <c r="J77" s="112"/>
-      <c r="K77" s="112"/>
-      <c r="L77" s="112"/>
+      <c r="G77" s="107" t="s">
+        <v>194</v>
+      </c>
+      <c r="H77" s="107"/>
+      <c r="I77" s="107"/>
+      <c r="J77" s="110"/>
+      <c r="K77" s="110"/>
+      <c r="L77" s="110"/>
       <c r="M77" s="40"/>
       <c r="N77" s="40"/>
     </row>
@@ -6857,14 +6724,10 @@
       </c>
       <c r="F78" s="40"/>
       <c r="G78" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="H78" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="I78" s="40" t="s">
-        <v>203</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="H78" s="40"/>
+      <c r="I78" s="40"/>
       <c r="J78" s="40"/>
       <c r="K78" s="40"/>
       <c r="M78" s="40"/>
@@ -6887,14 +6750,10 @@
       </c>
       <c r="F79" s="40"/>
       <c r="G79" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="H79" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="I79" s="40" t="s">
-        <v>202</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="H79" s="40"/>
+      <c r="I79" s="40"/>
       <c r="J79" s="40"/>
       <c r="K79" s="40"/>
       <c r="L79" s="40"/>
@@ -6918,14 +6777,10 @@
       </c>
       <c r="F80" s="40"/>
       <c r="G80" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="H80" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="I80" s="40" t="s">
-        <v>193</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="H80" s="40"/>
+      <c r="I80" s="40"/>
       <c r="J80" s="40"/>
       <c r="K80" s="40"/>
       <c r="L80" s="40"/>
@@ -6949,14 +6804,10 @@
       </c>
       <c r="F81" s="40"/>
       <c r="G81" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="H81" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="I81" s="40" t="s">
-        <v>192</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H81" s="40"/>
+      <c r="I81" s="40"/>
       <c r="J81" s="40"/>
       <c r="K81" s="40"/>
     </row>
@@ -7022,22 +6873,31 @@
       <c r="K84" s="40"/>
     </row>
     <row r="85" spans="2:11">
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
+      <c r="B85" s="108"/>
+      <c r="C85" s="108"/>
       <c r="D85" s="40"/>
       <c r="E85" s="40"/>
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
-      <c r="H85" s="105"/>
+      <c r="H85" s="102"/>
       <c r="I85" s="40"/>
       <c r="J85" s="40"/>
       <c r="K85" s="40"/>
     </row>
     <row r="86" spans="2:11">
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
+      <c r="B86" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" s="64">
+        <v>16</v>
+      </c>
+      <c r="D86" s="40">
+        <v>8</v>
+      </c>
+      <c r="E86" s="40">
+        <f>C86+2*D86</f>
+        <v>32</v>
+      </c>
       <c r="F86" s="40"/>
       <c r="G86" s="40"/>
       <c r="H86" s="40"/>
@@ -7046,10 +6906,19 @@
       <c r="K86" s="40"/>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40"/>
+      <c r="B87" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" s="40">
+        <v>18</v>
+      </c>
+      <c r="D87" s="40">
+        <v>7</v>
+      </c>
+      <c r="E87" s="40">
+        <f>C87+2*D87</f>
+        <v>32</v>
+      </c>
       <c r="F87" s="40"/>
       <c r="G87" s="40"/>
       <c r="H87" s="40"/>
@@ -7059,66 +6928,59 @@
     </row>
     <row r="88" spans="2:11">
       <c r="B88" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="C88" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="D88" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="E88" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="F88" s="40" t="s">
-        <v>210</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C88" s="40">
+        <v>21</v>
+      </c>
+      <c r="D88" s="40">
+        <v>5</v>
+      </c>
+      <c r="E88" s="40">
+        <f t="shared" ref="E88:E94" si="2">C88+2*D88</f>
+        <v>31</v>
+      </c>
+      <c r="F88" s="40"/>
       <c r="H88" s="40"/>
       <c r="I88" s="40"/>
       <c r="J88" s="40"/>
       <c r="K88" s="40"/>
     </row>
     <row r="89" spans="2:11">
-      <c r="B89" s="40">
-        <v>10</v>
+      <c r="B89" s="40" t="s">
+        <v>193</v>
       </c>
       <c r="C89" s="40">
-        <v>200</v>
+        <v>22</v>
       </c>
       <c r="D89" s="40">
-        <v>2000</v>
+        <v>5</v>
       </c>
       <c r="E89" s="40">
-        <f>12*200+936+70</f>
-        <v>3406</v>
-      </c>
-      <c r="F89" s="40">
-        <f>(55+130)*4+12*200*1.2*1.05</f>
-        <v>3764</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F89" s="40"/>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
       <c r="J89" s="40"/>
       <c r="K89" s="40"/>
     </row>
     <row r="90" spans="2:11">
-      <c r="B90" s="40">
-        <v>10</v>
-      </c>
-      <c r="C90" s="40">
-        <v>200</v>
+      <c r="B90" s="107" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" s="107">
+        <v>16</v>
       </c>
       <c r="D90" s="40">
-        <v>3000</v>
+        <v>8</v>
       </c>
       <c r="E90" s="40">
-        <f>12*200+936*1.5+70</f>
-        <v>3874</v>
-      </c>
-      <c r="F90" s="40">
-        <f>(55+130)*4+12*200*1.2*1.05</f>
-        <v>3764</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F90" s="40"/>
       <c r="G90" s="40"/>
       <c r="H90" s="40"/>
       <c r="I90" s="40"/>
@@ -7126,10 +6988,19 @@
       <c r="K90" s="40"/>
     </row>
     <row r="91" spans="2:11">
-      <c r="B91" s="40"/>
-      <c r="C91" s="40"/>
-      <c r="D91" s="40"/>
-      <c r="E91" s="40"/>
+      <c r="B91" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="C91" s="40">
+        <v>14</v>
+      </c>
+      <c r="D91" s="40">
+        <v>9</v>
+      </c>
+      <c r="E91" s="40">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="F91" s="40"/>
       <c r="G91" s="40"/>
       <c r="H91" s="40"/>
@@ -7138,10 +7009,19 @@
       <c r="K91" s="40"/>
     </row>
     <row r="92" spans="2:11">
-      <c r="B92" s="40"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
+      <c r="B92" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" s="40">
+        <v>20</v>
+      </c>
+      <c r="D92" s="40">
+        <v>6</v>
+      </c>
+      <c r="E92" s="40">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="F92" s="40"/>
       <c r="G92" s="40"/>
       <c r="H92" s="40"/>
@@ -7150,10 +7030,19 @@
       <c r="K92" s="40"/>
     </row>
     <row r="93" spans="2:11">
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="40"/>
+      <c r="B93" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C93" s="40">
+        <v>17</v>
+      </c>
+      <c r="D93" s="40">
+        <v>4</v>
+      </c>
+      <c r="E93" s="40">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="F93" s="40"/>
       <c r="G93" s="40"/>
       <c r="H93" s="40"/>
@@ -7162,11 +7051,20 @@
       <c r="K93" s="40"/>
     </row>
     <row r="94" spans="2:11">
-      <c r="B94" s="40"/>
-      <c r="C94" s="40"/>
-      <c r="D94" s="40"/>
-      <c r="E94" s="40"/>
-      <c r="F94" s="103"/>
+      <c r="B94" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" s="40">
+        <v>26</v>
+      </c>
+      <c r="D94" s="40">
+        <v>3</v>
+      </c>
+      <c r="E94" s="40">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F94" s="100"/>
       <c r="G94" s="40"/>
       <c r="H94" s="40"/>
       <c r="I94" s="40"/>
@@ -7197,7 +7095,7 @@
       <c r="C97" s="40"/>
       <c r="D97" s="40"/>
       <c r="E97" s="40"/>
-      <c r="F97" s="103"/>
+      <c r="F97" s="100"/>
       <c r="G97" s="40"/>
       <c r="H97" s="40"/>
       <c r="I97" s="40"/>
@@ -7242,7 +7140,7 @@
       <c r="C102" s="40"/>
       <c r="D102" s="40"/>
       <c r="E102" s="40"/>
-      <c r="F102" s="111"/>
+      <c r="F102" s="109"/>
     </row>
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
@@ -7299,7 +7197,7 @@
       <c r="F111" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="M3:N3"/>
@@ -7315,7 +7213,6 @@
     <mergeCell ref="K74:L74"/>
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="D84:G84"/>
-    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -7347,31 +7244,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7379,28 +7276,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7408,28 +7305,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7437,28 +7334,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7466,28 +7363,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7495,28 +7392,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7524,28 +7421,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7553,28 +7450,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7582,28 +7479,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7611,28 +7508,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7640,28 +7537,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7669,28 +7566,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7698,28 +7595,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7727,33 +7624,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>298</v>
-      </c>
       <c r="I14" s="6" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7785,34 +7682,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7820,31 +7717,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7852,31 +7749,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7884,31 +7781,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7916,31 +7813,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7948,31 +7845,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7980,31 +7877,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8012,31 +7909,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8044,31 +7941,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8076,31 +7973,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8108,31 +8005,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8140,31 +8037,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8172,31 +8069,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8204,63 +8101,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on Rogue rework
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180" activeTab="1"/>
+    <workbookView windowWidth="13545" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="407">
   <si>
     <t>1-Handed (base) (5.5 base + 3 stat = 8.5) (8.5 - 4 AC)*2 hands = 9</t>
   </si>
@@ -1033,18 +1033,71 @@
     <t>Feared</t>
   </si>
   <si>
-    <t>New Health</t>
-  </si>
-  <si>
-    <t>4 (2d4 - 1)</t>
-  </si>
-  <si>
-    <t>5 (1d8)</t>
-  </si>
-  <si>
-    <t>The double of another column
-should be 120% of that column
-E.g. 400XP HP = 1.2 * 2 * 200XP HP</t>
+    <t>18.5 (avg) + 3 (avg)</t>
+  </si>
+  <si>
+    <t>Health Regen (6 + 1 + 2*Level)</t>
+  </si>
+  <si>
+    <t>TODO: Setup some good</t>
+  </si>
+  <si>
+    <t>baseline damage for mobs</t>
+  </si>
+  <si>
+    <t>at e.g. 200, 300, etc</t>
+  </si>
+  <si>
+    <t>Go from there.</t>
+  </si>
+  <si>
+    <t>Calculate 80 or 85% like</t>
+  </si>
+  <si>
+    <t>normal epic monsters.</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Base Health</t>
+  </si>
+  <si>
+    <t>Health Regen</t>
+  </si>
+  <si>
+    <t>Total Health Per Adventure</t>
+  </si>
+  <si>
+    <t>Bertle</t>
+  </si>
+  <si>
+    <t>Davel</t>
+  </si>
+  <si>
+    <t>Dragonborn</t>
+  </si>
+  <si>
+    <t>Dwarf</t>
+  </si>
+  <si>
+    <t>Elf</t>
+  </si>
+  <si>
+    <t>Gnome</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Hollow</t>
+  </si>
+  <si>
+    <t>Orc</t>
+  </si>
+  <si>
+    <t>The double of another column should be 100% of that column
+E.g. 400XP HP = 1.0 * 2 * 200XP HP</t>
   </si>
   <si>
     <t>Epic HP multpliers are:
@@ -1059,40 +1112,48 @@
 E.g. 400XP dmg = 0.85 * 2 * 200XP dmg</t>
   </si>
   <si>
-    <t>18.5 + Might + Other</t>
-  </si>
-  <si>
-    <t>Reserve HP</t>
-  </si>
-  <si>
-    <t>Health Regen (6 - 2 + 2*Level)</t>
-  </si>
-  <si>
-    <t>Bertle</t>
-  </si>
-  <si>
-    <t>Davel</t>
-  </si>
-  <si>
-    <t>Dragonborn</t>
-  </si>
-  <si>
-    <t>Dwarf</t>
-  </si>
-  <si>
-    <t>Elf</t>
-  </si>
-  <si>
-    <t>Gnome</t>
-  </si>
-  <si>
-    <t>Hollow</t>
-  </si>
-  <si>
-    <t>Human</t>
-  </si>
-  <si>
-    <t>Orc</t>
+    <t>Players total XP</t>
+  </si>
+  <si>
+    <t>Monsters XP</t>
+  </si>
+  <si>
+    <t>(PREVIOUSLY) The double of another column
+should be 120% of that column
+E.g. 400XP HP = 1.2 * 2 * 200XP HP</t>
+  </si>
+  <si>
+    <t>900 (6 players)</t>
+  </si>
+  <si>
+    <t>800 (Koblods + Rats)</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>775 (Oni + 3 Sk)</t>
+  </si>
+  <si>
+    <t>900 (Goblins + Stg)</t>
+  </si>
+  <si>
+    <t>Easy-Medium</t>
+  </si>
+  <si>
+    <t>750 (5 players)</t>
+  </si>
+  <si>
+    <t>950 (Gnawls)</t>
+  </si>
+  <si>
+    <t>825 (5 or 6 players)</t>
+  </si>
+  <si>
+    <t>1125 (Lich + 3 Sk)</t>
+  </si>
+  <si>
+    <t>Hard</t>
   </si>
   <si>
     <t>1-Handed (+3)</t>
@@ -2624,7 +2685,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2913,6 +2974,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2925,12 +3004,42 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2949,8 +3058,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3335,7 +3444,7 @@
   <dimension ref="A2:N112"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -3440,7 +3549,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="102" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3456,10 +3565,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="96" t="s">
+      <c r="L8" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="96"/>
+      <c r="M8" s="102"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3492,13 +3601,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="135" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="136" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3510,7 +3619,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="120" t="s">
+      <c r="G10" s="136" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3521,13 +3630,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="135" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="136" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3539,7 +3648,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="120" t="s">
+      <c r="G11" s="136" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3550,13 +3659,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="137" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="138" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3568,7 +3677,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="122" t="s">
+      <c r="G12" s="138" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3853,8 +3962,8 @@
       <c r="H27" s="81"/>
       <c r="I27" s="81"/>
       <c r="J27" s="82"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="104"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3863,10 +3972,10 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="111" t="s">
+      <c r="C28" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="112"/>
+      <c r="D28" s="128"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -3967,7 +4076,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="118"/>
+      <c r="J32" s="134"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -4002,20 +4111,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="113" t="s">
+      <c r="A34" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="114">
+      <c r="B34" s="130">
         <v>1</v>
       </c>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="114"/>
+      <c r="C34" s="131"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="131"/>
+      <c r="F34" s="131"/>
+      <c r="G34" s="131"/>
+      <c r="H34" s="131"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="130"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -4114,17 +4223,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="116" t="s">
+      <c r="F40" s="132" t="s">
         <v>87</v>
       </c>
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="123" t="s">
+      <c r="I40" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="99"/>
-      <c r="K40" s="99"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="105"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4146,7 +4255,7 @@
       <c r="G41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="124" t="s">
+      <c r="I41" s="140" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4619,11 +4728,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="117" t="s">
+      <c r="C62" s="133" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="117" t="s">
+      <c r="F62" s="133" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4642,7 +4751,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="102" t="s">
+      <c r="E64" s="118" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4689,7 +4798,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="117" t="s">
+      <c r="C70" s="133" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4706,10 +4815,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="103"/>
-      <c r="B72" s="104"/>
-      <c r="C72" s="105"/>
-      <c r="D72" s="105"/>
+      <c r="A72" s="119"/>
+      <c r="B72" s="120"/>
+      <c r="C72" s="121"/>
+      <c r="D72" s="121"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4814,7 +4923,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="125" t="s">
+      <c r="D77" s="141" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4832,7 +4941,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="103"/>
+      <c r="A78" s="119"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4842,16 +4951,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="110"/>
+      <c r="E78" s="126"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="110"/>
-      <c r="H78" s="110"/>
-      <c r="I78" s="110"/>
-      <c r="J78" s="110"/>
-      <c r="K78" s="110"/>
-      <c r="L78" s="110"/>
+      <c r="G78" s="126"/>
+      <c r="H78" s="126"/>
+      <c r="I78" s="126"/>
+      <c r="J78" s="126"/>
+      <c r="K78" s="126"/>
+      <c r="L78" s="126"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -4908,7 +5017,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="125" t="s">
+      <c r="D81" s="141" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5181,8 +5290,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="109"/>
-      <c r="F103" s="109"/>
+      <c r="E103" s="125"/>
+      <c r="F103" s="125"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5266,21 +5375,22 @@
   <sheetPr/>
   <dimension ref="A2:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.7333333333333" customWidth="1"/>
+    <col min="1" max="1" width="17.2571428571429" customWidth="1"/>
     <col min="2" max="2" width="19.7333333333333" customWidth="1"/>
     <col min="3" max="3" width="24.4761904761905" customWidth="1"/>
-    <col min="4" max="4" width="25.9428571428571" customWidth="1"/>
+    <col min="4" max="4" width="26.8285714285714" customWidth="1"/>
     <col min="5" max="5" width="30.7904761904762" customWidth="1"/>
-    <col min="6" max="6" width="33.8952380952381" customWidth="1"/>
+    <col min="6" max="6" width="24.5809523809524" customWidth="1"/>
     <col min="7" max="7" width="27.9428571428571" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="10" width="17.4190476190476" customWidth="1"/>
+    <col min="9" max="9" width="25.952380952381" customWidth="1"/>
+    <col min="10" max="10" width="23.7238095238095" customWidth="1"/>
     <col min="11" max="11" width="17.152380952381" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
     <col min="13" max="13" width="14.152380952381" customWidth="1"/>
@@ -5372,7 +5482,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="102" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5388,10 +5498,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="96" t="s">
+      <c r="L8" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="96"/>
+      <c r="M8" s="102"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5424,13 +5534,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="135" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="136" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5442,7 +5552,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="120" t="s">
+      <c r="G10" s="136" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5453,13 +5563,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="135" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="136" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5471,7 +5581,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="120" t="s">
+      <c r="G11" s="136" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5482,13 +5592,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="137" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="138" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5500,7 +5610,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="122" t="s">
+      <c r="G12" s="138" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5599,10 +5709,7 @@
       <c r="F18" s="55">
         <v>-1</v>
       </c>
-      <c r="H18" s="57">
-        <f>6.5*2</f>
-        <v>13</v>
-      </c>
+      <c r="H18" s="57"/>
       <c r="K18" s="70">
         <v>4</v>
       </c>
@@ -5626,10 +5733,7 @@
       <c r="F19" s="55">
         <v>-2</v>
       </c>
-      <c r="H19" s="58">
-        <f>(14-5)*2</f>
-        <v>18</v>
-      </c>
+      <c r="H19" s="58"/>
       <c r="K19" s="70">
         <v>5</v>
       </c>
@@ -5653,7 +5757,14 @@
       <c r="F20" s="63">
         <v>-1</v>
       </c>
-      <c r="H20" s="57"/>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20" s="57">
+        <f>6.5+4</f>
+        <v>10.5</v>
+      </c>
+      <c r="J20" s="73"/>
       <c r="K20" s="70">
         <v>6</v>
       </c>
@@ -5767,7 +5878,7 @@
       <c r="H25" s="40"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
-      <c r="K25" s="97">
+      <c r="K25" s="103">
         <f>46/9</f>
         <v>5.11111111111111</v>
       </c>
@@ -5796,8 +5907,8 @@
       <c r="D27" s="81"/>
       <c r="E27" s="81"/>
       <c r="F27" s="82"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="104"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -5952,7 +6063,7 @@
       <c r="J37" s="40"/>
       <c r="K37" s="58"/>
     </row>
-    <row r="38" ht="16.5" spans="1:11">
+    <row r="38" ht="16.5" spans="1:12">
       <c r="A38" s="58"/>
       <c r="C38" s="67" t="s">
         <v>82</v>
@@ -5960,10 +6071,17 @@
       <c r="D38" s="89"/>
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
+      <c r="H38" s="72"/>
       <c r="I38" s="58"/>
       <c r="J38" s="40"/>
-      <c r="K38" s="58"/>
+      <c r="K38" s="58">
+        <f>550+225</f>
+        <v>775</v>
+      </c>
+      <c r="L38">
+        <f>150*5+200</f>
+        <v>950</v>
+      </c>
     </row>
     <row r="39" ht="15.75" spans="1:11">
       <c r="A39" s="72"/>
@@ -5974,17 +6092,18 @@
         <v>84</v>
       </c>
       <c r="D39" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="89" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="99"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="99"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="105"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
       <c r="A40" s="72"/>
@@ -5995,17 +6114,20 @@
         <v>7</v>
       </c>
       <c r="D40" s="40">
-        <f>FLOOR(C40*1.32,1)</f>
-        <v>9</v>
-      </c>
-      <c r="E40" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" s="93">
+        <v>1.5</v>
+      </c>
+      <c r="E40" s="93">
         <v>10</v>
       </c>
-      <c r="I40" s="58"/>
-      <c r="J40" s="40"/>
+      <c r="G40" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="H40" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" s="50" t="s">
+        <v>182</v>
+      </c>
       <c r="K40" s="58"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
@@ -6017,17 +6139,20 @@
         <v>14</v>
       </c>
       <c r="D41" s="40">
-        <f>FLOOR(C41*1.32,1)</f>
-        <v>18</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="F41" s="93">
+        <v>2.5</v>
+      </c>
+      <c r="E41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="58"/>
-      <c r="J41" s="40"/>
+      <c r="G41" s="39">
+        <v>1</v>
+      </c>
+      <c r="H41" s="55">
+        <v>21.5</v>
+      </c>
+      <c r="I41" s="55">
+        <v>7</v>
+      </c>
       <c r="K41" s="58"/>
     </row>
     <row r="42" ht="15.75" spans="1:11">
@@ -6036,20 +6161,23 @@
         <v>75</v>
       </c>
       <c r="C42" s="40">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D42" s="40">
-        <f t="shared" ref="D42:D60" si="0">FLOOR(C42*1.32,1)</f>
-        <v>27</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="93">
+        <v>3.5</v>
+      </c>
+      <c r="E42" s="93">
         <v>10</v>
       </c>
-      <c r="I42" s="58"/>
-      <c r="J42" s="40"/>
+      <c r="G42" s="39">
+        <v>2</v>
+      </c>
+      <c r="H42" s="55">
+        <v>25.5</v>
+      </c>
+      <c r="I42" s="55">
+        <v>9</v>
+      </c>
       <c r="K42" s="58"/>
     </row>
     <row r="43" ht="15.75" spans="1:11">
@@ -6060,20 +6188,23 @@
         <v>100</v>
       </c>
       <c r="C43" s="40">
-        <v>28</v>
-      </c>
-      <c r="D43" s="40">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E43" s="58" t="s">
-        <v>182</v>
-      </c>
-      <c r="F43" s="93">
+        <v>25</v>
+      </c>
+      <c r="D43" s="58">
+        <v>5</v>
+      </c>
+      <c r="E43" s="93">
         <v>10</v>
       </c>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="G43" s="39">
+        <v>3</v>
+      </c>
+      <c r="H43" s="55">
+        <v>29.5</v>
+      </c>
+      <c r="I43" s="55">
+        <v>11</v>
+      </c>
       <c r="K43" s="58"/>
     </row>
     <row r="44" ht="15.75" spans="1:11">
@@ -6084,20 +6215,23 @@
         <v>125</v>
       </c>
       <c r="C44" s="40">
-        <v>37</v>
-      </c>
-      <c r="D44" s="40">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="E44" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="F44" s="93">
+        <v>30</v>
+      </c>
+      <c r="D44" s="58">
+        <v>6.5</v>
+      </c>
+      <c r="E44" s="93">
         <v>10</v>
       </c>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="G44" s="39">
+        <v>4</v>
+      </c>
+      <c r="H44" s="55">
+        <v>33.5</v>
+      </c>
+      <c r="I44" s="55">
+        <v>13</v>
+      </c>
       <c r="K44" s="58"/>
     </row>
     <row r="45" ht="15.75" spans="1:11">
@@ -6108,20 +6242,23 @@
         <v>150</v>
       </c>
       <c r="C45" s="40">
-        <v>46</v>
-      </c>
-      <c r="D45" s="40">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="F45" s="93">
+        <v>35</v>
+      </c>
+      <c r="D45" s="58">
+        <v>7.5</v>
+      </c>
+      <c r="E45" s="93">
         <v>10</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="G45" s="39">
+        <v>5</v>
+      </c>
+      <c r="H45" s="55">
+        <v>37.5</v>
+      </c>
+      <c r="I45" s="55">
+        <v>15</v>
+      </c>
       <c r="K45" s="58"/>
     </row>
     <row r="46" ht="15.75" spans="1:11">
@@ -6132,20 +6269,26 @@
         <v>175</v>
       </c>
       <c r="C46" s="40">
-        <v>55</v>
-      </c>
-      <c r="D46" s="40">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="E46" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="93">
+        <v>40</v>
+      </c>
+      <c r="D46" s="58">
+        <v>8.5</v>
+      </c>
+      <c r="E46" s="93">
         <v>10</v>
       </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
+      <c r="F46" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" s="39">
+        <v>6</v>
+      </c>
+      <c r="H46" s="55">
+        <v>41.5</v>
+      </c>
+      <c r="I46" s="55">
+        <v>17</v>
+      </c>
       <c r="K46" s="58"/>
     </row>
     <row r="47" ht="15.75" spans="2:11">
@@ -6153,20 +6296,26 @@
         <v>200</v>
       </c>
       <c r="C47" s="40">
-        <v>65</v>
-      </c>
-      <c r="D47" s="40">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="93">
+        <v>45</v>
+      </c>
+      <c r="D47" s="58">
+        <v>9.5</v>
+      </c>
+      <c r="E47" s="93">
         <v>11</v>
       </c>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
+      <c r="F47" t="s">
+        <v>184</v>
+      </c>
+      <c r="G47" s="39">
+        <v>7</v>
+      </c>
+      <c r="H47" s="55">
+        <v>45.5</v>
+      </c>
+      <c r="I47" s="55">
+        <v>19</v>
+      </c>
       <c r="K47" s="58"/>
     </row>
     <row r="48" ht="15.75" spans="1:11">
@@ -6177,20 +6326,26 @@
         <v>225</v>
       </c>
       <c r="C48" s="40">
-        <v>75</v>
-      </c>
-      <c r="D48" s="40">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="E48" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="F48" s="93">
+        <v>50</v>
+      </c>
+      <c r="D48" s="58">
+        <v>10.5</v>
+      </c>
+      <c r="E48" s="93">
         <v>11</v>
       </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
+      <c r="F48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G48" s="39">
+        <v>8</v>
+      </c>
+      <c r="H48" s="55">
+        <v>49.5</v>
+      </c>
+      <c r="I48" s="55">
+        <v>21</v>
+      </c>
       <c r="K48" s="58"/>
     </row>
     <row r="49" ht="15.75" spans="1:11">
@@ -6201,20 +6356,26 @@
         <v>250</v>
       </c>
       <c r="C49" s="40">
-        <v>91</v>
-      </c>
-      <c r="D49" s="40">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="E49" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="F49" s="93">
+        <v>55</v>
+      </c>
+      <c r="D49" s="58">
+        <v>11.5</v>
+      </c>
+      <c r="E49" s="93">
         <v>11</v>
       </c>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
+      <c r="F49" t="s">
+        <v>186</v>
+      </c>
+      <c r="G49" s="39">
+        <v>9</v>
+      </c>
+      <c r="H49" s="55">
+        <v>53.5</v>
+      </c>
+      <c r="I49" s="55">
+        <v>23</v>
+      </c>
       <c r="K49" s="58"/>
     </row>
     <row r="50" ht="15.75" spans="2:11">
@@ -6222,20 +6383,26 @@
         <v>275</v>
       </c>
       <c r="C50" s="40">
-        <v>102</v>
-      </c>
-      <c r="D50" s="40">
-        <f t="shared" si="0"/>
-        <v>134</v>
-      </c>
-      <c r="E50" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F50" s="93">
+        <v>60</v>
+      </c>
+      <c r="D50" s="58">
+        <v>12.5</v>
+      </c>
+      <c r="E50" s="93">
         <v>11</v>
       </c>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
+      <c r="F50" t="s">
+        <v>187</v>
+      </c>
+      <c r="G50" s="44">
+        <v>10</v>
+      </c>
+      <c r="H50" s="43">
+        <v>57.5</v>
+      </c>
+      <c r="I50" s="43">
+        <v>25</v>
+      </c>
       <c r="K50" s="58"/>
     </row>
     <row r="51" ht="15.75" spans="1:13">
@@ -6246,20 +6413,21 @@
         <v>300</v>
       </c>
       <c r="C51" s="40">
-        <v>112</v>
-      </c>
-      <c r="D51" s="40">
-        <f t="shared" si="0"/>
-        <v>147</v>
-      </c>
-      <c r="E51" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="F51" s="41">
+        <v>65</v>
+      </c>
+      <c r="D51" s="58">
+        <v>13.5</v>
+      </c>
+      <c r="E51" s="41">
         <v>12</v>
       </c>
-      <c r="I51" s="58"/>
-      <c r="J51" s="70"/>
+      <c r="F51" t="s">
+        <v>188</v>
+      </c>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="106"/>
+      <c r="J51" s="106"/>
       <c r="K51" s="70"/>
       <c r="M51" s="58"/>
     </row>
@@ -6270,20 +6438,27 @@
       <c r="B52" s="95">
         <v>325</v>
       </c>
-      <c r="C52" s="95">
-        <v>120</v>
-      </c>
-      <c r="D52" s="95">
-        <f t="shared" si="0"/>
-        <v>158</v>
-      </c>
-      <c r="E52" s="95" t="s">
-        <v>121</v>
-      </c>
-      <c r="F52" s="41">
+      <c r="C52" s="40">
+        <v>70</v>
+      </c>
+      <c r="D52" s="58">
+        <v>14.5</v>
+      </c>
+      <c r="E52" s="41">
         <v>12</v>
       </c>
-      <c r="I52" s="40"/>
+      <c r="G52" s="96" t="s">
+        <v>189</v>
+      </c>
+      <c r="H52" s="96" t="s">
+        <v>190</v>
+      </c>
+      <c r="I52" s="107" t="s">
+        <v>191</v>
+      </c>
+      <c r="J52" s="108" t="s">
+        <v>192</v>
+      </c>
       <c r="M52" s="58"/>
     </row>
     <row r="53" ht="15.75" spans="1:13">
@@ -6294,171 +6469,243 @@
         <v>350</v>
       </c>
       <c r="C53" s="40">
-        <v>130</v>
-      </c>
-      <c r="D53" s="40">
-        <f t="shared" si="0"/>
-        <v>171</v>
-      </c>
-      <c r="E53" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="41">
+        <v>75</v>
+      </c>
+      <c r="D53" s="58">
+        <v>15.5</v>
+      </c>
+      <c r="E53" s="41">
         <v>12</v>
       </c>
-      <c r="I53" s="40"/>
+      <c r="G53" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="H53" s="97">
+        <v>16</v>
+      </c>
+      <c r="I53" s="109">
+        <v>8</v>
+      </c>
+      <c r="J53" s="110">
+        <f>H53+2*I53</f>
+        <v>32</v>
+      </c>
       <c r="M53" s="58"/>
     </row>
-    <row r="54" ht="16.5" spans="1:9">
+    <row r="54" ht="16.5" spans="1:10">
       <c r="A54" s="72" t="s">
         <v>123</v>
       </c>
       <c r="B54" s="65">
         <v>375</v>
       </c>
-      <c r="C54" s="45">
-        <v>140</v>
+      <c r="C54" s="98">
+        <v>80</v>
       </c>
       <c r="D54" s="45">
-        <f t="shared" si="0"/>
-        <v>184</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="F54" s="46">
+        <v>10.5</v>
+      </c>
+      <c r="E54" s="46">
         <v>12</v>
       </c>
-      <c r="I54" s="40"/>
-    </row>
-    <row r="55" spans="2:9">
+      <c r="G54" s="99" t="s">
+        <v>194</v>
+      </c>
+      <c r="H54" s="99">
+        <v>18</v>
+      </c>
+      <c r="I54" s="111">
+        <v>7</v>
+      </c>
+      <c r="J54" s="112">
+        <f>H54+2*I54</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
       <c r="B55" s="39">
         <v>400</v>
       </c>
       <c r="C55" s="40">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="D55" s="40">
-        <f t="shared" si="0"/>
-        <v>194</v>
-      </c>
-      <c r="E55" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="F55" s="41">
+        <v>11</v>
+      </c>
+      <c r="E55" s="41">
         <v>12</v>
       </c>
-      <c r="I55" s="40"/>
-    </row>
-    <row r="56" spans="2:9">
+      <c r="G55" s="99" t="s">
+        <v>195</v>
+      </c>
+      <c r="H55" s="99">
+        <v>21</v>
+      </c>
+      <c r="I55" s="111">
+        <v>5</v>
+      </c>
+      <c r="J55" s="112">
+        <f t="shared" ref="J55:J61" si="0">H55+2*I55</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
       <c r="B56" s="39">
         <v>425</v>
       </c>
       <c r="C56" s="40">
-        <v>165</v>
-      </c>
-      <c r="D56" s="40">
+        <v>90</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="41">
+        <v>12</v>
+      </c>
+      <c r="G56" s="99" t="s">
+        <v>196</v>
+      </c>
+      <c r="H56" s="99">
+        <v>22</v>
+      </c>
+      <c r="I56" s="111">
+        <v>5</v>
+      </c>
+      <c r="J56" s="112">
         <f t="shared" si="0"/>
-        <v>217</v>
-      </c>
-      <c r="E56" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="F56" s="41">
-        <v>12</v>
-      </c>
-      <c r="I56" s="40"/>
-    </row>
-    <row r="57" spans="2:9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
       <c r="B57" s="39">
         <v>450</v>
       </c>
       <c r="C57" s="40">
-        <v>182</v>
-      </c>
-      <c r="D57" s="40">
+        <v>95</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E57" s="41">
+        <v>12</v>
+      </c>
+      <c r="G57" s="100" t="s">
+        <v>197</v>
+      </c>
+      <c r="H57" s="100">
+        <v>16</v>
+      </c>
+      <c r="I57" s="111">
+        <v>8</v>
+      </c>
+      <c r="J57" s="112">
         <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="E57" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="F57" s="41">
-        <v>12</v>
-      </c>
-      <c r="I57" s="40"/>
-    </row>
-    <row r="58" spans="2:9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
       <c r="B58" s="39">
         <v>475</v>
       </c>
       <c r="C58" s="40">
-        <v>200</v>
-      </c>
-      <c r="D58" s="40">
+        <v>100</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="41">
+        <v>12</v>
+      </c>
+      <c r="G58" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="H58" s="99">
+        <v>14</v>
+      </c>
+      <c r="I58" s="111">
+        <v>9</v>
+      </c>
+      <c r="J58" s="112">
         <f t="shared" si="0"/>
-        <v>264</v>
-      </c>
-      <c r="E58" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="F58" s="41">
-        <v>12</v>
-      </c>
-      <c r="I58" s="40"/>
-    </row>
-    <row r="59" ht="15.75" spans="2:9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" spans="2:10">
       <c r="B59" s="52">
         <v>500</v>
       </c>
-      <c r="C59" s="95">
-        <v>218</v>
-      </c>
-      <c r="D59" s="95">
+      <c r="C59" s="40">
+        <v>105</v>
+      </c>
+      <c r="D59" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="41">
+        <v>12</v>
+      </c>
+      <c r="G59" s="99" t="s">
+        <v>199</v>
+      </c>
+      <c r="H59" s="99">
+        <v>20</v>
+      </c>
+      <c r="I59" s="111">
+        <v>6</v>
+      </c>
+      <c r="J59" s="112">
         <f t="shared" si="0"/>
-        <v>287</v>
-      </c>
-      <c r="E59" s="95" t="s">
-        <v>136</v>
-      </c>
-      <c r="F59" s="41">
-        <v>12</v>
-      </c>
-      <c r="I59" s="40"/>
-    </row>
-    <row r="60" ht="15.75" spans="2:9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" spans="2:10">
       <c r="B60" s="52">
         <v>600</v>
       </c>
       <c r="C60" s="95"/>
       <c r="D60" s="95">
-        <v>350</v>
-      </c>
-      <c r="E60" s="95">
         <v>14.5</v>
       </c>
-      <c r="F60" s="41">
+      <c r="E60" s="41">
         <v>13</v>
       </c>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-    </row>
-    <row r="61" ht="15.75" spans="2:9">
+      <c r="G60" s="99" t="s">
+        <v>200</v>
+      </c>
+      <c r="H60" s="99">
+        <v>17</v>
+      </c>
+      <c r="I60" s="111">
+        <v>4</v>
+      </c>
+      <c r="J60" s="112">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" spans="2:10">
       <c r="B61" s="52">
         <v>750</v>
       </c>
       <c r="C61" s="95"/>
       <c r="D61" s="95">
-        <v>441</v>
-      </c>
-      <c r="E61" s="95">
-        <v>17.25</v>
-      </c>
-      <c r="F61" s="41">
+        <v>15</v>
+      </c>
+      <c r="E61" s="41">
         <v>13</v>
       </c>
-      <c r="H61" s="40"/>
-      <c r="I61" s="100"/>
+      <c r="G61" s="101" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="101">
+        <v>26</v>
+      </c>
+      <c r="I61" s="113">
+        <v>3</v>
+      </c>
+      <c r="J61" s="114">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="62" ht="16.5" spans="2:9">
       <c r="B62" s="65">
@@ -6466,12 +6713,9 @@
       </c>
       <c r="C62" s="45"/>
       <c r="D62" s="45">
-        <v>688</v>
-      </c>
-      <c r="E62" s="45">
-        <v>21.5</v>
-      </c>
-      <c r="F62" s="46">
+        <v>15.5</v>
+      </c>
+      <c r="E62" s="46">
         <v>13</v>
       </c>
       <c r="H62" s="40"/>
@@ -6487,68 +6731,108 @@
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
     </row>
-    <row r="65" ht="90.75" spans="1:9">
+    <row r="65" ht="75.75" spans="1:10">
       <c r="A65">
         <f>147*2*0.8</f>
         <v>235.2</v>
       </c>
-      <c r="C65" s="101" t="s">
-        <v>184</v>
-      </c>
-      <c r="D65" s="101" t="s">
-        <v>185</v>
-      </c>
-      <c r="E65" s="101" t="s">
-        <v>186</v>
-      </c>
-      <c r="G65" s="40">
-        <f>350*4*0.8</f>
-        <v>1120</v>
-      </c>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-    </row>
-    <row r="66" spans="5:9">
+      <c r="C65" s="115" t="s">
+        <v>202</v>
+      </c>
+      <c r="D65" s="115" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" s="115" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" s="40"/>
+      <c r="H65" s="116" t="s">
+        <v>205</v>
+      </c>
+      <c r="I65" t="s">
+        <v>206</v>
+      </c>
+      <c r="J65" s="58"/>
+    </row>
+    <row r="66" ht="90.75" spans="3:10">
+      <c r="C66" s="115" t="s">
+        <v>207</v>
+      </c>
       <c r="E66" s="40"/>
       <c r="F66" s="40"/>
       <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
-    </row>
-    <row r="67" spans="5:9">
-      <c r="E67" s="102"/>
+      <c r="H66" s="117" t="s">
+        <v>208</v>
+      </c>
+      <c r="I66" t="s">
+        <v>209</v>
+      </c>
+      <c r="J66" s="40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10">
+      <c r="E67" s="118"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
-    </row>
-    <row r="68" spans="3:9">
+      <c r="H67" s="117" t="s">
+        <v>208</v>
+      </c>
+      <c r="I67" t="s">
+        <v>211</v>
+      </c>
+      <c r="J67" s="40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10">
       <c r="C68" s="40"/>
       <c r="E68" s="40"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
-      <c r="I68" s="40"/>
-    </row>
-    <row r="69" ht="13" customHeight="1" spans="5:9">
+      <c r="H68" s="117" t="s">
+        <v>208</v>
+      </c>
+      <c r="I68" t="s">
+        <v>212</v>
+      </c>
+      <c r="J68" s="40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" ht="13" customHeight="1" spans="5:10">
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
       <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
-    </row>
-    <row r="70" spans="5:9">
+      <c r="H69" s="117" t="s">
+        <v>214</v>
+      </c>
+      <c r="I69" s="125" t="s">
+        <v>215</v>
+      </c>
+      <c r="J69" s="40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10">
       <c r="E70" s="40"/>
       <c r="F70" s="40"/>
       <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
+      <c r="H70" s="117" t="s">
+        <v>216</v>
+      </c>
+      <c r="I70" s="125" t="s">
+        <v>217</v>
+      </c>
+      <c r="J70" s="40" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="71" ht="15.75" spans="1:14">
-      <c r="A71" s="103"/>
-      <c r="B71" s="104"/>
-      <c r="C71" s="105"/>
-      <c r="D71" s="105"/>
+      <c r="A71" s="119"/>
+      <c r="B71" s="120"/>
+      <c r="C71" s="121"/>
+      <c r="D71" s="121"/>
       <c r="E71" s="58"/>
       <c r="F71" s="58"/>
       <c r="G71" s="58"/>
@@ -6561,12 +6845,6 @@
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="40"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
       <c r="F72" s="40"/>
       <c r="G72" s="40"/>
       <c r="H72" s="40"/>
@@ -6578,24 +6856,12 @@
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="40"/>
-      <c r="B73" s="74" t="s">
-        <v>144</v>
-      </c>
-      <c r="C73" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="D73" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="E73" s="50" t="s">
-        <v>189</v>
-      </c>
       <c r="F73" s="40"/>
-      <c r="G73" s="106" t="s">
-        <v>190</v>
-      </c>
-      <c r="H73" s="106"/>
-      <c r="I73" s="106"/>
+      <c r="G73" s="122" t="s">
+        <v>193</v>
+      </c>
+      <c r="H73" s="122"/>
+      <c r="I73" s="122"/>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
       <c r="M73" s="40"/>
@@ -6603,21 +6869,9 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="40"/>
-      <c r="B74" s="39">
-        <v>1</v>
-      </c>
-      <c r="C74" s="55">
-        <v>22</v>
-      </c>
-      <c r="D74" s="55">
-        <v>10</v>
-      </c>
-      <c r="E74" s="55">
-        <v>6</v>
-      </c>
       <c r="F74" s="40"/>
       <c r="G74" s="40" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H74" s="40"/>
       <c r="I74" s="40"/>
@@ -6629,22 +6883,9 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="40"/>
-      <c r="B75" s="39">
-        <v>2</v>
-      </c>
-      <c r="C75" s="55">
-        <v>27</v>
-      </c>
-      <c r="D75" s="55">
-        <f>FLOOR(C75/2,1)</f>
-        <v>13</v>
-      </c>
-      <c r="E75" s="55">
-        <v>8</v>
-      </c>
       <c r="F75" s="40"/>
       <c r="G75" s="40" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H75" s="40"/>
       <c r="I75" s="40"/>
@@ -6656,22 +6897,9 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="40"/>
-      <c r="B76" s="39">
-        <v>3</v>
-      </c>
-      <c r="C76" s="55">
-        <v>32</v>
-      </c>
-      <c r="D76" s="55">
-        <f t="shared" ref="D76:D83" si="1">FLOOR(C76/2,1)</f>
-        <v>16</v>
-      </c>
-      <c r="E76" s="55">
-        <v>10</v>
-      </c>
       <c r="F76" s="40"/>
       <c r="G76" s="40" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H76" s="40"/>
       <c r="I76" s="40"/>
@@ -6681,50 +6909,24 @@
       <c r="N76" s="40"/>
     </row>
     <row r="77" ht="15.75" spans="1:14">
-      <c r="A77" s="103"/>
-      <c r="B77" s="39">
-        <v>4</v>
-      </c>
-      <c r="C77" s="55">
-        <v>37</v>
-      </c>
-      <c r="D77" s="55">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="E77" s="55">
-        <v>12</v>
-      </c>
+      <c r="A77" s="119"/>
       <c r="F77" s="40"/>
-      <c r="G77" s="107" t="s">
-        <v>194</v>
-      </c>
-      <c r="H77" s="107"/>
-      <c r="I77" s="107"/>
-      <c r="J77" s="110"/>
-      <c r="K77" s="110"/>
-      <c r="L77" s="110"/>
+      <c r="G77" s="123" t="s">
+        <v>197</v>
+      </c>
+      <c r="H77" s="123"/>
+      <c r="I77" s="123"/>
+      <c r="J77" s="126"/>
+      <c r="K77" s="126"/>
+      <c r="L77" s="126"/>
       <c r="M77" s="40"/>
       <c r="N77" s="40"/>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="40"/>
-      <c r="B78" s="39">
-        <v>5</v>
-      </c>
-      <c r="C78" s="55">
-        <v>42</v>
-      </c>
-      <c r="D78" s="55">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="E78" s="55">
-        <v>14</v>
-      </c>
       <c r="F78" s="40"/>
       <c r="G78" s="40" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H78" s="40"/>
       <c r="I78" s="40"/>
@@ -6735,22 +6937,9 @@
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="40"/>
-      <c r="B79" s="39">
-        <v>6</v>
-      </c>
-      <c r="C79" s="55">
-        <v>47</v>
-      </c>
-      <c r="D79" s="55">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="E79" s="55">
-        <v>16</v>
-      </c>
       <c r="F79" s="40"/>
       <c r="G79" s="40" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="40"/>
@@ -6762,22 +6951,9 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="40"/>
-      <c r="B80" s="39">
-        <v>7</v>
-      </c>
-      <c r="C80" s="55">
-        <v>52</v>
-      </c>
-      <c r="D80" s="55">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="E80" s="55">
-        <v>18</v>
-      </c>
       <c r="F80" s="40"/>
       <c r="G80" s="40" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H80" s="40"/>
       <c r="I80" s="40"/>
@@ -6789,22 +6965,9 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="40"/>
-      <c r="B81" s="39">
-        <v>8</v>
-      </c>
-      <c r="C81" s="55">
-        <v>57</v>
-      </c>
-      <c r="D81" s="55">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="E81" s="55">
-        <v>20</v>
-      </c>
       <c r="F81" s="40"/>
       <c r="G81" s="40" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H81" s="40"/>
       <c r="I81" s="40"/>
@@ -6813,19 +6976,6 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="40"/>
-      <c r="B82" s="39">
-        <v>9</v>
-      </c>
-      <c r="C82" s="55">
-        <v>62</v>
-      </c>
-      <c r="D82" s="55">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="E82" s="55">
-        <v>22</v>
-      </c>
       <c r="F82" s="40"/>
       <c r="G82" s="40"/>
       <c r="H82" s="40"/>
@@ -6833,21 +6983,8 @@
       <c r="J82" s="40"/>
       <c r="K82" s="40"/>
     </row>
-    <row r="83" ht="15.75" spans="1:11">
+    <row r="83" spans="1:11">
       <c r="A83" s="40"/>
-      <c r="B83" s="44">
-        <v>10</v>
-      </c>
-      <c r="C83" s="43">
-        <v>67</v>
-      </c>
-      <c r="D83" s="43">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="E83" s="43">
-        <v>24</v>
-      </c>
       <c r="F83" s="40"/>
       <c r="G83" s="40"/>
       <c r="H83" s="40"/>
@@ -6857,12 +6994,8 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="40"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="40"/>
-      <c r="F84" s="40"/>
-      <c r="G84" s="40"/>
+      <c r="F84" s="106"/>
+      <c r="G84" s="106"/>
       <c r="H84" s="40">
         <v>5</v>
       </c>
@@ -6872,32 +7005,15 @@
       <c r="J84" s="40"/>
       <c r="K84" s="40"/>
     </row>
-    <row r="85" spans="2:11">
-      <c r="B85" s="108"/>
-      <c r="C85" s="108"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="40"/>
+    <row r="85" spans="6:11">
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
-      <c r="H85" s="102"/>
+      <c r="H85" s="118"/>
       <c r="I85" s="40"/>
       <c r="J85" s="40"/>
       <c r="K85" s="40"/>
     </row>
-    <row r="86" spans="2:11">
-      <c r="B86" s="64" t="s">
-        <v>190</v>
-      </c>
-      <c r="C86" s="64">
-        <v>16</v>
-      </c>
-      <c r="D86" s="40">
-        <v>8</v>
-      </c>
-      <c r="E86" s="40">
-        <f>C86+2*D86</f>
-        <v>32</v>
-      </c>
+    <row r="86" spans="6:11">
       <c r="F86" s="40"/>
       <c r="G86" s="40"/>
       <c r="H86" s="40"/>
@@ -6905,20 +7021,7 @@
       <c r="J86" s="40"/>
       <c r="K86" s="40"/>
     </row>
-    <row r="87" spans="2:11">
-      <c r="B87" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="C87" s="40">
-        <v>18</v>
-      </c>
-      <c r="D87" s="40">
-        <v>7</v>
-      </c>
-      <c r="E87" s="40">
-        <f>C87+2*D87</f>
-        <v>32</v>
-      </c>
+    <row r="87" spans="6:11">
       <c r="F87" s="40"/>
       <c r="G87" s="40"/>
       <c r="H87" s="40"/>
@@ -6926,60 +7029,21 @@
       <c r="J87" s="40"/>
       <c r="K87" s="40"/>
     </row>
-    <row r="88" spans="2:11">
-      <c r="B88" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="C88" s="40">
-        <v>21</v>
-      </c>
-      <c r="D88" s="40">
-        <v>5</v>
-      </c>
-      <c r="E88" s="40">
-        <f t="shared" ref="E88:E94" si="2">C88+2*D88</f>
-        <v>31</v>
-      </c>
+    <row r="88" spans="6:11">
       <c r="F88" s="40"/>
       <c r="H88" s="40"/>
       <c r="I88" s="40"/>
       <c r="J88" s="40"/>
       <c r="K88" s="40"/>
     </row>
-    <row r="89" spans="2:11">
-      <c r="B89" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="C89" s="40">
-        <v>22</v>
-      </c>
-      <c r="D89" s="40">
-        <v>5</v>
-      </c>
-      <c r="E89" s="40">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
+    <row r="89" spans="6:11">
       <c r="F89" s="40"/>
       <c r="H89" s="40"/>
       <c r="I89" s="40"/>
       <c r="J89" s="40"/>
       <c r="K89" s="40"/>
     </row>
-    <row r="90" spans="2:11">
-      <c r="B90" s="107" t="s">
-        <v>194</v>
-      </c>
-      <c r="C90" s="107">
-        <v>16</v>
-      </c>
-      <c r="D90" s="40">
-        <v>8</v>
-      </c>
-      <c r="E90" s="40">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
+    <row r="90" spans="6:11">
       <c r="F90" s="40"/>
       <c r="G90" s="40"/>
       <c r="H90" s="40"/>
@@ -6987,20 +7051,7 @@
       <c r="J90" s="40"/>
       <c r="K90" s="40"/>
     </row>
-    <row r="91" spans="2:11">
-      <c r="B91" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C91" s="40">
-        <v>14</v>
-      </c>
-      <c r="D91" s="40">
-        <v>9</v>
-      </c>
-      <c r="E91" s="40">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
+    <row r="91" spans="6:11">
       <c r="F91" s="40"/>
       <c r="G91" s="40"/>
       <c r="H91" s="40"/>
@@ -7008,20 +7059,7 @@
       <c r="J91" s="40"/>
       <c r="K91" s="40"/>
     </row>
-    <row r="92" spans="2:11">
-      <c r="B92" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C92" s="40">
-        <v>20</v>
-      </c>
-      <c r="D92" s="40">
-        <v>6</v>
-      </c>
-      <c r="E92" s="40">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
+    <row r="92" spans="6:11">
       <c r="F92" s="40"/>
       <c r="G92" s="40"/>
       <c r="H92" s="40"/>
@@ -7029,20 +7067,7 @@
       <c r="J92" s="40"/>
       <c r="K92" s="40"/>
     </row>
-    <row r="93" spans="2:11">
-      <c r="B93" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C93" s="40">
-        <v>17</v>
-      </c>
-      <c r="D93" s="40">
-        <v>4</v>
-      </c>
-      <c r="E93" s="40">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
+    <row r="93" spans="6:11">
       <c r="F93" s="40"/>
       <c r="G93" s="40"/>
       <c r="H93" s="40"/>
@@ -7050,21 +7075,8 @@
       <c r="J93" s="40"/>
       <c r="K93" s="40"/>
     </row>
-    <row r="94" spans="2:11">
-      <c r="B94" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="C94" s="40">
-        <v>26</v>
-      </c>
-      <c r="D94" s="40">
-        <v>3</v>
-      </c>
-      <c r="E94" s="40">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="F94" s="100"/>
+    <row r="94" spans="6:11">
+      <c r="F94" s="124"/>
       <c r="G94" s="40"/>
       <c r="H94" s="40"/>
       <c r="I94" s="40"/>
@@ -7073,8 +7085,14 @@
     </row>
     <row r="95" spans="2:11">
       <c r="B95" s="40"/>
-      <c r="C95" s="40"/>
-      <c r="D95" s="40"/>
+      <c r="C95" s="40">
+        <f>AVERAGE(H53:H61)</f>
+        <v>18.8888888888889</v>
+      </c>
+      <c r="D95" s="40">
+        <f>AVERAGE(I53:I61)</f>
+        <v>6.11111111111111</v>
+      </c>
       <c r="E95" s="40"/>
       <c r="F95" s="40"/>
       <c r="G95" s="40"/>
@@ -7095,7 +7113,7 @@
       <c r="C97" s="40"/>
       <c r="D97" s="40"/>
       <c r="E97" s="40"/>
-      <c r="F97" s="100"/>
+      <c r="F97" s="124"/>
       <c r="G97" s="40"/>
       <c r="H97" s="40"/>
       <c r="I97" s="40"/>
@@ -7140,7 +7158,7 @@
       <c r="C102" s="40"/>
       <c r="D102" s="40"/>
       <c r="E102" s="40"/>
-      <c r="F102" s="109"/>
+      <c r="F102" s="125"/>
     </row>
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
@@ -7197,7 +7215,7 @@
       <c r="F111" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="M3:N3"/>
@@ -7212,7 +7230,6 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="K74:L74"/>
     <mergeCell ref="K75:L75"/>
-    <mergeCell ref="D84:G84"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -7225,7 +7242,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="18.75"/>
@@ -7244,31 +7261,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7276,28 +7293,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7305,28 +7322,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7334,28 +7351,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7363,28 +7380,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7392,28 +7409,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7421,28 +7438,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7450,28 +7467,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7479,28 +7496,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7508,28 +7525,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7537,28 +7554,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7566,28 +7583,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -7595,28 +7612,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" ht="19.5" spans="1:9">
@@ -7624,33 +7641,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" ht="19.5" spans="1:9">
       <c r="A15" s="8" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>4</v>
@@ -7682,34 +7699,34 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7717,31 +7734,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7749,31 +7766,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7781,31 +7798,31 @@
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7813,31 +7830,31 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7845,31 +7862,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7877,31 +7894,31 @@
         <v>5</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7909,31 +7926,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7941,31 +7958,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7973,31 +7990,31 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8005,31 +8022,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8037,31 +8054,31 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8069,31 +8086,31 @@
         <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8101,63 +8118,63 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="8" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP level 10 talents.
</commit_message>
<xml_diff>
--- a/Design/Tables.xlsx
+++ b/Design/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13545" windowHeight="11730" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2685,7 +2685,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2980,18 +2980,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3013,33 +3001,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3061,9 +3028,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3071,12 +3035,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3549,7 +3507,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="102" t="s">
+      <c r="L7" s="98" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -3565,10 +3523,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="102" t="s">
+      <c r="L8" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="102"/>
+      <c r="M8" s="98"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -3601,13 +3559,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="121" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="136" t="s">
+      <c r="C10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -3619,7 +3577,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="136" t="s">
+      <c r="G10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -3630,13 +3588,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="121" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -3648,7 +3606,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="136" t="s">
+      <c r="G11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -3659,13 +3617,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="123" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -3677,7 +3635,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="138" t="s">
+      <c r="G12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -3962,8 +3920,8 @@
       <c r="H27" s="81"/>
       <c r="I27" s="81"/>
       <c r="J27" s="82"/>
-      <c r="K27" s="104"/>
-      <c r="L27" s="104"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -3972,10 +3930,10 @@
       <c r="B28" s="40">
         <v>0</v>
       </c>
-      <c r="C28" s="127" t="s">
+      <c r="C28" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="128"/>
+      <c r="D28" s="116"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -4076,7 +4034,7 @@
       <c r="H32" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="134"/>
+      <c r="J32" s="120"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="44">
@@ -4111,20 +4069,20 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:14">
-      <c r="A34" s="129" t="s">
+      <c r="A34" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="130">
+      <c r="B34" s="104">
         <v>1</v>
       </c>
-      <c r="C34" s="131"/>
-      <c r="D34" s="131"/>
-      <c r="E34" s="131"/>
-      <c r="F34" s="131"/>
-      <c r="G34" s="131"/>
-      <c r="H34" s="131"/>
-      <c r="I34" s="131"/>
-      <c r="J34" s="130"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="104"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -4223,17 +4181,17 @@
       <c r="E40" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="132" t="s">
+      <c r="F40" s="118" t="s">
         <v>87</v>
       </c>
       <c r="G40" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="139" t="s">
+      <c r="I40" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="105"/>
-      <c r="K40" s="105"/>
+      <c r="J40" s="101"/>
+      <c r="K40" s="101"/>
     </row>
     <row r="41" ht="15.75" spans="1:11">
       <c r="A41" s="72"/>
@@ -4255,7 +4213,7 @@
       <c r="G41" s="93">
         <v>10</v>
       </c>
-      <c r="I41" s="140" t="s">
+      <c r="I41" s="126" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="40"/>
@@ -4728,11 +4686,11 @@
       <c r="I61" s="40"/>
     </row>
     <row r="62" ht="75" spans="3:9">
-      <c r="C62" s="133" t="s">
+      <c r="C62" s="119" t="s">
         <v>138</v>
       </c>
       <c r="E62" s="40"/>
-      <c r="F62" s="133" t="s">
+      <c r="F62" s="119" t="s">
         <v>139</v>
       </c>
       <c r="G62" s="40"/>
@@ -4751,7 +4709,7 @@
         <f>20+6*9</f>
         <v>74</v>
       </c>
-      <c r="E64" s="118" t="s">
+      <c r="E64" s="107" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="40"/>
@@ -4798,7 +4756,7 @@
       <c r="I69" s="40"/>
     </row>
     <row r="70" ht="102" customHeight="1" spans="3:9">
-      <c r="C70" s="133" t="s">
+      <c r="C70" s="119" t="s">
         <v>142</v>
       </c>
       <c r="E70" s="40"/>
@@ -4815,10 +4773,10 @@
       <c r="I71" s="40"/>
     </row>
     <row r="72" ht="15.75" spans="1:14">
-      <c r="A72" s="119"/>
-      <c r="B72" s="120"/>
-      <c r="C72" s="121"/>
-      <c r="D72" s="121"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="110"/>
+      <c r="D72" s="110"/>
       <c r="E72" s="58"/>
       <c r="F72" s="58" t="s">
         <v>143</v>
@@ -4923,7 +4881,7 @@
       <c r="C77" s="40">
         <v>30</v>
       </c>
-      <c r="D77" s="141" t="s">
+      <c r="D77" s="127" t="s">
         <v>150</v>
       </c>
       <c r="E77" s="40"/>
@@ -4941,7 +4899,7 @@
       <c r="N77" s="40"/>
     </row>
     <row r="78" ht="15.75" spans="1:14">
-      <c r="A78" s="119"/>
+      <c r="A78" s="108"/>
       <c r="B78" s="40">
         <v>4</v>
       </c>
@@ -4951,16 +4909,16 @@
       <c r="D78" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="126"/>
+      <c r="E78" s="114"/>
       <c r="F78" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="126"/>
-      <c r="H78" s="126"/>
-      <c r="I78" s="126"/>
-      <c r="J78" s="126"/>
-      <c r="K78" s="126"/>
-      <c r="L78" s="126"/>
+      <c r="G78" s="114"/>
+      <c r="H78" s="114"/>
+      <c r="I78" s="114"/>
+      <c r="J78" s="114"/>
+      <c r="K78" s="114"/>
+      <c r="L78" s="114"/>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
     </row>
@@ -5017,7 +4975,7 @@
       <c r="C81" s="40">
         <v>50</v>
       </c>
-      <c r="D81" s="141" t="s">
+      <c r="D81" s="127" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="40"/>
@@ -5290,8 +5248,8 @@
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>
       <c r="D103" s="40"/>
-      <c r="E103" s="125"/>
-      <c r="F103" s="125"/>
+      <c r="E103" s="106"/>
+      <c r="F103" s="106"/>
     </row>
     <row r="104" spans="3:6">
       <c r="C104" s="40"/>
@@ -5376,7 +5334,7 @@
   <dimension ref="A2:N111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15238095238095" defaultRowHeight="15"/>
@@ -5482,7 +5440,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="L7" s="102" t="s">
+      <c r="L7" s="98" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="58" t="s">
@@ -5498,10 +5456,10 @@
       <c r="E8" s="31"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
-      <c r="L8" s="102" t="s">
+      <c r="L8" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="102"/>
+      <c r="M8" s="98"/>
       <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:9">
@@ -5534,13 +5492,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="121" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39">
         <v>5.5</v>
       </c>
-      <c r="C10" s="136" t="s">
+      <c r="C10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="40">
@@ -5552,7 +5510,7 @@
       <c r="F10" s="42">
         <v>10.5</v>
       </c>
-      <c r="G10" s="136" t="s">
+      <c r="G10" s="122" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="40">
@@ -5563,13 +5521,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="121" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>5.5</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="40">
@@ -5581,7 +5539,7 @@
       <c r="F11" s="42">
         <v>10.5</v>
       </c>
-      <c r="G11" s="136" t="s">
+      <c r="G11" s="122" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40">
@@ -5592,13 +5550,13 @@
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:9">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="123" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="44">
         <v>5.5</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="45">
@@ -5610,7 +5568,7 @@
       <c r="F12" s="47">
         <v>10.5</v>
       </c>
-      <c r="G12" s="138" t="s">
+      <c r="G12" s="124" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="45">
@@ -5757,12 +5715,10 @@
       <c r="F20" s="63">
         <v>-1</v>
       </c>
-      <c r="G20">
-        <v>12</v>
-      </c>
+      <c r="G20"/>
       <c r="H20" s="57">
-        <f>6.5+4</f>
-        <v>10.5</v>
+        <f>5.5*3</f>
+        <v>16.5</v>
       </c>
       <c r="J20" s="73"/>
       <c r="K20" s="70">
@@ -5878,7 +5834,7 @@
       <c r="H25" s="40"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
-      <c r="K25" s="103">
+      <c r="K25" s="99">
         <f>46/9</f>
         <v>5.11111111111111</v>
       </c>
@@ -5907,8 +5863,8 @@
       <c r="D27" s="81"/>
       <c r="E27" s="81"/>
       <c r="F27" s="82"/>
-      <c r="K27" s="104"/>
-      <c r="L27" s="104"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="39">
@@ -6083,7 +6039,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="39" ht="15.75" spans="1:11">
+    <row r="39" ht="16.5" spans="1:11">
       <c r="A39" s="72"/>
       <c r="B39" s="74" t="s">
         <v>83</v>
@@ -6103,7 +6059,7 @@
       </c>
       <c r="I39" s="40"/>
       <c r="J39" s="40"/>
-      <c r="K39" s="105"/>
+      <c r="K39" s="101"/>
     </row>
     <row r="40" ht="15.75" spans="1:11">
       <c r="A40" s="72"/>
@@ -6378,7 +6334,7 @@
       </c>
       <c r="K49" s="58"/>
     </row>
-    <row r="50" ht="15.75" spans="2:11">
+    <row r="50" ht="16.5" spans="2:11">
       <c r="B50" s="39">
         <v>275</v>
       </c>
@@ -6405,7 +6361,7 @@
       </c>
       <c r="K50" s="58"/>
     </row>
-    <row r="51" ht="15.75" spans="1:13">
+    <row r="51" ht="16.5" spans="1:13">
       <c r="A51" s="94" t="s">
         <v>115</v>
       </c>
@@ -6426,12 +6382,12 @@
       </c>
       <c r="G51" s="40"/>
       <c r="H51" s="40"/>
-      <c r="I51" s="106"/>
-      <c r="J51" s="106"/>
+      <c r="I51" s="102"/>
+      <c r="J51" s="102"/>
       <c r="K51" s="70"/>
       <c r="M51" s="58"/>
     </row>
-    <row r="52" ht="15.75" spans="1:13">
+    <row r="52" ht="16.5" spans="1:13">
       <c r="A52" s="94" t="s">
         <v>117</v>
       </c>
@@ -6453,10 +6409,10 @@
       <c r="H52" s="96" t="s">
         <v>190</v>
       </c>
-      <c r="I52" s="107" t="s">
+      <c r="I52" s="103" t="s">
         <v>191</v>
       </c>
-      <c r="J52" s="108" t="s">
+      <c r="J52" s="104" t="s">
         <v>192</v>
       </c>
       <c r="M52" s="58"/>
@@ -6483,10 +6439,10 @@
       <c r="H53" s="97">
         <v>16</v>
       </c>
-      <c r="I53" s="109">
+      <c r="I53" s="50">
         <v>8</v>
       </c>
-      <c r="J53" s="110">
+      <c r="J53" s="83">
         <f>H53+2*I53</f>
         <v>32</v>
       </c>
@@ -6499,7 +6455,7 @@
       <c r="B54" s="65">
         <v>375</v>
       </c>
-      <c r="C54" s="98">
+      <c r="C54" s="45">
         <v>80</v>
       </c>
       <c r="D54" s="45">
@@ -6508,16 +6464,16 @@
       <c r="E54" s="46">
         <v>12</v>
       </c>
-      <c r="G54" s="99" t="s">
+      <c r="G54" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="H54" s="99">
+      <c r="H54" s="39">
         <v>18</v>
       </c>
-      <c r="I54" s="111">
+      <c r="I54" s="55">
         <v>7</v>
       </c>
-      <c r="J54" s="112">
+      <c r="J54" s="41">
         <f>H54+2*I54</f>
         <v>32</v>
       </c>
@@ -6535,16 +6491,16 @@
       <c r="E55" s="41">
         <v>12</v>
       </c>
-      <c r="G55" s="99" t="s">
+      <c r="G55" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="H55" s="99">
+      <c r="H55" s="39">
         <v>21</v>
       </c>
-      <c r="I55" s="111">
+      <c r="I55" s="55">
         <v>5</v>
       </c>
-      <c r="J55" s="112">
+      <c r="J55" s="41">
         <f t="shared" ref="J55:J61" si="0">H55+2*I55</f>
         <v>31</v>
       </c>
@@ -6562,16 +6518,16 @@
       <c r="E56" s="41">
         <v>12</v>
       </c>
-      <c r="G56" s="99" t="s">
+      <c r="G56" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="H56" s="99">
+      <c r="H56" s="39">
         <v>22</v>
       </c>
-      <c r="I56" s="111">
+      <c r="I56" s="55">
         <v>5</v>
       </c>
-      <c r="J56" s="112">
+      <c r="J56" s="41">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6589,16 +6545,16 @@
       <c r="E57" s="41">
         <v>12</v>
       </c>
-      <c r="G57" s="100" t="s">
+      <c r="G57" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="H57" s="100">
+      <c r="H57" s="42">
         <v>16</v>
       </c>
-      <c r="I57" s="111">
+      <c r="I57" s="55">
         <v>8</v>
       </c>
-      <c r="J57" s="112">
+      <c r="J57" s="41">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6616,16 +6572,16 @@
       <c r="E58" s="41">
         <v>12</v>
       </c>
-      <c r="G58" s="99" t="s">
+      <c r="G58" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="H58" s="99">
+      <c r="H58" s="39">
         <v>14</v>
       </c>
-      <c r="I58" s="111">
+      <c r="I58" s="55">
         <v>9</v>
       </c>
-      <c r="J58" s="112">
+      <c r="J58" s="41">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6643,16 +6599,16 @@
       <c r="E59" s="41">
         <v>12</v>
       </c>
-      <c r="G59" s="99" t="s">
+      <c r="G59" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="H59" s="99">
+      <c r="H59" s="39">
         <v>20</v>
       </c>
-      <c r="I59" s="111">
+      <c r="I59" s="55">
         <v>6</v>
       </c>
-      <c r="J59" s="112">
+      <c r="J59" s="41">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6668,21 +6624,21 @@
       <c r="E60" s="41">
         <v>13</v>
       </c>
-      <c r="G60" s="99" t="s">
+      <c r="G60" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="H60" s="99">
+      <c r="H60" s="39">
         <v>17</v>
       </c>
-      <c r="I60" s="111">
+      <c r="I60" s="55">
         <v>4</v>
       </c>
-      <c r="J60" s="112">
+      <c r="J60" s="41">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="61" ht="15.75" spans="2:10">
+    <row r="61" ht="16.5" spans="2:10">
       <c r="B61" s="52">
         <v>750</v>
       </c>
@@ -6693,16 +6649,16 @@
       <c r="E61" s="41">
         <v>13</v>
       </c>
-      <c r="G61" s="101" t="s">
+      <c r="G61" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="H61" s="101">
+      <c r="H61" s="44">
         <v>26</v>
       </c>
-      <c r="I61" s="113">
+      <c r="I61" s="43">
         <v>3</v>
       </c>
-      <c r="J61" s="114">
+      <c r="J61" s="46">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6736,17 +6692,17 @@
         <f>147*2*0.8</f>
         <v>235.2</v>
       </c>
-      <c r="C65" s="115" t="s">
+      <c r="C65" s="105" t="s">
         <v>202</v>
       </c>
-      <c r="D65" s="115" t="s">
+      <c r="D65" s="105" t="s">
         <v>203</v>
       </c>
-      <c r="E65" s="115" t="s">
+      <c r="E65" s="105" t="s">
         <v>204</v>
       </c>
       <c r="G65" s="40"/>
-      <c r="H65" s="116" t="s">
+      <c r="H65" s="106" t="s">
         <v>205</v>
       </c>
       <c r="I65" t="s">
@@ -6755,13 +6711,13 @@
       <c r="J65" s="58"/>
     </row>
     <row r="66" ht="90.75" spans="3:10">
-      <c r="C66" s="115" t="s">
+      <c r="C66" s="105" t="s">
         <v>207</v>
       </c>
       <c r="E66" s="40"/>
       <c r="F66" s="40"/>
       <c r="G66" s="40"/>
-      <c r="H66" s="117" t="s">
+      <c r="H66" s="40" t="s">
         <v>208</v>
       </c>
       <c r="I66" t="s">
@@ -6772,10 +6728,10 @@
       </c>
     </row>
     <row r="67" spans="5:10">
-      <c r="E67" s="118"/>
+      <c r="E67" s="107"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
-      <c r="H67" s="117" t="s">
+      <c r="H67" s="40" t="s">
         <v>208</v>
       </c>
       <c r="I67" t="s">
@@ -6790,7 +6746,7 @@
       <c r="E68" s="40"/>
       <c r="F68" s="40"/>
       <c r="G68" s="40"/>
-      <c r="H68" s="117" t="s">
+      <c r="H68" s="40" t="s">
         <v>208</v>
       </c>
       <c r="I68" t="s">
@@ -6804,10 +6760,10 @@
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
       <c r="G69" s="40"/>
-      <c r="H69" s="117" t="s">
+      <c r="H69" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="I69" s="125" t="s">
+      <c r="I69" s="106" t="s">
         <v>215</v>
       </c>
       <c r="J69" s="40" t="s">
@@ -6818,10 +6774,10 @@
       <c r="E70" s="40"/>
       <c r="F70" s="40"/>
       <c r="G70" s="40"/>
-      <c r="H70" s="117" t="s">
+      <c r="H70" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="I70" s="125" t="s">
+      <c r="I70" s="106" t="s">
         <v>217</v>
       </c>
       <c r="J70" s="40" t="s">
@@ -6829,10 +6785,10 @@
       </c>
     </row>
     <row r="71" ht="15.75" spans="1:14">
-      <c r="A71" s="119"/>
-      <c r="B71" s="120"/>
-      <c r="C71" s="121"/>
-      <c r="D71" s="121"/>
+      <c r="A71" s="108"/>
+      <c r="B71" s="109"/>
+      <c r="C71" s="110"/>
+      <c r="D71" s="110"/>
       <c r="E71" s="58"/>
       <c r="F71" s="58"/>
       <c r="G71" s="58"/>
@@ -6857,11 +6813,11 @@
     <row r="73" spans="1:14">
       <c r="A73" s="40"/>
       <c r="F73" s="40"/>
-      <c r="G73" s="122" t="s">
+      <c r="G73" s="111" t="s">
         <v>193</v>
       </c>
-      <c r="H73" s="122"/>
-      <c r="I73" s="122"/>
+      <c r="H73" s="111"/>
+      <c r="I73" s="111"/>
       <c r="J73" s="40"/>
       <c r="K73" s="40"/>
       <c r="M73" s="40"/>
@@ -6909,16 +6865,16 @@
       <c r="N76" s="40"/>
     </row>
     <row r="77" ht="15.75" spans="1:14">
-      <c r="A77" s="119"/>
+      <c r="A77" s="108"/>
       <c r="F77" s="40"/>
-      <c r="G77" s="123" t="s">
+      <c r="G77" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="H77" s="123"/>
-      <c r="I77" s="123"/>
-      <c r="J77" s="126"/>
-      <c r="K77" s="126"/>
-      <c r="L77" s="126"/>
+      <c r="H77" s="112"/>
+      <c r="I77" s="112"/>
+      <c r="J77" s="114"/>
+      <c r="K77" s="114"/>
+      <c r="L77" s="114"/>
       <c r="M77" s="40"/>
       <c r="N77" s="40"/>
     </row>
@@ -6994,8 +6950,8 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="40"/>
-      <c r="F84" s="106"/>
-      <c r="G84" s="106"/>
+      <c r="F84" s="102"/>
+      <c r="G84" s="102"/>
       <c r="H84" s="40">
         <v>5</v>
       </c>
@@ -7008,7 +6964,7 @@
     <row r="85" spans="6:11">
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
-      <c r="H85" s="118"/>
+      <c r="H85" s="107"/>
       <c r="I85" s="40"/>
       <c r="J85" s="40"/>
       <c r="K85" s="40"/>
@@ -7076,7 +7032,7 @@
       <c r="K93" s="40"/>
     </row>
     <row r="94" spans="6:11">
-      <c r="F94" s="124"/>
+      <c r="F94" s="113"/>
       <c r="G94" s="40"/>
       <c r="H94" s="40"/>
       <c r="I94" s="40"/>
@@ -7113,7 +7069,7 @@
       <c r="C97" s="40"/>
       <c r="D97" s="40"/>
       <c r="E97" s="40"/>
-      <c r="F97" s="124"/>
+      <c r="F97" s="113"/>
       <c r="G97" s="40"/>
       <c r="H97" s="40"/>
       <c r="I97" s="40"/>
@@ -7158,7 +7114,7 @@
       <c r="C102" s="40"/>
       <c r="D102" s="40"/>
       <c r="E102" s="40"/>
-      <c r="F102" s="125"/>
+      <c r="F102" s="106"/>
     </row>
     <row r="103" spans="3:6">
       <c r="C103" s="40"/>

</xml_diff>